<commit_message>
Enhance charlson_icd10 with RCS version. See #44.
</commit_message>
<xml_diff>
--- a/data-raw/classcodes.xlsx
+++ b/data-raw/classcodes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="charlson_icd10" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="131">
   <si>
     <t>group</t>
   </si>
@@ -376,6 +376,49 @@
   </si>
   <si>
     <t>^F(204|3(1[345]|[23]|41)|4[13]2)</t>
+  </si>
+  <si>
+    <t>regex_rcs</t>
+  </si>
+  <si>
+    <t>^I2([1-3]|52)</t>
+  </si>
+  <si>
+    <t>^I(1[13]|255|4[23]|5(0|17))</t>
+  </si>
+  <si>
+    <t>^((I7([0-3]|7[01]))|K55[189]|R02|Z95[89])</t>
+  </si>
+  <si>
+    <t>^(G4[56]|I6)</t>
+  </si>
+  <si>
+    <t>^(A810|F0([0-3]|51)|G3[01])</t>
+  </si>
+  <si>
+    <t>^Not included by RCS$</t>
+  </si>
+  <si>
+    <t>^Grouped with other liver disease$</t>
+  </si>
+  <si>
+    <t>^Grouped with other diabetes$</t>
+  </si>
+  <si>
+    <t>^G(114|8[1-3])</t>
+  </si>
+  <si>
+    <t>^(I1[23]|N(0[13578]|17[12]|1[89]|25)|Z(49|9(40|92)))</t>
+  </si>
+  <si>
+    <t>^E1[0-4]</t>
+  </si>
+  <si>
+    <t>^B2[0-4]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">^(B18|I(8(5|64)|982)|K7([016]|2[19])|R162|Z944)
+</t>
   </si>
 </sst>
 </file>
@@ -419,12 +462,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -707,26 +753,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMJ18"/>
+  <dimension ref="A1:AMK18"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.42578125" customWidth="1"/>
-    <col min="2" max="3" width="55.7109375" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" customWidth="1"/>
-    <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1"/>
-    <col min="10" max="1025" width="8.5703125" customWidth="1"/>
+    <col min="2" max="2" width="55.7109375" customWidth="1"/>
+    <col min="3" max="3" width="61.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.7109375" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" customWidth="1"/>
+    <col min="7" max="7" width="11" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" customWidth="1"/>
+    <col min="11" max="1026" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10 1025:1025" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -737,26 +785,29 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="AMJ1"/>
-    </row>
-    <row r="2" spans="1:1024" x14ac:dyDescent="0.25">
+      <c r="AMK1"/>
+    </row>
+    <row r="2" spans="1:10 1025:1025" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -766,8 +817,8 @@
       <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="D2">
-        <v>1</v>
+      <c r="D2" t="s">
+        <v>118</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -782,10 +833,13 @@
         <v>1</v>
       </c>
       <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1024" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10 1025:1025" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -795,8 +849,8 @@
       <c r="C3" t="s">
         <v>14</v>
       </c>
-      <c r="D3">
-        <v>1</v>
+      <c r="D3" t="s">
+        <v>119</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -805,16 +859,19 @@
         <v>1</v>
       </c>
       <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
         <v>4</v>
       </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
       <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1024" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10 1025:1025" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -824,8 +881,8 @@
       <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="D4">
-        <v>1</v>
+      <c r="D4" t="s">
+        <v>120</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -834,16 +891,19 @@
         <v>1</v>
       </c>
       <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
         <v>2</v>
       </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
       <c r="I4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1024" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10 1025:1025" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -853,8 +913,8 @@
       <c r="C5" t="s">
         <v>20</v>
       </c>
-      <c r="D5">
-        <v>1</v>
+      <c r="D5" t="s">
+        <v>121</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -869,10 +929,13 @@
         <v>1</v>
       </c>
       <c r="I5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1024" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10 1025:1025" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -882,8 +945,8 @@
       <c r="C6" t="s">
         <v>23</v>
       </c>
-      <c r="D6">
-        <v>1</v>
+      <c r="D6" t="s">
+        <v>122</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -892,16 +955,19 @@
         <v>1</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:1024" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10 1025:1025" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -911,8 +977,8 @@
       <c r="C7" t="s">
         <v>26</v>
       </c>
-      <c r="D7">
-        <v>1</v>
+      <c r="D7" t="s">
+        <v>26</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -921,16 +987,19 @@
         <v>1</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:1024" ht="45" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10 1025:1025" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -940,8 +1009,8 @@
       <c r="C8" t="s">
         <v>29</v>
       </c>
-      <c r="D8">
-        <v>1</v>
+      <c r="D8" t="s">
+        <v>29</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -950,16 +1019,19 @@
         <v>1</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:1024" ht="30" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10 1025:1025" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -969,8 +1041,8 @@
       <c r="C9" t="s">
         <v>32</v>
       </c>
-      <c r="D9">
-        <v>1</v>
+      <c r="D9" t="s">
+        <v>123</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -979,16 +1051,19 @@
         <v>1</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1024" ht="30" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10 1025:1025" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -998,8 +1073,8 @@
       <c r="C10" t="s">
         <v>35</v>
       </c>
-      <c r="D10">
-        <v>1</v>
+      <c r="D10" t="s">
+        <v>124</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -1008,16 +1083,19 @@
         <v>1</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:1024" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10 1025:1025" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -1027,8 +1105,8 @@
       <c r="C11" t="s">
         <v>38</v>
       </c>
-      <c r="D11">
-        <v>1</v>
+      <c r="D11" t="s">
+        <v>125</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -1037,16 +1115,19 @@
         <v>1</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1024" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10 1025:1025" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -1056,26 +1137,29 @@
       <c r="C12" t="s">
         <v>41</v>
       </c>
-      <c r="D12">
+      <c r="D12" t="s">
+        <v>126</v>
+      </c>
+      <c r="E12">
         <v>2</v>
       </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
       <c r="F12">
         <v>1</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I12">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:1024" ht="45" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10 1025:1025" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -1085,26 +1169,29 @@
       <c r="C13" t="s">
         <v>44</v>
       </c>
-      <c r="D13">
+      <c r="D13" t="s">
+        <v>127</v>
+      </c>
+      <c r="E13">
         <v>2</v>
       </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
       <c r="F13">
         <v>1</v>
       </c>
       <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
         <v>3</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>2</v>
       </c>
-      <c r="I13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1024" ht="30" x14ac:dyDescent="0.25">
+      <c r="J13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10 1025:1025" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -1114,26 +1201,29 @@
       <c r="C14" t="s">
         <v>47</v>
       </c>
-      <c r="D14">
+      <c r="D14" t="s">
+        <v>128</v>
+      </c>
+      <c r="E14">
         <v>2</v>
       </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
       <c r="F14">
         <v>1</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
         <v>2</v>
       </c>
-      <c r="I14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1024" ht="30" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10 1025:1025" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -1143,26 +1233,29 @@
       <c r="C15" t="s">
         <v>50</v>
       </c>
-      <c r="D15">
+      <c r="D15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15">
         <v>2</v>
       </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
       <c r="F15">
         <v>1</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I15">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:1024" ht="30" x14ac:dyDescent="0.25">
+      <c r="J15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10 1025:1025" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -1172,26 +1265,29 @@
       <c r="C16" t="s">
         <v>53</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E16">
         <v>3</v>
       </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
       <c r="F16">
         <v>1</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
         <v>3</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>54</v>
       </c>
@@ -1201,26 +1297,29 @@
       <c r="C17" t="s">
         <v>56</v>
       </c>
-      <c r="D17">
+      <c r="D17" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17">
         <v>6</v>
       </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
       <c r="F17">
         <v>1</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I17">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>57</v>
       </c>
@@ -1230,22 +1329,25 @@
       <c r="C18" t="s">
         <v>59</v>
       </c>
-      <c r="D18">
+      <c r="D18" t="s">
+        <v>129</v>
+      </c>
+      <c r="E18">
         <v>6</v>
       </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
       <c r="F18">
         <v>1</v>
       </c>
       <c r="G18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
         <v>6</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>4</v>
       </c>
     </row>
@@ -1259,8 +1361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fix #34. Updated classcodes for adverse events.
</commit_message>
<xml_diff>
--- a/data-raw/classcodes.xlsx
+++ b/data-raw/classcodes.xlsx
@@ -9,23 +9,22 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="charlson_icd10" sheetId="1" r:id="rId1"/>
     <sheet name="elix_icd10" sheetId="2" r:id="rId2"/>
+    <sheet name="hip.ae_icd10" sheetId="3" r:id="rId3"/>
+    <sheet name="hip.ae_kva" sheetId="4" r:id="rId4"/>
+    <sheet name="knee.ae_icd10" sheetId="5" r:id="rId5"/>
+    <sheet name="knee.ae_kva" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="159">
   <si>
     <t>group</t>
   </si>
@@ -428,13 +427,88 @@
   </si>
   <si>
     <t>ahrq_readm</t>
+  </si>
+  <si>
+    <t>condition</t>
+  </si>
+  <si>
+    <t>DA surgical complications</t>
+  </si>
+  <si>
+    <t>DB1 hip related</t>
+  </si>
+  <si>
+    <t>DB2 hip related</t>
+  </si>
+  <si>
+    <t>DC CVD</t>
+  </si>
+  <si>
+    <t>DM1 other</t>
+  </si>
+  <si>
+    <t>DM2 other</t>
+  </si>
+  <si>
+    <t>hbdia1_hdia</t>
+  </si>
+  <si>
+    <t>late_hdia</t>
+  </si>
+  <si>
+    <t>^(G(97[89])|M96(6F|[89])|(T8((1([02-9]|8W))|(4([03578]F?)|[49])|(8[89]))))$</t>
+  </si>
+  <si>
+    <t>^(G57[0-2]|M((00(0F?|[289]F))|(24(3|4F?)))|S7([4-6][0-9]{0,2}|30))$</t>
+  </si>
+  <si>
+    <t>^(M(24[056]F|6(10|21|6[23])F|8((43|6[01])F|66F?|95E)))$</t>
+  </si>
+  <si>
+    <t>^(I((2([14][[:alnum:]]*|6[09]))|4(6[019]|90)|6([0-35-6]|49)|7([24]|7[0-2]))|J8[01]9)|T811$</t>
+  </si>
+  <si>
+    <t>^(I80[[:alnum:]]*|J((1[3-8][[:alnum:]]*)|9(5[23589]|6[[:alnum:]]*|81))|K2[5-7][[:alnum:]]*|L89[[:alnum:]]*|N(99[089]|(17[[:alnum:]]*))|R339)$</t>
+  </si>
+  <si>
+    <t>^NF([CF-HJ-MS-TW]\\d{2}|A(02|1[12]|2[0-2])|Q09|U[013489]9)|QD(A10|B(0[05]|99)|E35|G30)|TNF(05|10)$</t>
+  </si>
+  <si>
+    <t>post_op</t>
+  </si>
+  <si>
+    <t>knee ae kva</t>
+  </si>
+  <si>
+    <t>hip ae kva</t>
+  </si>
+  <si>
+    <t>^(N(FQ[019]9|G([ACEGHJLSUW]|B59|F(0[12]|1[0-2]|9[12])|K[01]9|[MQ]09|T[01]9))|QD(A10|B[^1]|E35|G)|TNG(05|10))</t>
+  </si>
+  <si>
+    <t>DB1 knee related</t>
+  </si>
+  <si>
+    <t>DB2 knee related</t>
+  </si>
+  <si>
+    <t>^(G(97[89])|M96(6G|[89])|(T8((1([02-9]|8W))|(4([03-578]G?)|9)|(8[89]))))$</t>
+  </si>
+  <si>
+    <t>^(G57[34]|M(24[34])|M(00(0G?|[289]G)|2(2[01]|36|44G)|6(21|6[23])G|843G)|S(342|724|8([01]0|2[01]|3([01]|4[LM]|5[RSX])|4[01])))$</t>
+  </si>
+  <si>
+    <t>^M(2(35|4[056]|56)|659G|8((6[01]G|6G?)|95G))$</t>
+  </si>
+  <si>
+    <t>^(J2[0-2][[:alnum:]]*|K(590|29[[:alnum:]]*)|N991)$</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -449,6 +523,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -468,10 +549,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -482,9 +564,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1370,7 +1454,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -2313,4 +2397,281 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="131.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>140</v>
+      </c>
+      <c r="B7" t="s">
+        <v>158</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="98.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="131.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>140</v>
+      </c>
+      <c r="B7" t="s">
+        <v>158</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="99.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
* Better documentation for AE (Fix #52). * AE fractture codes based on ordinary hip codes (Fix #55). * Moved all classcocdes into Excel-file (Fix #54).
</commit_message>
<xml_diff>
--- a/data-raw/classcodes.xlsx
+++ b/data-raw/classcodes.xlsx
@@ -9,22 +9,26 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="charlson_icd10" sheetId="1" r:id="rId1"/>
-    <sheet name="elix_icd10" sheetId="2" r:id="rId2"/>
-    <sheet name="hip.ae_icd10" sheetId="3" r:id="rId3"/>
-    <sheet name="hip.ae_kva" sheetId="4" r:id="rId4"/>
-    <sheet name="knee.ae_icd10" sheetId="5" r:id="rId5"/>
-    <sheet name="knee.ae_kva" sheetId="6" r:id="rId6"/>
+    <sheet name="ex.carbrands_excars" sheetId="10" r:id="rId1"/>
+    <sheet name="charlson_icd10" sheetId="1" r:id="rId2"/>
+    <sheet name="elix_icd10" sheetId="2" r:id="rId3"/>
+    <sheet name="hip.ae_icd10" sheetId="3" r:id="rId4"/>
+    <sheet name="hip.ae_kva" sheetId="4" r:id="rId5"/>
+    <sheet name="knee.ae_icd10" sheetId="5" r:id="rId6"/>
+    <sheet name="knee.ae_kva" sheetId="6" r:id="rId7"/>
+    <sheet name="rxriskv_atc" sheetId="7" r:id="rId8"/>
+    <sheet name="rxriskv.modified_atc" sheetId="8" r:id="rId9"/>
+    <sheet name="cps_icd10" sheetId="9" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="288">
   <si>
     <t>group</t>
   </si>
@@ -502,6 +506,393 @@
   </si>
   <si>
     <t>^(J2[0-2][[:alnum:]]*|K(590|29[[:alnum:]]*)|N991)$</t>
+  </si>
+  <si>
+    <t>alcoholdependence</t>
+  </si>
+  <si>
+    <t>allergies</t>
+  </si>
+  <si>
+    <t>anticoagulationtherapy</t>
+  </si>
+  <si>
+    <t>antiplatelettherapy</t>
+  </si>
+  <si>
+    <t>anxiety</t>
+  </si>
+  <si>
+    <t>arrhythmia</t>
+  </si>
+  <si>
+    <t>benignprostatehypertrophy</t>
+  </si>
+  <si>
+    <t>bipolardisorder</t>
+  </si>
+  <si>
+    <t>chronicheartfailure</t>
+  </si>
+  <si>
+    <t>diabetes</t>
+  </si>
+  <si>
+    <t>endstagerenaldisease</t>
+  </si>
+  <si>
+    <t>epilepsy</t>
+  </si>
+  <si>
+    <t>gastricoesophagealrefluxdisorder</t>
+  </si>
+  <si>
+    <t>glaucoma</t>
+  </si>
+  <si>
+    <t>gout</t>
+  </si>
+  <si>
+    <t>hepatitisC</t>
+  </si>
+  <si>
+    <t>HIV</t>
+  </si>
+  <si>
+    <t>hyperkalcemia</t>
+  </si>
+  <si>
+    <t>hyperlipidemia</t>
+  </si>
+  <si>
+    <t>hypertension</t>
+  </si>
+  <si>
+    <t>hyperthyroidism</t>
+  </si>
+  <si>
+    <t>angina</t>
+  </si>
+  <si>
+    <t>ischaemicheartdiseasehypertension</t>
+  </si>
+  <si>
+    <t>inflammatoryboweldisease</t>
+  </si>
+  <si>
+    <t>malignancies</t>
+  </si>
+  <si>
+    <t>malnutrition</t>
+  </si>
+  <si>
+    <t>osteoporosispagets</t>
+  </si>
+  <si>
+    <t>pain</t>
+  </si>
+  <si>
+    <t>inflammationpain</t>
+  </si>
+  <si>
+    <t>pancreaticinsufficiency</t>
+  </si>
+  <si>
+    <t>parkinsonsdisease</t>
+  </si>
+  <si>
+    <t>psoriasis</t>
+  </si>
+  <si>
+    <t>chronicairwaysdisease</t>
+  </si>
+  <si>
+    <t>smokingcessation</t>
+  </si>
+  <si>
+    <t>steroidresponsivediseases</t>
+  </si>
+  <si>
+    <t>transplant</t>
+  </si>
+  <si>
+    <t>tuberculosis</t>
+  </si>
+  <si>
+    <t>^(N07BB0[34])|(V03AA01)|(R05CB01)$</t>
+  </si>
+  <si>
+    <t>^R0[16]A[CDEX][0125][1-35-9]$</t>
+  </si>
+  <si>
+    <t>^B01A[AB]0[1-6]$</t>
+  </si>
+  <si>
+    <t>^B01AC[0-3][0-4679]$</t>
+  </si>
+  <si>
+    <t>^N05BA[01][1246]$</t>
+  </si>
+  <si>
+    <t>^C01[AB][A-D]0[1345]$</t>
+  </si>
+  <si>
+    <t>^G04CA0[23]$</t>
+  </si>
+  <si>
+    <t>^N06AX$</t>
+  </si>
+  <si>
+    <t>^C0[39][AC]{2}[01][0-79]$</t>
+  </si>
+  <si>
+    <t>^N04DA0[2-4]$</t>
+  </si>
+  <si>
+    <t>^N06A[ABGX][0-2][0-689]$</t>
+  </si>
+  <si>
+    <t>^A10[AB][A-G][01][1-8]$</t>
+  </si>
+  <si>
+    <t>^B03XA0[12]|A11CC0[1-4]$</t>
+  </si>
+  <si>
+    <t>^N03A[ABD-GX][01][0-59]$</t>
+  </si>
+  <si>
+    <t>^A02B[A-DX][05][1-6]$</t>
+  </si>
+  <si>
+    <t>^S01E[A-EX][05][1-5]$</t>
+  </si>
+  <si>
+    <t>^M04A[A-C]01$</t>
+  </si>
+  <si>
+    <t>^J05AB54$</t>
+  </si>
+  <si>
+    <t>^J05A[EFGRX]0[1-9]$</t>
+  </si>
+  <si>
+    <t>^V03AE01$</t>
+  </si>
+  <si>
+    <t>^C10[AB][ABCX][01][1-579]$</t>
+  </si>
+  <si>
+    <t>^C0[239][A-EK][ABCX][01][1-9]$</t>
+  </si>
+  <si>
+    <t>^H03AA0[12]$</t>
+  </si>
+  <si>
+    <t>^C01DA[01][248]$</t>
+  </si>
+  <si>
+    <t>^C0[78][ACDF][ABG][01][1-35-7]$</t>
+  </si>
+  <si>
+    <t>^A07E[AC]0[1-4]$</t>
+  </si>
+  <si>
+    <t>^L01[A-DX][A-EX][0-35][[:digit:]]$</t>
+  </si>
+  <si>
+    <t>^B05BA03$</t>
+  </si>
+  <si>
+    <t>^M05B[AB]0[1-46-8]$</t>
+  </si>
+  <si>
+    <t>^N02A[ABEFGX][05][12359]$</t>
+  </si>
+  <si>
+    <t>^M01A[BCEH][015][1-6]$</t>
+  </si>
+  <si>
+    <t>^A09AA02$</t>
+  </si>
+  <si>
+    <t>^N04[AB][ACDX]0[1-79]$</t>
+  </si>
+  <si>
+    <t>^D05[AB][BX]0[12]|D05AA$</t>
+  </si>
+  <si>
+    <t>^R03[A-D][ABCKL][01][0-46-9]$</t>
+  </si>
+  <si>
+    <t>^N07BA0[12]$</t>
+  </si>
+  <si>
+    <t>^H02AB[01][01246-9]$</t>
+  </si>
+  <si>
+    <t>^L04AA[0-2][013468]$</t>
+  </si>
+  <si>
+    <t>^J04A[BCK]0[124]$</t>
+  </si>
+  <si>
+    <t>hyperkalaemia</t>
+  </si>
+  <si>
+    <t>liverfailure</t>
+  </si>
+  <si>
+    <t>migraine</t>
+  </si>
+  <si>
+    <t>psychoticillness</t>
+  </si>
+  <si>
+    <t>^N07BB0[1345]$</t>
+  </si>
+  <si>
+    <t>^B01A[AB][01][0-69]$</t>
+  </si>
+  <si>
+    <t>^B01AC[0-4679]$</t>
+  </si>
+  <si>
+    <t>^C01[AB][A-D]0[13457]$</t>
+  </si>
+  <si>
+    <t>^G04CA0[1-3]$</t>
+  </si>
+  <si>
+    <t>^N0[35]A[EGHNX][01][1-49]$</t>
+  </si>
+  <si>
+    <t>^C0[39][ACD][AC][01][0-79]$</t>
+  </si>
+  <si>
+    <t>^N04D[AX]0[1-4]$</t>
+  </si>
+  <si>
+    <t>^N06A[ABGX][012][0-689]$</t>
+  </si>
+  <si>
+    <t>^A10[AB][A-HX][01][[:digit:]]$</t>
+  </si>
+  <si>
+    <t>^(B03XA0[1-3])|(A11CC0[1-4])$</t>
+  </si>
+  <si>
+    <t>^N03A[ABDEFGX][01][0-59]$</t>
+  </si>
+  <si>
+    <t>^A02B[A-DX][015][1-6]$</t>
+  </si>
+  <si>
+    <t>^J05A[ABEX][0156][12457]$</t>
+  </si>
+  <si>
+    <t>^J05A[EFGRX][016][[:digit:]]$</t>
+  </si>
+  <si>
+    <t>^C0[239][ABDEKX][ABCX][01][1-9]$</t>
+  </si>
+  <si>
+    <t>^C0[78][ACDF][ABG][01][1-7]$</t>
+  </si>
+  <si>
+    <t>^A07E[AC]0[1-46]$</t>
+  </si>
+  <si>
+    <t>^A06AD11$</t>
+  </si>
+  <si>
+    <t>^L01[A-DX][A-EX][0-5][[:digit:]]$</t>
+  </si>
+  <si>
+    <t>^B05BA[01][03]$</t>
+  </si>
+  <si>
+    <t>^N02C[ACX]0[1-6]$</t>
+  </si>
+  <si>
+    <t>^M05B[ABX]0[1-46-8]$</t>
+  </si>
+  <si>
+    <t>^N02A[ABEFGX][05][123569]$</t>
+  </si>
+  <si>
+    <t>^M01A[BCEHX][015][1-6]$</t>
+  </si>
+  <si>
+    <t>^D05[AB][ABX][05][12]$</t>
+  </si>
+  <si>
+    <t>^N05A[ABDEFHNX][01][1-68]$</t>
+  </si>
+  <si>
+    <t>^R03[A-D][ABCKLX][01][[:digit:]]$</t>
+  </si>
+  <si>
+    <t>^N07BA0[1-3]$</t>
+  </si>
+  <si>
+    <t>^H02AB(0[1246-9]|10)$</t>
+  </si>
+  <si>
+    <t>^L04AA[012][013468]$</t>
+  </si>
+  <si>
+    <t>^J04A[A-CKM]0[12456]$</t>
+  </si>
+  <si>
+    <t>oridinary</t>
+  </si>
+  <si>
+    <t>special</t>
+  </si>
+  <si>
+    <t>^[[:upper:]][0-9]{2}.?[0-9]{0,2}[[:upper:]]?$</t>
+  </si>
+  <si>
+    <t>^U[ABP][0-9]{2,4}$</t>
+  </si>
+  <si>
+    <t>only_ordinary</t>
+  </si>
+  <si>
+    <t>Mazda</t>
+  </si>
+  <si>
+    <t>Mer-Ben</t>
+  </si>
+  <si>
+    <t>Ford</t>
+  </si>
+  <si>
+    <t>Fiat</t>
+  </si>
+  <si>
+    <t>Toyota</t>
+  </si>
+  <si>
+    <t>Volksw</t>
+  </si>
+  <si>
+    <t>Geely</t>
+  </si>
+  <si>
+    <t>Merc</t>
+  </si>
+  <si>
+    <t>Ford|Lincoln</t>
+  </si>
+  <si>
+    <t>Chrysler|Fiat|Dodge|Ferrari|Maserati,</t>
+  </si>
+  <si>
+    <t>Porsche</t>
+  </si>
+  <si>
+    <t>Volvo|Lotus</t>
   </si>
 </sst>
 </file>
@@ -846,6 +1237,140 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="36.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>276</v>
+      </c>
+      <c r="B2" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>277</v>
+      </c>
+      <c r="B3" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>278</v>
+      </c>
+      <c r="B4" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>279</v>
+      </c>
+      <c r="B5" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>280</v>
+      </c>
+      <c r="B6" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>281</v>
+      </c>
+      <c r="B7" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>282</v>
+      </c>
+      <c r="B8" t="s">
+        <v>287</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>271</v>
+      </c>
+      <c r="B2" t="s">
+        <v>273</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>272</v>
+      </c>
+      <c r="B3" t="s">
+        <v>274</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -1450,7 +1975,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I32"/>
   <sheetViews>
@@ -2399,12 +2924,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2496,7 +3021,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -2537,7 +3062,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -2634,12 +3159,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2674,4 +3199,706 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B4" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B6" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>164</v>
+      </c>
+      <c r="B7" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>165</v>
+      </c>
+      <c r="B8" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>166</v>
+      </c>
+      <c r="B9" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>167</v>
+      </c>
+      <c r="B10" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>90</v>
+      </c>
+      <c r="B12" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>168</v>
+      </c>
+      <c r="B13" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>169</v>
+      </c>
+      <c r="B14" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>170</v>
+      </c>
+      <c r="B15" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>171</v>
+      </c>
+      <c r="B16" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>172</v>
+      </c>
+      <c r="B17" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>173</v>
+      </c>
+      <c r="B18" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>174</v>
+      </c>
+      <c r="B19" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>175</v>
+      </c>
+      <c r="B20" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>176</v>
+      </c>
+      <c r="B21" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>177</v>
+      </c>
+      <c r="B22" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>178</v>
+      </c>
+      <c r="B23" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>179</v>
+      </c>
+      <c r="B24" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>180</v>
+      </c>
+      <c r="B25" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>181</v>
+      </c>
+      <c r="B26" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>182</v>
+      </c>
+      <c r="B27" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>183</v>
+      </c>
+      <c r="B28" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>184</v>
+      </c>
+      <c r="B29" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>185</v>
+      </c>
+      <c r="B30" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>186</v>
+      </c>
+      <c r="B31" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>187</v>
+      </c>
+      <c r="B32" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>188</v>
+      </c>
+      <c r="B33" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>189</v>
+      </c>
+      <c r="B34" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>190</v>
+      </c>
+      <c r="B35" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>191</v>
+      </c>
+      <c r="B36" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>192</v>
+      </c>
+      <c r="B37" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>193</v>
+      </c>
+      <c r="B38" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>194</v>
+      </c>
+      <c r="B39" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>195</v>
+      </c>
+      <c r="B40" t="s">
+        <v>234</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B4" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B5" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>163</v>
+      </c>
+      <c r="B6" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>164</v>
+      </c>
+      <c r="B7" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>165</v>
+      </c>
+      <c r="B8" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>166</v>
+      </c>
+      <c r="B9" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>167</v>
+      </c>
+      <c r="B10" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>90</v>
+      </c>
+      <c r="B12" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>168</v>
+      </c>
+      <c r="B13" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>169</v>
+      </c>
+      <c r="B14" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>170</v>
+      </c>
+      <c r="B15" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>171</v>
+      </c>
+      <c r="B16" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>172</v>
+      </c>
+      <c r="B17" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>173</v>
+      </c>
+      <c r="B18" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>174</v>
+      </c>
+      <c r="B19" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>175</v>
+      </c>
+      <c r="B20" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>235</v>
+      </c>
+      <c r="B21" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>177</v>
+      </c>
+      <c r="B22" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>178</v>
+      </c>
+      <c r="B23" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>179</v>
+      </c>
+      <c r="B24" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>180</v>
+      </c>
+      <c r="B25" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>181</v>
+      </c>
+      <c r="B26" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>182</v>
+      </c>
+      <c r="B27" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>236</v>
+      </c>
+      <c r="B28" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>183</v>
+      </c>
+      <c r="B29" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>184</v>
+      </c>
+      <c r="B30" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>237</v>
+      </c>
+      <c r="B31" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>185</v>
+      </c>
+      <c r="B32" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>186</v>
+      </c>
+      <c r="B33" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>187</v>
+      </c>
+      <c r="B34" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>188</v>
+      </c>
+      <c r="B35" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>189</v>
+      </c>
+      <c r="B36" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>190</v>
+      </c>
+      <c r="B37" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>238</v>
+      </c>
+      <c r="B38" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>191</v>
+      </c>
+      <c r="B39" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>192</v>
+      </c>
+      <c r="B40" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>193</v>
+      </c>
+      <c r="B41" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>194</v>
+      </c>
+      <c r="B42" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>195</v>
+      </c>
+      <c r="B43" t="s">
+        <v>270</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
* corrections made to Elixhauser nonclomplicated hypertension and psycoses. * incl elix.short_icd10 for testing purposes. See #59
</commit_message>
<xml_diff>
--- a/data-raw/classcodes.xlsx
+++ b/data-raw/classcodes.xlsx
@@ -9,26 +9,27 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ex.carbrands_excars" sheetId="10" r:id="rId1"/>
     <sheet name="charlson_icd10" sheetId="1" r:id="rId2"/>
     <sheet name="elix_icd10" sheetId="2" r:id="rId3"/>
-    <sheet name="hip.ae_icd10" sheetId="3" r:id="rId4"/>
-    <sheet name="hip.ae_kva" sheetId="4" r:id="rId5"/>
-    <sheet name="knee.ae_icd10" sheetId="5" r:id="rId6"/>
-    <sheet name="knee.ae_kva" sheetId="6" r:id="rId7"/>
-    <sheet name="rxriskv_atc" sheetId="7" r:id="rId8"/>
-    <sheet name="rxriskv.modified_atc" sheetId="8" r:id="rId9"/>
-    <sheet name="cps_icd10" sheetId="9" r:id="rId10"/>
+    <sheet name="elix.short_icd10" sheetId="11" r:id="rId4"/>
+    <sheet name="hip.ae_icd10" sheetId="3" r:id="rId5"/>
+    <sheet name="hip.ae_kva" sheetId="4" r:id="rId6"/>
+    <sheet name="knee.ae_icd10" sheetId="5" r:id="rId7"/>
+    <sheet name="knee.ae_kva" sheetId="6" r:id="rId8"/>
+    <sheet name="rxriskv_atc" sheetId="7" r:id="rId9"/>
+    <sheet name="rxriskv.modified_atc" sheetId="8" r:id="rId10"/>
+    <sheet name="cps_icd10" sheetId="9" r:id="rId11"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="311">
   <si>
     <t>group</t>
   </si>
@@ -312,9 +313,6 @@
     <t>I(2([67]|8[089]))</t>
   </si>
   <si>
-    <t>^I10[0-9]</t>
-  </si>
-  <si>
     <t>^I1[1-35]</t>
   </si>
   <si>
@@ -373,9 +371,6 @@
   </si>
   <si>
     <t>^(F1[1-689]|Z7(15|22))</t>
-  </si>
-  <si>
-    <t>^F(2[0-589]|3([01]2|15))</t>
   </si>
   <si>
     <t>^F(204|3(1[345]|[23]|41)|4[13]2)</t>
@@ -893,6 +888,81 @@
   </si>
   <si>
     <t>Volvo|Lotus</t>
+  </si>
+  <si>
+    <t>^(I(4[457-9])|R00|T82|Z[49]5)</t>
+  </si>
+  <si>
+    <t>^I2[678]</t>
+  </si>
+  <si>
+    <t>^(I7[01389]|K55|Z95)</t>
+  </si>
+  <si>
+    <t>^I10</t>
+  </si>
+  <si>
+    <t>^G(04|11|8[0-3])</t>
+  </si>
+  <si>
+    <t>^(G(1[0-3]|2[0125]|3[125-7]|4[01]|93)|R47|R56)</t>
+  </si>
+  <si>
+    <t>^(I27|(J([46][0-7]|68)|70))</t>
+  </si>
+  <si>
+    <t>^E(0[0-3]|89)</t>
+  </si>
+  <si>
+    <t>^(I(1[23])|N(1[89]|25)|Z(49|9[49]))</t>
+  </si>
+  <si>
+    <t>^(B18|I(8[56]|98)|K7[0-467]|Z94)</t>
+  </si>
+  <si>
+    <t>^B2[0-24]</t>
+  </si>
+  <si>
+    <t>^C(8[1-58]|9[06])</t>
+  </si>
+  <si>
+    <t>^(L94|M(0[568]|12|3[0-5]|4[56]))</t>
+  </si>
+  <si>
+    <t>^D6[5-9]</t>
+  </si>
+  <si>
+    <t>^(E4[0-6]|R6[34])</t>
+  </si>
+  <si>
+    <t>^E(22|8[67])</t>
+  </si>
+  <si>
+    <t>^D50</t>
+  </si>
+  <si>
+    <t>^D5[0-3]</t>
+  </si>
+  <si>
+    <t>^(F10|E52|G62|I42|K(29|70)|T51|Z(50|7[12]))</t>
+  </si>
+  <si>
+    <t>^(F1[1-689]|Z7[12])</t>
+  </si>
+  <si>
+    <t>^F(20|3[1-4]|4[13])</t>
+  </si>
+  <si>
+    <t>^F(2[02-589]|3([01]2|15))</t>
+  </si>
+  <si>
+    <t>^F(2[02-589]|3[015])</t>
+  </si>
+  <si>
+    <t>^(A52|I(0[5-9]|3[4-9]|Q23|Z95))</t>
+  </si>
+  <si>
+    <t>^(I(09|1[13]|25|4[23]|50)|P29)</t>
   </si>
 </sst>
 </file>
@@ -1239,7 +1309,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -1258,58 +1328,58 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B3" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B4" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B5" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B6" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B7" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B8" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -1318,6 +1388,369 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>159</v>
+      </c>
+      <c r="B4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>160</v>
+      </c>
+      <c r="B5" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>161</v>
+      </c>
+      <c r="B6" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>162</v>
+      </c>
+      <c r="B7" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B8" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>164</v>
+      </c>
+      <c r="B9" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>165</v>
+      </c>
+      <c r="B10" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>90</v>
+      </c>
+      <c r="B12" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>166</v>
+      </c>
+      <c r="B13" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>167</v>
+      </c>
+      <c r="B14" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>168</v>
+      </c>
+      <c r="B15" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>169</v>
+      </c>
+      <c r="B16" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>170</v>
+      </c>
+      <c r="B17" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>171</v>
+      </c>
+      <c r="B18" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>172</v>
+      </c>
+      <c r="B19" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>173</v>
+      </c>
+      <c r="B20" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>233</v>
+      </c>
+      <c r="B21" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>175</v>
+      </c>
+      <c r="B22" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>176</v>
+      </c>
+      <c r="B23" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>177</v>
+      </c>
+      <c r="B24" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>178</v>
+      </c>
+      <c r="B25" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>179</v>
+      </c>
+      <c r="B26" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>180</v>
+      </c>
+      <c r="B27" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>234</v>
+      </c>
+      <c r="B28" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>181</v>
+      </c>
+      <c r="B29" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>182</v>
+      </c>
+      <c r="B30" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>235</v>
+      </c>
+      <c r="B31" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>183</v>
+      </c>
+      <c r="B32" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>184</v>
+      </c>
+      <c r="B33" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>185</v>
+      </c>
+      <c r="B34" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>186</v>
+      </c>
+      <c r="B35" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>187</v>
+      </c>
+      <c r="B36" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>188</v>
+      </c>
+      <c r="B37" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>236</v>
+      </c>
+      <c r="B38" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>189</v>
+      </c>
+      <c r="B39" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>190</v>
+      </c>
+      <c r="B40" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>191</v>
+      </c>
+      <c r="B41" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>192</v>
+      </c>
+      <c r="B42" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>193</v>
+      </c>
+      <c r="B43" t="s">
+        <v>268</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -1339,15 +1772,15 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B2" t="s">
         <v>271</v>
-      </c>
-      <c r="B2" t="s">
-        <v>273</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1355,10 +1788,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>270</v>
+      </c>
+      <c r="B3" t="s">
         <v>272</v>
-      </c>
-      <c r="B3" t="s">
-        <v>274</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1403,7 +1836,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -1436,7 +1869,7 @@
         <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -1468,7 +1901,7 @@
         <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1500,7 +1933,7 @@
         <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -1532,7 +1965,7 @@
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -1564,7 +1997,7 @@
         <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -1660,7 +2093,7 @@
         <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -1692,7 +2125,7 @@
         <v>35</v>
       </c>
       <c r="D10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -1724,7 +2157,7 @@
         <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -1756,7 +2189,7 @@
         <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E12">
         <v>2</v>
@@ -1788,7 +2221,7 @@
         <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E13">
         <v>2</v>
@@ -1820,7 +2253,7 @@
         <v>47</v>
       </c>
       <c r="D14" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E14">
         <v>2</v>
@@ -1884,7 +2317,7 @@
         <v>53</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E16">
         <v>3</v>
@@ -1948,7 +2381,7 @@
         <v>59</v>
       </c>
       <c r="D18" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E18">
         <v>6</v>
@@ -1980,7 +2413,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2002,7 +2435,7 @@
         <v>60</v>
       </c>
       <c r="D1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E1" t="s">
         <v>61</v>
@@ -2014,10 +2447,10 @@
         <v>63</v>
       </c>
       <c r="H1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="I1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2170,7 +2603,7 @@
         <v>68</v>
       </c>
       <c r="B7" t="s">
-        <v>94</v>
+        <v>289</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -2199,7 +2632,7 @@
         <v>69</v>
       </c>
       <c r="B8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -2257,7 +2690,7 @@
         <v>71</v>
       </c>
       <c r="B10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -2286,7 +2719,7 @@
         <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -2315,7 +2748,7 @@
         <v>72</v>
       </c>
       <c r="B12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -2344,7 +2777,7 @@
         <v>73</v>
       </c>
       <c r="B13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -2373,7 +2806,7 @@
         <v>74</v>
       </c>
       <c r="B14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -2402,7 +2835,7 @@
         <v>75</v>
       </c>
       <c r="B15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -2431,7 +2864,7 @@
         <v>76</v>
       </c>
       <c r="B16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -2460,7 +2893,7 @@
         <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -2518,7 +2951,7 @@
         <v>77</v>
       </c>
       <c r="B19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -2576,7 +3009,7 @@
         <v>79</v>
       </c>
       <c r="B21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -2605,7 +3038,7 @@
         <v>80</v>
       </c>
       <c r="B22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -2634,7 +3067,7 @@
         <v>81</v>
       </c>
       <c r="B23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -2663,7 +3096,7 @@
         <v>82</v>
       </c>
       <c r="B24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -2692,7 +3125,7 @@
         <v>83</v>
       </c>
       <c r="B25" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -2721,7 +3154,7 @@
         <v>84</v>
       </c>
       <c r="B26" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -2750,7 +3183,7 @@
         <v>85</v>
       </c>
       <c r="B27" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -2779,7 +3212,7 @@
         <v>86</v>
       </c>
       <c r="B28" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -2808,7 +3241,7 @@
         <v>87</v>
       </c>
       <c r="B29" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -2837,7 +3270,7 @@
         <v>88</v>
       </c>
       <c r="B30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -2866,7 +3299,7 @@
         <v>89</v>
       </c>
       <c r="B31" t="s">
-        <v>115</v>
+        <v>307</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -2895,7 +3328,7 @@
         <v>90</v>
       </c>
       <c r="B32" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -2926,10 +3359,959 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.28515625" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" t="s">
+        <v>130</v>
+      </c>
+      <c r="I1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>310</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>7</v>
+      </c>
+      <c r="F2">
+        <v>9</v>
+      </c>
+      <c r="G2">
+        <v>9</v>
+      </c>
+      <c r="H2">
+        <v>9</v>
+      </c>
+      <c r="I2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" t="s">
+        <v>286</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
+        <v>309</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>-1</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" t="s">
+        <v>287</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5">
+        <v>6</v>
+      </c>
+      <c r="I5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" t="s">
+        <v>288</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="H6">
+        <v>3</v>
+      </c>
+      <c r="I6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" t="s">
+        <v>289</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>-2</v>
+      </c>
+      <c r="G7">
+        <v>-1</v>
+      </c>
+      <c r="H7">
+        <v>-1</v>
+      </c>
+      <c r="I7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>-2</v>
+      </c>
+      <c r="G8">
+        <v>-1</v>
+      </c>
+      <c r="H8">
+        <v>-1</v>
+      </c>
+      <c r="I8">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" t="s">
+        <v>290</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>7</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
+      </c>
+      <c r="H9">
+        <v>5</v>
+      </c>
+      <c r="I9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10" t="s">
+        <v>291</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>6</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+      <c r="G10">
+        <v>4</v>
+      </c>
+      <c r="H10">
+        <v>5</v>
+      </c>
+      <c r="I10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
+        <v>292</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <v>3</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+      <c r="H11">
+        <v>3</v>
+      </c>
+      <c r="I11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" t="s">
+        <v>126</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>-1</v>
+      </c>
+      <c r="H13">
+        <v>-3</v>
+      </c>
+      <c r="I13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" t="s">
+        <v>293</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" t="s">
+        <v>294</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>5</v>
+      </c>
+      <c r="F15">
+        <v>7</v>
+      </c>
+      <c r="G15">
+        <v>6</v>
+      </c>
+      <c r="H15">
+        <v>6</v>
+      </c>
+      <c r="I15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" t="s">
+        <v>295</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>11</v>
+      </c>
+      <c r="F16">
+        <v>7</v>
+      </c>
+      <c r="G16">
+        <v>5</v>
+      </c>
+      <c r="H16">
+        <v>4</v>
+      </c>
+      <c r="I16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" t="s">
+        <v>296</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>77</v>
+      </c>
+      <c r="B19" t="s">
+        <v>297</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>9</v>
+      </c>
+      <c r="F19">
+        <v>8</v>
+      </c>
+      <c r="G19">
+        <v>6</v>
+      </c>
+      <c r="H19">
+        <v>6</v>
+      </c>
+      <c r="I19">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>12</v>
+      </c>
+      <c r="F20">
+        <v>17</v>
+      </c>
+      <c r="G20">
+        <v>13</v>
+      </c>
+      <c r="H20">
+        <v>14</v>
+      </c>
+      <c r="I20">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>79</v>
+      </c>
+      <c r="B21" t="s">
+        <v>104</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>4</v>
+      </c>
+      <c r="F21">
+        <v>10</v>
+      </c>
+      <c r="G21">
+        <v>8</v>
+      </c>
+      <c r="H21">
+        <v>7</v>
+      </c>
+      <c r="I21">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" t="s">
+        <v>298</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>81</v>
+      </c>
+      <c r="B23" t="s">
+        <v>299</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>3</v>
+      </c>
+      <c r="F23">
+        <v>12</v>
+      </c>
+      <c r="G23">
+        <v>9</v>
+      </c>
+      <c r="H23">
+        <v>11</v>
+      </c>
+      <c r="I23">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" t="s">
+        <v>107</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>-4</v>
+      </c>
+      <c r="F24">
+        <v>-5</v>
+      </c>
+      <c r="G24">
+        <v>-4</v>
+      </c>
+      <c r="H24">
+        <v>-5</v>
+      </c>
+      <c r="I24">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>83</v>
+      </c>
+      <c r="B25" t="s">
+        <v>300</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>6</v>
+      </c>
+      <c r="F25">
+        <v>10</v>
+      </c>
+      <c r="G25">
+        <v>8</v>
+      </c>
+      <c r="H25">
+        <v>9</v>
+      </c>
+      <c r="I25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>84</v>
+      </c>
+      <c r="B26" t="s">
+        <v>301</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>5</v>
+      </c>
+      <c r="F26">
+        <v>11</v>
+      </c>
+      <c r="G26">
+        <v>9</v>
+      </c>
+      <c r="H26">
+        <v>11</v>
+      </c>
+      <c r="I26">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>85</v>
+      </c>
+      <c r="B27" t="s">
+        <v>302</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>-2</v>
+      </c>
+      <c r="F27">
+        <v>-3</v>
+      </c>
+      <c r="G27">
+        <v>-2</v>
+      </c>
+      <c r="H27">
+        <v>-3</v>
+      </c>
+      <c r="I27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>86</v>
+      </c>
+      <c r="B28" t="s">
+        <v>303</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>-2</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>-2</v>
+      </c>
+      <c r="I28">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>87</v>
+      </c>
+      <c r="B29" t="s">
+        <v>304</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>-2</v>
+      </c>
+      <c r="H29">
+        <v>-1</v>
+      </c>
+      <c r="I29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>88</v>
+      </c>
+      <c r="B30" t="s">
+        <v>305</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>-7</v>
+      </c>
+      <c r="F30">
+        <v>-11</v>
+      </c>
+      <c r="G30">
+        <v>-8</v>
+      </c>
+      <c r="H30">
+        <v>-7</v>
+      </c>
+      <c r="I30">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>89</v>
+      </c>
+      <c r="B31" t="s">
+        <v>308</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>-6</v>
+      </c>
+      <c r="G31">
+        <v>-4</v>
+      </c>
+      <c r="H31">
+        <v>-5</v>
+      </c>
+      <c r="I31">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32" t="s">
+        <v>306</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>-3</v>
+      </c>
+      <c r="F32">
+        <v>-5</v>
+      </c>
+      <c r="G32">
+        <v>-4</v>
+      </c>
+      <c r="H32">
+        <v>-5</v>
+      </c>
+      <c r="I32">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2947,73 +4329,73 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>139</v>
-      </c>
-      <c r="B6" t="s">
-        <v>147</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>140</v>
-      </c>
-      <c r="B7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -3021,7 +4403,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -3043,18 +4425,18 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -3062,7 +4444,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -3085,73 +4467,73 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>137</v>
+      </c>
+      <c r="B6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>139</v>
-      </c>
-      <c r="B6" t="s">
-        <v>147</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>140</v>
-      </c>
-      <c r="B7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -3159,7 +4541,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -3170,7 +4552,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="99.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="110" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3182,18 +4564,18 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2" t="s">
         <v>150</v>
       </c>
-      <c r="B2" t="s">
-        <v>152</v>
-      </c>
       <c r="C2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -3201,7 +4583,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B40"/>
   <sheetViews>
@@ -3225,74 +4607,74 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B7" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B8" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B9" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B10" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -3300,7 +4682,7 @@
         <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -3308,498 +4690,159 @@
         <v>90</v>
       </c>
       <c r="B12" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B13" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B14" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B15" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B16" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B17" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B18" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B19" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B20" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B21" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B22" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B23" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B24" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B25" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B26" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B27" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B28" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B29" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B30" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B31" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>187</v>
-      </c>
-      <c r="B32" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>188</v>
-      </c>
-      <c r="B33" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>189</v>
-      </c>
-      <c r="B34" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>190</v>
-      </c>
-      <c r="B35" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>191</v>
-      </c>
-      <c r="B36" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>192</v>
-      </c>
-      <c r="B37" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>193</v>
-      </c>
-      <c r="B38" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>194</v>
-      </c>
-      <c r="B39" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>195</v>
-      </c>
-      <c r="B40" t="s">
-        <v>234</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B43"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>159</v>
-      </c>
-      <c r="B2" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>160</v>
-      </c>
-      <c r="B3" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>161</v>
-      </c>
-      <c r="B4" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>162</v>
-      </c>
-      <c r="B5" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>163</v>
-      </c>
-      <c r="B6" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>164</v>
-      </c>
-      <c r="B7" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>165</v>
-      </c>
-      <c r="B8" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>166</v>
-      </c>
-      <c r="B9" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>167</v>
-      </c>
-      <c r="B10" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>90</v>
-      </c>
-      <c r="B12" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>168</v>
-      </c>
-      <c r="B13" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>169</v>
-      </c>
-      <c r="B14" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>170</v>
-      </c>
-      <c r="B15" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>171</v>
-      </c>
-      <c r="B16" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>172</v>
-      </c>
-      <c r="B17" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>173</v>
-      </c>
-      <c r="B18" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>174</v>
-      </c>
-      <c r="B19" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>175</v>
-      </c>
-      <c r="B20" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>235</v>
-      </c>
-      <c r="B21" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>177</v>
-      </c>
-      <c r="B22" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>178</v>
-      </c>
-      <c r="B23" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>179</v>
-      </c>
-      <c r="B24" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>180</v>
-      </c>
-      <c r="B25" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>181</v>
-      </c>
-      <c r="B26" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>182</v>
-      </c>
-      <c r="B27" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>236</v>
-      </c>
-      <c r="B28" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>183</v>
-      </c>
-      <c r="B29" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>184</v>
-      </c>
-      <c r="B30" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>237</v>
-      </c>
-      <c r="B31" t="s">
-        <v>260</v>
+        <v>223</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -3807,7 +4850,7 @@
         <v>185</v>
       </c>
       <c r="B32" t="s">
-        <v>261</v>
+        <v>224</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -3815,7 +4858,7 @@
         <v>186</v>
       </c>
       <c r="B33" t="s">
-        <v>262</v>
+        <v>225</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -3823,7 +4866,7 @@
         <v>187</v>
       </c>
       <c r="B34" t="s">
-        <v>263</v>
+        <v>226</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -3847,55 +4890,31 @@
         <v>190</v>
       </c>
       <c r="B37" t="s">
-        <v>264</v>
+        <v>229</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>238</v>
+        <v>191</v>
       </c>
       <c r="B38" t="s">
-        <v>265</v>
+        <v>230</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B39" t="s">
-        <v>266</v>
+        <v>231</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B40" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>193</v>
-      </c>
-      <c r="B41" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>194</v>
-      </c>
-      <c r="B42" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>195</v>
-      </c>
-      <c r="B43" t="s">
-        <v>270</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
code fix in elix.short_icd10 and fixed random seeds for reproducibility.
</commit_message>
<xml_diff>
--- a/data-raw/classcodes.xlsx
+++ b/data-raw/classcodes.xlsx
@@ -24,7 +24,7 @@
     <sheet name="rxriskv.modified_atc" sheetId="8" r:id="rId10"/>
     <sheet name="cps_icd10" sheetId="9" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -959,10 +959,10 @@
     <t>^F(2[02-589]|3[015])</t>
   </si>
   <si>
-    <t>^(A52|I(0[5-9]|3[4-9]|Q23|Z95))</t>
-  </si>
-  <si>
     <t>^(I(09|1[13]|25|4[23]|50)|P29)</t>
+  </si>
+  <si>
+    <t>^(A52|I(0[5-9]|3[4-9])|Q23|Z95)</t>
   </si>
 </sst>
 </file>
@@ -3362,7 +3362,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3407,7 +3407,7 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -3465,7 +3465,7 @@
         <v>67</v>
       </c>
       <c r="B4" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C4">
         <v>1</v>

</xml_diff>

<commit_message>
Fix #45. Add ICD-8 and ICD-9 codes for Charlson.
</commit_message>
<xml_diff>
--- a/data-raw/classcodes.xlsx
+++ b/data-raw/classcodes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ex.carbrands_excars" sheetId="10" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="389">
   <si>
     <t>group</t>
   </si>
@@ -1123,6 +1123,81 @@
   </si>
   <si>
     <t>index_pratt</t>
+  </si>
+  <si>
+    <t>41[02]</t>
+  </si>
+  <si>
+    <t>4(02|2[589])</t>
+  </si>
+  <si>
+    <t>44[0-7]|785E|V43D</t>
+  </si>
+  <si>
+    <t>362C|43[0-8]</t>
+  </si>
+  <si>
+    <t>29[04]</t>
+  </si>
+  <si>
+    <t>416|49[0-6]|50([0-5]|6D)</t>
+  </si>
+  <si>
+    <t>71[0-4]|725</t>
+  </si>
+  <si>
+    <t>070|456[A-C]|57[1-3]</t>
+  </si>
+  <si>
+    <t>34[2-4]</t>
+  </si>
+  <si>
+    <t>40[34]|58[0-68]|V4(20|51)</t>
+  </si>
+  <si>
+    <t>1([4-68][0-9]|7[0-24-9]|9[0-5])|20[0-8]</t>
+  </si>
+  <si>
+    <t>19[6-9]</t>
+  </si>
+  <si>
+    <t>279K</t>
+  </si>
+  <si>
+    <t>regex_icd9_brusselaers</t>
+  </si>
+  <si>
+    <t>regex_icd8_brusselaers</t>
+  </si>
+  <si>
+    <t>41[0-2]</t>
+  </si>
+  <si>
+    <t>4270|428</t>
+  </si>
+  <si>
+    <t>44[0-5]</t>
+  </si>
+  <si>
+    <t>43[0-8]</t>
+  </si>
+  <si>
+    <t>290[01]</t>
+  </si>
+  <si>
+    <t>49[0-3]|51[5-8]</t>
+  </si>
+  <si>
+    <t>7(1[0-2]|34)</t>
+  </si>
+  <si>
+    <t>070|4560|51[1-3]</t>
+  </si>
+  <si>
+    <t>40[34]|58[0-3]|792</t>
+  </si>
+  <si>
+    <t>1([4-68][0-9]|7[0-24-9]|9[0-4])|20[0-7]</t>
   </si>
 </sst>
 </file>
@@ -1549,28 +1624,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK18"/>
+  <dimension ref="A1:AMM18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.42578125" customWidth="1"/>
-    <col min="2" max="2" width="55.7109375" customWidth="1"/>
-    <col min="3" max="3" width="61.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="55.7109375" customWidth="1"/>
-    <col min="5" max="5" width="8.42578125" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" customWidth="1"/>
-    <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" customWidth="1"/>
-    <col min="11" max="1026" width="8.5703125" customWidth="1"/>
+    <col min="2" max="2" width="53.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="61.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="61.42578125" customWidth="1"/>
+    <col min="6" max="6" width="55.7109375" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" customWidth="1"/>
+    <col min="9" max="9" width="11" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" customWidth="1"/>
+    <col min="11" max="11" width="17.5703125" customWidth="1"/>
+    <col min="12" max="12" width="14.42578125" customWidth="1"/>
+    <col min="13" max="1028" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10 1025:1025" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12 1027:1027" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1584,26 +1660,32 @@
         <v>113</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="AMK1"/>
-    </row>
-    <row r="2" spans="1:10 1025:1025" x14ac:dyDescent="0.25">
+      <c r="AMM1"/>
+    </row>
+    <row r="2" spans="1:12 1027:1027" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1616,11 +1698,11 @@
       <c r="D2" t="s">
         <v>114</v>
       </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
+      <c r="E2" t="s">
+        <v>379</v>
+      </c>
+      <c r="F2" t="s">
+        <v>364</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -1632,10 +1714,16 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10 1025:1025" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12 1027:1027" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1648,26 +1736,32 @@
       <c r="D3" t="s">
         <v>115</v>
       </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
+      <c r="E3" t="s">
+        <v>380</v>
+      </c>
+      <c r="F3" t="s">
+        <v>365</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
         <v>4</v>
       </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10 1025:1025" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12 1027:1027" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1680,26 +1774,32 @@
       <c r="D4" t="s">
         <v>116</v>
       </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
+      <c r="E4" t="s">
+        <v>381</v>
+      </c>
+      <c r="F4" t="s">
+        <v>366</v>
       </c>
       <c r="G4">
         <v>1</v>
       </c>
       <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
         <v>2</v>
       </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10 1025:1025" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12 1027:1027" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1712,11 +1812,11 @@
       <c r="D5" t="s">
         <v>117</v>
       </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
+      <c r="E5" t="s">
+        <v>382</v>
+      </c>
+      <c r="F5" t="s">
+        <v>367</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -1728,10 +1828,16 @@
         <v>1</v>
       </c>
       <c r="J5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10 1025:1025" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12 1027:1027" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1744,26 +1850,32 @@
       <c r="D6" t="s">
         <v>118</v>
       </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
+      <c r="E6" t="s">
+        <v>383</v>
+      </c>
+      <c r="F6" t="s">
+        <v>368</v>
       </c>
       <c r="G6">
         <v>1</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6">
         <v>1</v>
       </c>
       <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:10 1025:1025" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12 1027:1027" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1776,26 +1888,32 @@
       <c r="D7" t="s">
         <v>26</v>
       </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
+      <c r="E7" t="s">
+        <v>384</v>
+      </c>
+      <c r="F7" t="s">
+        <v>369</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7">
         <v>1</v>
       </c>
       <c r="J7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10 1025:1025" ht="45" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12 1027:1027" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -1808,26 +1926,32 @@
       <c r="D8" t="s">
         <v>29</v>
       </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
+      <c r="E8" t="s">
+        <v>385</v>
+      </c>
+      <c r="F8" t="s">
+        <v>370</v>
       </c>
       <c r="G8">
         <v>1</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8">
         <v>1</v>
       </c>
       <c r="J8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10 1025:1025" ht="30" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12 1027:1027" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -1837,17 +1961,11 @@
       <c r="C9" t="s">
         <v>32</v>
       </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
       <c r="G9">
         <v>1</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9">
         <v>1</v>
@@ -1855,8 +1973,14 @@
       <c r="J9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:10 1025:1025" ht="30" x14ac:dyDescent="0.25">
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12 1027:1027" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -1866,26 +1990,26 @@
       <c r="C10" t="s">
         <v>35</v>
       </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
       <c r="G10">
         <v>1</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10">
         <v>1</v>
       </c>
       <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:10 1025:1025" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12 1027:1027" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -1895,17 +2019,11 @@
       <c r="C11" t="s">
         <v>38</v>
       </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
       <c r="G11">
         <v>1</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11">
         <v>1</v>
@@ -1913,8 +2031,14 @@
       <c r="J11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:10 1025:1025" x14ac:dyDescent="0.25">
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12 1027:1027" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -1928,25 +2052,31 @@
         <v>119</v>
       </c>
       <c r="E12">
+        <v>344</v>
+      </c>
+      <c r="F12" t="s">
+        <v>372</v>
+      </c>
+      <c r="G12">
         <v>2</v>
       </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
       <c r="H12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
         <v>2</v>
       </c>
-      <c r="J12">
+      <c r="L12">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:10 1025:1025" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12 1027:1027" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -1959,26 +2089,32 @@
       <c r="D13" t="s">
         <v>120</v>
       </c>
-      <c r="E13">
+      <c r="E13" t="s">
+        <v>387</v>
+      </c>
+      <c r="F13" t="s">
+        <v>373</v>
+      </c>
+      <c r="G13">
         <v>2</v>
       </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
       <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
         <v>3</v>
       </c>
-      <c r="I13">
+      <c r="K13">
         <v>2</v>
       </c>
-      <c r="J13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10 1025:1025" ht="30" x14ac:dyDescent="0.25">
+      <c r="L13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12 1027:1027" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -1992,25 +2128,31 @@
         <v>121</v>
       </c>
       <c r="E14">
+        <v>250</v>
+      </c>
+      <c r="F14">
+        <v>250</v>
+      </c>
+      <c r="G14">
         <v>2</v>
       </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
       <c r="H14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
         <v>2</v>
       </c>
-      <c r="J14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10 1025:1025" ht="30" x14ac:dyDescent="0.25">
+      <c r="L14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12 1027:1027" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>241</v>
       </c>
@@ -2023,26 +2165,32 @@
       <c r="D15" t="s">
         <v>49</v>
       </c>
-      <c r="E15">
+      <c r="E15" t="s">
+        <v>388</v>
+      </c>
+      <c r="F15" t="s">
+        <v>374</v>
+      </c>
+      <c r="G15">
         <v>2</v>
       </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
       <c r="H15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
         <v>2</v>
       </c>
-      <c r="J15">
+      <c r="L15">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:10 1025:1025" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12 1027:1027" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>50</v>
       </c>
@@ -2055,26 +2203,32 @@
       <c r="D16" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="G16">
         <v>3</v>
       </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
       <c r="H16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
         <v>3</v>
       </c>
-      <c r="J16">
+      <c r="L16">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -2087,26 +2241,32 @@
       <c r="D17" t="s">
         <v>55</v>
       </c>
-      <c r="E17">
+      <c r="E17" t="s">
+        <v>375</v>
+      </c>
+      <c r="F17" t="s">
+        <v>375</v>
+      </c>
+      <c r="G17">
         <v>6</v>
       </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
       <c r="H17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
         <v>6</v>
       </c>
-      <c r="J17">
+      <c r="L17">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -2119,22 +2279,25 @@
       <c r="D18" t="s">
         <v>122</v>
       </c>
-      <c r="E18">
+      <c r="F18" t="s">
+        <v>376</v>
+      </c>
+      <c r="G18">
         <v>6</v>
       </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="G18">
-        <v>1</v>
-      </c>
       <c r="H18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
         <v>6</v>
       </c>
-      <c r="J18">
+      <c r="L18">
         <v>4</v>
       </c>
     </row>
@@ -3471,7 +3634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Remove hard coded classification names from classcodes. Fix #64. Changed datasets names to include "." instead of "_". Modified summary.classcodes to only print a defined number of characters. Fix #65.
</commit_message>
<xml_diff>
--- a/data-raw/classcodes.xlsx
+++ b/data-raw/classcodes.xlsx
@@ -9,28 +9,26 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="ex.carbrands_excars" sheetId="10" r:id="rId1"/>
-    <sheet name="charlson_icd10" sheetId="1" r:id="rId2"/>
-    <sheet name="elix_icd10" sheetId="2" r:id="rId3"/>
-    <sheet name="hip.ae_icd10" sheetId="3" r:id="rId4"/>
-    <sheet name="hip.ae_kva" sheetId="4" r:id="rId5"/>
-    <sheet name="knee.ae_icd10" sheetId="5" r:id="rId6"/>
-    <sheet name="knee.ae_kva" sheetId="6" r:id="rId7"/>
-    <sheet name="rxriskv_atc" sheetId="7" r:id="rId8"/>
-    <sheet name="cps_icd10" sheetId="9" r:id="rId9"/>
+    <sheet name="ex_carbrands" sheetId="10" r:id="rId1"/>
+    <sheet name="charlson" sheetId="1" r:id="rId2"/>
+    <sheet name="elixhauser" sheetId="2" r:id="rId3"/>
+    <sheet name="hip_ae" sheetId="3" r:id="rId4"/>
+    <sheet name="knee_ae" sheetId="5" r:id="rId5"/>
+    <sheet name="rxriskv" sheetId="7" r:id="rId6"/>
+    <sheet name="cps" sheetId="9" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">rxriskv_atc!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">rxriskv!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="404">
   <si>
     <t>group</t>
   </si>
@@ -369,9 +367,6 @@
   </si>
   <si>
     <t>^F(204|3(1[345]|[23]|41)|4[13]2)</t>
-  </si>
-  <si>
-    <t>regex_rcs</t>
   </si>
   <si>
     <t>^I2([1-3]|52)</t>
@@ -462,12 +457,6 @@
     <t>post_op</t>
   </si>
   <si>
-    <t>knee ae kva</t>
-  </si>
-  <si>
-    <t>hip ae kva</t>
-  </si>
-  <si>
     <t>^(N(FQ[019]9|G([ACEGHJLSUW]|B59|F(0[12]|1[0-2]|9[12])|K[01]9|[MQ]09|T[01]9))|QD(A10|B[^1]|E35|G)|TNG(05|10))</t>
   </si>
   <si>
@@ -1198,6 +1187,60 @@
   </si>
   <si>
     <t>1([4-68][0-9]|7[0-24-9]|9[0-4])|20[0-7]</t>
+  </si>
+  <si>
+    <t>regex_icd10_rcs</t>
+  </si>
+  <si>
+    <t>regex_icd9cm_deyo</t>
+  </si>
+  <si>
+    <t>regex_icd9cm_enhanced</t>
+  </si>
+  <si>
+    <t>44(39|1)|7854|V434</t>
+  </si>
+  <si>
+    <t>490|50([0-5]|64)</t>
+  </si>
+  <si>
+    <t>7(1(0[014]|4([0-2]|81))|25)</t>
+  </si>
+  <si>
+    <t>53[1-4]</t>
+  </si>
+  <si>
+    <t>571[24-6]</t>
+  </si>
+  <si>
+    <t>250[0-37]</t>
+  </si>
+  <si>
+    <t>250[4-6]</t>
+  </si>
+  <si>
+    <t>34(41|2)</t>
+  </si>
+  <si>
+    <t>58([2568]|3[0-7])</t>
+  </si>
+  <si>
+    <t>(1([4-68]|7[0-24-9]|9([0-4]|5[0-8])))|20[0-8]</t>
+  </si>
+  <si>
+    <t>456[01]|572[2-8]</t>
+  </si>
+  <si>
+    <t>19([6-8]|9[01])</t>
+  </si>
+  <si>
+    <t>04[2-4]</t>
+  </si>
+  <si>
+    <t>KVA</t>
+  </si>
+  <si>
+    <t>regex_kva</t>
   </si>
 </sst>
 </file>
@@ -1249,18 +1292,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1545,7 +1593,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1563,58 +1611,58 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B3" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B4" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B5" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B7" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B8" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -1624,29 +1672,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMM18"/>
+  <dimension ref="A1:AMO18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.42578125" customWidth="1"/>
-    <col min="2" max="2" width="53.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="61.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" style="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="61.42578125" customWidth="1"/>
-    <col min="6" max="6" width="55.7109375" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" customWidth="1"/>
-    <col min="9" max="9" width="11" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" customWidth="1"/>
-    <col min="11" max="11" width="17.5703125" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" customWidth="1"/>
-    <col min="13" max="1028" width="8.5703125" customWidth="1"/>
+    <col min="6" max="6" width="61.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="61.42578125" customWidth="1"/>
+    <col min="8" max="8" width="55.7109375" customWidth="1"/>
+    <col min="9" max="9" width="8.42578125" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" customWidth="1"/>
+    <col min="11" max="11" width="11" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" customWidth="1"/>
+    <col min="13" max="13" width="17.5703125" customWidth="1"/>
+    <col min="14" max="14" width="14.42578125" customWidth="1"/>
+    <col min="15" max="1030" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12 1027:1027" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14 1029:1029" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1656,59 +1707,62 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>113</v>
+      <c r="D1" s="6" t="s">
+        <v>387</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>378</v>
+        <v>388</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>377</v>
+        <v>386</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="AMM1"/>
-    </row>
-    <row r="2" spans="1:12 1027:1027" x14ac:dyDescent="0.25">
+      <c r="AMO1"/>
+    </row>
+    <row r="2" spans="1:14 1029:1029" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E2" t="s">
-        <v>379</v>
+      <c r="D2" s="7" t="s">
+        <v>361</v>
       </c>
       <c r="F2" t="s">
-        <v>364</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
+        <v>113</v>
+      </c>
+      <c r="G2" t="s">
+        <v>376</v>
+      </c>
+      <c r="H2" t="s">
+        <v>361</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -1720,109 +1774,118 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12 1027:1027" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14 1029:1029" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
-        <v>115</v>
-      </c>
-      <c r="E3" t="s">
-        <v>380</v>
+      <c r="D3" s="7">
+        <v>428</v>
       </c>
       <c r="F3" t="s">
-        <v>365</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
+        <v>114</v>
+      </c>
+      <c r="G3" t="s">
+        <v>377</v>
+      </c>
+      <c r="H3" t="s">
+        <v>362</v>
       </c>
       <c r="I3">
         <v>1</v>
       </c>
       <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
         <v>4</v>
       </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3">
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:12 1027:1027" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14 1029:1029" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="D4" t="s">
-        <v>116</v>
-      </c>
-      <c r="E4" t="s">
-        <v>381</v>
+      <c r="D4" s="7" t="s">
+        <v>389</v>
       </c>
       <c r="F4" t="s">
-        <v>366</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
+        <v>115</v>
+      </c>
+      <c r="G4" t="s">
+        <v>378</v>
+      </c>
+      <c r="H4" t="s">
+        <v>363</v>
       </c>
       <c r="I4">
         <v>1</v>
       </c>
       <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
         <v>2</v>
       </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12 1027:1027" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14 1029:1029" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C5" t="s">
         <v>20</v>
       </c>
-      <c r="D5" t="s">
-        <v>117</v>
-      </c>
-      <c r="E5" t="s">
-        <v>382</v>
+      <c r="D5" s="7" t="s">
+        <v>379</v>
       </c>
       <c r="F5" t="s">
-        <v>367</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
+        <v>116</v>
+      </c>
+      <c r="G5" t="s">
+        <v>379</v>
+      </c>
+      <c r="H5" t="s">
+        <v>364</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -1834,144 +1897,156 @@
         <v>1</v>
       </c>
       <c r="L5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12 1027:1027" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14 1029:1029" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C6" t="s">
         <v>23</v>
       </c>
-      <c r="D6" t="s">
-        <v>118</v>
-      </c>
-      <c r="E6" t="s">
-        <v>383</v>
+      <c r="D6" s="7">
+        <v>290</v>
       </c>
       <c r="F6" t="s">
-        <v>368</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
+        <v>117</v>
+      </c>
+      <c r="G6" t="s">
+        <v>380</v>
+      </c>
+      <c r="H6" t="s">
+        <v>365</v>
       </c>
       <c r="I6">
         <v>1</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6">
         <v>1</v>
       </c>
       <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:12 1027:1027" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14 1029:1029" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C7" t="s">
         <v>26</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="7" t="s">
+        <v>390</v>
+      </c>
+      <c r="F7" t="s">
         <v>26</v>
       </c>
-      <c r="E7" t="s">
-        <v>384</v>
-      </c>
-      <c r="F7" t="s">
-        <v>369</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
+      <c r="G7" t="s">
+        <v>381</v>
+      </c>
+      <c r="H7" t="s">
+        <v>366</v>
       </c>
       <c r="I7">
         <v>1</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7">
         <v>1</v>
       </c>
       <c r="L7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12 1027:1027" ht="45" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14 1029:1029" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C8" t="s">
         <v>29</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="7" t="s">
+        <v>391</v>
+      </c>
+      <c r="F8" t="s">
         <v>29</v>
       </c>
-      <c r="E8" t="s">
-        <v>385</v>
-      </c>
-      <c r="F8" t="s">
-        <v>370</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
+      <c r="G8" t="s">
+        <v>382</v>
+      </c>
+      <c r="H8" t="s">
+        <v>367</v>
       </c>
       <c r="I8">
         <v>1</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8">
         <v>1</v>
       </c>
       <c r="L8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12 1027:1027" ht="30" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14 1029:1029" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C9" t="s">
         <v>32</v>
       </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
+      <c r="D9" s="7" t="s">
+        <v>392</v>
       </c>
       <c r="I9">
         <v>1</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9">
         <v>1</v>
@@ -1979,57 +2054,63 @@
       <c r="L9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:12 1027:1027" ht="30" x14ac:dyDescent="0.25">
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14 1029:1029" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C10" t="s">
         <v>35</v>
       </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10">
-        <v>1</v>
+      <c r="D10" s="7" t="s">
+        <v>393</v>
       </c>
       <c r="I10">
         <v>1</v>
       </c>
       <c r="J10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10">
         <v>1</v>
       </c>
       <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:12 1027:1027" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14 1029:1029" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="4" t="s">
         <v>37</v>
       </c>
       <c r="C11" t="s">
         <v>38</v>
       </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11">
-        <v>1</v>
+      <c r="D11" s="7" t="s">
+        <v>394</v>
       </c>
       <c r="I11">
         <v>1</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11">
         <v>1</v>
@@ -2037,267 +2118,294 @@
       <c r="L11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:12 1027:1027" x14ac:dyDescent="0.25">
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14 1029:1029" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C12" t="s">
         <v>41</v>
       </c>
-      <c r="D12" t="s">
-        <v>119</v>
-      </c>
-      <c r="E12">
+      <c r="D12" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="F12" t="s">
+        <v>118</v>
+      </c>
+      <c r="G12">
         <v>344</v>
       </c>
-      <c r="F12" t="s">
-        <v>372</v>
-      </c>
-      <c r="G12">
+      <c r="H12" t="s">
+        <v>369</v>
+      </c>
+      <c r="I12">
         <v>2</v>
       </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
       <c r="J12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
         <v>2</v>
       </c>
-      <c r="L12">
+      <c r="N12">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:12 1027:1027" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14 1029:1029" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="4" t="s">
         <v>43</v>
       </c>
       <c r="C13" t="s">
         <v>44</v>
       </c>
-      <c r="D13" t="s">
-        <v>120</v>
-      </c>
-      <c r="E13" t="s">
-        <v>387</v>
+      <c r="D13" s="7" t="s">
+        <v>397</v>
       </c>
       <c r="F13" t="s">
-        <v>373</v>
-      </c>
-      <c r="G13">
+        <v>119</v>
+      </c>
+      <c r="G13" t="s">
+        <v>384</v>
+      </c>
+      <c r="H13" t="s">
+        <v>370</v>
+      </c>
+      <c r="I13">
         <v>2</v>
       </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
-      <c r="I13">
-        <v>1</v>
-      </c>
       <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
         <v>3</v>
       </c>
-      <c r="K13">
+      <c r="M13">
         <v>2</v>
       </c>
-      <c r="L13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12 1027:1027" ht="30" x14ac:dyDescent="0.25">
+      <c r="N13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14 1029:1029" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="4" t="s">
         <v>46</v>
       </c>
       <c r="C14" t="s">
         <v>47</v>
       </c>
-      <c r="D14" t="s">
-        <v>121</v>
-      </c>
-      <c r="E14">
+      <c r="D14" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="F14" t="s">
+        <v>120</v>
+      </c>
+      <c r="G14">
         <v>250</v>
       </c>
-      <c r="F14">
+      <c r="H14">
         <v>250</v>
       </c>
-      <c r="G14">
+      <c r="I14">
         <v>2</v>
       </c>
-      <c r="H14">
-        <v>1</v>
-      </c>
-      <c r="I14">
-        <v>1</v>
-      </c>
       <c r="J14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
         <v>2</v>
       </c>
-      <c r="L14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12 1027:1027" ht="30" x14ac:dyDescent="0.25">
+      <c r="N14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14 1029:1029" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>241</v>
-      </c>
-      <c r="B15" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>48</v>
       </c>
       <c r="C15" t="s">
         <v>49</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="F15" t="s">
         <v>49</v>
       </c>
-      <c r="E15" t="s">
-        <v>388</v>
-      </c>
-      <c r="F15" t="s">
-        <v>374</v>
-      </c>
-      <c r="G15">
+      <c r="G15" t="s">
+        <v>385</v>
+      </c>
+      <c r="H15" t="s">
+        <v>371</v>
+      </c>
+      <c r="I15">
         <v>2</v>
       </c>
-      <c r="H15">
-        <v>1</v>
-      </c>
-      <c r="I15">
-        <v>1</v>
-      </c>
       <c r="J15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
         <v>2</v>
       </c>
-      <c r="L15">
+      <c r="N15">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:12 1027:1027" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14 1029:1029" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C16" t="s">
         <v>52</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>386</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>371</v>
-      </c>
-      <c r="G16">
+      <c r="D16" s="7" t="s">
+        <v>399</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="I16">
         <v>3</v>
       </c>
-      <c r="H16">
-        <v>1</v>
-      </c>
-      <c r="I16">
-        <v>1</v>
-      </c>
       <c r="J16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
         <v>3</v>
       </c>
-      <c r="L16">
+      <c r="N16">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="4" t="s">
         <v>54</v>
       </c>
       <c r="C17" t="s">
         <v>55</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="7" t="s">
+        <v>400</v>
+      </c>
+      <c r="F17" t="s">
         <v>55</v>
       </c>
-      <c r="E17" t="s">
-        <v>375</v>
-      </c>
-      <c r="F17" t="s">
-        <v>375</v>
-      </c>
-      <c r="G17">
+      <c r="G17" t="s">
+        <v>372</v>
+      </c>
+      <c r="H17" t="s">
+        <v>372</v>
+      </c>
+      <c r="I17">
         <v>6</v>
       </c>
-      <c r="H17">
-        <v>1</v>
-      </c>
-      <c r="I17">
-        <v>1</v>
-      </c>
       <c r="J17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
         <v>6</v>
       </c>
-      <c r="L17">
+      <c r="N17">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="4" t="s">
         <v>57</v>
       </c>
       <c r="C18" t="s">
         <v>58</v>
       </c>
-      <c r="D18" t="s">
-        <v>122</v>
+      <c r="D18" s="7" t="s">
+        <v>401</v>
       </c>
       <c r="F18" t="s">
-        <v>376</v>
-      </c>
-      <c r="G18">
+        <v>121</v>
+      </c>
+      <c r="H18" t="s">
+        <v>373</v>
+      </c>
+      <c r="I18">
         <v>6</v>
       </c>
-      <c r="H18">
-        <v>1</v>
-      </c>
-      <c r="I18">
-        <v>1</v>
-      </c>
       <c r="J18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
         <v>6</v>
       </c>
-      <c r="L18">
+      <c r="N18">
         <v>4</v>
       </c>
     </row>
@@ -2332,13 +2440,13 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D1" t="s">
         <v>59</v>
       </c>
       <c r="E1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F1" t="s">
         <v>60</v>
@@ -2350,10 +2458,10 @@
         <v>62</v>
       </c>
       <c r="I1" t="s">
+        <v>124</v>
+      </c>
+      <c r="J1" t="s">
         <v>125</v>
-      </c>
-      <c r="J1" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -2364,7 +2472,7 @@
         <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -2396,7 +2504,7 @@
         <v>90</v>
       </c>
       <c r="C3" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -2428,7 +2536,7 @@
         <v>91</v>
       </c>
       <c r="C4" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -2457,10 +2565,10 @@
         <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C5" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -2492,7 +2600,7 @@
         <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -2521,10 +2629,10 @@
         <v>67</v>
       </c>
       <c r="B7" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C7" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -2588,7 +2696,7 @@
         <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -2620,7 +2728,7 @@
         <v>93</v>
       </c>
       <c r="C10" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -2652,7 +2760,7 @@
         <v>94</v>
       </c>
       <c r="C11" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -2684,7 +2792,7 @@
         <v>95</v>
       </c>
       <c r="C12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -2716,7 +2824,7 @@
         <v>96</v>
       </c>
       <c r="C13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -2748,7 +2856,7 @@
         <v>97</v>
       </c>
       <c r="C14" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -2780,7 +2888,7 @@
         <v>98</v>
       </c>
       <c r="C15" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -2812,7 +2920,7 @@
         <v>99</v>
       </c>
       <c r="C16" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -2876,7 +2984,7 @@
         <v>58</v>
       </c>
       <c r="C18" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -2908,7 +3016,7 @@
         <v>101</v>
       </c>
       <c r="C19" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -3004,7 +3112,7 @@
         <v>103</v>
       </c>
       <c r="C22" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -3036,7 +3144,7 @@
         <v>104</v>
       </c>
       <c r="C23" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -3100,7 +3208,7 @@
         <v>106</v>
       </c>
       <c r="C25" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -3132,7 +3240,7 @@
         <v>107</v>
       </c>
       <c r="C26" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -3164,7 +3272,7 @@
         <v>108</v>
       </c>
       <c r="C27" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -3196,7 +3304,7 @@
         <v>109</v>
       </c>
       <c r="C28" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -3228,7 +3336,7 @@
         <v>110</v>
       </c>
       <c r="C29" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -3260,7 +3368,7 @@
         <v>111</v>
       </c>
       <c r="C30" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -3289,10 +3397,10 @@
         <v>88</v>
       </c>
       <c r="B31" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C31" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -3324,7 +3432,7 @@
         <v>112</v>
       </c>
       <c r="C32" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -3355,20 +3463,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="131.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="99.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3376,73 +3485,87 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>403</v>
+      </c>
+      <c r="D1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>128</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>136</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D3" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>129</v>
-      </c>
-      <c r="B3" t="s">
-        <v>137</v>
-      </c>
-      <c r="C3" s="4" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6" t="s">
+        <v>139</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>132</v>
+      </c>
+      <c r="B7" t="s">
+        <v>148</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>130</v>
-      </c>
-      <c r="B4" t="s">
-        <v>138</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>131</v>
-      </c>
-      <c r="B5" t="s">
-        <v>139</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>132</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>402</v>
+      </c>
+      <c r="C8" t="s">
         <v>140</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>133</v>
-      </c>
-      <c r="B7" t="s">
-        <v>151</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>135</v>
+      <c r="D8" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -3452,19 +3575,21 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="98.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="131.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="110" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3472,18 +3597,87 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>403</v>
+      </c>
+      <c r="D1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>144</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6" t="s">
+        <v>139</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>132</v>
+      </c>
+      <c r="B7" t="s">
+        <v>148</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>402</v>
+      </c>
+      <c r="C8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D8" t="s">
         <v>141</v>
-      </c>
-      <c r="C2" t="s">
-        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -3492,145 +3686,6 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="131.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B2" t="s">
-        <v>148</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>146</v>
-      </c>
-      <c r="B3" t="s">
-        <v>149</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>147</v>
-      </c>
-      <c r="B4" t="s">
-        <v>150</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>131</v>
-      </c>
-      <c r="B5" t="s">
-        <v>139</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>132</v>
-      </c>
-      <c r="B6" t="s">
-        <v>140</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>133</v>
-      </c>
-      <c r="B7" t="s">
-        <v>151</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="110" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B2" t="s">
-        <v>145</v>
-      </c>
-      <c r="C2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E47"/>
   <sheetViews>
@@ -3655,27 +3710,27 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="D1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="E1" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B2" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C2" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="D2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E2">
         <v>6</v>
@@ -3683,16 +3738,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B3" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C3" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="D3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E3">
         <v>-1</v>
@@ -3700,16 +3755,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B4" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C4" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="D4" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -3717,16 +3772,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B5" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C5" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="D5" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -3734,16 +3789,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B6" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C6" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D6" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -3751,16 +3806,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B7" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C7" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="D7" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -3768,16 +3823,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B8" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C8" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D8" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -3785,16 +3840,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B9" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C9" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D9" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E9">
         <v>-1</v>
@@ -3802,16 +3857,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B10" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C10" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D10" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="E10">
         <v>2</v>
@@ -3819,16 +3874,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B11" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C11" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="D11" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E11">
         <v>2</v>
@@ -3836,16 +3891,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B12" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C12" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D12" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E12">
         <v>2</v>
@@ -3853,16 +3908,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B13" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C13" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="D13" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E13">
         <v>2</v>
@@ -3870,16 +3925,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B14" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C14" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="D14" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E14">
         <v>2</v>
@@ -3887,16 +3942,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B15" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C15" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="D15" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -3904,16 +3959,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B16" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C16" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D16" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -3921,16 +3976,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B17" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C17" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="D17" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -3938,16 +3993,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B18" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C18" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="D18" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -3955,38 +4010,38 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="B19" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B20" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C20" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D20" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B21" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C21" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="D21" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -3994,16 +4049,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B22" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C22" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D22" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E22">
         <v>4</v>
@@ -4011,16 +4066,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B23" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C23" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="D23" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E23">
         <v>-1</v>
@@ -4028,16 +4083,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B24" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C24" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D24" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E24">
         <v>-1</v>
@@ -4045,16 +4100,16 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B25" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C25" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D25" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E25">
         <v>2</v>
@@ -4062,10 +4117,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B26" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -4073,10 +4128,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="B27" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -4084,16 +4139,16 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B28" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C28" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D28" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E28">
         <v>-1</v>
@@ -4101,16 +4156,16 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B29" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C29" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="D29" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -4118,16 +4173,16 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B30" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C30" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="D30" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E30">
         <v>-1</v>
@@ -4135,16 +4190,16 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B31" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C31" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D31" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E31">
         <v>2</v>
@@ -4152,16 +4207,16 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B32" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C32" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D32" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E32">
         <v>3</v>
@@ -4169,16 +4224,16 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B33" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C33" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="D33" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="E33">
         <v>2</v>
@@ -4186,16 +4241,16 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B34" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C34" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D34" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E34">
         <v>0</v>
@@ -4203,16 +4258,16 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B35" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C35" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="D35" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E35">
         <v>-1</v>
@@ -4220,16 +4275,16 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B36" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C36" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="D36" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E36">
         <v>-1</v>
@@ -4237,16 +4292,16 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B37" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C37" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="D37" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E37">
         <v>3</v>
@@ -4254,16 +4309,16 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B38" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C38" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D38" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -4271,16 +4326,16 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B39" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C39" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="D39" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E39">
         <v>3</v>
@@ -4288,16 +4343,16 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B40" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C40" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="D40" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E40">
         <v>0</v>
@@ -4305,16 +4360,16 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B41" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C41" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="D41" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E41">
         <v>6</v>
@@ -4322,10 +4377,10 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B42" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="E42">
         <v>6</v>
@@ -4333,16 +4388,16 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B43" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C43" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="D43" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E43">
         <v>6</v>
@@ -4350,16 +4405,16 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B44" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C44" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D44" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E44">
         <v>6</v>
@@ -4367,16 +4422,16 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B45" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C45" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="D45" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="E45">
         <v>2</v>
@@ -4384,16 +4439,16 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B46" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C46" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="D46" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E46">
         <v>0</v>
@@ -4401,16 +4456,16 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B47" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C47" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="D47" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -4422,12 +4477,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4444,15 +4499,15 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -4460,10 +4515,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B3" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C3">
         <v>0</v>

</xml_diff>

<commit_message>
Add possibility to remove all non LPHnumeric characters from codes. Fix #53.
</commit_message>
<xml_diff>
--- a/data-raw/classcodes.xlsx
+++ b/data-raw/classcodes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ex_carbrands" sheetId="10" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="417">
   <si>
     <t>group</t>
   </si>
@@ -1241,6 +1241,45 @@
   </si>
   <si>
     <t>regex_kva</t>
+  </si>
+  <si>
+    <t>39891|4(0(2([01]1|91)|4([019][13]))|2(5[4-9]|8))</t>
+  </si>
+  <si>
+    <t>0930|4(373|4[01]|3[1-9]|471)|557[19]|V434</t>
+  </si>
+  <si>
+    <t>36234|43[0-8]</t>
+  </si>
+  <si>
+    <t>29(0|41)|3312</t>
+  </si>
+  <si>
+    <t>4(16[89]|90)|50([0-5]|64|8[18])</t>
+  </si>
+  <si>
+    <t>4465|7(1(0[0-4]|4[0-28])|25)</t>
+  </si>
+  <si>
+    <t>070([23]{2}|[45]4|[69])|57([01]|3[3489])|V427</t>
+  </si>
+  <si>
+    <t>250[0-389]</t>
+  </si>
+  <si>
+    <t>250[4-7]</t>
+  </si>
+  <si>
+    <t>3(341|4([23]|4[0-69]))</t>
+  </si>
+  <si>
+    <t>40(3([019]1)|4([019][23]))|58([256]|3[0-7]|80)|V(4(20|51)|56)</t>
+  </si>
+  <si>
+    <t>1([4-68]|7[0-24-9]|9([0-4]|5[0-8]))|2(0[0-8]|386)</t>
+  </si>
+  <si>
+    <t>456[0-2]|572[2-8]</t>
   </si>
 </sst>
 </file>
@@ -1674,8 +1713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMO18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1755,6 +1794,9 @@
       <c r="D2" s="7" t="s">
         <v>361</v>
       </c>
+      <c r="E2" s="7" t="s">
+        <v>361</v>
+      </c>
       <c r="F2" t="s">
         <v>113</v>
       </c>
@@ -1796,6 +1838,9 @@
       <c r="D3" s="7">
         <v>428</v>
       </c>
+      <c r="E3" t="s">
+        <v>404</v>
+      </c>
       <c r="F3" t="s">
         <v>114</v>
       </c>
@@ -1837,6 +1882,9 @@
       <c r="D4" s="7" t="s">
         <v>389</v>
       </c>
+      <c r="E4" t="s">
+        <v>405</v>
+      </c>
       <c r="F4" t="s">
         <v>115</v>
       </c>
@@ -1878,6 +1926,9 @@
       <c r="D5" s="7" t="s">
         <v>379</v>
       </c>
+      <c r="E5" t="s">
+        <v>406</v>
+      </c>
       <c r="F5" t="s">
         <v>116</v>
       </c>
@@ -1919,6 +1970,9 @@
       <c r="D6" s="7">
         <v>290</v>
       </c>
+      <c r="E6" t="s">
+        <v>407</v>
+      </c>
       <c r="F6" t="s">
         <v>117</v>
       </c>
@@ -1960,6 +2014,9 @@
       <c r="D7" s="7" t="s">
         <v>390</v>
       </c>
+      <c r="E7" t="s">
+        <v>408</v>
+      </c>
       <c r="F7" t="s">
         <v>26</v>
       </c>
@@ -2001,6 +2058,9 @@
       <c r="D8" s="7" t="s">
         <v>391</v>
       </c>
+      <c r="E8" t="s">
+        <v>409</v>
+      </c>
       <c r="F8" t="s">
         <v>29</v>
       </c>
@@ -2042,6 +2102,9 @@
       <c r="D9" s="7" t="s">
         <v>392</v>
       </c>
+      <c r="E9" t="s">
+        <v>392</v>
+      </c>
       <c r="I9">
         <v>1</v>
       </c>
@@ -2074,6 +2137,9 @@
       <c r="D10" s="7" t="s">
         <v>393</v>
       </c>
+      <c r="E10" t="s">
+        <v>410</v>
+      </c>
       <c r="I10">
         <v>1</v>
       </c>
@@ -2106,6 +2172,9 @@
       <c r="D11" s="7" t="s">
         <v>394</v>
       </c>
+      <c r="E11" t="s">
+        <v>411</v>
+      </c>
       <c r="I11">
         <v>1</v>
       </c>
@@ -2138,6 +2207,9 @@
       <c r="D12" s="7" t="s">
         <v>396</v>
       </c>
+      <c r="E12" t="s">
+        <v>413</v>
+      </c>
       <c r="F12" t="s">
         <v>118</v>
       </c>
@@ -2179,6 +2251,9 @@
       <c r="D13" s="7" t="s">
         <v>397</v>
       </c>
+      <c r="E13" t="s">
+        <v>414</v>
+      </c>
       <c r="F13" t="s">
         <v>119</v>
       </c>
@@ -2220,6 +2295,9 @@
       <c r="D14" s="7" t="s">
         <v>395</v>
       </c>
+      <c r="E14" t="s">
+        <v>412</v>
+      </c>
       <c r="F14" t="s">
         <v>120</v>
       </c>
@@ -2261,6 +2339,9 @@
       <c r="D15" s="7" t="s">
         <v>398</v>
       </c>
+      <c r="E15" t="s">
+        <v>415</v>
+      </c>
       <c r="F15" t="s">
         <v>49</v>
       </c>
@@ -2302,6 +2383,9 @@
       <c r="D16" s="7" t="s">
         <v>399</v>
       </c>
+      <c r="E16" t="s">
+        <v>416</v>
+      </c>
       <c r="F16" s="2" t="s">
         <v>122</v>
       </c>
@@ -2343,6 +2427,9 @@
       <c r="D17" s="7" t="s">
         <v>400</v>
       </c>
+      <c r="E17" t="s">
+        <v>372</v>
+      </c>
       <c r="F17" t="s">
         <v>55</v>
       </c>
@@ -2382,6 +2469,9 @@
         <v>58</v>
       </c>
       <c r="D18" s="7" t="s">
+        <v>401</v>
+      </c>
+      <c r="E18" t="s">
         <v>401</v>
       </c>
       <c r="F18" t="s">
@@ -3465,7 +3555,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Some bug fixes and updates as well as fix #67.
</commit_message>
<xml_diff>
--- a/data-raw/classcodes.xlsx
+++ b/data-raw/classcodes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="ex_carbrands" sheetId="10" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="418">
   <si>
     <t>group</t>
   </si>
@@ -63,150 +63,99 @@
     <t>Acute myocardial infarction. Old myocardial infarction.</t>
   </si>
   <si>
-    <t>^I2([12]|52)</t>
-  </si>
-  <si>
     <t>congestive heart failure</t>
   </si>
   <si>
     <t>Heart failure.</t>
   </si>
   <si>
-    <t>^(I(099|1(10|3[02])|255|4(2[05-9]|3)|50)|P290)</t>
-  </si>
-  <si>
     <t>peripheral vascular disease</t>
   </si>
   <si>
     <t>Peripheral vascular disease, incl. intermittent claudication. Aortic aneurysm. Gangrene. Blood vessel replaced by prosthesis. Resection and replacement of lower limb arteries.</t>
   </si>
   <si>
-    <t>^(I7([01]|3[189]|71|9[02])|K55[189]|Z95[89])</t>
-  </si>
-  <si>
     <t>cerebrovascular disease</t>
   </si>
   <si>
     <t>Cerebrovascular disease.</t>
   </si>
   <si>
-    <t>^(G4[56]|H340|I6)</t>
-  </si>
-  <si>
     <t>dementia</t>
   </si>
   <si>
     <t>Senile and presenile dementias.</t>
   </si>
   <si>
-    <t>^(F0([0-3]|51)|G3(0|11))</t>
-  </si>
-  <si>
     <t>chronic pulmonary disease</t>
   </si>
   <si>
     <t>Chronic obstructive pulmonary disease. Pneumoconioses. Chronic respiratory conditions due to fumes and vapors.</t>
   </si>
   <si>
-    <t>^((I27[89])|J(4[0-7]|6([0-7]|84)|70[13]))</t>
-  </si>
-  <si>
     <t>rheumatic disease</t>
   </si>
   <si>
     <t xml:space="preserve">Systemic lupus erythematosus. Systemic sclerosis. Polymyositis. Adult rheumatoid arthritis. Rheumatoid lung. Polymyalgia rheumatica. </t>
   </si>
   <si>
-    <t>^M(0[56]|3(15|[2-4]|5[13]|60))</t>
-  </si>
-  <si>
     <t>peptic ulcer disease</t>
   </si>
   <si>
     <t xml:space="preserve">Gastric, duodenal and gastrojejunal ulcers. Chronic forms of peptic ulcer disease (subset of above listing). </t>
   </si>
   <si>
-    <t>^K2[5-8]</t>
-  </si>
-  <si>
     <t>mild liver disease</t>
   </si>
   <si>
     <t>Alcoholic cirrhosis. Cirrhosis without mention of alcohol. Biliary cirrhosis. Chronic hepatitis.</t>
   </si>
   <si>
-    <t>^(B18|K7(0[0-39]|1[3457]|[34]|6[023489])|Z944)</t>
-  </si>
-  <si>
     <t>diabetes without complication</t>
   </si>
   <si>
     <t>Diabetes with or without acute metabolic disturbances. Diabetes with peripheral circulatory disorders.</t>
   </si>
   <si>
-    <t>^E1[0-4][01689]</t>
-  </si>
-  <si>
     <t>hemiplegia or paraplegia</t>
   </si>
   <si>
     <t>Paraplegia. Hemiplegia.</t>
   </si>
   <si>
-    <t>^G(041|114|8(0[12]|[12]|3[0-49]))</t>
-  </si>
-  <si>
     <t>renal disease</t>
   </si>
   <si>
     <t>Chronic glomerulonephritis. Nephritis and nephropathy Chronic renal failure. Renal failure, unspecified. Disorders resulting from impaired renal function.</t>
   </si>
   <si>
-    <t>^(I1(20|31)|N(0([35][2-7])|1[89]|250)|Z(49[012]|9(40|92)))</t>
-  </si>
-  <si>
     <t>diabetes complication</t>
   </si>
   <si>
     <t>Diabetes with renal, ophthalmic, or neurological manifestations.</t>
   </si>
   <si>
-    <t>^E1[0-4][2-57]</t>
-  </si>
-  <si>
     <t>Malignant neoplasms. Malignant neoplasms. Leukemia and lymphoma</t>
   </si>
   <si>
-    <t>^C([01]|2[0-6]|3[0-47-9]|4[0135-9]|5[0-8]|6|7[0-6]|8[1-58]|9[0-7])</t>
-  </si>
-  <si>
     <t>moderate or severe liver disease</t>
   </si>
   <si>
     <t>Hepatic coma, portal hypertension, other sequelae of chronic liver disease. Esophageal varices.</t>
   </si>
   <si>
-    <t>^(I(8(5[09]|64)|982)|K7(04|[12]1|29|6[5-7]))</t>
-  </si>
-  <si>
     <t>metastatic solid tumor</t>
   </si>
   <si>
     <t>Secondary malignant neoplasm of lymph nodes and other organs</t>
   </si>
   <si>
-    <t>^C(7[7-9]|80)</t>
-  </si>
-  <si>
     <t>AIDS/HIV</t>
   </si>
   <si>
     <t>HIV infection with related specified conditions.</t>
   </si>
   <si>
-    <t>^B2[0124]</t>
-  </si>
-  <si>
     <t>sum_all</t>
   </si>
   <si>
@@ -300,986 +249,1040 @@
     <t>depression</t>
   </si>
   <si>
-    <t>^(I(44[1-3]|456|459|4[7-9])|R00[018]|T821|Z[49]50)</t>
-  </si>
-  <si>
-    <t>^(A520|I(0[5-8]|09[18]|3[4-9])|Q23[0-3]|Z95[2-4])</t>
-  </si>
-  <si>
-    <t>^I1[1-35]</t>
-  </si>
-  <si>
-    <t>^(G(1[0-3]|2([012]|5[45])|3(1[289]|[25-7])|4[01]|93[14])|R470|R56)</t>
-  </si>
-  <si>
-    <t>^((I27[89])|(J(4[0-7]|6([0-7]|84)|70[13])))</t>
-  </si>
-  <si>
-    <t>^E1[0-4][019]</t>
-  </si>
-  <si>
-    <t>^E1[0-4][23-8]</t>
-  </si>
-  <si>
-    <t>^E(0[0-3]|890)</t>
-  </si>
-  <si>
-    <t>^(I(120|131)|N(1[89]|250)|Z(49[012]|9(40|92)))</t>
-  </si>
-  <si>
-    <t>^(B18|I(8(5|64)|982)|K7(0|1[13457]|[234]|6[02-9])|Z944)</t>
-  </si>
-  <si>
-    <t>^K2[5-8][79]</t>
-  </si>
-  <si>
-    <t>^C(8[1-58]|9(6|0[02]))</t>
-  </si>
-  <si>
-    <t>^C([01]|2[0-6]|3[0-47-9]|4[0135-9]|5[0-8]|6|7[0-6]|97)</t>
-  </si>
-  <si>
-    <t>^(L94[013]|M(0[568]|12[03]|3(0|1[0-3]|[2-5])|4(5|6[189])))</t>
-  </si>
-  <si>
-    <t>^D6([5-8]|9[13-6])</t>
-  </si>
-  <si>
-    <t>^E66</t>
-  </si>
-  <si>
-    <t>^(E4[0-6]|R63?4)</t>
-  </si>
-  <si>
-    <t>^E(222|8[67])</t>
-  </si>
-  <si>
-    <t>^D500</t>
-  </si>
-  <si>
-    <t>^D5(0[89]|[123])</t>
-  </si>
-  <si>
-    <t>^(F10|E52|G621|I426|K(292|70[039])|T51|Z(502|7(14|21)))</t>
-  </si>
-  <si>
-    <t>^(F1[1-689]|Z7(15|22))</t>
-  </si>
-  <si>
-    <t>^F(204|3(1[345]|[23]|41)|4[13]2)</t>
-  </si>
-  <si>
-    <t>^I2([1-3]|52)</t>
-  </si>
-  <si>
-    <t>^I(1[13]|255|4[23]|5(0|17))</t>
-  </si>
-  <si>
-    <t>^((I7([0-3]|7[01]))|K55[189]|R02|Z95[89])</t>
-  </si>
-  <si>
-    <t>^(G4[56]|I6)</t>
-  </si>
-  <si>
-    <t>^(A810|F0([0-3]|51)|G3[01])</t>
-  </si>
-  <si>
-    <t>^G(114|8[1-3])</t>
-  </si>
-  <si>
-    <t>^(I1[23]|N(0[13578]|17[12]|1[89]|25)|Z(49|9(40|92)))</t>
-  </si>
-  <si>
-    <t>^E1[0-4]</t>
-  </si>
-  <si>
-    <t>^B2[0-4]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">^(B18|I(8(5|64)|982)|K7([016]|2[19])|R162|Z944)
+    <t>sum_all_ahrq</t>
+  </si>
+  <si>
+    <t>ahrq_mort</t>
+  </si>
+  <si>
+    <t>ahrq_readm</t>
+  </si>
+  <si>
+    <t>condition</t>
+  </si>
+  <si>
+    <t>DA surgical complications</t>
+  </si>
+  <si>
+    <t>DB1 hip related</t>
+  </si>
+  <si>
+    <t>DB2 hip related</t>
+  </si>
+  <si>
+    <t>DC CVD</t>
+  </si>
+  <si>
+    <t>DM1 other</t>
+  </si>
+  <si>
+    <t>DM2 other</t>
+  </si>
+  <si>
+    <t>hbdia1_hdia</t>
+  </si>
+  <si>
+    <t>late_hdia</t>
+  </si>
+  <si>
+    <t>^NF([CF-HJ-MS-TW]\\d{2}|A(02|1[12]|2[0-2])|Q09|U[013489]9)|QD(A10|B(0[05]|99)|E35|G30)|TNF(05|10)$</t>
+  </si>
+  <si>
+    <t>post_op</t>
+  </si>
+  <si>
+    <t>^(N(FQ[019]9|G([ACEGHJLSUW]|B59|F(0[12]|1[0-2]|9[12])|K[01]9|[MQ]09|T[01]9))|QD(A10|B[^1]|E35|G)|TNG(05|10))</t>
+  </si>
+  <si>
+    <t>DB1 knee related</t>
+  </si>
+  <si>
+    <t>DB2 knee related</t>
+  </si>
+  <si>
+    <t>HIV</t>
+  </si>
+  <si>
+    <t>oridinary</t>
+  </si>
+  <si>
+    <t>special</t>
+  </si>
+  <si>
+    <t>only_ordinary</t>
+  </si>
+  <si>
+    <t>Mazda</t>
+  </si>
+  <si>
+    <t>Mer-Ben</t>
+  </si>
+  <si>
+    <t>Ford</t>
+  </si>
+  <si>
+    <t>Fiat</t>
+  </si>
+  <si>
+    <t>Toyota</t>
+  </si>
+  <si>
+    <t>Volksw</t>
+  </si>
+  <si>
+    <t>Geely</t>
+  </si>
+  <si>
+    <t>Merc</t>
+  </si>
+  <si>
+    <t>Ford|Lincoln</t>
+  </si>
+  <si>
+    <t>Chrysler|Fiat|Dodge|Ferrari|Maserati,</t>
+  </si>
+  <si>
+    <t>Porsche</t>
+  </si>
+  <si>
+    <t>Volvo|Lotus</t>
+  </si>
+  <si>
+    <t>malignancy</t>
+  </si>
+  <si>
+    <t>regex_short</t>
+  </si>
+  <si>
+    <t>regex_garland</t>
+  </si>
+  <si>
+    <t>Alcohol dependence</t>
+  </si>
+  <si>
+    <t>Allergies</t>
+  </si>
+  <si>
+    <t>Anticoagulants</t>
+  </si>
+  <si>
+    <t>Antiplatelets</t>
+  </si>
+  <si>
+    <t>Anxiety</t>
+  </si>
+  <si>
+    <t>Arrhythmia</t>
+  </si>
+  <si>
+    <t>Benign prostatic hyperplasia</t>
+  </si>
+  <si>
+    <t>Bipolar disorder</t>
+  </si>
+  <si>
+    <t>Chronic airways disease</t>
+  </si>
+  <si>
+    <t>Congestive heart failure</t>
+  </si>
+  <si>
+    <t>Dementia</t>
+  </si>
+  <si>
+    <t>Depression</t>
+  </si>
+  <si>
+    <t>Diabetes</t>
+  </si>
+  <si>
+    <t>Renal disease</t>
+  </si>
+  <si>
+    <t>Epilepsy</t>
+  </si>
+  <si>
+    <t>Gastrooesophageal reflux disease</t>
+  </si>
+  <si>
+    <t>Glaucoma</t>
+  </si>
+  <si>
+    <t>Gout</t>
+  </si>
+  <si>
+    <t>Hepatitis C</t>
+  </si>
+  <si>
+    <t>Hyperkalaemia</t>
+  </si>
+  <si>
+    <t>Hyperlipidaemia</t>
+  </si>
+  <si>
+    <t>Hypertension</t>
+  </si>
+  <si>
+    <t>Hyperthyroidism</t>
+  </si>
+  <si>
+    <t>Inflammation/pain</t>
+  </si>
+  <si>
+    <t>Irritable bowel syndrome</t>
+  </si>
+  <si>
+    <t>Ischaemic heart disease: hypertension</t>
+  </si>
+  <si>
+    <t>Ischemic heart disease: angina</t>
+  </si>
+  <si>
+    <t>Liver failure</t>
+  </si>
+  <si>
+    <t>Malignancies</t>
+  </si>
+  <si>
+    <t>Malnutrition</t>
+  </si>
+  <si>
+    <t>Migraine</t>
+  </si>
+  <si>
+    <t>Osteoporosis/Paget's</t>
+  </si>
+  <si>
+    <t>Pain</t>
+  </si>
+  <si>
+    <t>Pancreatic insufficiency</t>
+  </si>
+  <si>
+    <t>Parkinson's disease</t>
+  </si>
+  <si>
+    <t>Psoriasis</t>
+  </si>
+  <si>
+    <t>Psychotic illness</t>
+  </si>
+  <si>
+    <t>Smoking cessation</t>
+  </si>
+  <si>
+    <t>Steroid-responsive disease</t>
+  </si>
+  <si>
+    <t>Transplant</t>
+  </si>
+  <si>
+    <t>Tuberculosis</t>
+  </si>
+  <si>
+    <t>Hepatitis B</t>
+  </si>
+  <si>
+    <t>Pulmonary hypertension</t>
+  </si>
+  <si>
+    <t>regex_caughey</t>
+  </si>
+  <si>
+    <t>Hypothyroidism</t>
+  </si>
+  <si>
+    <t>Incontinence</t>
+  </si>
+  <si>
+    <t>index_pratt</t>
+  </si>
+  <si>
+    <t>41[02]</t>
+  </si>
+  <si>
+    <t>4(02|2[589])</t>
+  </si>
+  <si>
+    <t>44[0-7]|785E|V43D</t>
+  </si>
+  <si>
+    <t>362C|43[0-8]</t>
+  </si>
+  <si>
+    <t>29[04]</t>
+  </si>
+  <si>
+    <t>416|49[0-6]|50([0-5]|6D)</t>
+  </si>
+  <si>
+    <t>71[0-4]|725</t>
+  </si>
+  <si>
+    <t>070|456[A-C]|57[1-3]</t>
+  </si>
+  <si>
+    <t>34[2-4]</t>
+  </si>
+  <si>
+    <t>40[34]|58[0-68]|V4(20|51)</t>
+  </si>
+  <si>
+    <t>1([4-68][0-9]|7[0-24-9]|9[0-5])|20[0-8]</t>
+  </si>
+  <si>
+    <t>19[6-9]</t>
+  </si>
+  <si>
+    <t>279K</t>
+  </si>
+  <si>
+    <t>regex_icd9_brusselaers</t>
+  </si>
+  <si>
+    <t>regex_icd8_brusselaers</t>
+  </si>
+  <si>
+    <t>41[0-2]</t>
+  </si>
+  <si>
+    <t>4270|428</t>
+  </si>
+  <si>
+    <t>44[0-5]</t>
+  </si>
+  <si>
+    <t>43[0-8]</t>
+  </si>
+  <si>
+    <t>290[01]</t>
+  </si>
+  <si>
+    <t>49[0-3]|51[5-8]</t>
+  </si>
+  <si>
+    <t>7(1[0-2]|34)</t>
+  </si>
+  <si>
+    <t>070|4560|51[1-3]</t>
+  </si>
+  <si>
+    <t>40[34]|58[0-3]|792</t>
+  </si>
+  <si>
+    <t>1([4-68][0-9]|7[0-24-9]|9[0-4])|20[0-7]</t>
+  </si>
+  <si>
+    <t>regex_icd10_rcs</t>
+  </si>
+  <si>
+    <t>regex_icd9cm_deyo</t>
+  </si>
+  <si>
+    <t>regex_icd9cm_enhanced</t>
+  </si>
+  <si>
+    <t>44(39|1)|7854|V434</t>
+  </si>
+  <si>
+    <t>490|50([0-5]|64)</t>
+  </si>
+  <si>
+    <t>7(1(0[014]|4([0-2]|81))|25)</t>
+  </si>
+  <si>
+    <t>53[1-4]</t>
+  </si>
+  <si>
+    <t>571[24-6]</t>
+  </si>
+  <si>
+    <t>250[0-37]</t>
+  </si>
+  <si>
+    <t>250[4-6]</t>
+  </si>
+  <si>
+    <t>34(41|2)</t>
+  </si>
+  <si>
+    <t>58([2568]|3[0-7])</t>
+  </si>
+  <si>
+    <t>(1([4-68]|7[0-24-9]|9([0-4]|5[0-8])))|20[0-8]</t>
+  </si>
+  <si>
+    <t>456[01]|572[2-8]</t>
+  </si>
+  <si>
+    <t>19([6-8]|9[01])</t>
+  </si>
+  <si>
+    <t>04[2-4]</t>
+  </si>
+  <si>
+    <t>KVA</t>
+  </si>
+  <si>
+    <t>regex_kva</t>
+  </si>
+  <si>
+    <t>39891|4(0(2([01]1|91)|4([019][13]))|2(5[4-9]|8))</t>
+  </si>
+  <si>
+    <t>0930|4(373|4[01]|3[1-9]|471)|557[19]|V434</t>
+  </si>
+  <si>
+    <t>36234|43[0-8]</t>
+  </si>
+  <si>
+    <t>29(0|41)|3312</t>
+  </si>
+  <si>
+    <t>4(16[89]|90)|50([0-5]|64|8[18])</t>
+  </si>
+  <si>
+    <t>4465|7(1(0[0-4]|4[0-28])|25)</t>
+  </si>
+  <si>
+    <t>070([23]{2}|[45]4|[69])|57([01]|3[3489])|V427</t>
+  </si>
+  <si>
+    <t>250[0-389]</t>
+  </si>
+  <si>
+    <t>250[4-7]</t>
+  </si>
+  <si>
+    <t>3(341|4([23]|4[0-69]))</t>
+  </si>
+  <si>
+    <t>40(3([019]1)|4([019][23]))|58([256]|3[0-7]|80)|V(4(20|51)|56)</t>
+  </si>
+  <si>
+    <t>1([4-68]|7[0-24-9]|9([0-4]|5[0-8]))|2(0[0-8]|386)</t>
+  </si>
+  <si>
+    <t>456[0-2]|572[2-8]</t>
+  </si>
+  <si>
+    <t>I2([12]|52)</t>
+  </si>
+  <si>
+    <t>I(1[13]|255|4[23]|5(0|17))</t>
+  </si>
+  <si>
+    <t>I2([1-3]|52)</t>
+  </si>
+  <si>
+    <t>M(0[56]|3(15|[2-4]|5[13]|60))</t>
+  </si>
+  <si>
+    <t>K2[5-8]</t>
+  </si>
+  <si>
+    <t>E1[0-4][01689]</t>
+  </si>
+  <si>
+    <t>G(041|114|8(0[12]|[12]|3[0-49]))</t>
+  </si>
+  <si>
+    <t>G(114|8[1-3])</t>
+  </si>
+  <si>
+    <t>E1[0-4][2-57]</t>
+  </si>
+  <si>
+    <t>E1[0-4]</t>
+  </si>
+  <si>
+    <t>C([01]|2[0-6]|3[0-47-9]|4[0135-9]|5[0-8]|6|7[0-6]|8[1-58]|9[0-7])</t>
+  </si>
+  <si>
+    <t>C(7[7-9]|80)</t>
+  </si>
+  <si>
+    <t>B2[0124]</t>
+  </si>
+  <si>
+    <t>B2[0-4]</t>
+  </si>
+  <si>
+    <t>I(099|1(10|3[02])|255|4(2[05-9]|3)|50)|P290</t>
+  </si>
+  <si>
+    <t>I7([01]|3[189]|71|9[02])|K55[189]|Z95[89]</t>
+  </si>
+  <si>
+    <t>G4[56]|H340|I6</t>
+  </si>
+  <si>
+    <t>F0([0-3]|51)|G3(0|11)</t>
+  </si>
+  <si>
+    <t>(I27[89])|J(4[0-7]|6([0-7]|84)|70[13])</t>
+  </si>
+  <si>
+    <t>B18|K7(0[0-39]|1[3457]|[34]|6[023489])|Z944</t>
+  </si>
+  <si>
+    <t>I1(20|31)|N(0([35][2-7])|1[89]|250)|Z(49[012]|9(40|92))</t>
+  </si>
+  <si>
+    <t>I(8(5[09]|64)|982)|K7(04|[12]1|29|6[5-7])</t>
+  </si>
+  <si>
+    <t>(I7([0-3]|7[01]))|K55[189]|R02|Z95[89]</t>
+  </si>
+  <si>
+    <t>G4[56]|I6</t>
+  </si>
+  <si>
+    <t>A810|F0([0-3]|51)|G3[01]</t>
+  </si>
+  <si>
+    <t>I1[23]|N(0[13578]|17[12]|1[89]|25)|Z(49|9(40|92))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B18|I(8(5|64)|982)|K7([016]|2[19])|R162|Z944
 </t>
   </si>
   <si>
-    <t>sum_all_ahrq</t>
-  </si>
-  <si>
-    <t>ahrq_mort</t>
-  </si>
-  <si>
-    <t>ahrq_readm</t>
-  </si>
-  <si>
-    <t>condition</t>
-  </si>
-  <si>
-    <t>DA surgical complications</t>
-  </si>
-  <si>
-    <t>DB1 hip related</t>
-  </si>
-  <si>
-    <t>DB2 hip related</t>
-  </si>
-  <si>
-    <t>DC CVD</t>
-  </si>
-  <si>
-    <t>DM1 other</t>
-  </si>
-  <si>
-    <t>DM2 other</t>
-  </si>
-  <si>
-    <t>hbdia1_hdia</t>
-  </si>
-  <si>
-    <t>late_hdia</t>
-  </si>
-  <si>
-    <t>^(G(97[89])|M96(6F|[89])|(T8((1([02-9]|8W))|(4([03578]F?)|[49])|(8[89]))))$</t>
-  </si>
-  <si>
-    <t>^(G57[0-2]|M((00(0F?|[289]F))|(24(3|4F?)))|S7([4-6][0-9]{0,2}|30))$</t>
-  </si>
-  <si>
-    <t>^(M(24[056]F|6(10|21|6[23])F|8((43|6[01])F|66F?|95E)))$</t>
-  </si>
-  <si>
-    <t>^(I((2([14][[:alnum:]]*|6[09]))|4(6[019]|90)|6([0-35-6]|49)|7([24]|7[0-2]))|J8[01]9)|T811$</t>
-  </si>
-  <si>
-    <t>^(I80[[:alnum:]]*|J((1[3-8][[:alnum:]]*)|9(5[23589]|6[[:alnum:]]*|81))|K2[5-7][[:alnum:]]*|L89[[:alnum:]]*|N(99[089]|(17[[:alnum:]]*))|R339)$</t>
-  </si>
-  <si>
-    <t>^NF([CF-HJ-MS-TW]\\d{2}|A(02|1[12]|2[0-2])|Q09|U[013489]9)|QD(A10|B(0[05]|99)|E35|G30)|TNF(05|10)$</t>
-  </si>
-  <si>
-    <t>post_op</t>
-  </si>
-  <si>
-    <t>^(N(FQ[019]9|G([ACEGHJLSUW]|B59|F(0[12]|1[0-2]|9[12])|K[01]9|[MQ]09|T[01]9))|QD(A10|B[^1]|E35|G)|TNG(05|10))</t>
-  </si>
-  <si>
-    <t>DB1 knee related</t>
-  </si>
-  <si>
-    <t>DB2 knee related</t>
-  </si>
-  <si>
-    <t>^(G(97[89])|M96(6G|[89])|(T8((1([02-9]|8W))|(4([03-578]G?)|9)|(8[89]))))$</t>
-  </si>
-  <si>
-    <t>^(G57[34]|M(24[34])|M(00(0G?|[289]G)|2(2[01]|36|44G)|6(21|6[23])G|843G)|S(342|724|8([01]0|2[01]|3([01]|4[LM]|5[RSX])|4[01])))$</t>
-  </si>
-  <si>
-    <t>^M(2(35|4[056]|56)|659G|8((6[01]G|6G?)|95G))$</t>
-  </si>
-  <si>
-    <t>^(J2[0-2][[:alnum:]]*|K(590|29[[:alnum:]]*)|N991)$</t>
-  </si>
-  <si>
-    <t>HIV</t>
-  </si>
-  <si>
-    <t>^R0[16]A[CDEX][0125][1-35-9]$</t>
-  </si>
-  <si>
-    <t>^N05BA[01][1246]$</t>
-  </si>
-  <si>
-    <t>^G04CA0[23]$</t>
-  </si>
-  <si>
-    <t>^N06AX$</t>
-  </si>
-  <si>
-    <t>^S01E[A-EX][05][1-5]$</t>
-  </si>
-  <si>
-    <t>^M04A[A-C]01$</t>
-  </si>
-  <si>
-    <t>^J05AB54$</t>
-  </si>
-  <si>
-    <t>^V03AE01$</t>
-  </si>
-  <si>
-    <t>^C10[AB][ABCX][01][1-579]$</t>
-  </si>
-  <si>
-    <t>^H03AA0[12]$</t>
-  </si>
-  <si>
-    <t>^C01DA[01][248]$</t>
-  </si>
-  <si>
-    <t>^B05BA03$</t>
-  </si>
-  <si>
-    <t>^A09AA02$</t>
-  </si>
-  <si>
-    <t>^N04[AB][ACDX]0[1-79]$</t>
-  </si>
-  <si>
-    <t>^N07BB0[1345]$</t>
-  </si>
-  <si>
-    <t>^B01A[AB][01][0-69]$</t>
-  </si>
-  <si>
-    <t>^B01AC[0-4679]$</t>
-  </si>
-  <si>
-    <t>^C01[AB][A-D]0[13457]$</t>
-  </si>
-  <si>
-    <t>^G04CA0[1-3]$</t>
-  </si>
-  <si>
-    <t>^N0[35]A[EGHNX][01][1-49]$</t>
-  </si>
-  <si>
-    <t>^C0[39][ACD][AC][01][0-79]$</t>
-  </si>
-  <si>
-    <t>^N04D[AX]0[1-4]$</t>
-  </si>
-  <si>
-    <t>^N06A[ABGX][012][0-689]$</t>
-  </si>
-  <si>
-    <t>^A10[AB][A-HX][01][[:digit:]]$</t>
-  </si>
-  <si>
-    <t>^(B03XA0[1-3])|(A11CC0[1-4])$</t>
-  </si>
-  <si>
-    <t>^N03A[ABDEFGX][01][0-59]$</t>
-  </si>
-  <si>
-    <t>^A02B[A-DX][015][1-6]$</t>
-  </si>
-  <si>
-    <t>^J05A[ABEX][0156][12457]$</t>
-  </si>
-  <si>
-    <t>^J05A[EFGRX][016][[:digit:]]$</t>
-  </si>
-  <si>
-    <t>^C0[239][ABDEKX][ABCX][01][1-9]$</t>
-  </si>
-  <si>
-    <t>^C0[78][ACDF][ABG][01][1-7]$</t>
-  </si>
-  <si>
-    <t>^A07E[AC]0[1-46]$</t>
-  </si>
-  <si>
-    <t>^A06AD11$</t>
-  </si>
-  <si>
-    <t>^L01[A-DX][A-EX][0-5][[:digit:]]$</t>
-  </si>
-  <si>
-    <t>^B05BA[01][03]$</t>
-  </si>
-  <si>
-    <t>^N02C[ACX]0[1-6]$</t>
-  </si>
-  <si>
-    <t>^M05B[ABX]0[1-46-8]$</t>
-  </si>
-  <si>
-    <t>^N02A[ABEFGX][05][123569]$</t>
-  </si>
-  <si>
-    <t>^M01A[BCEHX][015][1-6]$</t>
-  </si>
-  <si>
-    <t>^D05[AB][ABX][05][12]$</t>
-  </si>
-  <si>
-    <t>^N05A[ABDEFHNX][01][1-68]$</t>
-  </si>
-  <si>
-    <t>^R03[A-D][ABCKLX][01][[:digit:]]$</t>
-  </si>
-  <si>
-    <t>^N07BA0[1-3]$</t>
-  </si>
-  <si>
-    <t>^H02AB(0[1246-9]|10)$</t>
-  </si>
-  <si>
-    <t>^L04AA[012][013468]$</t>
-  </si>
-  <si>
-    <t>^J04A[A-CKM]0[12456]$</t>
-  </si>
-  <si>
-    <t>oridinary</t>
-  </si>
-  <si>
-    <t>special</t>
-  </si>
-  <si>
-    <t>^[[:upper:]][0-9]{2}.?[0-9]{0,2}[[:upper:]]?$</t>
-  </si>
-  <si>
-    <t>^U[ABP][0-9]{2,4}$</t>
-  </si>
-  <si>
-    <t>only_ordinary</t>
-  </si>
-  <si>
-    <t>Mazda</t>
-  </si>
-  <si>
-    <t>Mer-Ben</t>
-  </si>
-  <si>
-    <t>Ford</t>
-  </si>
-  <si>
-    <t>Fiat</t>
-  </si>
-  <si>
-    <t>Toyota</t>
-  </si>
-  <si>
-    <t>Volksw</t>
-  </si>
-  <si>
-    <t>Geely</t>
-  </si>
-  <si>
-    <t>Merc</t>
-  </si>
-  <si>
-    <t>Ford|Lincoln</t>
-  </si>
-  <si>
-    <t>Chrysler|Fiat|Dodge|Ferrari|Maserati,</t>
-  </si>
-  <si>
-    <t>Porsche</t>
-  </si>
-  <si>
-    <t>Volvo|Lotus</t>
-  </si>
-  <si>
-    <t>^(I(4[457-9])|R00|T82|Z[49]5)</t>
-  </si>
-  <si>
-    <t>^I2[678]</t>
-  </si>
-  <si>
-    <t>^(I7[01389]|K55|Z95)</t>
-  </si>
-  <si>
-    <t>^I10</t>
-  </si>
-  <si>
-    <t>^G(04|11|8[0-3])</t>
-  </si>
-  <si>
-    <t>^(G(1[0-3]|2[0125]|3[125-7]|4[01]|93)|R47|R56)</t>
-  </si>
-  <si>
-    <t>^(I27|(J([46][0-7]|68)|70))</t>
-  </si>
-  <si>
-    <t>^E(0[0-3]|89)</t>
-  </si>
-  <si>
-    <t>^(I(1[23])|N(1[89]|25)|Z(49|9[49]))</t>
-  </si>
-  <si>
-    <t>^(B18|I(8[56]|98)|K7[0-467]|Z94)</t>
-  </si>
-  <si>
-    <t>^B2[0-24]</t>
-  </si>
-  <si>
-    <t>^C(8[1-58]|9[06])</t>
-  </si>
-  <si>
-    <t>^(L94|M(0[568]|12|3[0-5]|4[56]))</t>
-  </si>
-  <si>
-    <t>^D6[5-9]</t>
-  </si>
-  <si>
-    <t>^(E4[0-6]|R6[34])</t>
-  </si>
-  <si>
-    <t>^E(22|8[67])</t>
-  </si>
-  <si>
-    <t>^D50</t>
-  </si>
-  <si>
-    <t>^D5[0-3]</t>
-  </si>
-  <si>
-    <t>^(F10|E52|G62|I42|K(29|70)|T51|Z(50|7[12]))</t>
-  </si>
-  <si>
-    <t>^(F1[1-689]|Z7[12])</t>
-  </si>
-  <si>
-    <t>^F(20|3[1-4]|4[13])</t>
-  </si>
-  <si>
-    <t>^F(2[02-589]|3([01]2|15))</t>
-  </si>
-  <si>
-    <t>^F(2[02-589]|3[015])</t>
-  </si>
-  <si>
-    <t>^(I(09|1[13]|25|4[23]|50)|P29)</t>
-  </si>
-  <si>
-    <t>^(A52|I(0[5-9]|3[4-9])|Q23|Z95)</t>
-  </si>
-  <si>
-    <t>malignancy</t>
-  </si>
-  <si>
-    <t>^I(2([67]|8[089]))</t>
-  </si>
-  <si>
-    <t>regex_short</t>
-  </si>
-  <si>
-    <t>regex_garland</t>
-  </si>
-  <si>
-    <t>Alcohol dependence</t>
-  </si>
-  <si>
-    <t>Allergies</t>
-  </si>
-  <si>
-    <t>Anticoagulants</t>
-  </si>
-  <si>
-    <t>Antiplatelets</t>
-  </si>
-  <si>
-    <t>Anxiety</t>
-  </si>
-  <si>
-    <t>Arrhythmia</t>
-  </si>
-  <si>
-    <t>Benign prostatic hyperplasia</t>
-  </si>
-  <si>
-    <t>Bipolar disorder</t>
-  </si>
-  <si>
-    <t>Chronic airways disease</t>
-  </si>
-  <si>
-    <t>Congestive heart failure</t>
-  </si>
-  <si>
-    <t>Dementia</t>
-  </si>
-  <si>
-    <t>Depression</t>
-  </si>
-  <si>
-    <t>Diabetes</t>
-  </si>
-  <si>
-    <t>Renal disease</t>
-  </si>
-  <si>
-    <t>Epilepsy</t>
-  </si>
-  <si>
-    <t>Gastrooesophageal reflux disease</t>
-  </si>
-  <si>
-    <t>Glaucoma</t>
-  </si>
-  <si>
-    <t>Gout</t>
-  </si>
-  <si>
-    <t>Hepatitis C</t>
-  </si>
-  <si>
-    <t>Hyperkalaemia</t>
-  </si>
-  <si>
-    <t>Hyperlipidaemia</t>
-  </si>
-  <si>
-    <t>Hypertension</t>
-  </si>
-  <si>
-    <t>Hyperthyroidism</t>
-  </si>
-  <si>
-    <t>Inflammation/pain</t>
-  </si>
-  <si>
-    <t>Irritable bowel syndrome</t>
-  </si>
-  <si>
-    <t>Ischaemic heart disease: hypertension</t>
-  </si>
-  <si>
-    <t>Ischemic heart disease: angina</t>
-  </si>
-  <si>
-    <t>Liver failure</t>
-  </si>
-  <si>
-    <t>Malignancies</t>
-  </si>
-  <si>
-    <t>Malnutrition</t>
-  </si>
-  <si>
-    <t>Migraine</t>
-  </si>
-  <si>
-    <t>Osteoporosis/Paget's</t>
-  </si>
-  <si>
-    <t>Pain</t>
-  </si>
-  <si>
-    <t>Pancreatic insufficiency</t>
-  </si>
-  <si>
-    <t>Parkinson's disease</t>
-  </si>
-  <si>
-    <t>Psoriasis</t>
-  </si>
-  <si>
-    <t>Psychotic illness</t>
-  </si>
-  <si>
-    <t>Smoking cessation</t>
-  </si>
-  <si>
-    <t>Steroid-responsive disease</t>
-  </si>
-  <si>
-    <t>Transplant</t>
-  </si>
-  <si>
-    <t>Tuberculosis</t>
-  </si>
-  <si>
-    <t>Hepatitis B</t>
-  </si>
-  <si>
-    <t>Pulmonary hypertension</t>
-  </si>
-  <si>
-    <t xml:space="preserve">^J05AF(08|1[01])$ </t>
-  </si>
-  <si>
-    <t>^C02KX0[1-5]$</t>
-  </si>
-  <si>
-    <t>regex_caughey</t>
-  </si>
-  <si>
-    <t>^N07BB\\d{2}$</t>
-  </si>
-  <si>
-    <t>^R0(1A[CD]([0-5]\\d|60)|(6A([D-X]([01]\\d|2[0-7])|B04)))$</t>
-  </si>
-  <si>
-    <t>^B01A((A(0[3-9]|[1-9]\\d)|B0[0-6])|E07|F0[12]|X05)$</t>
-  </si>
-  <si>
-    <t>^B01AC(0[5-9]|[1-2]\\d|30)$</t>
-  </si>
-  <si>
-    <t>^N05B(A(0[1-9]|1[0-2])|E01)$</t>
-  </si>
-  <si>
-    <t>^C0(1(AA05|B([A-C]\\d{2}|D0[01]))|7AA07)$</t>
-  </si>
-  <si>
-    <t>^G04C(A\\d{2}|B0[12])$</t>
-  </si>
-  <si>
-    <t>^N05AN01$</t>
-  </si>
-  <si>
-    <t>^R03([A-D]([A-V]\\d{2}}|X05))$</t>
-  </si>
-  <si>
-    <t>^C0(3(DA(0[2-9]|\\d{2})|C([AB]\\d{2}|C01))|7A(B(0[27]|12)|G02)|9C[A-X]\\d{2})$</t>
-  </si>
-  <si>
-    <t>^N06A([A-F]\\d{2}|G0[0-2]|X(0[3-9]|1[0138])|2[1-6])$</t>
-  </si>
-  <si>
-    <t>^N06AD(A0[2-4]|X01)$</t>
-  </si>
-  <si>
-    <t>^S01E(A\\d{2}|B0[0-3]|C(0[3-9]|[1-9]\\d)|[D-X]\\d{2})$</t>
-  </si>
-  <si>
-    <t>^A02B([A-W]\\d{2}|X0[0-5])$</t>
-  </si>
-  <si>
-    <t>^M04A([AB]\\d{2}|C0[01])$</t>
-  </si>
-  <si>
-    <t>^A10[AB][[:alnum:]]{3}$</t>
-  </si>
-  <si>
-    <t>^N03A[[:alnum:]]{3}$</t>
-  </si>
-  <si>
-    <t>^H03B(A02|B01)$</t>
-  </si>
-  <si>
-    <t>Hypothyroidism</t>
-  </si>
-  <si>
-    <t>^A10BH03|C10([AB][A-W]\\d{2}|X0\\d)$</t>
-  </si>
-  <si>
-    <t>^(J05A(B54|E1[124]|X(1[45]|65)|B04)|L03AB[16][01])$</t>
-  </si>
-  <si>
-    <t>^J05A(E(0[1-9]|10)|F(0[1-79]|1[2-9]|[2-9]\\d)|G0[0-5]|R\\d{2}|X(0[7-9]|12)|)$</t>
-  </si>
-  <si>
-    <t>^C0(2(A(B\\d{2}|C0[0-5])|DB(0[2-9]|[1-9]\\d))|3(A([A-Z]\\d{2}|BA(0\\d|1[01]))|DB(01|99)|C([AB]\\d{2}|C0[01])|EA01)|9(BA0[2-9]|DA0[2-8]|C[A-X]\\d{2}))$</t>
-  </si>
-  <si>
-    <t>^(A07E(A0[1-26]|C0[1-4]|)|L04AA33)$</t>
-  </si>
-  <si>
-    <t>^C0(1D(A(0[2-9]|1[0-4])|X16)|8EX02)$</t>
-  </si>
-  <si>
-    <t>^C(0(7A(A(0[1-689]|[1-9]\\d)|B0[0-3]|G01)|8(C[A-Z]\\d{2}|DB0[01])|9(BB(0[2-9]|10)|D(B0[1-4]|X0[13])))|10BX03)$</t>
-  </si>
-  <si>
-    <t>^G04BD\\d{2}$</t>
-  </si>
-  <si>
-    <t>Incontinence</t>
-  </si>
-  <si>
-    <t>^M01A([B-G]\\d{2}|H0[0-6])$</t>
-  </si>
-  <si>
-    <t>^A0(6AD11|7AA11)$</t>
-  </si>
-  <si>
-    <t>^L01[A-X]{2}\\d{2}$</t>
-  </si>
-  <si>
-    <t>^B05BA(0[1-9]|10)$</t>
-  </si>
-  <si>
-    <t>^N02C[A-X]\\d{2}$</t>
-  </si>
-  <si>
-    <t>^(G03XC01|H05AA02|M05B(A\\d{2}|B0[0-5]|X0[34]))$</t>
-  </si>
-  <si>
-    <t>^N02(A([A-W]\\d{1}|X(0[26]|52))|BE51)$</t>
-  </si>
-  <si>
-    <t>^N04[AB][A-DX]\\d{2}$</t>
-  </si>
-  <si>
-    <t>^D05(A(A\\d{2}|C([0-4]\\d|5[01])|X[05]2)|BB0[12])$</t>
-  </si>
-  <si>
-    <t>^N05A(A\\d{2}|B(0[0-26-9]|[1-9]\\d)|[C-K]\\d{2}|L0[0-7]|X(0[7-9]|1[0-3]))$</t>
-  </si>
-  <si>
-    <t>^(A11CC0[1-4]|B03XA0[1-3]|V03AE0[235])$</t>
-  </si>
-  <si>
-    <t>^N0(7BA0[1-3]|6AX12)$</t>
-  </si>
-  <si>
-    <t>^H02AB(0\\d|10)$</t>
-  </si>
-  <si>
-    <t>^L04A(A(06|1[08])|D0[12])$</t>
-  </si>
-  <si>
-    <t>^J04A(C([0-4]\\d|5[01])|M\\d{2})$</t>
-  </si>
-  <si>
-    <t>^N07BB0[34]|V03AA01$</t>
-  </si>
-  <si>
-    <t>^R0(1A(C\\d{2}|D([0-5]\\d|60))|6A([D-W]\\d{2}|X([01]\\d|2[0-6])))$</t>
-  </si>
-  <si>
-    <t>^B01A(A(0[3-9]|[1-9]\\d)|B0[0-6])$</t>
-  </si>
-  <si>
-    <t>^B01AC(0[4-9]|[12]\\d|30)$</t>
-  </si>
-  <si>
-    <t>^N05BA(0\\d|1[0-2])$</t>
-  </si>
-  <si>
-    <t>^C01(AA05|B([A-C]\\d{2}|D0[01]))$</t>
-  </si>
-  <si>
-    <t>^C0(3(C([AB]\\d{2}|C0[01]))|9(AA(0\\d|10)|CA0[67]))$</t>
-  </si>
-  <si>
-    <t>^N06DA0[2-4]$</t>
-  </si>
-  <si>
-    <t>^N06A([A-F]\\d{2}|G0[0-2]|X(0\\d|1[0-8]))$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">^A10(A[A-X]\\d{2}|B([A-F]\\d{2}|G0[0-3]))$ </t>
-  </si>
-  <si>
-    <t>^(B03XA0[12]|A11CC0[1-4]|V03AE02)$</t>
-  </si>
-  <si>
-    <t>^N03A([A-W]\\d{2}|X14)$</t>
-  </si>
-  <si>
-    <t>^A02B([A-W]\\d{2}|X05)$</t>
-  </si>
-  <si>
-    <t>^S01E(A\\d{2}|B0[0-3]|C(0[3-9]|[[:alnum:]]{1,3}))$</t>
-  </si>
-  <si>
-    <t>^J05A(E(0[0-8])?|F\\d{2}|G0[0-3]|R.*|X07)$</t>
-  </si>
-  <si>
-    <t>^C10(A[A-X]\\d{2}|B[A-W]\\d{2}|X0[0-3])$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">^C0(2(A(B\\d{2}|C0[0-5])|[D-J][A-X]\\d{2}|K([A-W]\\d{2}|X0[10]))|3([AD][A-X]\\d{2}|BA(0\\d|1[01])|EA0[01])|9(BA0[2-9]|DA0[2-7]))$ </t>
-  </si>
-  <si>
-    <t>^C01DA0[2-4]$</t>
-  </si>
-  <si>
-    <t>^C0(7(A((A\\d{2}|B0[0-3])|[G-X]\\d{2})|[B-X][A-X]\\d{2})|8([A-C][A-X]\\d{2}|D(A\\d{2}|B0[01])))$</t>
-  </si>
-  <si>
-    <t>^N07BA0[1]$</t>
-  </si>
-  <si>
-    <t>^A07E(C0[1-4]|A0[12])$</t>
-  </si>
-  <si>
-    <t>^M05B(A\\d{2}|B0[0-3])$</t>
-  </si>
-  <si>
-    <t>^N02A[A-X]\\d{2}$</t>
-  </si>
-  <si>
-    <t>^N04([AB][A-X]\\d{2})$</t>
-  </si>
-  <si>
-    <t>^D05(A(A|X02)|BB0[12])$</t>
-  </si>
-  <si>
-    <t>^N05A(A\\d{2}|B(0[0-26-9]|[1-9]\\d)|[C-X]\\d{2})$</t>
-  </si>
-  <si>
-    <t>^R03(A(C(0[2-9]|[1-9]\\d)|[D-X]\\d{2})|[BC][A-X]\\d{2}|D([AB]\\d{2}|C0[0-3]))$</t>
-  </si>
-  <si>
-    <t>^L04AA([01]\\d|2[01])$</t>
-  </si>
-  <si>
-    <t>^J04A([B-J]\\d{2}|K0[0-2])$</t>
-  </si>
-  <si>
-    <t>index_pratt</t>
-  </si>
-  <si>
-    <t>41[02]</t>
-  </si>
-  <si>
-    <t>4(02|2[589])</t>
-  </si>
-  <si>
-    <t>44[0-7]|785E|V43D</t>
-  </si>
-  <si>
-    <t>362C|43[0-8]</t>
-  </si>
-  <si>
-    <t>29[04]</t>
-  </si>
-  <si>
-    <t>416|49[0-6]|50([0-5]|6D)</t>
-  </si>
-  <si>
-    <t>71[0-4]|725</t>
-  </si>
-  <si>
-    <t>070|456[A-C]|57[1-3]</t>
-  </si>
-  <si>
-    <t>34[2-4]</t>
-  </si>
-  <si>
-    <t>40[34]|58[0-68]|V4(20|51)</t>
-  </si>
-  <si>
-    <t>1([4-68][0-9]|7[0-24-9]|9[0-5])|20[0-8]</t>
-  </si>
-  <si>
-    <t>19[6-9]</t>
-  </si>
-  <si>
-    <t>279K</t>
-  </si>
-  <si>
-    <t>regex_icd9_brusselaers</t>
-  </si>
-  <si>
-    <t>regex_icd8_brusselaers</t>
-  </si>
-  <si>
-    <t>41[0-2]</t>
-  </si>
-  <si>
-    <t>4270|428</t>
-  </si>
-  <si>
-    <t>44[0-5]</t>
-  </si>
-  <si>
-    <t>43[0-8]</t>
-  </si>
-  <si>
-    <t>290[01]</t>
-  </si>
-  <si>
-    <t>49[0-3]|51[5-8]</t>
-  </si>
-  <si>
-    <t>7(1[0-2]|34)</t>
-  </si>
-  <si>
-    <t>070|4560|51[1-3]</t>
-  </si>
-  <si>
-    <t>40[34]|58[0-3]|792</t>
-  </si>
-  <si>
-    <t>1([4-68][0-9]|7[0-24-9]|9[0-4])|20[0-7]</t>
-  </si>
-  <si>
-    <t>regex_icd10_rcs</t>
-  </si>
-  <si>
-    <t>regex_icd9cm_deyo</t>
-  </si>
-  <si>
-    <t>regex_icd9cm_enhanced</t>
-  </si>
-  <si>
-    <t>44(39|1)|7854|V434</t>
-  </si>
-  <si>
-    <t>490|50([0-5]|64)</t>
-  </si>
-  <si>
-    <t>7(1(0[014]|4([0-2]|81))|25)</t>
-  </si>
-  <si>
-    <t>53[1-4]</t>
-  </si>
-  <si>
-    <t>571[24-6]</t>
-  </si>
-  <si>
-    <t>250[0-37]</t>
-  </si>
-  <si>
-    <t>250[4-6]</t>
-  </si>
-  <si>
-    <t>34(41|2)</t>
-  </si>
-  <si>
-    <t>58([2568]|3[0-7])</t>
-  </si>
-  <si>
-    <t>(1([4-68]|7[0-24-9]|9([0-4]|5[0-8])))|20[0-8]</t>
-  </si>
-  <si>
-    <t>456[01]|572[2-8]</t>
-  </si>
-  <si>
-    <t>19([6-8]|9[01])</t>
-  </si>
-  <si>
-    <t>04[2-4]</t>
-  </si>
-  <si>
-    <t>KVA</t>
-  </si>
-  <si>
-    <t>regex_kva</t>
-  </si>
-  <si>
-    <t>39891|4(0(2([01]1|91)|4([019][13]))|2(5[4-9]|8))</t>
-  </si>
-  <si>
-    <t>0930|4(373|4[01]|3[1-9]|471)|557[19]|V434</t>
-  </si>
-  <si>
-    <t>36234|43[0-8]</t>
-  </si>
-  <si>
-    <t>29(0|41)|3312</t>
-  </si>
-  <si>
-    <t>4(16[89]|90)|50([0-5]|64|8[18])</t>
-  </si>
-  <si>
-    <t>4465|7(1(0[0-4]|4[0-28])|25)</t>
-  </si>
-  <si>
-    <t>070([23]{2}|[45]4|[69])|57([01]|3[3489])|V427</t>
-  </si>
-  <si>
-    <t>250[0-389]</t>
-  </si>
-  <si>
-    <t>250[4-7]</t>
-  </si>
-  <si>
-    <t>3(341|4([23]|4[0-69]))</t>
-  </si>
-  <si>
-    <t>40(3([019]1)|4([019][23]))|58([256]|3[0-7]|80)|V(4(20|51)|56)</t>
-  </si>
-  <si>
-    <t>1([4-68]|7[0-24-9]|9([0-4]|5[0-8]))|2(0[0-8]|386)</t>
-  </si>
-  <si>
-    <t>456[0-2]|572[2-8]</t>
+    <t>I(2([67]|8[089]))</t>
+  </si>
+  <si>
+    <t>I2[678]</t>
+  </si>
+  <si>
+    <t>I10</t>
+  </si>
+  <si>
+    <t>I1[1-35]</t>
+  </si>
+  <si>
+    <t>G(04|11|8[0-3])</t>
+  </si>
+  <si>
+    <t>E1[0-4][019]</t>
+  </si>
+  <si>
+    <t>E1[0-4][23-8]</t>
+  </si>
+  <si>
+    <t>E(0[0-3]|890)</t>
+  </si>
+  <si>
+    <t>E(0[0-3]|89)</t>
+  </si>
+  <si>
+    <t>K2[5-8][79]</t>
+  </si>
+  <si>
+    <t>B2[0-24]</t>
+  </si>
+  <si>
+    <t>C(8[1-58]|9(6|0[02]))</t>
+  </si>
+  <si>
+    <t>C(8[1-58]|9[06])</t>
+  </si>
+  <si>
+    <t>C([01]|2[0-6]|3[0-47-9]|4[0135-9]|5[0-8]|6|7[0-6]|97)</t>
+  </si>
+  <si>
+    <t>D6([5-8]|9[13-6])</t>
+  </si>
+  <si>
+    <t>D6[5-9]</t>
+  </si>
+  <si>
+    <t>E66</t>
+  </si>
+  <si>
+    <t>E(222|8[67])</t>
+  </si>
+  <si>
+    <t>E(22|8[67])</t>
+  </si>
+  <si>
+    <t>D500</t>
+  </si>
+  <si>
+    <t>D50</t>
+  </si>
+  <si>
+    <t>D5(0[89]|[123])</t>
+  </si>
+  <si>
+    <t>D5[0-3]</t>
+  </si>
+  <si>
+    <t>F(2[02-589]|3([01]2|15))</t>
+  </si>
+  <si>
+    <t>F(2[02-589]|3[015])</t>
+  </si>
+  <si>
+    <t>F(204|3(1[345]|[23]|41)|4[13]2)</t>
+  </si>
+  <si>
+    <t>F(20|3[1-4]|4[13])</t>
+  </si>
+  <si>
+    <t>I(44[1-3]|456|459|4[7-9])|R00[018]|T821|Z[49]50</t>
+  </si>
+  <si>
+    <t>A520|I(0[5-8]|09[18]|3[4-9])|Q23[0-3]|Z95[2-4]</t>
+  </si>
+  <si>
+    <t>G(1[0-3]|2([012]|5[45])|3(1[289]|[25-7])|4[01]|93[14])|R470|R56</t>
+  </si>
+  <si>
+    <t>(I27[89])|(J(4[0-7]|6([0-7]|84)|70[13]))</t>
+  </si>
+  <si>
+    <t>I(120|131)|N(1[89]|250)|Z(49[012]|9(40|92))</t>
+  </si>
+  <si>
+    <t>B18|I(8(5|64)|982)|K7(0|1[13457]|[234]|6[02-9])|Z944</t>
+  </si>
+  <si>
+    <t>L94[013]|M(0[568]|12[03]|3(0|1[0-3]|[2-5])|4(5|6[189]))</t>
+  </si>
+  <si>
+    <t>E4[0-6]|R63?4</t>
+  </si>
+  <si>
+    <t>F10|E52|G621|I426|K(292|70[039])|T51|Z(502|7(14|21))</t>
+  </si>
+  <si>
+    <t>F1[1-689]|Z7(15|22)</t>
+  </si>
+  <si>
+    <t>I(09|1[13]|25|4[23]|50)|P29</t>
+  </si>
+  <si>
+    <t>I(4[457-9])|R00|T82|Z[49]5</t>
+  </si>
+  <si>
+    <t>A52|I(0[5-9]|3[4-9])|Q23|Z95</t>
+  </si>
+  <si>
+    <t>I7[01389]|K55|Z95</t>
+  </si>
+  <si>
+    <t>G(1[0-3]|2[0125]|3[125-7]|4[01]|93)|R47|R56</t>
+  </si>
+  <si>
+    <t>I27|(J([46][0-7]|68)|70)</t>
+  </si>
+  <si>
+    <t>I(1[23])|N(1[89]|25)|Z(49|9[49])</t>
+  </si>
+  <si>
+    <t>B18|I(8[56]|98)|K7[0-467]|Z94</t>
+  </si>
+  <si>
+    <t>L94|M(0[568]|12|3[0-5]|4[56])</t>
+  </si>
+  <si>
+    <t>E4[0-6]|R6[34]</t>
+  </si>
+  <si>
+    <t>F10|E52|G62|I42|K(29|70)|T51|Z(50|7[12])</t>
+  </si>
+  <si>
+    <t>F1[1-689]|Z7[12]</t>
+  </si>
+  <si>
+    <t>G(97[89])|M96(6F|[89])|(T8((1([02-9]|8W))|(4([03578]F?)|[49])|(8[89])))</t>
+  </si>
+  <si>
+    <t>G57[0-2]|M((00(0F?|[289]F))|(24(3|4F?)))|S7([4-6][0-9]{0,2}|30)</t>
+  </si>
+  <si>
+    <t>M(24[056]F|6(10|21|6[23])F|8((43|6[01])F|66F?|95E))</t>
+  </si>
+  <si>
+    <t>I((2([14][[:alnum:]]*|6[09]))|4(6[019]|90)|6([0-35-6]|49)|7([24]|7[0-2]))|J8[01]9)|T81</t>
+  </si>
+  <si>
+    <t>I80[[:alnum:]]*|J((1[3-8][[:alnum:]]*)|9(5[23589]|6[[:alnum:]]*|81))|K2[5-7][[:alnum:]]*|L89[[:alnum:]]*|N(99[089]|(17[[:alnum:]]*))|R339</t>
+  </si>
+  <si>
+    <t>J2[0-2][[:alnum:]]*|K(590|29[[:alnum:]]*)|N991</t>
+  </si>
+  <si>
+    <t>G(97[89])|M96(6G|[89])|(T8((1([02-9]|8W))|(4([03-578]G?)|9)|(8[89])))</t>
+  </si>
+  <si>
+    <t>G57[34]|M(24[34])|M(00(0G?|[289]G)|2(2[01]|36|44G)|6(21|6[23])G|843G)|S(342|724|8([01]0|2[01]|3([01]|4[LM]|5[RSX])|4[01]))</t>
+  </si>
+  <si>
+    <t>M(2(35|4[056]|56)|659G|8((6[01]G|6G?)|95G))</t>
+  </si>
+  <si>
+    <t>(I((2([14][[:alnum:]]*|6[09]))|4(6[019]|90)|6([0-35-6]|49)|7([24]|7[0-2]))|J8[01]9)|T811</t>
+  </si>
+  <si>
+    <t>N07BB\\d{2}</t>
+  </si>
+  <si>
+    <t>N07BB0[34]|V03AA01</t>
+  </si>
+  <si>
+    <t>N07BB0[1345]</t>
+  </si>
+  <si>
+    <t>R0(1A[CD]([0-5]\\d|60)|(6A([D-X]([01]\\d|2[0-7])|B04)))</t>
+  </si>
+  <si>
+    <t>R0(1A(C\\d{2}|D([0-5]\\d|60))|6A([D-W]\\d{2}|X([01]\\d|2[0-6])))</t>
+  </si>
+  <si>
+    <t>R0[16]A[CDEX][0125][1-35-9]</t>
+  </si>
+  <si>
+    <t>B01A((A(0[3-9]|[1-9]\\d)|B0[0-6])|E07|F0[12]|X05)</t>
+  </si>
+  <si>
+    <t>B01A(A(0[3-9]|[1-9]\\d)|B0[0-6])</t>
+  </si>
+  <si>
+    <t>B01A[AB][01][0-69]</t>
+  </si>
+  <si>
+    <t>B01AC(0[5-9]|[1-2]\\d|30)</t>
+  </si>
+  <si>
+    <t>B01AC(0[4-9]|[12]\\d|30)</t>
+  </si>
+  <si>
+    <t>B01AC[0-4679]</t>
+  </si>
+  <si>
+    <t>N05B(A(0[1-9]|1[0-2])|E01)</t>
+  </si>
+  <si>
+    <t>N05BA(0\\d|1[0-2])</t>
+  </si>
+  <si>
+    <t>N05BA[01][1246]</t>
+  </si>
+  <si>
+    <t>C0(1(AA05|B([A-C]\\d{2}|D0[01]))|7AA07)</t>
+  </si>
+  <si>
+    <t>C01(AA05|B([A-C]\\d{2}|D0[01]))</t>
+  </si>
+  <si>
+    <t>C01[AB][A-D]0[13457]</t>
+  </si>
+  <si>
+    <t>G04C(A\\d{2}|B0[12])</t>
+  </si>
+  <si>
+    <t>G04CA0[23]</t>
+  </si>
+  <si>
+    <t>G04CA0[1-3]</t>
+  </si>
+  <si>
+    <t>N05AN01</t>
+  </si>
+  <si>
+    <t>N06AX</t>
+  </si>
+  <si>
+    <t>N0[35]A[EGHNX][01][1-49]</t>
+  </si>
+  <si>
+    <t>R03([A-D]([A-V]\\d{2}}|X05))</t>
+  </si>
+  <si>
+    <t>R03(A(C(0[2-9]|[1-9]\\d)|[D-X]\\d{2})|[BC][A-X]\\d{2}|D([AB]\\d{2}|C0[0-3]))</t>
+  </si>
+  <si>
+    <t>R03[A-D][ABCKLX][01][[:digit:]]</t>
+  </si>
+  <si>
+    <t>C0(3(DA(0[2-9]|\\d{2})|C([AB]\\d{2}|C01))|7A(B(0[27]|12)|G02)|9C[A-X]\\d{2})</t>
+  </si>
+  <si>
+    <t>C0(3(C([AB]\\d{2}|C0[01]))|9(AA(0\\d|10)|CA0[67]))</t>
+  </si>
+  <si>
+    <t>C0[39][ACD][AC][01][0-79]</t>
+  </si>
+  <si>
+    <t>N06AD(A0[2-4]|X01)</t>
+  </si>
+  <si>
+    <t>N06DA0[2-4]</t>
+  </si>
+  <si>
+    <t>N04D[AX]0[1-4]</t>
+  </si>
+  <si>
+    <t>N06A([A-F]\\d{2}|G0[0-2]|X(0[3-9]|1[0138])|2[1-6])</t>
+  </si>
+  <si>
+    <t>N06A([A-F]\\d{2}|G0[0-2]|X(0\\d|1[0-8]))</t>
+  </si>
+  <si>
+    <t>N06A[ABGX][012][0-689]</t>
+  </si>
+  <si>
+    <t>A10[AB][[:alnum:]]{3}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A10(A[A-X]\\d{2}|B([A-F]\\d{2}|G0[0-3])) </t>
+  </si>
+  <si>
+    <t>A10[AB][A-HX][01][[:digit:]]</t>
+  </si>
+  <si>
+    <t>N03A[[:alnum:]]{3}</t>
+  </si>
+  <si>
+    <t>N03A([A-W]\\d{2}|X14)</t>
+  </si>
+  <si>
+    <t>N03A[ABDEFGX][01][0-59]</t>
+  </si>
+  <si>
+    <t>A02B([A-W]\\d{2}|X0[0-5])</t>
+  </si>
+  <si>
+    <t>A02B([A-W]\\d{2}|X05)</t>
+  </si>
+  <si>
+    <t>A02B[A-DX][015][1-6]</t>
+  </si>
+  <si>
+    <t>S01E(A\\d{2}|B0[0-3]|C(0[3-9]|[1-9]\\d)|[D-X]\\d{2})</t>
+  </si>
+  <si>
+    <t>S01E(A\\d{2}|B0[0-3]|C(0[3-9]|[[:alnum:]]{1,3}))</t>
+  </si>
+  <si>
+    <t>S01E[A-EX][05][1-5]</t>
+  </si>
+  <si>
+    <t>M04A([AB]\\d{2}|C0[01])</t>
+  </si>
+  <si>
+    <t>M04A[A-C]01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J05AF(08|1[01]) </t>
+  </si>
+  <si>
+    <t>J05AB54</t>
+  </si>
+  <si>
+    <t>J05A[ABEX][0156][12457]</t>
+  </si>
+  <si>
+    <t>J05A(E(0[1-9]|10)|F(0[1-79]|1[2-9]|[2-9]\\d)|G0[0-5]|R\\d{2}|X(0[7-9]|12)|)</t>
+  </si>
+  <si>
+    <t>J05A(E(0[0-8])?|F\\d{2}|G0[0-3]|R.*|X07)</t>
+  </si>
+  <si>
+    <t>J05A[EFGRX][016][[:digit:]]</t>
+  </si>
+  <si>
+    <t>V03AE01</t>
+  </si>
+  <si>
+    <t>A10BH03|C10([AB][A-W]\\d{2}|X0\\d)</t>
+  </si>
+  <si>
+    <t>C10(A[A-X]\\d{2}|B[A-W]\\d{2}|X0[0-3])</t>
+  </si>
+  <si>
+    <t>C10[AB][ABCX][01][1-579]</t>
+  </si>
+  <si>
+    <t>C0(2(A(B\\d{2}|C0[0-5])|DB(0[2-9]|[1-9]\\d))|3(A([A-Z]\\d{2}|BA(0\\d|1[01]))|DB(01|99)|C([AB]\\d{2}|C0[01])|EA01)|9(BA0[2-9]|DA0[2-8]|C[A-X]\\d{2}))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C0(2(A(B\\d{2}|C0[0-5])|[D-J][A-X]\\d{2}|K([A-W]\\d{2}|X0[10]))|3([AD][A-X]\\d{2}|BA(0\\d|1[01])|EA0[01])|9(BA0[2-9]|DA0[2-7])) </t>
+  </si>
+  <si>
+    <t>C0[239][ABDEKX][ABCX][01][1-9]</t>
+  </si>
+  <si>
+    <t>H03AA0[12]</t>
+  </si>
+  <si>
+    <t>H03B(A02|B01)</t>
+  </si>
+  <si>
+    <t>G04BD\\d{2}</t>
+  </si>
+  <si>
+    <t>M01A([B-G]\\d{2}|H0[0-6])</t>
+  </si>
+  <si>
+    <t>M01A[BCEHX][015][1-6]</t>
+  </si>
+  <si>
+    <t>A07E(C0[1-4]|A0[12])</t>
+  </si>
+  <si>
+    <t>A07E[AC]0[1-46]</t>
+  </si>
+  <si>
+    <t>C(0(7A(A(0[1-689]|[1-9]\\d)|B0[0-3]|G01)|8(C[A-Z]\\d{2}|DB0[01])|9(BB(0[2-9]|10)|D(B0[1-4]|X0[13])))|10BX03)</t>
+  </si>
+  <si>
+    <t>C0(7(A((A\\d{2}|B0[0-3])|[G-X]\\d{2})|[B-X][A-X]\\d{2})|8([A-C][A-X]\\d{2}|D(A\\d{2}|B0[01])))</t>
+  </si>
+  <si>
+    <t>C0[78][ACDF][ABG][01][1-7]</t>
+  </si>
+  <si>
+    <t>C0(1D(A(0[2-9]|1[0-4])|X16)|8EX02)</t>
+  </si>
+  <si>
+    <t>C01DA0[2-4]</t>
+  </si>
+  <si>
+    <t>C01DA[01][248]</t>
+  </si>
+  <si>
+    <t>A0(6AD11|7AA11)</t>
+  </si>
+  <si>
+    <t>A06AD11</t>
+  </si>
+  <si>
+    <t>L01[A-X]{2}\\d{2}</t>
+  </si>
+  <si>
+    <t>L01[A-DX][A-EX][0-5][[:digit:]]</t>
+  </si>
+  <si>
+    <t>B05BA(0[1-9]|10)</t>
+  </si>
+  <si>
+    <t>B05BA03</t>
+  </si>
+  <si>
+    <t>B05BA[01][03]</t>
+  </si>
+  <si>
+    <t>N02C[A-X]\\d{2}</t>
+  </si>
+  <si>
+    <t>N02C[ACX]0[1-6]</t>
+  </si>
+  <si>
+    <t>M05B(A\\d{2}|B0[0-3])</t>
+  </si>
+  <si>
+    <t>M05B[ABX]0[1-46-8]</t>
+  </si>
+  <si>
+    <t>N02(A([A-W]\\d{1}|X(0[26]|52))|BE51)</t>
+  </si>
+  <si>
+    <t>N02A[A-X]\\d{2}</t>
+  </si>
+  <si>
+    <t>N02A[ABEFGX][05][123569]</t>
+  </si>
+  <si>
+    <t>A09AA02</t>
+  </si>
+  <si>
+    <t>N04[AB][A-DX]\\d{2}</t>
+  </si>
+  <si>
+    <t>N04([AB][A-X]\\d{2})</t>
+  </si>
+  <si>
+    <t>N04[AB][ACDX]0[1-79]</t>
+  </si>
+  <si>
+    <t>D05(A(A\\d{2}|C([0-4]\\d|5[01])|X[05]2)|BB0[12])</t>
+  </si>
+  <si>
+    <t>D05(A(A|X02)|BB0[12])</t>
+  </si>
+  <si>
+    <t>D05[AB][ABX][05][12]</t>
+  </si>
+  <si>
+    <t>N05A(A\\d{2}|B(0[0-26-9]|[1-9]\\d)|[C-K]\\d{2}|L0[0-7]|X(0[7-9]|1[0-3]))</t>
+  </si>
+  <si>
+    <t>N05A(A\\d{2}|B(0[0-26-9]|[1-9]\\d)|[C-X]\\d{2})</t>
+  </si>
+  <si>
+    <t>N05A[ABDEFHNX][01][1-68]</t>
+  </si>
+  <si>
+    <t>C02KX0[1-5]</t>
+  </si>
+  <si>
+    <t>(B03XA0[1-3])|(A11CC0[1-4])</t>
+  </si>
+  <si>
+    <t>N0(7BA0[1-3]|6AX12)</t>
+  </si>
+  <si>
+    <t>N07BA0[1]</t>
+  </si>
+  <si>
+    <t>N07BA0[1-3]</t>
+  </si>
+  <si>
+    <t>H02AB(0\\d|10)</t>
+  </si>
+  <si>
+    <t>H02AB(0[1246-9]|10)</t>
+  </si>
+  <si>
+    <t>L04A(A(06|1[08])|D0[12])</t>
+  </si>
+  <si>
+    <t>L04AA([01]\\d|2[01])</t>
+  </si>
+  <si>
+    <t>L04AA[012][013468]</t>
+  </si>
+  <si>
+    <t>J04A(C([0-4]\\d|5[01])|M\\d{2})</t>
+  </si>
+  <si>
+    <t>J04A([B-J]\\d{2}|K0[0-2])</t>
+  </si>
+  <si>
+    <t>J04A[A-CKM]0[12456]</t>
+  </si>
+  <si>
+    <t>J05A(B54|E1[124]|X(1[45]|65)|B04)|L03AB[16][01]</t>
+  </si>
+  <si>
+    <t>A07E(A0[1-26]|C0[1-4]|)|L04AA33</t>
+  </si>
+  <si>
+    <t>G03XC01|H05AA02|M05B(A\\d{2}|B0[0-5]|X0[34])</t>
+  </si>
+  <si>
+    <t>A11CC0[1-4]|B03XA0[1-3]|V03AE0[235]</t>
+  </si>
+  <si>
+    <t>B03XA0[12]|A11CC0[1-4]|V03AE02</t>
+  </si>
+  <si>
+    <t>[[:upper:]][0-9]{2}.?[0-9]{0,2}[[:upper:]]?</t>
+  </si>
+  <si>
+    <t>U[ABP][0-9]{2,4}</t>
   </si>
 </sst>
 </file>
@@ -1336,9 +1339,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -1347,6 +1347,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1650,58 +1653,58 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>201</v>
+        <v>94</v>
       </c>
       <c r="B2" t="s">
-        <v>201</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>202</v>
+        <v>95</v>
       </c>
       <c r="B3" t="s">
-        <v>208</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>203</v>
+        <v>96</v>
       </c>
       <c r="B4" t="s">
-        <v>209</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>204</v>
+        <v>97</v>
       </c>
       <c r="B5" t="s">
-        <v>210</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>205</v>
+        <v>98</v>
       </c>
       <c r="B6" t="s">
-        <v>205</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>206</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>211</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>207</v>
+        <v>100</v>
       </c>
       <c r="B8" t="s">
-        <v>212</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1713,20 +1716,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMO18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.42578125" customWidth="1"/>
-    <col min="2" max="2" width="53.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="61.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="61.42578125" customWidth="1"/>
-    <col min="6" max="6" width="61.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="61.42578125" customWidth="1"/>
-    <col min="8" max="8" width="55.7109375" customWidth="1"/>
+    <col min="6" max="6" width="61.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="61.42578125" style="6" customWidth="1"/>
+    <col min="8" max="8" width="55.7109375" style="6" customWidth="1"/>
     <col min="9" max="9" width="8.42578125" customWidth="1"/>
     <col min="10" max="10" width="14.140625" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
@@ -1746,20 +1749,20 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>387</v>
+      <c r="D1" s="5" t="s">
+        <v>182</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>388</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>374</v>
+        <v>183</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>169</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>3</v>
@@ -1785,26 +1788,26 @@
       <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>361</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>361</v>
-      </c>
-      <c r="F2" t="s">
-        <v>113</v>
-      </c>
-      <c r="G2" t="s">
-        <v>376</v>
-      </c>
-      <c r="H2" t="s">
-        <v>361</v>
+        <v>212</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>156</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -1827,28 +1830,28 @@
     </row>
     <row r="3" spans="1:14 1029:1029" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>13</v>
-      </c>
       <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="7">
+        <v>226</v>
+      </c>
+      <c r="D3" s="6">
         <v>428</v>
       </c>
       <c r="E3" t="s">
-        <v>404</v>
-      </c>
-      <c r="F3" t="s">
-        <v>114</v>
-      </c>
-      <c r="G3" t="s">
-        <v>377</v>
-      </c>
-      <c r="H3" t="s">
-        <v>362</v>
+        <v>199</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>157</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -1871,28 +1874,28 @@
     </row>
     <row r="4" spans="1:14 1029:1029" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>389</v>
+        <v>227</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>184</v>
       </c>
       <c r="E4" t="s">
-        <v>405</v>
-      </c>
-      <c r="F4" t="s">
-        <v>115</v>
-      </c>
-      <c r="G4" t="s">
-        <v>378</v>
-      </c>
-      <c r="H4" t="s">
-        <v>363</v>
+        <v>200</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>158</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -1915,28 +1918,28 @@
     </row>
     <row r="5" spans="1:14 1029:1029" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>19</v>
+        <v>15</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>379</v>
+        <v>228</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>174</v>
       </c>
       <c r="E5" t="s">
-        <v>406</v>
-      </c>
-      <c r="F5" t="s">
-        <v>116</v>
-      </c>
-      <c r="G5" t="s">
-        <v>379</v>
-      </c>
-      <c r="H5" t="s">
-        <v>364</v>
+        <v>201</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>159</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -1959,28 +1962,28 @@
     </row>
     <row r="6" spans="1:14 1029:1029" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="7">
+        <v>229</v>
+      </c>
+      <c r="D6" s="6">
         <v>290</v>
       </c>
       <c r="E6" t="s">
-        <v>407</v>
-      </c>
-      <c r="F6" t="s">
-        <v>117</v>
-      </c>
-      <c r="G6" t="s">
-        <v>380</v>
-      </c>
-      <c r="H6" t="s">
-        <v>365</v>
+        <v>202</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>160</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -2003,28 +2006,28 @@
     </row>
     <row r="7" spans="1:14 1029:1029" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>25</v>
+        <v>19</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>390</v>
+        <v>230</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>185</v>
       </c>
       <c r="E7" t="s">
-        <v>408</v>
-      </c>
-      <c r="F7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" t="s">
-        <v>381</v>
-      </c>
-      <c r="H7" t="s">
-        <v>366</v>
+        <v>203</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>161</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -2047,28 +2050,28 @@
     </row>
     <row r="8" spans="1:14 1029:1029" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>28</v>
+        <v>21</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>391</v>
+        <v>215</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>186</v>
       </c>
       <c r="E8" t="s">
-        <v>409</v>
-      </c>
-      <c r="F8" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" t="s">
-        <v>382</v>
-      </c>
-      <c r="H8" t="s">
-        <v>367</v>
+        <v>204</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>162</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -2091,19 +2094,19 @@
     </row>
     <row r="9" spans="1:14 1029:1029" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>31</v>
+        <v>23</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>392</v>
+        <v>216</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>187</v>
       </c>
       <c r="E9" t="s">
-        <v>392</v>
+        <v>187</v>
       </c>
       <c r="I9">
         <v>1</v>
@@ -2126,19 +2129,19 @@
     </row>
     <row r="10" spans="1:14 1029:1029" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>34</v>
+        <v>25</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>393</v>
+        <v>231</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>188</v>
       </c>
       <c r="E10" t="s">
-        <v>410</v>
+        <v>205</v>
       </c>
       <c r="I10">
         <v>1</v>
@@ -2161,19 +2164,19 @@
     </row>
     <row r="11" spans="1:14 1029:1029" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>37</v>
+        <v>27</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>394</v>
+        <v>217</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>189</v>
       </c>
       <c r="E11" t="s">
-        <v>411</v>
+        <v>206</v>
       </c>
       <c r="I11">
         <v>1</v>
@@ -2196,28 +2199,28 @@
     </row>
     <row r="12" spans="1:14 1029:1029" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>40</v>
+        <v>29</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>396</v>
+        <v>218</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>191</v>
       </c>
       <c r="E12" t="s">
-        <v>413</v>
-      </c>
-      <c r="F12" t="s">
-        <v>118</v>
-      </c>
-      <c r="G12">
+        <v>208</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="G12" s="6">
         <v>344</v>
       </c>
-      <c r="H12" t="s">
-        <v>369</v>
+      <c r="H12" s="6" t="s">
+        <v>164</v>
       </c>
       <c r="I12">
         <v>2</v>
@@ -2240,28 +2243,28 @@
     </row>
     <row r="13" spans="1:14 1029:1029" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>43</v>
+        <v>31</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>397</v>
+        <v>232</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>192</v>
       </c>
       <c r="E13" t="s">
-        <v>414</v>
-      </c>
-      <c r="F13" t="s">
-        <v>119</v>
-      </c>
-      <c r="G13" t="s">
-        <v>384</v>
-      </c>
-      <c r="H13" t="s">
-        <v>370</v>
+        <v>209</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>165</v>
       </c>
       <c r="I13">
         <v>2</v>
@@ -2284,27 +2287,27 @@
     </row>
     <row r="14" spans="1:14 1029:1029" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>46</v>
+        <v>33</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>395</v>
+        <v>220</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>190</v>
       </c>
       <c r="E14" t="s">
-        <v>412</v>
-      </c>
-      <c r="F14" t="s">
-        <v>120</v>
-      </c>
-      <c r="G14">
+        <v>207</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="G14" s="6">
         <v>250</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="6">
         <v>250</v>
       </c>
       <c r="I14">
@@ -2328,28 +2331,28 @@
     </row>
     <row r="15" spans="1:14 1029:1029" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>238</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>48</v>
+        <v>106</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>398</v>
+        <v>222</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>193</v>
       </c>
       <c r="E15" t="s">
-        <v>415</v>
-      </c>
-      <c r="F15" t="s">
-        <v>49</v>
-      </c>
-      <c r="G15" t="s">
-        <v>385</v>
-      </c>
-      <c r="H15" t="s">
-        <v>371</v>
+        <v>210</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>166</v>
       </c>
       <c r="I15">
         <v>2</v>
@@ -2372,28 +2375,28 @@
     </row>
     <row r="16" spans="1:14 1029:1029" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>51</v>
+        <v>36</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="C16" t="s">
-        <v>52</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>399</v>
+        <v>233</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>194</v>
       </c>
       <c r="E16" t="s">
-        <v>416</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>368</v>
+        <v>211</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>163</v>
       </c>
       <c r="I16">
         <v>3</v>
@@ -2416,28 +2419,28 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>53</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>54</v>
+        <v>38</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>400</v>
+        <v>223</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>195</v>
       </c>
       <c r="E17" t="s">
-        <v>372</v>
-      </c>
-      <c r="F17" t="s">
-        <v>55</v>
-      </c>
-      <c r="G17" t="s">
-        <v>372</v>
-      </c>
-      <c r="H17" t="s">
-        <v>372</v>
+        <v>167</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>167</v>
       </c>
       <c r="I17">
         <v>6</v>
@@ -2460,25 +2463,25 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>56</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>57</v>
+        <v>40</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="C18" t="s">
-        <v>58</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>401</v>
+        <v>224</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>196</v>
       </c>
       <c r="E18" t="s">
-        <v>401</v>
-      </c>
-      <c r="F18" t="s">
-        <v>121</v>
-      </c>
-      <c r="H18" t="s">
-        <v>373</v>
+        <v>196</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>168</v>
       </c>
       <c r="I18">
         <v>6</v>
@@ -2510,7 +2513,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2530,39 +2533,39 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>240</v>
+        <v>107</v>
       </c>
       <c r="D1" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="E1" t="s">
-        <v>123</v>
+        <v>73</v>
       </c>
       <c r="F1" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="G1" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="H1" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="I1" t="s">
-        <v>124</v>
+        <v>74</v>
       </c>
       <c r="J1" t="s">
-        <v>125</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>226</v>
       </c>
       <c r="C2" t="s">
-        <v>236</v>
+        <v>276</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -2588,13 +2591,13 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>90</v>
+        <v>266</v>
       </c>
       <c r="C3" t="s">
-        <v>213</v>
+        <v>277</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -2620,13 +2623,13 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>91</v>
+        <v>267</v>
       </c>
       <c r="C4" t="s">
-        <v>237</v>
+        <v>278</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -2652,13 +2655,13 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
         <v>239</v>
       </c>
       <c r="C5" t="s">
-        <v>214</v>
+        <v>240</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -2684,13 +2687,13 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>227</v>
       </c>
       <c r="C6" t="s">
-        <v>215</v>
+        <v>279</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -2716,13 +2719,13 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C7" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -2748,13 +2751,13 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>92</v>
+        <v>242</v>
       </c>
       <c r="C8" t="s">
-        <v>92</v>
+        <v>242</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -2780,13 +2783,13 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>218</v>
       </c>
       <c r="C9" t="s">
-        <v>217</v>
+        <v>243</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -2812,13 +2815,13 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="B10" t="s">
-        <v>93</v>
+        <v>268</v>
       </c>
       <c r="C10" t="s">
-        <v>218</v>
+        <v>280</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -2844,13 +2847,13 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>94</v>
+        <v>269</v>
       </c>
       <c r="C11" t="s">
-        <v>219</v>
+        <v>281</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -2876,13 +2879,13 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>95</v>
+        <v>244</v>
       </c>
       <c r="C12" t="s">
-        <v>120</v>
+        <v>221</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -2908,13 +2911,13 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="B13" t="s">
-        <v>96</v>
+        <v>245</v>
       </c>
       <c r="C13" t="s">
-        <v>120</v>
+        <v>221</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -2940,13 +2943,13 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="B14" t="s">
-        <v>97</v>
+        <v>246</v>
       </c>
       <c r="C14" t="s">
-        <v>220</v>
+        <v>247</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -2972,13 +2975,13 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="B15" t="s">
-        <v>98</v>
+        <v>270</v>
       </c>
       <c r="C15" t="s">
-        <v>221</v>
+        <v>282</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -3004,13 +3007,13 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="B16" t="s">
-        <v>99</v>
+        <v>271</v>
       </c>
       <c r="C16" t="s">
-        <v>222</v>
+        <v>283</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -3036,13 +3039,13 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>100</v>
+        <v>248</v>
       </c>
       <c r="C17" t="s">
-        <v>32</v>
+        <v>216</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -3068,13 +3071,13 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="B18" t="s">
-        <v>58</v>
+        <v>224</v>
       </c>
       <c r="C18" t="s">
-        <v>223</v>
+        <v>249</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -3100,13 +3103,13 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="B19" t="s">
-        <v>101</v>
+        <v>250</v>
       </c>
       <c r="C19" t="s">
-        <v>224</v>
+        <v>251</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -3132,13 +3135,13 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="B20" t="s">
-        <v>55</v>
+        <v>223</v>
       </c>
       <c r="C20" t="s">
-        <v>55</v>
+        <v>223</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -3164,13 +3167,13 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="B21" t="s">
-        <v>102</v>
+        <v>252</v>
       </c>
       <c r="C21" t="s">
-        <v>102</v>
+        <v>252</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -3196,13 +3199,13 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="B22" t="s">
-        <v>103</v>
+        <v>272</v>
       </c>
       <c r="C22" t="s">
-        <v>225</v>
+        <v>284</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -3228,13 +3231,13 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="B23" t="s">
-        <v>104</v>
+        <v>253</v>
       </c>
       <c r="C23" t="s">
-        <v>226</v>
+        <v>254</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -3260,13 +3263,13 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="B24" t="s">
-        <v>105</v>
+        <v>255</v>
       </c>
       <c r="C24" t="s">
-        <v>105</v>
+        <v>255</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -3292,13 +3295,13 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="B25" t="s">
-        <v>106</v>
+        <v>273</v>
       </c>
       <c r="C25" t="s">
-        <v>227</v>
+        <v>285</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -3324,13 +3327,13 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="B26" t="s">
-        <v>107</v>
+        <v>256</v>
       </c>
       <c r="C26" t="s">
-        <v>228</v>
+        <v>257</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -3356,13 +3359,13 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="B27" t="s">
-        <v>108</v>
+        <v>258</v>
       </c>
       <c r="C27" t="s">
-        <v>229</v>
+        <v>259</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -3388,13 +3391,13 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="B28" t="s">
-        <v>109</v>
+        <v>260</v>
       </c>
       <c r="C28" t="s">
-        <v>230</v>
+        <v>261</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -3420,13 +3423,13 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="B29" t="s">
-        <v>110</v>
+        <v>274</v>
       </c>
       <c r="C29" t="s">
-        <v>231</v>
+        <v>286</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -3452,13 +3455,13 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="B30" t="s">
-        <v>111</v>
+        <v>275</v>
       </c>
       <c r="C30" t="s">
-        <v>232</v>
+        <v>287</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -3484,13 +3487,13 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="B31" t="s">
-        <v>234</v>
+        <v>262</v>
       </c>
       <c r="C31" t="s">
-        <v>235</v>
+        <v>263</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -3516,13 +3519,13 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="B32" t="s">
-        <v>112</v>
+        <v>264</v>
       </c>
       <c r="C32" t="s">
-        <v>233</v>
+        <v>265</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -3556,7 +3559,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3575,87 +3578,87 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>403</v>
+        <v>198</v>
       </c>
       <c r="D1" t="s">
-        <v>126</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>127</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>133</v>
+        <v>288</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>128</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>136</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>133</v>
+        <v>289</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>129</v>
+        <v>79</v>
       </c>
       <c r="B4" t="s">
-        <v>137</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>134</v>
+        <v>290</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="B5" t="s">
-        <v>138</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>133</v>
+        <v>291</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>131</v>
+        <v>81</v>
       </c>
       <c r="B6" t="s">
-        <v>139</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>133</v>
+        <v>292</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>132</v>
+        <v>82</v>
       </c>
       <c r="B7" t="s">
-        <v>148</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>134</v>
+        <v>293</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>402</v>
+        <v>197</v>
       </c>
       <c r="C8" t="s">
-        <v>140</v>
+        <v>85</v>
       </c>
       <c r="D8" t="s">
-        <v>141</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -3668,7 +3671,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3687,87 +3690,87 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>403</v>
+        <v>198</v>
       </c>
       <c r="D1" t="s">
-        <v>126</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>127</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
-        <v>145</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>133</v>
+        <v>294</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>143</v>
+        <v>88</v>
       </c>
       <c r="B3" t="s">
-        <v>146</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>133</v>
+        <v>295</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>144</v>
+        <v>89</v>
       </c>
       <c r="B4" t="s">
-        <v>147</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>134</v>
+        <v>296</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="B5" t="s">
-        <v>138</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>133</v>
+        <v>297</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>131</v>
+        <v>81</v>
       </c>
       <c r="B6" t="s">
-        <v>139</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>133</v>
+        <v>292</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>132</v>
+        <v>82</v>
       </c>
       <c r="B7" t="s">
-        <v>148</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>134</v>
+        <v>293</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>402</v>
+        <v>197</v>
       </c>
       <c r="C8" t="s">
-        <v>142</v>
+        <v>87</v>
       </c>
       <c r="D8" t="s">
-        <v>141</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -3779,8 +3782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3800,27 +3803,27 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>287</v>
+        <v>152</v>
       </c>
       <c r="D1" t="s">
-        <v>241</v>
+        <v>108</v>
       </c>
       <c r="E1" t="s">
-        <v>360</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>242</v>
+        <v>109</v>
       </c>
       <c r="B2" t="s">
-        <v>288</v>
+        <v>298</v>
       </c>
       <c r="C2" t="s">
-        <v>331</v>
+        <v>299</v>
       </c>
       <c r="D2" t="s">
-        <v>164</v>
+        <v>300</v>
       </c>
       <c r="E2">
         <v>6</v>
@@ -3828,16 +3831,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>243</v>
+        <v>110</v>
       </c>
       <c r="B3" t="s">
-        <v>289</v>
+        <v>301</v>
       </c>
       <c r="C3" t="s">
-        <v>332</v>
+        <v>302</v>
       </c>
       <c r="D3" t="s">
-        <v>150</v>
+        <v>303</v>
       </c>
       <c r="E3">
         <v>-1</v>
@@ -3845,16 +3848,16 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>244</v>
+        <v>111</v>
       </c>
       <c r="B4" t="s">
-        <v>290</v>
+        <v>304</v>
       </c>
       <c r="C4" t="s">
-        <v>333</v>
+        <v>305</v>
       </c>
       <c r="D4" t="s">
-        <v>165</v>
+        <v>306</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -3862,16 +3865,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>245</v>
+        <v>112</v>
       </c>
       <c r="B5" t="s">
-        <v>291</v>
+        <v>307</v>
       </c>
       <c r="C5" t="s">
-        <v>334</v>
+        <v>308</v>
       </c>
       <c r="D5" t="s">
-        <v>166</v>
+        <v>309</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -3879,16 +3882,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>246</v>
+        <v>113</v>
       </c>
       <c r="B6" t="s">
-        <v>292</v>
+        <v>310</v>
       </c>
       <c r="C6" t="s">
-        <v>335</v>
+        <v>311</v>
       </c>
       <c r="D6" t="s">
-        <v>151</v>
+        <v>312</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -3896,16 +3899,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>247</v>
+        <v>114</v>
       </c>
       <c r="B7" t="s">
-        <v>293</v>
+        <v>313</v>
       </c>
       <c r="C7" t="s">
-        <v>336</v>
+        <v>314</v>
       </c>
       <c r="D7" t="s">
-        <v>167</v>
+        <v>315</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -3913,16 +3916,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>248</v>
+        <v>115</v>
       </c>
       <c r="B8" t="s">
-        <v>294</v>
+        <v>316</v>
       </c>
       <c r="C8" t="s">
-        <v>152</v>
+        <v>317</v>
       </c>
       <c r="D8" t="s">
-        <v>168</v>
+        <v>318</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -3930,16 +3933,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>249</v>
+        <v>116</v>
       </c>
       <c r="B9" t="s">
-        <v>295</v>
+        <v>319</v>
       </c>
       <c r="C9" t="s">
-        <v>153</v>
+        <v>320</v>
       </c>
       <c r="D9" t="s">
-        <v>169</v>
+        <v>321</v>
       </c>
       <c r="E9">
         <v>-1</v>
@@ -3947,16 +3950,16 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>250</v>
+        <v>117</v>
       </c>
       <c r="B10" t="s">
-        <v>296</v>
+        <v>322</v>
       </c>
       <c r="C10" t="s">
-        <v>357</v>
+        <v>323</v>
       </c>
       <c r="D10" t="s">
-        <v>191</v>
+        <v>324</v>
       </c>
       <c r="E10">
         <v>2</v>
@@ -3964,16 +3967,16 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>251</v>
+        <v>118</v>
       </c>
       <c r="B11" t="s">
-        <v>297</v>
+        <v>325</v>
       </c>
       <c r="C11" t="s">
-        <v>337</v>
+        <v>326</v>
       </c>
       <c r="D11" t="s">
-        <v>170</v>
+        <v>327</v>
       </c>
       <c r="E11">
         <v>2</v>
@@ -3981,16 +3984,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>252</v>
+        <v>119</v>
       </c>
       <c r="B12" t="s">
-        <v>299</v>
+        <v>328</v>
       </c>
       <c r="C12" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="D12" t="s">
-        <v>171</v>
+        <v>330</v>
       </c>
       <c r="E12">
         <v>2</v>
@@ -3998,16 +4001,16 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>253</v>
+        <v>120</v>
       </c>
       <c r="B13" t="s">
-        <v>298</v>
+        <v>331</v>
       </c>
       <c r="C13" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="D13" t="s">
-        <v>172</v>
+        <v>333</v>
       </c>
       <c r="E13">
         <v>2</v>
@@ -4015,16 +4018,16 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>254</v>
+        <v>121</v>
       </c>
       <c r="B14" t="s">
-        <v>303</v>
+        <v>334</v>
       </c>
       <c r="C14" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="D14" t="s">
-        <v>173</v>
+        <v>336</v>
       </c>
       <c r="E14">
         <v>2</v>
@@ -4032,16 +4035,16 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>256</v>
+        <v>123</v>
       </c>
       <c r="B15" t="s">
-        <v>304</v>
+        <v>337</v>
       </c>
       <c r="C15" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="D15" t="s">
-        <v>175</v>
+        <v>339</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -4049,16 +4052,16 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>257</v>
+        <v>124</v>
       </c>
       <c r="B16" t="s">
-        <v>301</v>
+        <v>340</v>
       </c>
       <c r="C16" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D16" t="s">
-        <v>176</v>
+        <v>342</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -4066,16 +4069,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>258</v>
+        <v>125</v>
       </c>
       <c r="B17" t="s">
-        <v>300</v>
+        <v>343</v>
       </c>
       <c r="C17" t="s">
         <v>344</v>
       </c>
       <c r="D17" t="s">
-        <v>154</v>
+        <v>345</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -4083,16 +4086,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>259</v>
+        <v>126</v>
       </c>
       <c r="B18" t="s">
-        <v>302</v>
+        <v>346</v>
       </c>
       <c r="C18" t="s">
-        <v>302</v>
+        <v>346</v>
       </c>
       <c r="D18" t="s">
-        <v>155</v>
+        <v>347</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -4100,38 +4103,38 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>283</v>
+        <v>150</v>
       </c>
       <c r="B19" t="s">
-        <v>285</v>
+        <v>348</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>260</v>
+        <v>127</v>
       </c>
       <c r="B20" t="s">
-        <v>308</v>
+        <v>411</v>
       </c>
       <c r="C20" t="s">
-        <v>156</v>
+        <v>349</v>
       </c>
       <c r="D20" t="s">
-        <v>177</v>
+        <v>350</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>149</v>
+        <v>90</v>
       </c>
       <c r="B21" t="s">
-        <v>309</v>
+        <v>351</v>
       </c>
       <c r="C21" t="s">
-        <v>345</v>
+        <v>352</v>
       </c>
       <c r="D21" t="s">
-        <v>178</v>
+        <v>353</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -4139,16 +4142,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>261</v>
+        <v>128</v>
       </c>
       <c r="B22" t="s">
-        <v>157</v>
+        <v>354</v>
       </c>
       <c r="C22" t="s">
-        <v>157</v>
+        <v>354</v>
       </c>
       <c r="D22" t="s">
-        <v>157</v>
+        <v>354</v>
       </c>
       <c r="E22">
         <v>4</v>
@@ -4156,16 +4159,16 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>262</v>
+        <v>129</v>
       </c>
       <c r="B23" t="s">
-        <v>307</v>
+        <v>355</v>
       </c>
       <c r="C23" t="s">
-        <v>346</v>
+        <v>356</v>
       </c>
       <c r="D23" t="s">
-        <v>158</v>
+        <v>357</v>
       </c>
       <c r="E23">
         <v>-1</v>
@@ -4173,16 +4176,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>263</v>
+        <v>130</v>
       </c>
       <c r="B24" t="s">
-        <v>310</v>
+        <v>358</v>
       </c>
       <c r="C24" t="s">
-        <v>347</v>
+        <v>359</v>
       </c>
       <c r="D24" t="s">
-        <v>179</v>
+        <v>360</v>
       </c>
       <c r="E24">
         <v>-1</v>
@@ -4190,16 +4193,16 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>264</v>
+        <v>131</v>
       </c>
       <c r="B25" t="s">
-        <v>159</v>
+        <v>361</v>
       </c>
       <c r="C25" t="s">
-        <v>159</v>
+        <v>361</v>
       </c>
       <c r="D25" t="s">
-        <v>159</v>
+        <v>361</v>
       </c>
       <c r="E25">
         <v>2</v>
@@ -4207,10 +4210,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>306</v>
+        <v>153</v>
       </c>
       <c r="B26" t="s">
-        <v>305</v>
+        <v>362</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -4218,10 +4221,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>315</v>
+        <v>154</v>
       </c>
       <c r="B27" t="s">
-        <v>314</v>
+        <v>363</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -4229,16 +4232,16 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>265</v>
+        <v>132</v>
       </c>
       <c r="B28" t="s">
-        <v>316</v>
+        <v>364</v>
       </c>
       <c r="C28" t="s">
-        <v>316</v>
+        <v>364</v>
       </c>
       <c r="D28" t="s">
-        <v>188</v>
+        <v>365</v>
       </c>
       <c r="E28">
         <v>-1</v>
@@ -4246,16 +4249,16 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>266</v>
+        <v>133</v>
       </c>
       <c r="B29" t="s">
-        <v>311</v>
+        <v>412</v>
       </c>
       <c r="C29" t="s">
-        <v>351</v>
+        <v>366</v>
       </c>
       <c r="D29" t="s">
-        <v>181</v>
+        <v>367</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -4263,16 +4266,16 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>267</v>
+        <v>134</v>
       </c>
       <c r="B30" t="s">
-        <v>313</v>
+        <v>368</v>
       </c>
       <c r="C30" t="s">
-        <v>349</v>
+        <v>369</v>
       </c>
       <c r="D30" t="s">
-        <v>180</v>
+        <v>370</v>
       </c>
       <c r="E30">
         <v>-1</v>
@@ -4280,16 +4283,16 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>268</v>
+        <v>135</v>
       </c>
       <c r="B31" t="s">
-        <v>312</v>
+        <v>371</v>
       </c>
       <c r="C31" t="s">
-        <v>348</v>
+        <v>372</v>
       </c>
       <c r="D31" t="s">
-        <v>160</v>
+        <v>373</v>
       </c>
       <c r="E31">
         <v>2</v>
@@ -4297,16 +4300,16 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>269</v>
+        <v>136</v>
       </c>
       <c r="B32" t="s">
-        <v>317</v>
+        <v>374</v>
       </c>
       <c r="C32" t="s">
-        <v>182</v>
+        <v>375</v>
       </c>
       <c r="D32" t="s">
-        <v>182</v>
+        <v>375</v>
       </c>
       <c r="E32">
         <v>3</v>
@@ -4314,16 +4317,16 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>270</v>
+        <v>137</v>
       </c>
       <c r="B33" t="s">
-        <v>318</v>
+        <v>376</v>
       </c>
       <c r="C33" t="s">
-        <v>318</v>
+        <v>376</v>
       </c>
       <c r="D33" t="s">
-        <v>183</v>
+        <v>377</v>
       </c>
       <c r="E33">
         <v>2</v>
@@ -4331,16 +4334,16 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>271</v>
+        <v>138</v>
       </c>
       <c r="B34" t="s">
-        <v>319</v>
+        <v>378</v>
       </c>
       <c r="C34" t="s">
-        <v>161</v>
+        <v>379</v>
       </c>
       <c r="D34" t="s">
-        <v>184</v>
+        <v>380</v>
       </c>
       <c r="E34">
         <v>0</v>
@@ -4348,16 +4351,16 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>272</v>
+        <v>139</v>
       </c>
       <c r="B35" t="s">
-        <v>320</v>
+        <v>381</v>
       </c>
       <c r="C35" t="s">
-        <v>320</v>
+        <v>381</v>
       </c>
       <c r="D35" t="s">
-        <v>185</v>
+        <v>382</v>
       </c>
       <c r="E35">
         <v>-1</v>
@@ -4365,16 +4368,16 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>273</v>
+        <v>140</v>
       </c>
       <c r="B36" t="s">
-        <v>321</v>
+        <v>413</v>
       </c>
       <c r="C36" t="s">
-        <v>352</v>
+        <v>383</v>
       </c>
       <c r="D36" t="s">
-        <v>186</v>
+        <v>384</v>
       </c>
       <c r="E36">
         <v>-1</v>
@@ -4382,16 +4385,16 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>274</v>
+        <v>141</v>
       </c>
       <c r="B37" t="s">
-        <v>322</v>
+        <v>385</v>
       </c>
       <c r="C37" t="s">
-        <v>353</v>
+        <v>386</v>
       </c>
       <c r="D37" t="s">
-        <v>187</v>
+        <v>387</v>
       </c>
       <c r="E37">
         <v>3</v>
@@ -4399,16 +4402,16 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>275</v>
+        <v>142</v>
       </c>
       <c r="B38" t="s">
-        <v>162</v>
+        <v>388</v>
       </c>
       <c r="C38" t="s">
-        <v>162</v>
+        <v>388</v>
       </c>
       <c r="D38" t="s">
-        <v>162</v>
+        <v>388</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -4416,16 +4419,16 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>276</v>
+        <v>143</v>
       </c>
       <c r="B39" t="s">
-        <v>323</v>
+        <v>389</v>
       </c>
       <c r="C39" t="s">
-        <v>354</v>
+        <v>390</v>
       </c>
       <c r="D39" t="s">
-        <v>163</v>
+        <v>391</v>
       </c>
       <c r="E39">
         <v>3</v>
@@ -4433,16 +4436,16 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>277</v>
+        <v>144</v>
       </c>
       <c r="B40" t="s">
-        <v>324</v>
+        <v>392</v>
       </c>
       <c r="C40" t="s">
-        <v>355</v>
+        <v>393</v>
       </c>
       <c r="D40" t="s">
-        <v>189</v>
+        <v>394</v>
       </c>
       <c r="E40">
         <v>0</v>
@@ -4450,16 +4453,16 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>278</v>
+        <v>145</v>
       </c>
       <c r="B41" t="s">
-        <v>325</v>
+        <v>395</v>
       </c>
       <c r="C41" t="s">
-        <v>356</v>
+        <v>396</v>
       </c>
       <c r="D41" t="s">
-        <v>190</v>
+        <v>397</v>
       </c>
       <c r="E41">
         <v>6</v>
@@ -4467,10 +4470,10 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>284</v>
+        <v>151</v>
       </c>
       <c r="B42" t="s">
-        <v>286</v>
+        <v>398</v>
       </c>
       <c r="E42">
         <v>6</v>
@@ -4478,16 +4481,16 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>255</v>
+        <v>122</v>
       </c>
       <c r="B43" t="s">
-        <v>326</v>
+        <v>414</v>
       </c>
       <c r="C43" t="s">
-        <v>341</v>
+        <v>415</v>
       </c>
       <c r="D43" t="s">
-        <v>174</v>
+        <v>399</v>
       </c>
       <c r="E43">
         <v>6</v>
@@ -4495,16 +4498,16 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>279</v>
+        <v>146</v>
       </c>
       <c r="B44" t="s">
-        <v>327</v>
+        <v>400</v>
       </c>
       <c r="C44" t="s">
-        <v>350</v>
+        <v>401</v>
       </c>
       <c r="D44" t="s">
-        <v>192</v>
+        <v>402</v>
       </c>
       <c r="E44">
         <v>6</v>
@@ -4512,16 +4515,16 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>280</v>
+        <v>147</v>
       </c>
       <c r="B45" t="s">
-        <v>328</v>
+        <v>403</v>
       </c>
       <c r="C45" t="s">
-        <v>328</v>
+        <v>403</v>
       </c>
       <c r="D45" t="s">
-        <v>193</v>
+        <v>404</v>
       </c>
       <c r="E45">
         <v>2</v>
@@ -4529,16 +4532,16 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>281</v>
+        <v>148</v>
       </c>
       <c r="B46" t="s">
-        <v>329</v>
+        <v>405</v>
       </c>
       <c r="C46" t="s">
-        <v>358</v>
+        <v>406</v>
       </c>
       <c r="D46" t="s">
-        <v>194</v>
+        <v>407</v>
       </c>
       <c r="E46">
         <v>0</v>
@@ -4546,16 +4549,16 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>282</v>
+        <v>149</v>
       </c>
       <c r="B47" t="s">
-        <v>330</v>
+        <v>408</v>
       </c>
       <c r="C47" t="s">
-        <v>359</v>
+        <v>409</v>
       </c>
       <c r="D47" t="s">
-        <v>195</v>
+        <v>410</v>
       </c>
     </row>
   </sheetData>
@@ -4571,8 +4574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4589,15 +4592,15 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>200</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>196</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
-        <v>198</v>
+        <v>416</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -4605,10 +4608,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>197</v>
+        <v>92</v>
       </c>
       <c r="B3" t="s">
-        <v>199</v>
+        <v>417</v>
       </c>
       <c r="C3">
         <v>0</v>

</xml_diff>

<commit_message>
Include hip_ae-hailer. Fix #69.E
</commit_message>
<xml_diff>
--- a/data-raw/classcodes.xlsx
+++ b/data-raw/classcodes.xlsx
@@ -9,26 +9,27 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ex_carbrands" sheetId="10" r:id="rId1"/>
     <sheet name="charlson" sheetId="1" r:id="rId2"/>
     <sheet name="elixhauser" sheetId="2" r:id="rId3"/>
     <sheet name="hip_ae" sheetId="3" r:id="rId4"/>
-    <sheet name="knee_ae" sheetId="5" r:id="rId5"/>
-    <sheet name="rxriskv" sheetId="7" r:id="rId6"/>
-    <sheet name="cps" sheetId="9" r:id="rId7"/>
+    <sheet name="hip_ae_hailer" sheetId="11" r:id="rId5"/>
+    <sheet name="knee_ae" sheetId="5" r:id="rId6"/>
+    <sheet name="rxriskv" sheetId="7" r:id="rId7"/>
+    <sheet name="cps" sheetId="9" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">rxriskv!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">rxriskv!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="424">
   <si>
     <t>group</t>
   </si>
@@ -1283,6 +1284,24 @@
   </si>
   <si>
     <t>U[ABP][0-9]{2,4}</t>
+  </si>
+  <si>
+    <t>Infection</t>
+  </si>
+  <si>
+    <t>(M(00(1|[0289]F?)|86([01]F|6F?)))|T(8(14|4(5[FX]?|7F?)))</t>
+  </si>
+  <si>
+    <t>NFS\\d{0,2}</t>
+  </si>
+  <si>
+    <t>Dislocation</t>
+  </si>
+  <si>
+    <t>M24(3|4F?)|S730|T933</t>
+  </si>
+  <si>
+    <t>NFH([02]{2}|21)</t>
   </si>
 </sst>
 </file>
@@ -1716,7 +1735,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMO18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -3559,7 +3578,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3667,6 +3686,60 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>418</v>
+      </c>
+      <c r="B2" t="s">
+        <v>419</v>
+      </c>
+      <c r="C2" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>421</v>
+      </c>
+      <c r="B3" t="s">
+        <v>422</v>
+      </c>
+      <c r="C3" t="s">
+        <v>423</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
@@ -3778,7 +3851,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E47"/>
   <sheetViews>
@@ -4570,11 +4643,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Remove documentation for regex-unknown from rxriskv and add index "sum-all". Fix #70.
</commit_message>
<xml_diff>
--- a/data-raw/classcodes.xlsx
+++ b/data-raw/classcodes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="ex_carbrands" sheetId="10" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="424">
   <si>
     <t>group</t>
   </si>
@@ -3689,8 +3689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3853,10 +3853,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3868,7 +3868,7 @@
     <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3884,8 +3884,11 @@
       <c r="E1" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>109</v>
       </c>
@@ -3901,8 +3904,11 @@
       <c r="E2">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>110</v>
       </c>
@@ -3918,8 +3924,11 @@
       <c r="E3">
         <v>-1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>111</v>
       </c>
@@ -3935,8 +3944,11 @@
       <c r="E4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>112</v>
       </c>
@@ -3952,8 +3964,11 @@
       <c r="E5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>113</v>
       </c>
@@ -3969,8 +3984,11 @@
       <c r="E6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>114</v>
       </c>
@@ -3986,8 +4004,11 @@
       <c r="E7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>115</v>
       </c>
@@ -4003,8 +4024,11 @@
       <c r="E8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>116</v>
       </c>
@@ -4020,8 +4044,11 @@
       <c r="E9">
         <v>-1</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>117</v>
       </c>
@@ -4037,8 +4064,11 @@
       <c r="E10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>118</v>
       </c>
@@ -4054,8 +4084,11 @@
       <c r="E11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>119</v>
       </c>
@@ -4071,8 +4104,11 @@
       <c r="E12">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>120</v>
       </c>
@@ -4088,8 +4124,11 @@
       <c r="E13">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>121</v>
       </c>
@@ -4105,8 +4144,11 @@
       <c r="E14">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>123</v>
       </c>
@@ -4122,8 +4164,11 @@
       <c r="E15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>124</v>
       </c>
@@ -4139,8 +4184,11 @@
       <c r="E16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>125</v>
       </c>
@@ -4156,8 +4204,11 @@
       <c r="E17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>126</v>
       </c>
@@ -4173,16 +4224,22 @@
       <c r="E18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>150</v>
       </c>
       <c r="B19" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>127</v>
       </c>
@@ -4195,8 +4252,11 @@
       <c r="D20" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>90</v>
       </c>
@@ -4212,8 +4272,11 @@
       <c r="E21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>128</v>
       </c>
@@ -4229,8 +4292,11 @@
       <c r="E22">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>129</v>
       </c>
@@ -4246,8 +4312,11 @@
       <c r="E23">
         <v>-1</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>130</v>
       </c>
@@ -4263,8 +4332,11 @@
       <c r="E24">
         <v>-1</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>131</v>
       </c>
@@ -4280,8 +4352,11 @@
       <c r="E25">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>153</v>
       </c>
@@ -4291,8 +4366,11 @@
       <c r="E26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>154</v>
       </c>
@@ -4302,8 +4380,11 @@
       <c r="E27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>132</v>
       </c>
@@ -4319,8 +4400,11 @@
       <c r="E28">
         <v>-1</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>133</v>
       </c>
@@ -4336,8 +4420,11 @@
       <c r="E29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>134</v>
       </c>
@@ -4353,8 +4440,11 @@
       <c r="E30">
         <v>-1</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>135</v>
       </c>
@@ -4370,8 +4460,11 @@
       <c r="E31">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>136</v>
       </c>
@@ -4387,8 +4480,11 @@
       <c r="E32">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>137</v>
       </c>
@@ -4404,8 +4500,11 @@
       <c r="E33">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>138</v>
       </c>
@@ -4421,8 +4520,11 @@
       <c r="E34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>139</v>
       </c>
@@ -4438,8 +4540,11 @@
       <c r="E35">
         <v>-1</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>140</v>
       </c>
@@ -4455,8 +4560,11 @@
       <c r="E36">
         <v>-1</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>141</v>
       </c>
@@ -4472,8 +4580,11 @@
       <c r="E37">
         <v>3</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>142</v>
       </c>
@@ -4489,8 +4600,11 @@
       <c r="E38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>143</v>
       </c>
@@ -4506,8 +4620,11 @@
       <c r="E39">
         <v>3</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>144</v>
       </c>
@@ -4523,8 +4640,11 @@
       <c r="E40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>145</v>
       </c>
@@ -4540,8 +4660,11 @@
       <c r="E41">
         <v>6</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>151</v>
       </c>
@@ -4551,8 +4674,11 @@
       <c r="E42">
         <v>6</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>122</v>
       </c>
@@ -4568,8 +4694,11 @@
       <c r="E43">
         <v>6</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>146</v>
       </c>
@@ -4585,8 +4714,11 @@
       <c r="E44">
         <v>6</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>147</v>
       </c>
@@ -4602,8 +4734,11 @@
       <c r="E45">
         <v>2</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>148</v>
       </c>
@@ -4619,8 +4754,11 @@
       <c r="E46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>149</v>
       </c>
@@ -4632,6 +4770,9 @@
       </c>
       <c r="D47" t="s">
         <v>410</v>
+      </c>
+      <c r="F47">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Suppress warning from clasify if called by categorize. Fix #71.
</commit_message>
<xml_diff>
--- a/data-raw/classcodes.xlsx
+++ b/data-raw/classcodes.xlsx
@@ -496,9 +496,6 @@
     <t>Incontinence</t>
   </si>
   <si>
-    <t>index_pratt</t>
-  </si>
-  <si>
     <t>41[02]</t>
   </si>
   <si>
@@ -1302,6 +1299,9 @@
   </si>
   <si>
     <t>NFH([02]{2}|21)</t>
+  </si>
+  <si>
+    <t>pratt</t>
   </si>
 </sst>
 </file>
@@ -1769,19 +1769,19 @@
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>183</v>
-      </c>
       <c r="F1" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>3</v>
@@ -1811,22 +1811,22 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -1855,22 +1855,22 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D3" s="6">
         <v>428</v>
       </c>
       <c r="E3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -1899,22 +1899,22 @@
         <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -1943,22 +1943,22 @@
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -1987,22 +1987,22 @@
         <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D6" s="6">
         <v>290</v>
       </c>
       <c r="E6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -2031,22 +2031,22 @@
         <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -2075,22 +2075,22 @@
         <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -2119,13 +2119,13 @@
         <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I9">
         <v>1</v>
@@ -2154,13 +2154,13 @@
         <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I10">
         <v>1</v>
@@ -2189,13 +2189,13 @@
         <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E11" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I11">
         <v>1</v>
@@ -2224,22 +2224,22 @@
         <v>30</v>
       </c>
       <c r="C12" t="s">
+        <v>217</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="E12" t="s">
+        <v>207</v>
+      </c>
+      <c r="F12" s="6" t="s">
         <v>218</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="E12" t="s">
-        <v>208</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>219</v>
       </c>
       <c r="G12" s="6">
         <v>344</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I12">
         <v>2</v>
@@ -2268,22 +2268,22 @@
         <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I13">
         <v>2</v>
@@ -2312,16 +2312,16 @@
         <v>34</v>
       </c>
       <c r="C14" t="s">
+        <v>219</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="E14" t="s">
+        <v>206</v>
+      </c>
+      <c r="F14" s="6" t="s">
         <v>220</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="E14" t="s">
-        <v>207</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>221</v>
       </c>
       <c r="G14" s="6">
         <v>250</v>
@@ -2356,22 +2356,22 @@
         <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E15" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I15">
         <v>2</v>
@@ -2400,22 +2400,22 @@
         <v>37</v>
       </c>
       <c r="C16" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E16" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I16">
         <v>3</v>
@@ -2444,22 +2444,22 @@
         <v>39</v>
       </c>
       <c r="C17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I17">
         <v>6</v>
@@ -2488,19 +2488,19 @@
         <v>41</v>
       </c>
       <c r="C18" t="s">
+        <v>223</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="E18" t="s">
+        <v>195</v>
+      </c>
+      <c r="F18" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="D18" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="E18" t="s">
-        <v>196</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>225</v>
-      </c>
       <c r="H18" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I18">
         <v>6</v>
@@ -2581,10 +2581,10 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -2613,10 +2613,10 @@
         <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D3">
         <v>1</v>
@@ -2645,10 +2645,10 @@
         <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -2677,10 +2677,10 @@
         <v>46</v>
       </c>
       <c r="B5" t="s">
+        <v>238</v>
+      </c>
+      <c r="C5" t="s">
         <v>239</v>
-      </c>
-      <c r="C5" t="s">
-        <v>240</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -2709,10 +2709,10 @@
         <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -2741,10 +2741,10 @@
         <v>50</v>
       </c>
       <c r="B7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -2773,10 +2773,10 @@
         <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -2805,10 +2805,10 @@
         <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -2837,10 +2837,10 @@
         <v>53</v>
       </c>
       <c r="B10" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C10" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -2869,10 +2869,10 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C11" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -2901,10 +2901,10 @@
         <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -2933,10 +2933,10 @@
         <v>55</v>
       </c>
       <c r="B13" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C13" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -2965,10 +2965,10 @@
         <v>56</v>
       </c>
       <c r="B14" t="s">
+        <v>245</v>
+      </c>
+      <c r="C14" t="s">
         <v>246</v>
-      </c>
-      <c r="C14" t="s">
-        <v>247</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -2997,10 +2997,10 @@
         <v>57</v>
       </c>
       <c r="B15" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C15" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -3029,10 +3029,10 @@
         <v>58</v>
       </c>
       <c r="B16" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C16" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -3061,10 +3061,10 @@
         <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C17" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -3093,10 +3093,10 @@
         <v>40</v>
       </c>
       <c r="B18" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C18" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -3125,10 +3125,10 @@
         <v>59</v>
       </c>
       <c r="B19" t="s">
+        <v>249</v>
+      </c>
+      <c r="C19" t="s">
         <v>250</v>
-      </c>
-      <c r="C19" t="s">
-        <v>251</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -3157,10 +3157,10 @@
         <v>60</v>
       </c>
       <c r="B20" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C20" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -3189,10 +3189,10 @@
         <v>61</v>
       </c>
       <c r="B21" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C21" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -3221,10 +3221,10 @@
         <v>62</v>
       </c>
       <c r="B22" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C22" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -3253,10 +3253,10 @@
         <v>63</v>
       </c>
       <c r="B23" t="s">
+        <v>252</v>
+      </c>
+      <c r="C23" t="s">
         <v>253</v>
-      </c>
-      <c r="C23" t="s">
-        <v>254</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -3285,10 +3285,10 @@
         <v>64</v>
       </c>
       <c r="B24" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C24" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -3317,10 +3317,10 @@
         <v>65</v>
       </c>
       <c r="B25" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C25" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -3349,10 +3349,10 @@
         <v>66</v>
       </c>
       <c r="B26" t="s">
+        <v>255</v>
+      </c>
+      <c r="C26" t="s">
         <v>256</v>
-      </c>
-      <c r="C26" t="s">
-        <v>257</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -3381,10 +3381,10 @@
         <v>67</v>
       </c>
       <c r="B27" t="s">
+        <v>257</v>
+      </c>
+      <c r="C27" t="s">
         <v>258</v>
-      </c>
-      <c r="C27" t="s">
-        <v>259</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -3413,10 +3413,10 @@
         <v>68</v>
       </c>
       <c r="B28" t="s">
+        <v>259</v>
+      </c>
+      <c r="C28" t="s">
         <v>260</v>
-      </c>
-      <c r="C28" t="s">
-        <v>261</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -3445,10 +3445,10 @@
         <v>69</v>
       </c>
       <c r="B29" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C29" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -3477,10 +3477,10 @@
         <v>70</v>
       </c>
       <c r="B30" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C30" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D30">
         <v>1</v>
@@ -3509,10 +3509,10 @@
         <v>71</v>
       </c>
       <c r="B31" t="s">
+        <v>261</v>
+      </c>
+      <c r="C31" t="s">
         <v>262</v>
-      </c>
-      <c r="C31" t="s">
-        <v>263</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -3541,10 +3541,10 @@
         <v>72</v>
       </c>
       <c r="B32" t="s">
+        <v>263</v>
+      </c>
+      <c r="C32" t="s">
         <v>264</v>
-      </c>
-      <c r="C32" t="s">
-        <v>265</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -3597,7 +3597,7 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D1" t="s">
         <v>76</v>
@@ -3608,7 +3608,7 @@
         <v>77</v>
       </c>
       <c r="B2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>83</v>
@@ -3619,7 +3619,7 @@
         <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>83</v>
@@ -3630,7 +3630,7 @@
         <v>79</v>
       </c>
       <c r="B4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>84</v>
@@ -3641,7 +3641,7 @@
         <v>80</v>
       </c>
       <c r="B5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>83</v>
@@ -3652,7 +3652,7 @@
         <v>81</v>
       </c>
       <c r="B6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>83</v>
@@ -3663,7 +3663,7 @@
         <v>82</v>
       </c>
       <c r="B7" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>84</v>
@@ -3671,7 +3671,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C8" t="s">
         <v>85</v>
@@ -3709,29 +3709,29 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>417</v>
+      </c>
+      <c r="B2" t="s">
         <v>418</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>419</v>
-      </c>
-      <c r="C2" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>420</v>
+      </c>
+      <c r="B3" t="s">
         <v>421</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>422</v>
-      </c>
-      <c r="C3" t="s">
-        <v>423</v>
       </c>
     </row>
   </sheetData>
@@ -3763,7 +3763,7 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D1" t="s">
         <v>76</v>
@@ -3774,7 +3774,7 @@
         <v>77</v>
       </c>
       <c r="B2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>83</v>
@@ -3785,7 +3785,7 @@
         <v>88</v>
       </c>
       <c r="B3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>83</v>
@@ -3796,7 +3796,7 @@
         <v>89</v>
       </c>
       <c r="B4" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>84</v>
@@ -3807,7 +3807,7 @@
         <v>80</v>
       </c>
       <c r="B5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>83</v>
@@ -3818,7 +3818,7 @@
         <v>81</v>
       </c>
       <c r="B6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>83</v>
@@ -3829,7 +3829,7 @@
         <v>82</v>
       </c>
       <c r="B7" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>84</v>
@@ -3837,7 +3837,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C8" t="s">
         <v>87</v>
@@ -3855,8 +3855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3882,7 +3882,7 @@
         <v>108</v>
       </c>
       <c r="E1" t="s">
-        <v>155</v>
+        <v>423</v>
       </c>
       <c r="F1" t="s">
         <v>42</v>
@@ -3893,13 +3893,13 @@
         <v>109</v>
       </c>
       <c r="B2" t="s">
+        <v>297</v>
+      </c>
+      <c r="C2" t="s">
         <v>298</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>299</v>
-      </c>
-      <c r="D2" t="s">
-        <v>300</v>
       </c>
       <c r="E2">
         <v>6</v>
@@ -3913,13 +3913,13 @@
         <v>110</v>
       </c>
       <c r="B3" t="s">
+        <v>300</v>
+      </c>
+      <c r="C3" t="s">
         <v>301</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>302</v>
-      </c>
-      <c r="D3" t="s">
-        <v>303</v>
       </c>
       <c r="E3">
         <v>-1</v>
@@ -3933,13 +3933,13 @@
         <v>111</v>
       </c>
       <c r="B4" t="s">
+        <v>303</v>
+      </c>
+      <c r="C4" t="s">
         <v>304</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>305</v>
-      </c>
-      <c r="D4" t="s">
-        <v>306</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -3953,13 +3953,13 @@
         <v>112</v>
       </c>
       <c r="B5" t="s">
+        <v>306</v>
+      </c>
+      <c r="C5" t="s">
         <v>307</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>308</v>
-      </c>
-      <c r="D5" t="s">
-        <v>309</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -3973,13 +3973,13 @@
         <v>113</v>
       </c>
       <c r="B6" t="s">
+        <v>309</v>
+      </c>
+      <c r="C6" t="s">
         <v>310</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>311</v>
-      </c>
-      <c r="D6" t="s">
-        <v>312</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -3993,13 +3993,13 @@
         <v>114</v>
       </c>
       <c r="B7" t="s">
+        <v>312</v>
+      </c>
+      <c r="C7" t="s">
         <v>313</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>314</v>
-      </c>
-      <c r="D7" t="s">
-        <v>315</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -4013,13 +4013,13 @@
         <v>115</v>
       </c>
       <c r="B8" t="s">
+        <v>315</v>
+      </c>
+      <c r="C8" t="s">
         <v>316</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>317</v>
-      </c>
-      <c r="D8" t="s">
-        <v>318</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -4033,13 +4033,13 @@
         <v>116</v>
       </c>
       <c r="B9" t="s">
+        <v>318</v>
+      </c>
+      <c r="C9" t="s">
         <v>319</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>320</v>
-      </c>
-      <c r="D9" t="s">
-        <v>321</v>
       </c>
       <c r="E9">
         <v>-1</v>
@@ -4053,13 +4053,13 @@
         <v>117</v>
       </c>
       <c r="B10" t="s">
+        <v>321</v>
+      </c>
+      <c r="C10" t="s">
         <v>322</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>323</v>
-      </c>
-      <c r="D10" t="s">
-        <v>324</v>
       </c>
       <c r="E10">
         <v>2</v>
@@ -4073,13 +4073,13 @@
         <v>118</v>
       </c>
       <c r="B11" t="s">
+        <v>324</v>
+      </c>
+      <c r="C11" t="s">
         <v>325</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>326</v>
-      </c>
-      <c r="D11" t="s">
-        <v>327</v>
       </c>
       <c r="E11">
         <v>2</v>
@@ -4093,13 +4093,13 @@
         <v>119</v>
       </c>
       <c r="B12" t="s">
+        <v>327</v>
+      </c>
+      <c r="C12" t="s">
         <v>328</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>329</v>
-      </c>
-      <c r="D12" t="s">
-        <v>330</v>
       </c>
       <c r="E12">
         <v>2</v>
@@ -4113,13 +4113,13 @@
         <v>120</v>
       </c>
       <c r="B13" t="s">
+        <v>330</v>
+      </c>
+      <c r="C13" t="s">
         <v>331</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>332</v>
-      </c>
-      <c r="D13" t="s">
-        <v>333</v>
       </c>
       <c r="E13">
         <v>2</v>
@@ -4133,13 +4133,13 @@
         <v>121</v>
       </c>
       <c r="B14" t="s">
+        <v>333</v>
+      </c>
+      <c r="C14" t="s">
         <v>334</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>335</v>
-      </c>
-      <c r="D14" t="s">
-        <v>336</v>
       </c>
       <c r="E14">
         <v>2</v>
@@ -4153,13 +4153,13 @@
         <v>123</v>
       </c>
       <c r="B15" t="s">
+        <v>336</v>
+      </c>
+      <c r="C15" t="s">
         <v>337</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>338</v>
-      </c>
-      <c r="D15" t="s">
-        <v>339</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -4173,13 +4173,13 @@
         <v>124</v>
       </c>
       <c r="B16" t="s">
+        <v>339</v>
+      </c>
+      <c r="C16" t="s">
         <v>340</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>341</v>
-      </c>
-      <c r="D16" t="s">
-        <v>342</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -4193,13 +4193,13 @@
         <v>125</v>
       </c>
       <c r="B17" t="s">
+        <v>342</v>
+      </c>
+      <c r="C17" t="s">
         <v>343</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>344</v>
-      </c>
-      <c r="D17" t="s">
-        <v>345</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -4213,13 +4213,13 @@
         <v>126</v>
       </c>
       <c r="B18" t="s">
+        <v>345</v>
+      </c>
+      <c r="C18" t="s">
+        <v>345</v>
+      </c>
+      <c r="D18" t="s">
         <v>346</v>
-      </c>
-      <c r="C18" t="s">
-        <v>346</v>
-      </c>
-      <c r="D18" t="s">
-        <v>347</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -4233,7 +4233,7 @@
         <v>150</v>
       </c>
       <c r="B19" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -4244,13 +4244,13 @@
         <v>127</v>
       </c>
       <c r="B20" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C20" t="s">
+        <v>348</v>
+      </c>
+      <c r="D20" t="s">
         <v>349</v>
-      </c>
-      <c r="D20" t="s">
-        <v>350</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -4261,13 +4261,13 @@
         <v>90</v>
       </c>
       <c r="B21" t="s">
+        <v>350</v>
+      </c>
+      <c r="C21" t="s">
         <v>351</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>352</v>
-      </c>
-      <c r="D21" t="s">
-        <v>353</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -4281,13 +4281,13 @@
         <v>128</v>
       </c>
       <c r="B22" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C22" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D22" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E22">
         <v>4</v>
@@ -4301,13 +4301,13 @@
         <v>129</v>
       </c>
       <c r="B23" t="s">
+        <v>354</v>
+      </c>
+      <c r="C23" t="s">
         <v>355</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>356</v>
-      </c>
-      <c r="D23" t="s">
-        <v>357</v>
       </c>
       <c r="E23">
         <v>-1</v>
@@ -4321,13 +4321,13 @@
         <v>130</v>
       </c>
       <c r="B24" t="s">
+        <v>357</v>
+      </c>
+      <c r="C24" t="s">
         <v>358</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>359</v>
-      </c>
-      <c r="D24" t="s">
-        <v>360</v>
       </c>
       <c r="E24">
         <v>-1</v>
@@ -4341,13 +4341,13 @@
         <v>131</v>
       </c>
       <c r="B25" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C25" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D25" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E25">
         <v>2</v>
@@ -4361,7 +4361,7 @@
         <v>153</v>
       </c>
       <c r="B26" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -4375,7 +4375,7 @@
         <v>154</v>
       </c>
       <c r="B27" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -4389,13 +4389,13 @@
         <v>132</v>
       </c>
       <c r="B28" t="s">
+        <v>363</v>
+      </c>
+      <c r="C28" t="s">
+        <v>363</v>
+      </c>
+      <c r="D28" t="s">
         <v>364</v>
-      </c>
-      <c r="C28" t="s">
-        <v>364</v>
-      </c>
-      <c r="D28" t="s">
-        <v>365</v>
       </c>
       <c r="E28">
         <v>-1</v>
@@ -4409,13 +4409,13 @@
         <v>133</v>
       </c>
       <c r="B29" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C29" t="s">
+        <v>365</v>
+      </c>
+      <c r="D29" t="s">
         <v>366</v>
-      </c>
-      <c r="D29" t="s">
-        <v>367</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -4429,13 +4429,13 @@
         <v>134</v>
       </c>
       <c r="B30" t="s">
+        <v>367</v>
+      </c>
+      <c r="C30" t="s">
         <v>368</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>369</v>
-      </c>
-      <c r="D30" t="s">
-        <v>370</v>
       </c>
       <c r="E30">
         <v>-1</v>
@@ -4449,13 +4449,13 @@
         <v>135</v>
       </c>
       <c r="B31" t="s">
+        <v>370</v>
+      </c>
+      <c r="C31" t="s">
         <v>371</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>372</v>
-      </c>
-      <c r="D31" t="s">
-        <v>373</v>
       </c>
       <c r="E31">
         <v>2</v>
@@ -4469,13 +4469,13 @@
         <v>136</v>
       </c>
       <c r="B32" t="s">
+        <v>373</v>
+      </c>
+      <c r="C32" t="s">
         <v>374</v>
       </c>
-      <c r="C32" t="s">
-        <v>375</v>
-      </c>
       <c r="D32" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E32">
         <v>3</v>
@@ -4489,13 +4489,13 @@
         <v>137</v>
       </c>
       <c r="B33" t="s">
+        <v>375</v>
+      </c>
+      <c r="C33" t="s">
+        <v>375</v>
+      </c>
+      <c r="D33" t="s">
         <v>376</v>
-      </c>
-      <c r="C33" t="s">
-        <v>376</v>
-      </c>
-      <c r="D33" t="s">
-        <v>377</v>
       </c>
       <c r="E33">
         <v>2</v>
@@ -4509,13 +4509,13 @@
         <v>138</v>
       </c>
       <c r="B34" t="s">
+        <v>377</v>
+      </c>
+      <c r="C34" t="s">
         <v>378</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>379</v>
-      </c>
-      <c r="D34" t="s">
-        <v>380</v>
       </c>
       <c r="E34">
         <v>0</v>
@@ -4529,13 +4529,13 @@
         <v>139</v>
       </c>
       <c r="B35" t="s">
+        <v>380</v>
+      </c>
+      <c r="C35" t="s">
+        <v>380</v>
+      </c>
+      <c r="D35" t="s">
         <v>381</v>
-      </c>
-      <c r="C35" t="s">
-        <v>381</v>
-      </c>
-      <c r="D35" t="s">
-        <v>382</v>
       </c>
       <c r="E35">
         <v>-1</v>
@@ -4549,13 +4549,13 @@
         <v>140</v>
       </c>
       <c r="B36" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C36" t="s">
+        <v>382</v>
+      </c>
+      <c r="D36" t="s">
         <v>383</v>
-      </c>
-      <c r="D36" t="s">
-        <v>384</v>
       </c>
       <c r="E36">
         <v>-1</v>
@@ -4569,13 +4569,13 @@
         <v>141</v>
       </c>
       <c r="B37" t="s">
+        <v>384</v>
+      </c>
+      <c r="C37" t="s">
         <v>385</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>386</v>
-      </c>
-      <c r="D37" t="s">
-        <v>387</v>
       </c>
       <c r="E37">
         <v>3</v>
@@ -4589,13 +4589,13 @@
         <v>142</v>
       </c>
       <c r="B38" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C38" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D38" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -4609,13 +4609,13 @@
         <v>143</v>
       </c>
       <c r="B39" t="s">
+        <v>388</v>
+      </c>
+      <c r="C39" t="s">
         <v>389</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>390</v>
-      </c>
-      <c r="D39" t="s">
-        <v>391</v>
       </c>
       <c r="E39">
         <v>3</v>
@@ -4629,13 +4629,13 @@
         <v>144</v>
       </c>
       <c r="B40" t="s">
+        <v>391</v>
+      </c>
+      <c r="C40" t="s">
         <v>392</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>393</v>
-      </c>
-      <c r="D40" t="s">
-        <v>394</v>
       </c>
       <c r="E40">
         <v>0</v>
@@ -4649,13 +4649,13 @@
         <v>145</v>
       </c>
       <c r="B41" t="s">
+        <v>394</v>
+      </c>
+      <c r="C41" t="s">
         <v>395</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>396</v>
-      </c>
-      <c r="D41" t="s">
-        <v>397</v>
       </c>
       <c r="E41">
         <v>6</v>
@@ -4669,7 +4669,7 @@
         <v>151</v>
       </c>
       <c r="B42" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E42">
         <v>6</v>
@@ -4683,13 +4683,13 @@
         <v>122</v>
       </c>
       <c r="B43" t="s">
+        <v>413</v>
+      </c>
+      <c r="C43" t="s">
         <v>414</v>
       </c>
-      <c r="C43" t="s">
-        <v>415</v>
-      </c>
       <c r="D43" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E43">
         <v>6</v>
@@ -4703,13 +4703,13 @@
         <v>146</v>
       </c>
       <c r="B44" t="s">
+        <v>399</v>
+      </c>
+      <c r="C44" t="s">
         <v>400</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>401</v>
-      </c>
-      <c r="D44" t="s">
-        <v>402</v>
       </c>
       <c r="E44">
         <v>6</v>
@@ -4723,13 +4723,13 @@
         <v>147</v>
       </c>
       <c r="B45" t="s">
+        <v>402</v>
+      </c>
+      <c r="C45" t="s">
+        <v>402</v>
+      </c>
+      <c r="D45" t="s">
         <v>403</v>
-      </c>
-      <c r="C45" t="s">
-        <v>403</v>
-      </c>
-      <c r="D45" t="s">
-        <v>404</v>
       </c>
       <c r="E45">
         <v>2</v>
@@ -4743,13 +4743,13 @@
         <v>148</v>
       </c>
       <c r="B46" t="s">
+        <v>404</v>
+      </c>
+      <c r="C46" t="s">
         <v>405</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>406</v>
-      </c>
-      <c r="D46" t="s">
-        <v>407</v>
       </c>
       <c r="E46">
         <v>0</v>
@@ -4763,13 +4763,13 @@
         <v>149</v>
       </c>
       <c r="B47" t="s">
+        <v>407</v>
+      </c>
+      <c r="C47" t="s">
         <v>408</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>409</v>
-      </c>
-      <c r="D47" t="s">
-        <v>410</v>
       </c>
       <c r="F47">
         <v>1</v>
@@ -4814,7 +4814,7 @@
         <v>91</v>
       </c>
       <c r="B2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -4825,7 +4825,7 @@
         <v>92</v>
       </c>
       <c r="B3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C3">
         <v>0</v>

</xml_diff>

<commit_message>
Merge ae_hip and ae_hip_fracture. Fix #78.
</commit_message>
<xml_diff>
--- a/data-raw/classcodes.xlsx
+++ b/data-raw/classcodes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erik_\Documents\GitHub\coder\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erikbulow/coder/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9858AD-CCBE-4335-94AA-DB609559802B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBBD5F1D-E62B-0541-8390-5963D76F117F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="11436" windowWidth="21264" windowHeight="18684" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24920" windowHeight="15540" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ex_carbrands" sheetId="10" r:id="rId1"/>
@@ -26,7 +26,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">rxriskv!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -288,9 +287,6 @@
     <t>late_hdia</t>
   </si>
   <si>
-    <t>^NF([CF-HJ-MS-TW]\\d{2}|A(02|1[12]|2[0-2])|Q09|U[013489]9)|QD(A10|B(0[05]|99)|E35|G30)|TNF(05|10)$</t>
-  </si>
-  <si>
     <t>post_op</t>
   </si>
   <si>
@@ -340,9 +336,6 @@
   </si>
   <si>
     <t>Ford|Lincoln</t>
-  </si>
-  <si>
-    <t>Chrysler|Fiat|Dodge|Ferrari|Maserati,</t>
   </si>
   <si>
     <t>Porsche</t>
@@ -1523,6 +1516,12 @@
   </si>
   <si>
     <t>29(6[235])|3(0(04|9)|11)</t>
+  </si>
+  <si>
+    <t>NF([CF-HJ-MS-TW]\\d{2}|A(02|1[12]|2[0-2])|Q09|U[013489]9)|QD(A10|B(0[05]|99)|E35|G30)|TNF(05|10)</t>
+  </si>
+  <si>
+    <t>Chrysler|Fiat|Dodge|Ferrari|Maserati</t>
   </si>
 </sst>
 </file>
@@ -1875,15 +1874,15 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="36.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1891,60 +1890,60 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>94</v>
       </c>
-      <c r="B2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>95</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>96</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" t="s">
         <v>103</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>98</v>
-      </c>
-      <c r="B6" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>99</v>
-      </c>
-      <c r="B7" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>100</v>
-      </c>
-      <c r="B8" t="s">
-        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1956,30 +1955,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMO18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37.44140625" customWidth="1"/>
-    <col min="2" max="2" width="53.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="61.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.5" customWidth="1"/>
+    <col min="2" max="2" width="53.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="61.44140625" customWidth="1"/>
-    <col min="6" max="6" width="61.44140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="61.44140625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="61.5" customWidth="1"/>
+    <col min="6" max="6" width="61.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="61.5" style="6" customWidth="1"/>
     <col min="8" max="8" width="55.6640625" style="6" customWidth="1"/>
-    <col min="9" max="9" width="8.44140625" customWidth="1"/>
-    <col min="10" max="10" width="14.109375" customWidth="1"/>
+    <col min="9" max="9" width="8.5" customWidth="1"/>
+    <col min="10" max="10" width="14.1640625" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
     <col min="12" max="12" width="13.6640625" customWidth="1"/>
-    <col min="13" max="13" width="17.5546875" customWidth="1"/>
-    <col min="14" max="14" width="14.44140625" customWidth="1"/>
-    <col min="15" max="1030" width="8.5546875" customWidth="1"/>
+    <col min="13" max="13" width="17.5" customWidth="1"/>
+    <col min="14" max="14" width="14.5" customWidth="1"/>
+    <col min="15" max="1030" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14 1029:1029" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14 1029:1029" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1990,19 +1989,19 @@
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>3</v>
@@ -2024,7 +2023,7 @@
       </c>
       <c r="AMO1"/>
     </row>
-    <row r="2" spans="1:14 1029:1029" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14 1029:1029" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -2032,22 +2031,22 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
+        <v>209</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>213</v>
-      </c>
       <c r="G2" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -2068,7 +2067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14 1029:1029" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14 1029:1029" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -2076,22 +2075,22 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D3" s="6">
         <v>428</v>
       </c>
       <c r="E3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -2112,7 +2111,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:14 1029:1029" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14 1029:1029" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -2120,22 +2119,22 @@
         <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -2156,7 +2155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14 1029:1029" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14 1029:1029" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -2164,22 +2163,22 @@
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -2200,7 +2199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14 1029:1029" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14 1029:1029" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -2208,22 +2207,22 @@
         <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D6" s="6">
         <v>290</v>
       </c>
       <c r="E6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -2244,7 +2243,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:14 1029:1029" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14 1029:1029" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -2252,22 +2251,22 @@
         <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -2288,7 +2287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14 1029:1029" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14 1029:1029" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -2296,22 +2295,22 @@
         <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E8" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -2332,7 +2331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14 1029:1029" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14 1029:1029" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -2340,13 +2339,13 @@
         <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E9" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I9">
         <v>1</v>
@@ -2367,7 +2366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14 1029:1029" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14 1029:1029" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -2375,13 +2374,13 @@
         <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E10" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="I10">
         <v>1</v>
@@ -2402,7 +2401,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:14 1029:1029" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14 1029:1029" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -2410,13 +2409,13 @@
         <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E11" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I11">
         <v>1</v>
@@ -2437,7 +2436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14 1029:1029" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14 1029:1029" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -2445,22 +2444,22 @@
         <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E12" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G12" s="6">
         <v>344</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="I12">
         <v>2</v>
@@ -2481,7 +2480,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:14 1029:1029" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14 1029:1029" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -2489,22 +2488,22 @@
         <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E13" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I13">
         <v>2</v>
@@ -2525,7 +2524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:14 1029:1029" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14 1029:1029" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -2533,16 +2532,16 @@
         <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E14" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G14" s="6">
         <v>250</v>
@@ -2569,30 +2568,30 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:14 1029:1029" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14 1029:1029" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C15" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E15" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="I15">
         <v>2</v>
@@ -2613,7 +2612,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:14 1029:1029" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14 1029:1029" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -2621,22 +2620,22 @@
         <v>37</v>
       </c>
       <c r="C16" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E16" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I16">
         <v>3</v>
@@ -2657,7 +2656,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -2665,22 +2664,22 @@
         <v>39</v>
       </c>
       <c r="C17" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E17" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="I17">
         <v>6</v>
@@ -2701,7 +2700,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>40</v>
       </c>
@@ -2709,19 +2708,19 @@
         <v>41</v>
       </c>
       <c r="C18" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E18" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I18">
         <v>6</v>
@@ -2752,20 +2751,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="62.44140625" customWidth="1"/>
+    <col min="2" max="2" width="62.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="62.5" customWidth="1"/>
     <col min="12" max="12" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2773,16 +2772,16 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="E1" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="F1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G1" t="s">
         <v>42</v>
@@ -2806,24 +2805,24 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D2" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="E2" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="F2" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -2847,21 +2846,21 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D3" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="F3" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -2885,24 +2884,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C4" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D4" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="E4" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="F4" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -2926,24 +2925,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D5" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="E5" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="F5" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -2967,24 +2966,24 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C6" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D6" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="E6" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="F6" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -3008,21 +3007,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>50</v>
       </c>
       <c r="B7" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C7" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D7" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="E7" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="F7">
         <v>401</v>
@@ -3049,24 +3048,24 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C8" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D8" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="E8" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="F8" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -3090,24 +3089,24 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>52</v>
       </c>
       <c r="B9" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C9" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D9" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E9" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="F9" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -3131,24 +3130,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>53</v>
       </c>
       <c r="B10" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C10" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D10" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="E10" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="F10" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -3172,24 +3171,24 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C11" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D11" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E11" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="F11" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -3213,24 +3212,24 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C12" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D12" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="E12" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="F12" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -3254,24 +3253,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>55</v>
       </c>
       <c r="B13" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C13" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D13" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="E13" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="F13" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -3295,24 +3294,24 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>56</v>
       </c>
       <c r="B14" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C14" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D14" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="E14" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="F14" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="G14">
         <v>1</v>
@@ -3336,24 +3335,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>57</v>
       </c>
       <c r="B15" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C15" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D15" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="E15" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="F15" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="G15">
         <v>1</v>
@@ -3377,24 +3376,24 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>58</v>
       </c>
       <c r="B16" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C16" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D16" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="E16" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="F16" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="G16">
         <v>1</v>
@@ -3418,24 +3417,24 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C17" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D17" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="E17" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="F17" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="G17">
         <v>1</v>
@@ -3459,24 +3458,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>40</v>
       </c>
       <c r="B18" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C18" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D18" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E18" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F18" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G18">
         <v>1</v>
@@ -3500,24 +3499,24 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>59</v>
       </c>
       <c r="B19" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C19" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D19" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="E19" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="F19" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="G19">
         <v>1</v>
@@ -3541,24 +3540,24 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>60</v>
       </c>
       <c r="B20" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C20" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D20" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E20" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F20" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -3582,24 +3581,24 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>61</v>
       </c>
       <c r="B21" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C21" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D21" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="E21" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="F21" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -3623,24 +3622,24 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>62</v>
       </c>
       <c r="B22" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C22" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D22" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E22" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="F22" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="G22">
         <v>1</v>
@@ -3664,24 +3663,24 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>63</v>
       </c>
       <c r="B23" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C23" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="D23" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="E23" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="F23" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -3705,15 +3704,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>64</v>
       </c>
       <c r="B24" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C24" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D24">
         <v>2780</v>
@@ -3746,24 +3745,24 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>65</v>
       </c>
       <c r="B25" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C25" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D25" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="E25" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="F25" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="G25">
         <v>1</v>
@@ -3787,15 +3786,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>66</v>
       </c>
       <c r="B26" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C26" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D26">
         <v>276</v>
@@ -3804,7 +3803,7 @@
         <v>276</v>
       </c>
       <c r="F26" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="G26">
         <v>1</v>
@@ -3828,21 +3827,21 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>67</v>
       </c>
       <c r="B27" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C27" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D27">
         <v>2800</v>
       </c>
       <c r="E27" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="F27">
         <v>2800</v>
@@ -3869,24 +3868,24 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>68</v>
       </c>
       <c r="B28" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C28" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D28" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="E28" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="F28" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="G28">
         <v>1</v>
@@ -3910,24 +3909,24 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>69</v>
       </c>
       <c r="B29" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C29" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D29" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E29" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="F29" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="G29">
         <v>1</v>
@@ -3951,24 +3950,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>70</v>
       </c>
       <c r="B30" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C30" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D30" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="E30" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="F30" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="G30">
         <v>1</v>
@@ -3992,24 +3991,24 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>71</v>
       </c>
       <c r="B31" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C31" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D31" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="E31" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="F31" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="G31">
         <v>1</v>
@@ -4033,27 +4032,27 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>72</v>
       </c>
       <c r="B32" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C32" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D32" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="E32" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="F32" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="G32" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="H32">
         <v>1</v>
@@ -4085,18 +4084,18 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="131.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="99.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="131.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="99.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4104,87 +4103,87 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>77</v>
       </c>
       <c r="B2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>79</v>
       </c>
       <c r="B4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>80</v>
       </c>
       <c r="B5" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>81</v>
       </c>
       <c r="B6" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>82</v>
       </c>
       <c r="B7" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C8" t="s">
+        <v>495</v>
+      </c>
+      <c r="D8" t="s">
         <v>85</v>
-      </c>
-      <c r="D8" t="s">
-        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -4196,19 +4195,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4216,29 +4215,29 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>415</v>
+      </c>
+      <c r="B2" t="s">
+        <v>416</v>
+      </c>
+      <c r="C2" t="s">
         <v>417</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>418</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B3" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
         <v>420</v>
-      </c>
-      <c r="B3" t="s">
-        <v>421</v>
-      </c>
-      <c r="C3" t="s">
-        <v>422</v>
       </c>
     </row>
   </sheetData>
@@ -4254,15 +4253,15 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="131.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="131.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="110" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4270,87 +4269,87 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>77</v>
       </c>
       <c r="B2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B4" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>80</v>
       </c>
       <c r="B5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>81</v>
       </c>
       <c r="B6" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>82</v>
       </c>
       <c r="B7" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -4366,16 +4365,16 @@
       <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="144.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="144.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4383,30 +4382,30 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="F1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
+        <v>295</v>
+      </c>
+      <c r="C2" t="s">
+        <v>296</v>
+      </c>
+      <c r="D2" t="s">
         <v>297</v>
-      </c>
-      <c r="C2" t="s">
-        <v>298</v>
-      </c>
-      <c r="D2" t="s">
-        <v>299</v>
       </c>
       <c r="E2">
         <v>6</v>
@@ -4415,18 +4414,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B3" t="s">
+        <v>298</v>
+      </c>
+      <c r="C3" t="s">
+        <v>299</v>
+      </c>
+      <c r="D3" t="s">
         <v>300</v>
-      </c>
-      <c r="C3" t="s">
-        <v>301</v>
-      </c>
-      <c r="D3" t="s">
-        <v>302</v>
       </c>
       <c r="E3">
         <v>-1</v>
@@ -4435,38 +4434,38 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B4" t="s">
+        <v>301</v>
+      </c>
+      <c r="C4" t="s">
+        <v>302</v>
+      </c>
+      <c r="D4" t="s">
         <v>303</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B5" t="s">
         <v>304</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C5" t="s">
         <v>305</v>
       </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>112</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>306</v>
-      </c>
-      <c r="C5" t="s">
-        <v>307</v>
-      </c>
-      <c r="D5" t="s">
-        <v>308</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -4475,38 +4474,38 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B6" t="s">
+        <v>307</v>
+      </c>
+      <c r="C6" t="s">
+        <v>308</v>
+      </c>
+      <c r="D6" t="s">
         <v>309</v>
       </c>
-      <c r="C6" t="s">
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B7" t="s">
         <v>310</v>
       </c>
-      <c r="D6" t="s">
+      <c r="C7" t="s">
         <v>311</v>
       </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
         <v>312</v>
-      </c>
-      <c r="C7" t="s">
-        <v>313</v>
-      </c>
-      <c r="D7" t="s">
-        <v>314</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -4515,38 +4514,38 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B8" t="s">
+        <v>313</v>
+      </c>
+      <c r="C8" t="s">
+        <v>314</v>
+      </c>
+      <c r="D8" t="s">
         <v>315</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B9" t="s">
         <v>316</v>
       </c>
-      <c r="D8" t="s">
+      <c r="C9" t="s">
         <v>317</v>
       </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>116</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="D9" t="s">
         <v>318</v>
-      </c>
-      <c r="C9" t="s">
-        <v>319</v>
-      </c>
-      <c r="D9" t="s">
-        <v>320</v>
       </c>
       <c r="E9">
         <v>-1</v>
@@ -4555,18 +4554,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B10" t="s">
+        <v>319</v>
+      </c>
+      <c r="C10" t="s">
+        <v>320</v>
+      </c>
+      <c r="D10" t="s">
         <v>321</v>
-      </c>
-      <c r="C10" t="s">
-        <v>322</v>
-      </c>
-      <c r="D10" t="s">
-        <v>323</v>
       </c>
       <c r="E10">
         <v>2</v>
@@ -4575,18 +4574,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B11" t="s">
+        <v>322</v>
+      </c>
+      <c r="C11" t="s">
+        <v>323</v>
+      </c>
+      <c r="D11" t="s">
         <v>324</v>
-      </c>
-      <c r="C11" t="s">
-        <v>325</v>
-      </c>
-      <c r="D11" t="s">
-        <v>326</v>
       </c>
       <c r="E11">
         <v>2</v>
@@ -4595,18 +4594,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B12" t="s">
+        <v>325</v>
+      </c>
+      <c r="C12" t="s">
+        <v>326</v>
+      </c>
+      <c r="D12" t="s">
         <v>327</v>
-      </c>
-      <c r="C12" t="s">
-        <v>328</v>
-      </c>
-      <c r="D12" t="s">
-        <v>329</v>
       </c>
       <c r="E12">
         <v>2</v>
@@ -4615,18 +4614,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B13" t="s">
+        <v>328</v>
+      </c>
+      <c r="C13" t="s">
+        <v>329</v>
+      </c>
+      <c r="D13" t="s">
         <v>330</v>
-      </c>
-      <c r="C13" t="s">
-        <v>331</v>
-      </c>
-      <c r="D13" t="s">
-        <v>332</v>
       </c>
       <c r="E13">
         <v>2</v>
@@ -4635,18 +4634,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B14" t="s">
+        <v>331</v>
+      </c>
+      <c r="C14" t="s">
+        <v>332</v>
+      </c>
+      <c r="D14" t="s">
         <v>333</v>
-      </c>
-      <c r="C14" t="s">
-        <v>334</v>
-      </c>
-      <c r="D14" t="s">
-        <v>335</v>
       </c>
       <c r="E14">
         <v>2</v>
@@ -4655,146 +4654,146 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>121</v>
+      </c>
+      <c r="B15" t="s">
+        <v>334</v>
+      </c>
+      <c r="C15" t="s">
+        <v>335</v>
+      </c>
+      <c r="D15" t="s">
+        <v>336</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>122</v>
+      </c>
+      <c r="B16" t="s">
+        <v>337</v>
+      </c>
+      <c r="C16" t="s">
+        <v>338</v>
+      </c>
+      <c r="D16" t="s">
+        <v>339</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>123</v>
       </c>
-      <c r="B15" t="s">
-        <v>336</v>
-      </c>
-      <c r="C15" t="s">
-        <v>337</v>
-      </c>
-      <c r="D15" t="s">
-        <v>338</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="B17" t="s">
+        <v>340</v>
+      </c>
+      <c r="C17" t="s">
+        <v>341</v>
+      </c>
+      <c r="D17" t="s">
+        <v>342</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>124</v>
       </c>
-      <c r="B16" t="s">
-        <v>339</v>
-      </c>
-      <c r="C16" t="s">
-        <v>340</v>
-      </c>
-      <c r="D16" t="s">
-        <v>341</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="B18" t="s">
+        <v>343</v>
+      </c>
+      <c r="C18" t="s">
+        <v>343</v>
+      </c>
+      <c r="D18" t="s">
+        <v>344</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>148</v>
+      </c>
+      <c r="B19" t="s">
+        <v>345</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>125</v>
       </c>
-      <c r="B17" t="s">
-        <v>342</v>
-      </c>
-      <c r="C17" t="s">
-        <v>343</v>
-      </c>
-      <c r="D17" t="s">
-        <v>344</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="B20" t="s">
+        <v>408</v>
+      </c>
+      <c r="C20" t="s">
+        <v>346</v>
+      </c>
+      <c r="D20" t="s">
+        <v>347</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" t="s">
+        <v>348</v>
+      </c>
+      <c r="C21" t="s">
+        <v>349</v>
+      </c>
+      <c r="D21" t="s">
+        <v>350</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>126</v>
       </c>
-      <c r="B18" t="s">
-        <v>345</v>
-      </c>
-      <c r="C18" t="s">
-        <v>345</v>
-      </c>
-      <c r="D18" t="s">
-        <v>346</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>150</v>
-      </c>
-      <c r="B19" t="s">
-        <v>347</v>
-      </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>127</v>
-      </c>
-      <c r="B20" t="s">
-        <v>410</v>
-      </c>
-      <c r="C20" t="s">
-        <v>348</v>
-      </c>
-      <c r="D20" t="s">
-        <v>349</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>90</v>
-      </c>
-      <c r="B21" t="s">
-        <v>350</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="B22" t="s">
         <v>351</v>
       </c>
-      <c r="D21" t="s">
-        <v>352</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>128</v>
-      </c>
-      <c r="B22" t="s">
-        <v>353</v>
-      </c>
       <c r="C22" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D22" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E22">
         <v>4</v>
@@ -4803,18 +4802,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B23" t="s">
+        <v>352</v>
+      </c>
+      <c r="C23" t="s">
+        <v>353</v>
+      </c>
+      <c r="D23" t="s">
         <v>354</v>
-      </c>
-      <c r="C23" t="s">
-        <v>355</v>
-      </c>
-      <c r="D23" t="s">
-        <v>356</v>
       </c>
       <c r="E23">
         <v>-1</v>
@@ -4823,18 +4822,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B24" t="s">
+        <v>355</v>
+      </c>
+      <c r="C24" t="s">
+        <v>356</v>
+      </c>
+      <c r="D24" t="s">
         <v>357</v>
-      </c>
-      <c r="C24" t="s">
-        <v>358</v>
-      </c>
-      <c r="D24" t="s">
-        <v>359</v>
       </c>
       <c r="E24">
         <v>-1</v>
@@ -4843,18 +4842,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B25" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C25" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D25" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E25">
         <v>2</v>
@@ -4863,46 +4862,46 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B26" t="s">
+        <v>359</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>152</v>
+      </c>
+      <c r="B27" t="s">
+        <v>360</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>130</v>
+      </c>
+      <c r="B28" t="s">
         <v>361</v>
       </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-      <c r="F26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>154</v>
-      </c>
-      <c r="B27" t="s">
+      <c r="C28" t="s">
+        <v>361</v>
+      </c>
+      <c r="D28" t="s">
         <v>362</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>132</v>
-      </c>
-      <c r="B28" t="s">
-        <v>363</v>
-      </c>
-      <c r="C28" t="s">
-        <v>363</v>
-      </c>
-      <c r="D28" t="s">
-        <v>364</v>
       </c>
       <c r="E28">
         <v>-1</v>
@@ -4911,38 +4910,38 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B29" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C29" t="s">
+        <v>363</v>
+      </c>
+      <c r="D29" t="s">
+        <v>364</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>132</v>
+      </c>
+      <c r="B30" t="s">
         <v>365</v>
       </c>
-      <c r="D29" t="s">
+      <c r="C30" t="s">
         <v>366</v>
       </c>
-      <c r="E29">
-        <v>0</v>
-      </c>
-      <c r="F29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>134</v>
-      </c>
-      <c r="B30" t="s">
+      <c r="D30" t="s">
         <v>367</v>
-      </c>
-      <c r="C30" t="s">
-        <v>368</v>
-      </c>
-      <c r="D30" t="s">
-        <v>369</v>
       </c>
       <c r="E30">
         <v>-1</v>
@@ -4951,18 +4950,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B31" t="s">
+        <v>368</v>
+      </c>
+      <c r="C31" t="s">
+        <v>369</v>
+      </c>
+      <c r="D31" t="s">
         <v>370</v>
-      </c>
-      <c r="C31" t="s">
-        <v>371</v>
-      </c>
-      <c r="D31" t="s">
-        <v>372</v>
       </c>
       <c r="E31">
         <v>2</v>
@@ -4971,18 +4970,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B32" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C32" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D32" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="E32">
         <v>3</v>
@@ -4991,18 +4990,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B33" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C33" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D33" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="E33">
         <v>2</v>
@@ -5011,38 +5010,38 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B34" t="s">
+        <v>375</v>
+      </c>
+      <c r="C34" t="s">
+        <v>376</v>
+      </c>
+      <c r="D34" t="s">
         <v>377</v>
       </c>
-      <c r="C34" t="s">
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>137</v>
+      </c>
+      <c r="B35" t="s">
         <v>378</v>
       </c>
-      <c r="D34" t="s">
+      <c r="C35" t="s">
+        <v>378</v>
+      </c>
+      <c r="D35" t="s">
         <v>379</v>
-      </c>
-      <c r="E34">
-        <v>0</v>
-      </c>
-      <c r="F34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>139</v>
-      </c>
-      <c r="B35" t="s">
-        <v>380</v>
-      </c>
-      <c r="C35" t="s">
-        <v>380</v>
-      </c>
-      <c r="D35" t="s">
-        <v>381</v>
       </c>
       <c r="E35">
         <v>-1</v>
@@ -5051,18 +5050,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B36" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C36" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D36" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="E36">
         <v>-1</v>
@@ -5071,18 +5070,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B37" t="s">
+        <v>382</v>
+      </c>
+      <c r="C37" t="s">
+        <v>383</v>
+      </c>
+      <c r="D37" t="s">
         <v>384</v>
-      </c>
-      <c r="C37" t="s">
-        <v>385</v>
-      </c>
-      <c r="D37" t="s">
-        <v>386</v>
       </c>
       <c r="E37">
         <v>3</v>
@@ -5091,38 +5090,38 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B38" t="s">
+        <v>385</v>
+      </c>
+      <c r="C38" t="s">
+        <v>385</v>
+      </c>
+      <c r="D38" t="s">
+        <v>385</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>141</v>
+      </c>
+      <c r="B39" t="s">
+        <v>386</v>
+      </c>
+      <c r="C39" t="s">
         <v>387</v>
       </c>
-      <c r="C38" t="s">
-        <v>387</v>
-      </c>
-      <c r="D38" t="s">
-        <v>387</v>
-      </c>
-      <c r="E38">
-        <v>0</v>
-      </c>
-      <c r="F38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>143</v>
-      </c>
-      <c r="B39" t="s">
+      <c r="D39" t="s">
         <v>388</v>
-      </c>
-      <c r="C39" t="s">
-        <v>389</v>
-      </c>
-      <c r="D39" t="s">
-        <v>390</v>
       </c>
       <c r="E39">
         <v>3</v>
@@ -5131,38 +5130,38 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B40" t="s">
+        <v>389</v>
+      </c>
+      <c r="C40" t="s">
+        <v>390</v>
+      </c>
+      <c r="D40" t="s">
         <v>391</v>
       </c>
-      <c r="C40" t="s">
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>143</v>
+      </c>
+      <c r="B41" t="s">
         <v>392</v>
       </c>
-      <c r="D40" t="s">
+      <c r="C41" t="s">
         <v>393</v>
       </c>
-      <c r="E40">
-        <v>0</v>
-      </c>
-      <c r="F40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>145</v>
-      </c>
-      <c r="B41" t="s">
+      <c r="D41" t="s">
         <v>394</v>
-      </c>
-      <c r="C41" t="s">
-        <v>395</v>
-      </c>
-      <c r="D41" t="s">
-        <v>396</v>
       </c>
       <c r="E41">
         <v>6</v>
@@ -5171,12 +5170,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B42" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="E42">
         <v>6</v>
@@ -5185,18 +5184,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B43" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C43" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D43" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="E43">
         <v>6</v>
@@ -5205,18 +5204,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B44" t="s">
+        <v>397</v>
+      </c>
+      <c r="C44" t="s">
+        <v>398</v>
+      </c>
+      <c r="D44" t="s">
         <v>399</v>
-      </c>
-      <c r="C44" t="s">
-        <v>400</v>
-      </c>
-      <c r="D44" t="s">
-        <v>401</v>
       </c>
       <c r="E44">
         <v>6</v>
@@ -5225,18 +5224,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B45" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C45" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D45" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="E45">
         <v>2</v>
@@ -5245,38 +5244,38 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B46" t="s">
+        <v>402</v>
+      </c>
+      <c r="C46" t="s">
+        <v>403</v>
+      </c>
+      <c r="D46" t="s">
         <v>404</v>
       </c>
-      <c r="C46" t="s">
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>147</v>
+      </c>
+      <c r="B47" t="s">
         <v>405</v>
       </c>
-      <c r="D46" t="s">
+      <c r="C47" t="s">
         <v>406</v>
       </c>
-      <c r="E46">
-        <v>0</v>
-      </c>
-      <c r="F46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>149</v>
-      </c>
-      <c r="B47" t="s">
+      <c r="D47" t="s">
         <v>407</v>
-      </c>
-      <c r="C47" t="s">
-        <v>408</v>
-      </c>
-      <c r="D47" t="s">
-        <v>409</v>
       </c>
       <c r="F47">
         <v>1</v>
@@ -5299,13 +5298,13 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="39.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5313,26 +5312,26 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" t="s">
+        <v>413</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>91</v>
       </c>
-      <c r="B2" t="s">
-        <v>415</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>92</v>
-      </c>
       <c r="B3" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C3">
         <v>0</v>

</xml_diff>

<commit_message>
Explicit column names with prefix "regex_" and "index_" used with classcodes objects. Fix #79. Fix #80.
</commit_message>
<xml_diff>
--- a/data-raw/classcodes.xlsx
+++ b/data-raw/classcodes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erikbulow/coder/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBBD5F1D-E62B-0541-8390-5963D76F117F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{089EAE29-9CA4-9043-8A15-3588199F345B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24920" windowHeight="15540" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24920" windowHeight="15540" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ex_carbrands" sheetId="10" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="499">
   <si>
     <t>group</t>
   </si>
@@ -41,24 +41,6 @@
     <t>regex</t>
   </si>
   <si>
-    <t>charlson</t>
-  </si>
-  <si>
-    <t>deyo_ramano</t>
-  </si>
-  <si>
-    <t>dhoore</t>
-  </si>
-  <si>
-    <t>ghali</t>
-  </si>
-  <si>
-    <t>quan_original</t>
-  </si>
-  <si>
-    <t>quan_updated</t>
-  </si>
-  <si>
     <t>myocardial infarction</t>
   </si>
   <si>
@@ -158,18 +140,6 @@
     <t>HIV infection with related specified conditions.</t>
   </si>
   <si>
-    <t>sum_all</t>
-  </si>
-  <si>
-    <t>walraven</t>
-  </si>
-  <si>
-    <t>sid29</t>
-  </si>
-  <si>
-    <t>sid30</t>
-  </si>
-  <si>
     <t>pulmonary circulation disorder</t>
   </si>
   <si>
@@ -251,15 +221,6 @@
     <t>depression</t>
   </si>
   <si>
-    <t>sum_all_ahrq</t>
-  </si>
-  <si>
-    <t>ahrq_mort</t>
-  </si>
-  <si>
-    <t>ahrq_readm</t>
-  </si>
-  <si>
     <t>condition</t>
   </si>
   <si>
@@ -308,9 +269,6 @@
     <t>special</t>
   </si>
   <si>
-    <t>only_ordinary</t>
-  </si>
-  <si>
     <t>Mazda</t>
   </si>
   <si>
@@ -341,13 +299,7 @@
     <t>Porsche</t>
   </si>
   <si>
-    <t>Volvo|Lotus</t>
-  </si>
-  <si>
     <t>malignancy</t>
-  </si>
-  <si>
-    <t>regex_short</t>
   </si>
   <si>
     <t>regex_garland</t>
@@ -1296,9 +1248,6 @@
     <t>NFH([02]{2}|21)</t>
   </si>
   <si>
-    <t>pratt</t>
-  </si>
-  <si>
     <t>regex_icd9cm</t>
   </si>
   <si>
@@ -1522,6 +1471,63 @@
   </si>
   <si>
     <t>Chrysler|Fiat|Dodge|Ferrari|Maserati</t>
+  </si>
+  <si>
+    <t>Volvo|Lotus|Polestar</t>
+  </si>
+  <si>
+    <t>regex_icd10</t>
+  </si>
+  <si>
+    <t>index_charlson</t>
+  </si>
+  <si>
+    <t>index_deyo_ramano</t>
+  </si>
+  <si>
+    <t>index_dhoore</t>
+  </si>
+  <si>
+    <t>index_ghali</t>
+  </si>
+  <si>
+    <t>index_quan_original</t>
+  </si>
+  <si>
+    <t>index_quan_updated</t>
+  </si>
+  <si>
+    <t>regex_icd10_short</t>
+  </si>
+  <si>
+    <t>index_sum_all</t>
+  </si>
+  <si>
+    <t>index_sum_all_ahrq</t>
+  </si>
+  <si>
+    <t>index_walraven</t>
+  </si>
+  <si>
+    <t>index_sid29</t>
+  </si>
+  <si>
+    <t>index_sid30</t>
+  </si>
+  <si>
+    <t>index_ahrq_mort</t>
+  </si>
+  <si>
+    <t>index_ahrq_readm</t>
+  </si>
+  <si>
+    <t>regex_pratt</t>
+  </si>
+  <si>
+    <t>index_pratt</t>
+  </si>
+  <si>
+    <t>index_only_ordinary</t>
   </si>
 </sst>
 </file>
@@ -1874,7 +1880,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1892,58 +1898,58 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="B5" t="s">
-        <v>496</v>
+        <v>479</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="B6" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="B7" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="B8" t="s">
-        <v>103</v>
+        <v>480</v>
       </c>
     </row>
   </sheetData>
@@ -1955,8 +1961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMO18"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1986,67 +1992,67 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>481</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>3</v>
+        <v>482</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>4</v>
+        <v>483</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>5</v>
+        <v>484</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>6</v>
+        <v>485</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>7</v>
+        <v>486</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>8</v>
+        <v>487</v>
       </c>
       <c r="AMO1"/>
     </row>
     <row r="2" spans="1:14 1029:1029" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>209</v>
+        <v>193</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -2069,28 +2075,28 @@
     </row>
     <row r="3" spans="1:14 1029:1029" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>223</v>
+        <v>207</v>
       </c>
       <c r="D3" s="6">
         <v>428</v>
       </c>
       <c r="E3" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -2113,28 +2119,28 @@
     </row>
     <row r="4" spans="1:14 1029:1029" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>224</v>
+        <v>208</v>
       </c>
       <c r="D4" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="E4" t="s">
         <v>181</v>
       </c>
-      <c r="E4" t="s">
-        <v>197</v>
-      </c>
       <c r="F4" s="6" t="s">
-        <v>231</v>
+        <v>215</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -2157,28 +2163,28 @@
     </row>
     <row r="5" spans="1:14 1029:1029" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>225</v>
+        <v>209</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
       <c r="E5" t="s">
-        <v>198</v>
+        <v>182</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>232</v>
+        <v>216</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -2201,28 +2207,28 @@
     </row>
     <row r="6" spans="1:14 1029:1029" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>226</v>
+        <v>210</v>
       </c>
       <c r="D6" s="6">
         <v>290</v>
       </c>
       <c r="E6" t="s">
-        <v>199</v>
+        <v>183</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>233</v>
+        <v>217</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -2245,28 +2251,28 @@
     </row>
     <row r="7" spans="1:14 1029:1029" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>227</v>
+        <v>211</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="E7" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>227</v>
+        <v>211</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -2289,28 +2295,28 @@
     </row>
     <row r="8" spans="1:14 1029:1029" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
       <c r="E8" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -2333,19 +2339,19 @@
     </row>
     <row r="9" spans="1:14 1029:1029" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="E9" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="I9">
         <v>1</v>
@@ -2368,19 +2374,19 @@
     </row>
     <row r="10" spans="1:14 1029:1029" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>228</v>
+        <v>212</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="E10" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="I10">
         <v>1</v>
@@ -2403,19 +2409,19 @@
     </row>
     <row r="11" spans="1:14 1029:1029" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>214</v>
+        <v>198</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="E11" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="I11">
         <v>1</v>
@@ -2438,28 +2444,28 @@
     </row>
     <row r="12" spans="1:14 1029:1029" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="E12" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="G12" s="6">
         <v>344</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
       <c r="I12">
         <v>2</v>
@@ -2482,28 +2488,28 @@
     </row>
     <row r="13" spans="1:14 1029:1029" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
       <c r="E13" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="I13">
         <v>2</v>
@@ -2526,22 +2532,22 @@
     </row>
     <row r="14" spans="1:14 1029:1029" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>217</v>
+        <v>201</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="E14" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>218</v>
+        <v>202</v>
       </c>
       <c r="G14" s="6">
         <v>250</v>
@@ -2570,28 +2576,28 @@
     </row>
     <row r="15" spans="1:14 1029:1029" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>219</v>
+        <v>203</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="E15" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>219</v>
+        <v>203</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="I15">
         <v>2</v>
@@ -2614,28 +2620,28 @@
     </row>
     <row r="16" spans="1:14 1029:1029" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>191</v>
+        <v>175</v>
       </c>
       <c r="E16" t="s">
-        <v>208</v>
+        <v>192</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>235</v>
+        <v>219</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="I16">
         <v>3</v>
@@ -2658,28 +2664,28 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>220</v>
+        <v>204</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>192</v>
+        <v>176</v>
       </c>
       <c r="E17" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>220</v>
+        <v>204</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="I17">
         <v>6</v>
@@ -2702,25 +2708,25 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>221</v>
+        <v>205</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="E18" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
       <c r="I18">
         <v>6</v>
@@ -2751,8 +2757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2769,60 +2775,60 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>481</v>
       </c>
       <c r="C1" t="s">
-        <v>105</v>
+        <v>488</v>
       </c>
       <c r="D1" t="s">
-        <v>422</v>
+        <v>405</v>
       </c>
       <c r="E1" t="s">
-        <v>446</v>
+        <v>429</v>
       </c>
       <c r="F1" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="G1" t="s">
-        <v>42</v>
+        <v>489</v>
       </c>
       <c r="H1" t="s">
-        <v>73</v>
+        <v>490</v>
       </c>
       <c r="I1" t="s">
-        <v>43</v>
+        <v>491</v>
       </c>
       <c r="J1" t="s">
-        <v>44</v>
+        <v>492</v>
       </c>
       <c r="K1" t="s">
-        <v>45</v>
+        <v>493</v>
       </c>
       <c r="L1" t="s">
-        <v>74</v>
+        <v>494</v>
       </c>
       <c r="M1" t="s">
-        <v>75</v>
+        <v>495</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>223</v>
+        <v>207</v>
       </c>
       <c r="C2" t="s">
-        <v>273</v>
+        <v>257</v>
       </c>
       <c r="D2" t="s">
-        <v>425</v>
+        <v>408</v>
       </c>
       <c r="E2" t="s">
-        <v>447</v>
+        <v>430</v>
       </c>
       <c r="F2" t="s">
-        <v>469</v>
+        <v>452</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -2848,19 +2854,19 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>263</v>
+        <v>247</v>
       </c>
       <c r="C3" t="s">
-        <v>274</v>
+        <v>258</v>
       </c>
       <c r="D3" t="s">
-        <v>470</v>
+        <v>453</v>
       </c>
       <c r="F3" t="s">
-        <v>471</v>
+        <v>454</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -2886,22 +2892,22 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>264</v>
+        <v>248</v>
       </c>
       <c r="C4" t="s">
-        <v>275</v>
+        <v>259</v>
       </c>
       <c r="D4" t="s">
-        <v>448</v>
+        <v>431</v>
       </c>
       <c r="E4" t="s">
-        <v>449</v>
+        <v>432</v>
       </c>
       <c r="F4" t="s">
-        <v>472</v>
+        <v>455</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -2927,22 +2933,22 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>236</v>
+        <v>220</v>
       </c>
       <c r="C5" t="s">
-        <v>237</v>
+        <v>221</v>
       </c>
       <c r="D5" t="s">
-        <v>426</v>
+        <v>409</v>
       </c>
       <c r="E5" t="s">
-        <v>426</v>
+        <v>409</v>
       </c>
       <c r="F5" t="s">
-        <v>473</v>
+        <v>456</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -2968,22 +2974,22 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>224</v>
+        <v>208</v>
       </c>
       <c r="C6" t="s">
-        <v>276</v>
+        <v>260</v>
       </c>
       <c r="D6" t="s">
-        <v>450</v>
+        <v>433</v>
       </c>
       <c r="E6" t="s">
-        <v>451</v>
+        <v>434</v>
       </c>
       <c r="F6" t="s">
-        <v>474</v>
+        <v>457</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -3009,19 +3015,19 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>238</v>
+        <v>222</v>
       </c>
       <c r="C7" t="s">
-        <v>238</v>
+        <v>222</v>
       </c>
       <c r="D7" t="s">
-        <v>423</v>
+        <v>406</v>
       </c>
       <c r="E7" t="s">
-        <v>452</v>
+        <v>435</v>
       </c>
       <c r="F7">
         <v>401</v>
@@ -3050,22 +3056,22 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
       <c r="C8" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
       <c r="D8" t="s">
-        <v>424</v>
+        <v>407</v>
       </c>
       <c r="E8" t="s">
-        <v>453</v>
+        <v>436</v>
       </c>
       <c r="F8" t="s">
-        <v>475</v>
+        <v>458</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -3091,22 +3097,22 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="C9" t="s">
-        <v>240</v>
+        <v>224</v>
       </c>
       <c r="D9" t="s">
-        <v>427</v>
+        <v>410</v>
       </c>
       <c r="E9" t="s">
-        <v>454</v>
+        <v>437</v>
       </c>
       <c r="F9" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -3132,22 +3138,22 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>265</v>
+        <v>249</v>
       </c>
       <c r="C10" t="s">
-        <v>277</v>
+        <v>261</v>
       </c>
       <c r="D10" t="s">
-        <v>428</v>
+        <v>411</v>
       </c>
       <c r="E10" t="s">
-        <v>455</v>
+        <v>438</v>
       </c>
       <c r="F10" t="s">
-        <v>476</v>
+        <v>459</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -3173,22 +3179,22 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>266</v>
+        <v>250</v>
       </c>
       <c r="C11" t="s">
-        <v>278</v>
+        <v>262</v>
       </c>
       <c r="D11" t="s">
-        <v>429</v>
+        <v>412</v>
       </c>
       <c r="E11" t="s">
-        <v>456</v>
+        <v>439</v>
       </c>
       <c r="F11" t="s">
-        <v>477</v>
+        <v>460</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -3214,22 +3220,22 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B12" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
       <c r="C12" t="s">
-        <v>218</v>
+        <v>202</v>
       </c>
       <c r="D12" t="s">
-        <v>430</v>
+        <v>413</v>
       </c>
       <c r="E12" t="s">
-        <v>457</v>
+        <v>440</v>
       </c>
       <c r="F12" t="s">
-        <v>430</v>
+        <v>413</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -3255,22 +3261,22 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>242</v>
+        <v>226</v>
       </c>
       <c r="C13" t="s">
-        <v>218</v>
+        <v>202</v>
       </c>
       <c r="D13" t="s">
-        <v>431</v>
+        <v>414</v>
       </c>
       <c r="E13" t="s">
-        <v>479</v>
+        <v>462</v>
       </c>
       <c r="F13" t="s">
-        <v>478</v>
+        <v>461</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -3296,22 +3302,22 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B14" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
       <c r="C14" t="s">
-        <v>244</v>
+        <v>228</v>
       </c>
       <c r="D14" t="s">
-        <v>432</v>
+        <v>415</v>
       </c>
       <c r="E14" t="s">
-        <v>458</v>
+        <v>441</v>
       </c>
       <c r="F14" t="s">
-        <v>480</v>
+        <v>463</v>
       </c>
       <c r="G14">
         <v>1</v>
@@ -3337,22 +3343,22 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>267</v>
+        <v>251</v>
       </c>
       <c r="C15" t="s">
-        <v>279</v>
+        <v>263</v>
       </c>
       <c r="D15" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="E15" t="s">
-        <v>481</v>
+        <v>464</v>
       </c>
       <c r="F15" t="s">
-        <v>482</v>
+        <v>465</v>
       </c>
       <c r="G15">
         <v>1</v>
@@ -3378,22 +3384,22 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B16" t="s">
-        <v>268</v>
+        <v>252</v>
       </c>
       <c r="C16" t="s">
-        <v>280</v>
+        <v>264</v>
       </c>
       <c r="D16" t="s">
-        <v>434</v>
+        <v>417</v>
       </c>
       <c r="E16" t="s">
-        <v>459</v>
+        <v>442</v>
       </c>
       <c r="F16" t="s">
-        <v>483</v>
+        <v>466</v>
       </c>
       <c r="G16">
         <v>1</v>
@@ -3419,22 +3425,22 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>245</v>
+        <v>229</v>
       </c>
       <c r="C17" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
       <c r="D17" t="s">
-        <v>435</v>
+        <v>418</v>
       </c>
       <c r="E17" t="s">
-        <v>460</v>
+        <v>443</v>
       </c>
       <c r="F17" t="s">
-        <v>484</v>
+        <v>467</v>
       </c>
       <c r="G17">
         <v>1</v>
@@ -3460,22 +3466,22 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>221</v>
+        <v>205</v>
       </c>
       <c r="C18" t="s">
-        <v>246</v>
+        <v>230</v>
       </c>
       <c r="D18" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="E18" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="F18" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="G18">
         <v>1</v>
@@ -3501,22 +3507,22 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B19" t="s">
-        <v>247</v>
+        <v>231</v>
       </c>
       <c r="C19" t="s">
-        <v>248</v>
+        <v>232</v>
       </c>
       <c r="D19" t="s">
-        <v>436</v>
+        <v>419</v>
       </c>
       <c r="E19" t="s">
-        <v>461</v>
+        <v>444</v>
       </c>
       <c r="F19" t="s">
-        <v>485</v>
+        <v>468</v>
       </c>
       <c r="G19">
         <v>1</v>
@@ -3542,22 +3548,22 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B20" t="s">
-        <v>220</v>
+        <v>204</v>
       </c>
       <c r="C20" t="s">
-        <v>220</v>
+        <v>204</v>
       </c>
       <c r="D20" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="E20" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="F20" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -3583,22 +3589,22 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B21" t="s">
-        <v>249</v>
+        <v>233</v>
       </c>
       <c r="C21" t="s">
-        <v>249</v>
+        <v>233</v>
       </c>
       <c r="D21" t="s">
-        <v>437</v>
+        <v>420</v>
       </c>
       <c r="E21" t="s">
-        <v>462</v>
+        <v>445</v>
       </c>
       <c r="F21" t="s">
-        <v>486</v>
+        <v>469</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -3624,22 +3630,22 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B22" t="s">
-        <v>269</v>
+        <v>253</v>
       </c>
       <c r="C22" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
       <c r="D22" t="s">
-        <v>438</v>
+        <v>421</v>
       </c>
       <c r="E22" t="s">
-        <v>438</v>
+        <v>421</v>
       </c>
       <c r="F22" t="s">
-        <v>487</v>
+        <v>470</v>
       </c>
       <c r="G22">
         <v>1</v>
@@ -3665,22 +3671,22 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B23" t="s">
-        <v>250</v>
+        <v>234</v>
       </c>
       <c r="C23" t="s">
-        <v>251</v>
+        <v>235</v>
       </c>
       <c r="D23" t="s">
-        <v>439</v>
+        <v>422</v>
       </c>
       <c r="E23" t="s">
-        <v>439</v>
+        <v>422</v>
       </c>
       <c r="F23" t="s">
-        <v>439</v>
+        <v>422</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -3706,13 +3712,13 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B24" t="s">
-        <v>252</v>
+        <v>236</v>
       </c>
       <c r="C24" t="s">
-        <v>252</v>
+        <v>236</v>
       </c>
       <c r="D24">
         <v>2780</v>
@@ -3747,22 +3753,22 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B25" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="C25" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
       <c r="D25" t="s">
-        <v>440</v>
+        <v>423</v>
       </c>
       <c r="E25" t="s">
-        <v>463</v>
+        <v>446</v>
       </c>
       <c r="F25" t="s">
-        <v>488</v>
+        <v>471</v>
       </c>
       <c r="G25">
         <v>1</v>
@@ -3788,13 +3794,13 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B26" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="C26" t="s">
-        <v>254</v>
+        <v>238</v>
       </c>
       <c r="D26">
         <v>276</v>
@@ -3803,7 +3809,7 @@
         <v>276</v>
       </c>
       <c r="F26" t="s">
-        <v>489</v>
+        <v>472</v>
       </c>
       <c r="G26">
         <v>1</v>
@@ -3829,19 +3835,19 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B27" t="s">
-        <v>255</v>
+        <v>239</v>
       </c>
       <c r="C27" t="s">
-        <v>256</v>
+        <v>240</v>
       </c>
       <c r="D27">
         <v>2800</v>
       </c>
       <c r="E27" t="s">
-        <v>464</v>
+        <v>447</v>
       </c>
       <c r="F27">
         <v>2800</v>
@@ -3870,22 +3876,22 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="B28" t="s">
-        <v>257</v>
+        <v>241</v>
       </c>
       <c r="C28" t="s">
-        <v>258</v>
+        <v>242</v>
       </c>
       <c r="D28" t="s">
-        <v>441</v>
+        <v>424</v>
       </c>
       <c r="E28" t="s">
-        <v>465</v>
+        <v>448</v>
       </c>
       <c r="F28" t="s">
-        <v>490</v>
+        <v>473</v>
       </c>
       <c r="G28">
         <v>1</v>
@@ -3911,22 +3917,22 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B29" t="s">
-        <v>271</v>
+        <v>255</v>
       </c>
       <c r="C29" t="s">
-        <v>283</v>
+        <v>267</v>
       </c>
       <c r="D29" t="s">
-        <v>442</v>
+        <v>425</v>
       </c>
       <c r="E29" t="s">
-        <v>466</v>
+        <v>449</v>
       </c>
       <c r="F29" t="s">
-        <v>491</v>
+        <v>474</v>
       </c>
       <c r="G29">
         <v>1</v>
@@ -3952,22 +3958,22 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B30" t="s">
-        <v>272</v>
+        <v>256</v>
       </c>
       <c r="C30" t="s">
-        <v>284</v>
+        <v>268</v>
       </c>
       <c r="D30" t="s">
-        <v>443</v>
+        <v>426</v>
       </c>
       <c r="E30" t="s">
-        <v>467</v>
+        <v>450</v>
       </c>
       <c r="F30" t="s">
-        <v>492</v>
+        <v>475</v>
       </c>
       <c r="G30">
         <v>1</v>
@@ -3993,22 +3999,22 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="B31" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
       <c r="C31" t="s">
-        <v>260</v>
+        <v>244</v>
       </c>
       <c r="D31" t="s">
-        <v>444</v>
+        <v>427</v>
       </c>
       <c r="E31" t="s">
-        <v>444</v>
+        <v>427</v>
       </c>
       <c r="F31" t="s">
-        <v>493</v>
+        <v>476</v>
       </c>
       <c r="G31">
         <v>1</v>
@@ -4034,25 +4040,25 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B32" t="s">
-        <v>261</v>
+        <v>245</v>
       </c>
       <c r="C32" t="s">
-        <v>262</v>
+        <v>246</v>
       </c>
       <c r="D32" t="s">
-        <v>445</v>
+        <v>428</v>
       </c>
       <c r="E32" t="s">
-        <v>445</v>
+        <v>428</v>
       </c>
       <c r="F32" t="s">
-        <v>494</v>
+        <v>477</v>
       </c>
       <c r="G32" t="s">
-        <v>468</v>
+        <v>451</v>
       </c>
       <c r="H32">
         <v>1</v>
@@ -4083,8 +4089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4100,90 +4106,90 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>481</v>
       </c>
       <c r="C1" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="D1" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>285</v>
+        <v>269</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
-        <v>286</v>
+        <v>270</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="B4" t="s">
-        <v>287</v>
+        <v>271</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s">
-        <v>288</v>
+        <v>272</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="B6" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B7" t="s">
-        <v>290</v>
+        <v>274</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>194</v>
+        <v>178</v>
       </c>
       <c r="C8" t="s">
-        <v>495</v>
+        <v>478</v>
       </c>
       <c r="D8" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -4195,8 +4201,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4212,32 +4218,32 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>481</v>
       </c>
       <c r="C1" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>415</v>
+        <v>399</v>
       </c>
       <c r="B2" t="s">
-        <v>416</v>
+        <v>400</v>
       </c>
       <c r="C2" t="s">
-        <v>417</v>
+        <v>401</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>418</v>
+        <v>402</v>
       </c>
       <c r="B3" t="s">
-        <v>419</v>
+        <v>403</v>
       </c>
       <c r="C3" t="s">
-        <v>420</v>
+        <v>404</v>
       </c>
     </row>
   </sheetData>
@@ -4250,7 +4256,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4266,90 +4272,90 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>481</v>
       </c>
       <c r="C1" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="D1" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>291</v>
+        <v>275</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>292</v>
+        <v>276</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s">
-        <v>293</v>
+        <v>277</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s">
-        <v>294</v>
+        <v>278</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="B6" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B7" t="s">
-        <v>290</v>
+        <v>274</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>194</v>
+        <v>178</v>
       </c>
       <c r="C8" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="D8" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -4361,8 +4367,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4379,33 +4385,33 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>496</v>
       </c>
       <c r="C1" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="D1" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="E1" t="s">
-        <v>421</v>
+        <v>497</v>
       </c>
       <c r="F1" t="s">
-        <v>42</v>
+        <v>489</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
-        <v>295</v>
+        <v>279</v>
       </c>
       <c r="C2" t="s">
-        <v>296</v>
+        <v>280</v>
       </c>
       <c r="D2" t="s">
-        <v>297</v>
+        <v>281</v>
       </c>
       <c r="E2">
         <v>6</v>
@@ -4416,16 +4422,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="B3" t="s">
-        <v>298</v>
+        <v>282</v>
       </c>
       <c r="C3" t="s">
-        <v>299</v>
+        <v>283</v>
       </c>
       <c r="D3" t="s">
-        <v>300</v>
+        <v>284</v>
       </c>
       <c r="E3">
         <v>-1</v>
@@ -4436,16 +4442,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="B4" t="s">
-        <v>301</v>
+        <v>285</v>
       </c>
       <c r="C4" t="s">
-        <v>302</v>
+        <v>286</v>
       </c>
       <c r="D4" t="s">
-        <v>303</v>
+        <v>287</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -4456,16 +4462,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="B5" t="s">
-        <v>304</v>
+        <v>288</v>
       </c>
       <c r="C5" t="s">
-        <v>305</v>
+        <v>289</v>
       </c>
       <c r="D5" t="s">
-        <v>306</v>
+        <v>290</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -4476,16 +4482,16 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="B6" t="s">
-        <v>307</v>
+        <v>291</v>
       </c>
       <c r="C6" t="s">
-        <v>308</v>
+        <v>292</v>
       </c>
       <c r="D6" t="s">
-        <v>309</v>
+        <v>293</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -4496,16 +4502,16 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="B7" t="s">
-        <v>310</v>
+        <v>294</v>
       </c>
       <c r="C7" t="s">
-        <v>311</v>
+        <v>295</v>
       </c>
       <c r="D7" t="s">
-        <v>312</v>
+        <v>296</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -4516,16 +4522,16 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="B8" t="s">
-        <v>313</v>
+        <v>297</v>
       </c>
       <c r="C8" t="s">
-        <v>314</v>
+        <v>298</v>
       </c>
       <c r="D8" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -4536,16 +4542,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="B9" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="C9" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="D9" t="s">
-        <v>318</v>
+        <v>302</v>
       </c>
       <c r="E9">
         <v>-1</v>
@@ -4556,16 +4562,16 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="B10" t="s">
-        <v>319</v>
+        <v>303</v>
       </c>
       <c r="C10" t="s">
-        <v>320</v>
+        <v>304</v>
       </c>
       <c r="D10" t="s">
-        <v>321</v>
+        <v>305</v>
       </c>
       <c r="E10">
         <v>2</v>
@@ -4576,16 +4582,16 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="B11" t="s">
-        <v>322</v>
+        <v>306</v>
       </c>
       <c r="C11" t="s">
-        <v>323</v>
+        <v>307</v>
       </c>
       <c r="D11" t="s">
-        <v>324</v>
+        <v>308</v>
       </c>
       <c r="E11">
         <v>2</v>
@@ -4596,16 +4602,16 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="B12" t="s">
-        <v>325</v>
+        <v>309</v>
       </c>
       <c r="C12" t="s">
-        <v>326</v>
+        <v>310</v>
       </c>
       <c r="D12" t="s">
-        <v>327</v>
+        <v>311</v>
       </c>
       <c r="E12">
         <v>2</v>
@@ -4616,16 +4622,16 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="B13" t="s">
-        <v>328</v>
+        <v>312</v>
       </c>
       <c r="C13" t="s">
-        <v>329</v>
+        <v>313</v>
       </c>
       <c r="D13" t="s">
-        <v>330</v>
+        <v>314</v>
       </c>
       <c r="E13">
         <v>2</v>
@@ -4636,16 +4642,16 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="B14" t="s">
-        <v>331</v>
+        <v>315</v>
       </c>
       <c r="C14" t="s">
-        <v>332</v>
+        <v>316</v>
       </c>
       <c r="D14" t="s">
-        <v>333</v>
+        <v>317</v>
       </c>
       <c r="E14">
         <v>2</v>
@@ -4656,16 +4662,16 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="B15" t="s">
-        <v>334</v>
+        <v>318</v>
       </c>
       <c r="C15" t="s">
-        <v>335</v>
+        <v>319</v>
       </c>
       <c r="D15" t="s">
-        <v>336</v>
+        <v>320</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -4676,16 +4682,16 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="B16" t="s">
-        <v>337</v>
+        <v>321</v>
       </c>
       <c r="C16" t="s">
-        <v>338</v>
+        <v>322</v>
       </c>
       <c r="D16" t="s">
-        <v>339</v>
+        <v>323</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -4696,16 +4702,16 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="B17" t="s">
-        <v>340</v>
+        <v>324</v>
       </c>
       <c r="C17" t="s">
-        <v>341</v>
+        <v>325</v>
       </c>
       <c r="D17" t="s">
-        <v>342</v>
+        <v>326</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -4716,16 +4722,16 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="B18" t="s">
-        <v>343</v>
+        <v>327</v>
       </c>
       <c r="C18" t="s">
-        <v>343</v>
+        <v>327</v>
       </c>
       <c r="D18" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -4736,10 +4742,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="B19" t="s">
-        <v>345</v>
+        <v>329</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -4747,16 +4753,16 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="B20" t="s">
-        <v>408</v>
+        <v>392</v>
       </c>
       <c r="C20" t="s">
-        <v>346</v>
+        <v>330</v>
       </c>
       <c r="D20" t="s">
-        <v>347</v>
+        <v>331</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -4764,16 +4770,16 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="B21" t="s">
-        <v>348</v>
+        <v>332</v>
       </c>
       <c r="C21" t="s">
-        <v>349</v>
+        <v>333</v>
       </c>
       <c r="D21" t="s">
-        <v>350</v>
+        <v>334</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -4784,16 +4790,16 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="B22" t="s">
-        <v>351</v>
+        <v>335</v>
       </c>
       <c r="C22" t="s">
-        <v>351</v>
+        <v>335</v>
       </c>
       <c r="D22" t="s">
-        <v>351</v>
+        <v>335</v>
       </c>
       <c r="E22">
         <v>4</v>
@@ -4804,16 +4810,16 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="B23" t="s">
-        <v>352</v>
+        <v>336</v>
       </c>
       <c r="C23" t="s">
-        <v>353</v>
+        <v>337</v>
       </c>
       <c r="D23" t="s">
-        <v>354</v>
+        <v>338</v>
       </c>
       <c r="E23">
         <v>-1</v>
@@ -4824,16 +4830,16 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="B24" t="s">
-        <v>355</v>
+        <v>339</v>
       </c>
       <c r="C24" t="s">
-        <v>356</v>
+        <v>340</v>
       </c>
       <c r="D24" t="s">
-        <v>357</v>
+        <v>341</v>
       </c>
       <c r="E24">
         <v>-1</v>
@@ -4844,16 +4850,16 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="B25" t="s">
-        <v>358</v>
+        <v>342</v>
       </c>
       <c r="C25" t="s">
-        <v>358</v>
+        <v>342</v>
       </c>
       <c r="D25" t="s">
-        <v>358</v>
+        <v>342</v>
       </c>
       <c r="E25">
         <v>2</v>
@@ -4864,10 +4870,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="B26" t="s">
-        <v>359</v>
+        <v>343</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -4878,10 +4884,10 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="B27" t="s">
-        <v>360</v>
+        <v>344</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -4892,16 +4898,16 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="B28" t="s">
-        <v>361</v>
+        <v>345</v>
       </c>
       <c r="C28" t="s">
-        <v>361</v>
+        <v>345</v>
       </c>
       <c r="D28" t="s">
-        <v>362</v>
+        <v>346</v>
       </c>
       <c r="E28">
         <v>-1</v>
@@ -4912,16 +4918,16 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="B29" t="s">
-        <v>409</v>
+        <v>393</v>
       </c>
       <c r="C29" t="s">
-        <v>363</v>
+        <v>347</v>
       </c>
       <c r="D29" t="s">
-        <v>364</v>
+        <v>348</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -4932,16 +4938,16 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="B30" t="s">
-        <v>365</v>
+        <v>349</v>
       </c>
       <c r="C30" t="s">
-        <v>366</v>
+        <v>350</v>
       </c>
       <c r="D30" t="s">
-        <v>367</v>
+        <v>351</v>
       </c>
       <c r="E30">
         <v>-1</v>
@@ -4952,16 +4958,16 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="B31" t="s">
-        <v>368</v>
+        <v>352</v>
       </c>
       <c r="C31" t="s">
-        <v>369</v>
+        <v>353</v>
       </c>
       <c r="D31" t="s">
-        <v>370</v>
+        <v>354</v>
       </c>
       <c r="E31">
         <v>2</v>
@@ -4972,16 +4978,16 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="B32" t="s">
-        <v>371</v>
+        <v>355</v>
       </c>
       <c r="C32" t="s">
-        <v>372</v>
+        <v>356</v>
       </c>
       <c r="D32" t="s">
-        <v>372</v>
+        <v>356</v>
       </c>
       <c r="E32">
         <v>3</v>
@@ -4992,16 +4998,16 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="B33" t="s">
-        <v>373</v>
+        <v>357</v>
       </c>
       <c r="C33" t="s">
-        <v>373</v>
+        <v>357</v>
       </c>
       <c r="D33" t="s">
-        <v>374</v>
+        <v>358</v>
       </c>
       <c r="E33">
         <v>2</v>
@@ -5012,16 +5018,16 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="B34" t="s">
-        <v>375</v>
+        <v>359</v>
       </c>
       <c r="C34" t="s">
-        <v>376</v>
+        <v>360</v>
       </c>
       <c r="D34" t="s">
-        <v>377</v>
+        <v>361</v>
       </c>
       <c r="E34">
         <v>0</v>
@@ -5032,16 +5038,16 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="B35" t="s">
-        <v>378</v>
+        <v>362</v>
       </c>
       <c r="C35" t="s">
-        <v>378</v>
+        <v>362</v>
       </c>
       <c r="D35" t="s">
-        <v>379</v>
+        <v>363</v>
       </c>
       <c r="E35">
         <v>-1</v>
@@ -5052,16 +5058,16 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="B36" t="s">
-        <v>410</v>
+        <v>394</v>
       </c>
       <c r="C36" t="s">
-        <v>380</v>
+        <v>364</v>
       </c>
       <c r="D36" t="s">
-        <v>381</v>
+        <v>365</v>
       </c>
       <c r="E36">
         <v>-1</v>
@@ -5072,16 +5078,16 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="B37" t="s">
-        <v>382</v>
+        <v>366</v>
       </c>
       <c r="C37" t="s">
-        <v>383</v>
+        <v>367</v>
       </c>
       <c r="D37" t="s">
-        <v>384</v>
+        <v>368</v>
       </c>
       <c r="E37">
         <v>3</v>
@@ -5092,16 +5098,16 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="B38" t="s">
-        <v>385</v>
+        <v>369</v>
       </c>
       <c r="C38" t="s">
-        <v>385</v>
+        <v>369</v>
       </c>
       <c r="D38" t="s">
-        <v>385</v>
+        <v>369</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -5112,16 +5118,16 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="B39" t="s">
-        <v>386</v>
+        <v>370</v>
       </c>
       <c r="C39" t="s">
-        <v>387</v>
+        <v>371</v>
       </c>
       <c r="D39" t="s">
-        <v>388</v>
+        <v>372</v>
       </c>
       <c r="E39">
         <v>3</v>
@@ -5132,16 +5138,16 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="B40" t="s">
-        <v>389</v>
+        <v>373</v>
       </c>
       <c r="C40" t="s">
-        <v>390</v>
+        <v>374</v>
       </c>
       <c r="D40" t="s">
-        <v>391</v>
+        <v>375</v>
       </c>
       <c r="E40">
         <v>0</v>
@@ -5152,16 +5158,16 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="B41" t="s">
-        <v>392</v>
+        <v>376</v>
       </c>
       <c r="C41" t="s">
-        <v>393</v>
+        <v>377</v>
       </c>
       <c r="D41" t="s">
-        <v>394</v>
+        <v>378</v>
       </c>
       <c r="E41">
         <v>6</v>
@@ -5172,10 +5178,10 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="B42" t="s">
-        <v>395</v>
+        <v>379</v>
       </c>
       <c r="E42">
         <v>6</v>
@@ -5186,16 +5192,16 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="B43" t="s">
-        <v>411</v>
+        <v>395</v>
       </c>
       <c r="C43" t="s">
-        <v>412</v>
+        <v>396</v>
       </c>
       <c r="D43" t="s">
-        <v>396</v>
+        <v>380</v>
       </c>
       <c r="E43">
         <v>6</v>
@@ -5206,16 +5212,16 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="B44" t="s">
-        <v>397</v>
+        <v>381</v>
       </c>
       <c r="C44" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="D44" t="s">
-        <v>399</v>
+        <v>383</v>
       </c>
       <c r="E44">
         <v>6</v>
@@ -5226,16 +5232,16 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="B45" t="s">
-        <v>400</v>
+        <v>384</v>
       </c>
       <c r="C45" t="s">
-        <v>400</v>
+        <v>384</v>
       </c>
       <c r="D45" t="s">
-        <v>401</v>
+        <v>385</v>
       </c>
       <c r="E45">
         <v>2</v>
@@ -5246,16 +5252,16 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="B46" t="s">
-        <v>402</v>
+        <v>386</v>
       </c>
       <c r="C46" t="s">
-        <v>403</v>
+        <v>387</v>
       </c>
       <c r="D46" t="s">
-        <v>404</v>
+        <v>388</v>
       </c>
       <c r="E46">
         <v>0</v>
@@ -5266,16 +5272,16 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="B47" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="C47" t="s">
-        <v>406</v>
+        <v>390</v>
       </c>
       <c r="D47" t="s">
-        <v>407</v>
+        <v>391</v>
       </c>
       <c r="F47">
         <v>1</v>
@@ -5294,8 +5300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5309,18 +5315,18 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>481</v>
       </c>
       <c r="C1" t="s">
-        <v>92</v>
+        <v>498</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -5328,10 +5334,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>414</v>
+        <v>398</v>
       </c>
       <c r="C3">
         <v>0</v>

</xml_diff>

<commit_message>
Compared all codes to JV and changed when needed.
</commit_message>
<xml_diff>
--- a/data-raw/classcodes.xlsx
+++ b/data-raw/classcodes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erik_\Documents\GitHub\coder\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93169436-405C-4E8E-8555-8A777655621B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A65391-0A99-4130-B081-D2B524FADE84}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="408" yWindow="2664" windowWidth="26700" windowHeight="18684" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32964" yWindow="0" windowWidth="14964" windowHeight="17868" tabRatio="500" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ex_carbrands" sheetId="10" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="500">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="501">
   <si>
     <t>group</t>
   </si>
@@ -582,9 +582,6 @@
   </si>
   <si>
     <t>29(0|41)|3312</t>
-  </si>
-  <si>
-    <t>4(16[89]|90)|50([0-5]|64|8[18])</t>
   </si>
   <si>
     <t>4465|7(1(0[0-4]|4[0-28])|25)</t>
@@ -849,9 +846,6 @@
     <t>M(24[056]F|6(10|21|6[23])F|8((43|6[01])F|66F?|95E))</t>
   </si>
   <si>
-    <t>I((2([14][[:alnum:]]*|6[09]))|4(6[019]|90)|6([0-35-6]|49)|7([24]|7[0-2]))|J8[01]9)|T81</t>
-  </si>
-  <si>
     <t>I80[[:alnum:]]*|J((1[3-8][[:alnum:]]*)|9(5[23589]|6[[:alnum:]]*|81))|K2[5-7][[:alnum:]]*|L89[[:alnum:]]*|N(99[089]|(17[[:alnum:]]*))|R339</t>
   </si>
   <si>
@@ -870,63 +864,30 @@
     <t>(I((2([14][[:alnum:]]*|6[09]))|4(6[019]|90)|6([0-35-6]|49)|7([24]|7[0-2]))|J8[01]9)|T811</t>
   </si>
   <si>
-    <t>N07BB\\d{2}</t>
-  </si>
-  <si>
     <t>N07BB0[34]|V03AA01</t>
   </si>
   <si>
     <t>N07BB0[1345]</t>
   </si>
   <si>
-    <t>R0(1A[CD]([0-5]\\d|60)|(6A([D-X]([01]\\d|2[0-7])|B04)))</t>
-  </si>
-  <si>
-    <t>R0(1A(C\\d{2}|D([0-5]\\d|60))|6A([D-W]\\d{2}|X([01]\\d|2[0-6])))</t>
-  </si>
-  <si>
     <t>R0[16]A[CDEX][0125][1-35-9]</t>
   </si>
   <si>
-    <t>B01A((A(0[3-9]|[1-9]\\d)|B0[0-6])|E07|F0[12]|X05)</t>
-  </si>
-  <si>
-    <t>B01A(A(0[3-9]|[1-9]\\d)|B0[0-6])</t>
-  </si>
-  <si>
     <t>B01A[AB][01][0-69]</t>
   </si>
   <si>
-    <t>B01AC(0[5-9]|[1-2]\\d|30)</t>
-  </si>
-  <si>
-    <t>B01AC(0[4-9]|[12]\\d|30)</t>
-  </si>
-  <si>
     <t>B01AC[0-4679]</t>
   </si>
   <si>
     <t>N05B(A(0[1-9]|1[0-2])|E01)</t>
   </si>
   <si>
-    <t>N05BA(0\\d|1[0-2])</t>
-  </si>
-  <si>
     <t>N05BA[01][1246]</t>
   </si>
   <si>
-    <t>C0(1(AA05|B([A-C]\\d{2}|D0[01]))|7AA07)</t>
-  </si>
-  <si>
-    <t>C01(AA05|B([A-C]\\d{2}|D0[01]))</t>
-  </si>
-  <si>
     <t>C01[AB][A-D]0[13457]</t>
   </si>
   <si>
-    <t>G04C(A\\d{2}|B0[12])</t>
-  </si>
-  <si>
     <t>G04CA0[23]</t>
   </si>
   <si>
@@ -942,81 +903,39 @@
     <t>N0[35]A[EGHNX][01][1-49]</t>
   </si>
   <si>
-    <t>R03([A-D]([A-V]\\d{2}}|X05))</t>
-  </si>
-  <si>
-    <t>R03(A(C(0[2-9]|[1-9]\\d)|[D-X]\\d{2})|[BC][A-X]\\d{2}|D([AB]\\d{2}|C0[0-3]))</t>
-  </si>
-  <si>
     <t>R03[A-D][ABCKLX][01][[:digit:]]</t>
   </si>
   <si>
-    <t>C0(3(DA(0[2-9]|\\d{2})|C([AB]\\d{2}|C01))|7A(B(0[27]|12)|G02)|9C[A-X]\\d{2})</t>
-  </si>
-  <si>
-    <t>C0(3(C([AB]\\d{2}|C0[01]))|9(AA(0\\d|10)|CA0[67]))</t>
-  </si>
-  <si>
     <t>C0[39][ACD][AC][01][0-79]</t>
   </si>
   <si>
-    <t>N06AD(A0[2-4]|X01)</t>
-  </si>
-  <si>
     <t>N06DA0[2-4]</t>
   </si>
   <si>
     <t>N04D[AX]0[1-4]</t>
   </si>
   <si>
-    <t>N06A([A-F]\\d{2}|G0[0-2]|X(0[3-9]|1[0138])|2[1-6])</t>
-  </si>
-  <si>
-    <t>N06A([A-F]\\d{2}|G0[0-2]|X(0\\d|1[0-8]))</t>
-  </si>
-  <si>
     <t>N06A[ABGX][012][0-689]</t>
   </si>
   <si>
     <t>A10[AB][[:alnum:]]{3}</t>
   </si>
   <si>
-    <t xml:space="preserve">A10(A[A-X]\\d{2}|B([A-F]\\d{2}|G0[0-3])) </t>
-  </si>
-  <si>
     <t>A10[AB][A-HX][01][[:digit:]]</t>
   </si>
   <si>
     <t>N03A[[:alnum:]]{3}</t>
   </si>
   <si>
-    <t>N03A([A-W]\\d{2}|X14)</t>
-  </si>
-  <si>
     <t>N03A[ABDEFGX][01][0-59]</t>
   </si>
   <si>
-    <t>A02B([A-W]\\d{2}|X0[0-5])</t>
-  </si>
-  <si>
-    <t>A02B([A-W]\\d{2}|X05)</t>
-  </si>
-  <si>
     <t>A02B[A-DX][015][1-6]</t>
   </si>
   <si>
-    <t>S01E(A\\d{2}|B0[0-3]|C(0[3-9]|[1-9]\\d)|[D-X]\\d{2})</t>
-  </si>
-  <si>
-    <t>S01E(A\\d{2}|B0[0-3]|C(0[3-9]|[[:alnum:]]{1,3}))</t>
-  </si>
-  <si>
     <t>S01E[A-EX][05][1-5]</t>
   </si>
   <si>
-    <t>M04A([AB]\\d{2}|C0[01])</t>
-  </si>
-  <si>
     <t>M04A[A-C]01</t>
   </si>
   <si>
@@ -1029,33 +948,15 @@
     <t>J05A[ABEX][0156][12457]</t>
   </si>
   <si>
-    <t>J05A(E(0[1-9]|10)|F(0[1-79]|1[2-9]|[2-9]\\d)|G0[0-5]|R\\d{2}|X(0[7-9]|12)|)</t>
-  </si>
-  <si>
-    <t>J05A(E(0[0-8])?|F\\d{2}|G0[0-3]|R.*|X07)</t>
-  </si>
-  <si>
     <t>J05A[EFGRX][016][[:digit:]]</t>
   </si>
   <si>
     <t>V03AE01</t>
   </si>
   <si>
-    <t>A10BH03|C10([AB][A-W]\\d{2}|X0\\d)</t>
-  </si>
-  <si>
-    <t>C10(A[A-X]\\d{2}|B[A-W]\\d{2}|X0[0-3])</t>
-  </si>
-  <si>
     <t>C10[AB][ABCX][01][1-579]</t>
   </si>
   <si>
-    <t>C0(2(A(B\\d{2}|C0[0-5])|DB(0[2-9]|[1-9]\\d))|3(A([A-Z]\\d{2}|BA(0\\d|1[01]))|DB(01|99)|C([AB]\\d{2}|C0[01])|EA01)|9(BA0[2-9]|DA0[2-8]|C[A-X]\\d{2}))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C0(2(A(B\\d{2}|C0[0-5])|[D-J][A-X]\\d{2}|K([A-W]\\d{2}|X0[10]))|3([AD][A-X]\\d{2}|BA(0\\d|1[01])|EA0[01])|9(BA0[2-9]|DA0[2-7])) </t>
-  </si>
-  <si>
     <t>C0[239][ABDEKX][ABCX][01][1-9]</t>
   </si>
   <si>
@@ -1065,12 +966,6 @@
     <t>H03B(A02|B01)</t>
   </si>
   <si>
-    <t>G04BD\\d{2}</t>
-  </si>
-  <si>
-    <t>M01A([B-G]\\d{2}|H0[0-6])</t>
-  </si>
-  <si>
     <t>M01A[BCEHX][015][1-6]</t>
   </si>
   <si>
@@ -1080,12 +975,6 @@
     <t>A07E[AC]0[1-46]</t>
   </si>
   <si>
-    <t>C(0(7A(A(0[1-689]|[1-9]\\d)|B0[0-3]|G01)|8(C[A-Z]\\d{2}|DB0[01])|9(BB(0[2-9]|10)|D(B0[1-4]|X0[13])))|10BX03)</t>
-  </si>
-  <si>
-    <t>C0(7(A((A\\d{2}|B0[0-3])|[G-X]\\d{2})|[B-X][A-X]\\d{2})|8([A-C][A-X]\\d{2}|D(A\\d{2}|B0[01])))</t>
-  </si>
-  <si>
     <t>C0[78][ACDF][ABG][01][1-7]</t>
   </si>
   <si>
@@ -1104,9 +993,6 @@
     <t>A06AD11</t>
   </si>
   <si>
-    <t>L01[A-X]{2}\\d{2}</t>
-  </si>
-  <si>
     <t>L01[A-DX][A-EX][0-5][[:digit:]]</t>
   </si>
   <si>
@@ -1119,54 +1005,27 @@
     <t>B05BA[01][03]</t>
   </si>
   <si>
-    <t>N02C[A-X]\\d{2}</t>
-  </si>
-  <si>
     <t>N02C[ACX]0[1-6]</t>
   </si>
   <si>
-    <t>M05B(A\\d{2}|B0[0-3])</t>
-  </si>
-  <si>
     <t>M05B[ABX]0[1-46-8]</t>
   </si>
   <si>
-    <t>N02(A([A-W]\\d{1}|X(0[26]|52))|BE51)</t>
-  </si>
-  <si>
-    <t>N02A[A-X]\\d{2}</t>
-  </si>
-  <si>
     <t>N02A[ABEFGX][05][123569]</t>
   </si>
   <si>
     <t>A09AA02</t>
   </si>
   <si>
-    <t>N04[AB][A-DX]\\d{2}</t>
-  </si>
-  <si>
-    <t>N04([AB][A-X]\\d{2})</t>
-  </si>
-  <si>
     <t>N04[AB][ACDX]0[1-79]</t>
   </si>
   <si>
-    <t>D05(A(A\\d{2}|C([0-4]\\d|5[01])|X[05]2)|BB0[12])</t>
-  </si>
-  <si>
     <t>D05(A(A|X02)|BB0[12])</t>
   </si>
   <si>
     <t>D05[AB][ABX][05][12]</t>
   </si>
   <si>
-    <t>N05A(A\\d{2}|B(0[0-26-9]|[1-9]\\d)|[C-K]\\d{2}|L0[0-7]|X(0[7-9]|1[0-3]))</t>
-  </si>
-  <si>
-    <t>N05A(A\\d{2}|B(0[0-26-9]|[1-9]\\d)|[C-X]\\d{2})</t>
-  </si>
-  <si>
     <t>N05A[ABDEFHNX][01][1-68]</t>
   </si>
   <si>
@@ -1185,27 +1044,15 @@
     <t>N07BA0[1-3]</t>
   </si>
   <si>
-    <t>H02AB(0\\d|10)</t>
-  </si>
-  <si>
     <t>H02AB(0[1246-9]|10)</t>
   </si>
   <si>
     <t>L04A(A(06|1[08])|D0[12])</t>
   </si>
   <si>
-    <t>L04AA([01]\\d|2[01])</t>
-  </si>
-  <si>
     <t>L04AA[012][013468]</t>
   </si>
   <si>
-    <t>J04A(C([0-4]\\d|5[01])|M\\d{2})</t>
-  </si>
-  <si>
-    <t>J04A([B-J]\\d{2}|K0[0-2])</t>
-  </si>
-  <si>
     <t>J04A[A-CKM]0[12456]</t>
   </si>
   <si>
@@ -1215,9 +1062,6 @@
     <t>A07E(A0[1-26]|C0[1-4]|)|L04AA33</t>
   </si>
   <si>
-    <t>G03XC01|H05AA02|M05B(A\\d{2}|B0[0-5]|X0[34])</t>
-  </si>
-  <si>
     <t>A11CC0[1-4]|B03XA0[1-3]|V03AE0[235]</t>
   </si>
   <si>
@@ -1317,9 +1161,6 @@
     <t>29([5-8]|91)</t>
   </si>
   <si>
-    <t>3(0(04|112|9[01])11</t>
-  </si>
-  <si>
     <t>regex_icd9cm_ahrqweb</t>
   </si>
   <si>
@@ -1347,9 +1188,6 @@
     <t>34[2-4]|438[2-5]</t>
   </si>
   <si>
-    <t>3(3([0145]|20|3[45])|4(0|1[1-9]|[47]))|78([04]3)</t>
-  </si>
-  <si>
     <t>49|50([0-5]|6[0-4])</t>
   </si>
   <si>
@@ -1380,18 +1218,12 @@
     <t>28(0[1-9]|1|5[29])</t>
   </si>
   <si>
-    <t>291[1-3589]|30(3|50)</t>
-  </si>
-  <si>
     <t>292(0|8[2-9]|9)|30(4|5[2-9])|6483</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>39891|4(0(2[019]1|4[019][13]|5[4-9])|28)</t>
-  </si>
-  <si>
     <t xml:space="preserve">42(6(1[013]|[2-46-8][0-9]|5[0-3])|7([029][0-9]|31|60))|7850|V(450|533) </t>
   </si>
   <si>
@@ -1425,21 +1257,12 @@
     <t>24(09|[34]|6[18])</t>
   </si>
   <si>
-    <t>40(3([019]1)|4[019][23]))|58[56]|V(4(20|51)|56)</t>
-  </si>
-  <si>
-    <t>40(3([019]1)|4[019][23]))|58([56]|80)|V(4(20|51)|56)</t>
-  </si>
-  <si>
     <t>070([23]{2}|[45]4|[69])|456([0-2])|57([01]|2([2-9]|[3-8])|3[3489])|V427</t>
   </si>
   <si>
     <t>53[1-4][79]</t>
   </si>
   <si>
-    <t>2(0([0-2]30)|386)</t>
-  </si>
-  <si>
     <t>1([4-68]|7[0-24-9]|9[0-5])</t>
   </si>
   <si>
@@ -1531,6 +1354,186 @@
   </si>
   <si>
     <t>3(0(04|112|9[01])|11)</t>
+  </si>
+  <si>
+    <t>R0(1A(C[[:digit:]]{2}|D([0-5][[:digit:]]|60))|6A([D-W][[:digit:]]{2}|X([01][[:digit:]]|2[0-6])))</t>
+  </si>
+  <si>
+    <t>B01A((A(0[3-9]|[1-9][[:digit:]])|B0[0-6])|E07|F0[12]|X05)</t>
+  </si>
+  <si>
+    <t>B01A(A(0[3-9]|[1-9][[:digit:]])|B0[0-6])</t>
+  </si>
+  <si>
+    <t>B01AC(0[4-9]|[12][[:digit:]]|30)</t>
+  </si>
+  <si>
+    <t>N05BA(0[[:digit:]]|1[0-2])</t>
+  </si>
+  <si>
+    <t>C0(1(AA05|B([A-C][[:digit:]]{2}|D0[01]))|7AA07)</t>
+  </si>
+  <si>
+    <t>C01(AA05|B([A-C][[:digit:]]{2}|D0[01]))</t>
+  </si>
+  <si>
+    <t>G04C(A[[:digit:]]{2}|B0[12])</t>
+  </si>
+  <si>
+    <t>R03(A(C(0[2-9]|[1-9][[:digit:]])|[D-X][[:digit:]]{2})|[BC][A-X][[:digit:]]{2}|D([AB][[:digit:]]{2}|C0[0-3]))</t>
+  </si>
+  <si>
+    <t>C0(3(C([AB][[:digit:]]{2}|C0[01]))|9(AA(0[[:digit:]]|10)|CA0[67]))</t>
+  </si>
+  <si>
+    <t>N06A([A-F][[:digit:]]{2}|G0[0-2]|X(0[[:digit:]]|1[0-8]))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A10(A[A-X][[:digit:]]{2}|B([A-F][[:digit:]]{2}|G0[0-3])) </t>
+  </si>
+  <si>
+    <t>N03A([A-W][[:digit:]]{2}|X14)</t>
+  </si>
+  <si>
+    <t>A02B([A-W][[:digit:]]{2}|X0[0-5])</t>
+  </si>
+  <si>
+    <t>A02B([A-W][[:digit:]]{2}|X05)</t>
+  </si>
+  <si>
+    <t>S01E(A[[:digit:]]{2}|B0[0-3]|C(0[3-9]|[1-9][[:digit:]])|[D-X][[:digit:]]{2})</t>
+  </si>
+  <si>
+    <t>S01E(A[[:digit:]]{2}|B0[0-3]|C(0[3-9]|[[:alnum:]]{1,3}))</t>
+  </si>
+  <si>
+    <t>M04A([AB][[:digit:]]{2}|C0[01])</t>
+  </si>
+  <si>
+    <t>J05A(E(0[1-9]|10)|F(0[1-79]|1[2-9]|[2-9][[:digit:]])|G0[0-5]|R[[:digit:]]{2}|X(0[7-9]|12)|)</t>
+  </si>
+  <si>
+    <t>J05A(E(0[0-8])?|F[[:digit:]]{2}|G0[0-3]|R.*|X07)</t>
+  </si>
+  <si>
+    <t>C10(A[A-X][[:digit:]]{2}|B[A-W][[:digit:]]{2}|X0[0-3])</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C0(2(A(B[[:digit:]]{2}|C0[0-5])|[D-J][A-X][[:digit:]]{2}|K([A-W][[:digit:]]{2}|X0[10]))|3([AD][A-X][[:digit:]]{2}|BA(0[[:digit:]]|1[01])|EA0[01])|9(BA0[2-9]|DA0[2-7])) </t>
+  </si>
+  <si>
+    <t>G04BD[[:digit:]]{2}</t>
+  </si>
+  <si>
+    <t>M01A([B-G][[:digit:]]{2}|H0[0-6])</t>
+  </si>
+  <si>
+    <t>C0(7(A((A[[:digit:]]{2}|B0[0-3])|[G-X][[:digit:]]{2})|[B-X][A-X][[:digit:]]{2})|8([A-C][A-X][[:digit:]]{2}|D(A[[:digit:]]{2}|B0[01])))</t>
+  </si>
+  <si>
+    <t>L01[A-X]{2}[[:digit:]]{2}</t>
+  </si>
+  <si>
+    <t>N02C[A-X][[:digit:]]{2}</t>
+  </si>
+  <si>
+    <t>G03XC01|H05AA02|M05B(A[[:digit:]]{2}|B0[0-5]|X0[34])</t>
+  </si>
+  <si>
+    <t>M05B(A[[:digit:]]{2}|B0[0-3])</t>
+  </si>
+  <si>
+    <t>N02A[A-X][[:digit:]]{2}</t>
+  </si>
+  <si>
+    <t>N04[AB][A-DX][[:digit:]]{2}</t>
+  </si>
+  <si>
+    <t>N04([AB][A-X][[:digit:]]{2})</t>
+  </si>
+  <si>
+    <t>D05(A(A[[:digit:]]{2}|C([0-4][[:digit:]]|5[01])|X[05]2)|BB0[12])</t>
+  </si>
+  <si>
+    <t>N05A(A[[:digit:]]{2}|B(0[0-26-9]|[1-9][[:digit:]])|[C-K][[:digit:]]{2}|L0[0-7]|X(0[7-9]|1[0-3]))</t>
+  </si>
+  <si>
+    <t>N05A(A[[:digit:]]{2}|B(0[0-26-9]|[1-9][[:digit:]])|[C-X][[:digit:]]{2})</t>
+  </si>
+  <si>
+    <t>H02AB(0[[:digit:]]|10)</t>
+  </si>
+  <si>
+    <t>L04AA([01][[:digit:]]|2[01])</t>
+  </si>
+  <si>
+    <t>J04A(C([0-4][[:digit:]]|5[01])|M[[:digit:]]{2})</t>
+  </si>
+  <si>
+    <t>J04A([B-J][[:digit:]]{2}|K0[0-2])</t>
+  </si>
+  <si>
+    <t>N07BB[[:digit:]]{2}</t>
+  </si>
+  <si>
+    <t>4(16[89]|9)|50([0-5]|64|8[18])</t>
+  </si>
+  <si>
+    <t>M(0[569]|120|3(15|[2-6]))</t>
+  </si>
+  <si>
+    <t>3(3([0145]|20|3[45])|4(1[1-9]|[057]))|78([04]3)</t>
+  </si>
+  <si>
+    <t>(I2[67])|J(4[0-7]|6([0-7]|84)|70[13])</t>
+  </si>
+  <si>
+    <t>39891|4(0(2[019]1|4[019][13]|5[4-9])|2(5[4-9]|8))</t>
+  </si>
+  <si>
+    <t>2(0([0-2]|30)|386)</t>
+  </si>
+  <si>
+    <t>291[0-3589]|30(3|50)</t>
+  </si>
+  <si>
+    <t>40(3([019]1)|4[019][23])|58[56]|V(4(20|51)|56)</t>
+  </si>
+  <si>
+    <t>40(3([019]1)|4[019][23])|58([56]|80)|V(4(20|51)|56)</t>
+  </si>
+  <si>
+    <t>I((2([14]|6[09]))|4(6[019]|90)|6([0-35-6]|49)|7([24]|7[0-2])|8(19|2)|97[89])|J8[01]9|T811</t>
+  </si>
+  <si>
+    <t>R0(1A(C[0-9]{2}|D([0-5][0-9]|60))|(6A(([D-V][0-9]{2}|X([01][0-9]|2[0-7]))|B04)))</t>
+  </si>
+  <si>
+    <t>B01AC(0[4-9]|[1-2][0-9]|30)</t>
+  </si>
+  <si>
+    <t>R03([A-D][A-V][0-9]{2}|DX05)</t>
+  </si>
+  <si>
+    <t>C0(3(DA[0-9]{2}|C([AB][0-9]{2}|C01))|7A(B(0[27]|12)|G02)|9([AC][A-Z][0-X]{2}))</t>
+  </si>
+  <si>
+    <t>N06D(A0[2-4]|X01)</t>
+  </si>
+  <si>
+    <t>N06A([A-F][0-9]{2}|G0[0-2]|X(0[3-9]|1[013-8]|2[1-6]))</t>
+  </si>
+  <si>
+    <t>A10BH03|C10([AB][A-Z][0-9]{2}|X0[0-9])</t>
+  </si>
+  <si>
+    <t>C0(2(A(B[0-9]{2}|C0[0-5])|DB(0[2-9]|[1-9][0-9]))|3((A[A-Z][0-9]{2}|BA(0[0-9]|1[01]))|DB(01|99)|C([AB][0-9]{2}|C0[01])|EA01)|9(BA0[2-9]|DA0[2-8]|C[A-X][0-9]{2}))</t>
+  </si>
+  <si>
+    <t>C(0(7A(A(0[1-689]|[1-9][0-9])|B0[0-3]|G01)|8(C[A-Z][0-9]{2}|D(A[0-9]{2}|B0[01]))|9(BB(0[2-9]|10)|D(B0[1-4]|X0[13])))|10BX03)</t>
+  </si>
+  <si>
+    <t>N02(A([A-W][0-9]{1}|X(0[0-26]|52))|BE51)</t>
   </si>
 </sst>
 </file>
@@ -1928,7 +1931,7 @@
         <v>82</v>
       </c>
       <c r="B5" t="s">
-        <v>479</v>
+        <v>420</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -1952,7 +1955,7 @@
         <v>85</v>
       </c>
       <c r="B8" t="s">
-        <v>480</v>
+        <v>421</v>
       </c>
     </row>
   </sheetData>
@@ -1965,7 +1968,8 @@
   <dimension ref="A1:AMO18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1995,7 +1999,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>481</v>
+        <v>422</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>163</v>
@@ -2013,22 +2017,22 @@
         <v>150</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>482</v>
+        <v>423</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>483</v>
+        <v>424</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>484</v>
+        <v>425</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>485</v>
+        <v>426</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>486</v>
+        <v>427</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>487</v>
+        <v>428</v>
       </c>
       <c r="AMO1"/>
     </row>
@@ -2040,7 +2044,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>137</v>
@@ -2049,7 +2053,7 @@
         <v>137</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>152</v>
@@ -2084,7 +2088,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D3" s="6">
         <v>428</v>
@@ -2093,7 +2097,7 @@
         <v>180</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>153</v>
@@ -2128,7 +2132,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>165</v>
@@ -2137,7 +2141,7 @@
         <v>181</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>154</v>
@@ -2172,7 +2176,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>155</v>
@@ -2181,7 +2185,7 @@
         <v>182</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>155</v>
@@ -2216,7 +2220,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D6" s="6">
         <v>290</v>
@@ -2225,7 +2229,7 @@
         <v>183</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>156</v>
@@ -2260,16 +2264,16 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>166</v>
       </c>
       <c r="E7" t="s">
-        <v>184</v>
+        <v>481</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>211</v>
+        <v>484</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>157</v>
@@ -2304,16 +2308,16 @@
         <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>167</v>
       </c>
       <c r="E8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>196</v>
+        <v>482</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>158</v>
@@ -2348,7 +2352,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>168</v>
@@ -2383,13 +2387,13 @@
         <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>169</v>
       </c>
       <c r="E10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I10">
         <v>1</v>
@@ -2418,13 +2422,13 @@
         <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>170</v>
       </c>
       <c r="E11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I11">
         <v>1</v>
@@ -2453,16 +2457,16 @@
         <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>172</v>
       </c>
       <c r="E12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G12" s="6">
         <v>344</v>
@@ -2497,16 +2501,16 @@
         <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>173</v>
       </c>
       <c r="E13" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G13" s="6" t="s">
         <v>160</v>
@@ -2541,16 +2545,16 @@
         <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>171</v>
       </c>
       <c r="E14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G14" s="6">
         <v>250</v>
@@ -2585,16 +2589,16 @@
         <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>174</v>
       </c>
       <c r="E15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G15" s="6" t="s">
         <v>161</v>
@@ -2629,16 +2633,16 @@
         <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>175</v>
       </c>
       <c r="E16" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G16" s="7" t="s">
         <v>159</v>
@@ -2673,7 +2677,7 @@
         <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>176</v>
@@ -2682,7 +2686,7 @@
         <v>148</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G17" s="6" t="s">
         <v>148</v>
@@ -2717,7 +2721,7 @@
         <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>177</v>
@@ -2726,7 +2730,7 @@
         <v>177</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H18" s="6" t="s">
         <v>149</v>
@@ -2760,8 +2764,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2778,40 +2783,40 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>481</v>
+        <v>422</v>
       </c>
       <c r="C1" t="s">
-        <v>488</v>
+        <v>429</v>
       </c>
       <c r="D1" t="s">
-        <v>405</v>
+        <v>353</v>
       </c>
       <c r="E1" t="s">
-        <v>429</v>
+        <v>376</v>
       </c>
       <c r="F1" t="s">
         <v>164</v>
       </c>
       <c r="G1" t="s">
-        <v>489</v>
+        <v>430</v>
       </c>
       <c r="H1" t="s">
-        <v>490</v>
+        <v>431</v>
       </c>
       <c r="I1" t="s">
-        <v>491</v>
+        <v>432</v>
       </c>
       <c r="J1" t="s">
-        <v>492</v>
+        <v>433</v>
       </c>
       <c r="K1" t="s">
-        <v>493</v>
+        <v>434</v>
       </c>
       <c r="L1" t="s">
-        <v>494</v>
+        <v>435</v>
       </c>
       <c r="M1" t="s">
-        <v>495</v>
+        <v>436</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -2819,19 +2824,19 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D2" t="s">
-        <v>408</v>
+        <v>356</v>
       </c>
       <c r="E2" t="s">
-        <v>430</v>
+        <v>377</v>
       </c>
       <c r="F2" t="s">
-        <v>452</v>
+        <v>485</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -2860,16 +2865,16 @@
         <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D3" t="s">
-        <v>453</v>
+        <v>397</v>
       </c>
       <c r="F3" t="s">
-        <v>454</v>
+        <v>398</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -2898,19 +2903,19 @@
         <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D4" t="s">
-        <v>431</v>
+        <v>378</v>
       </c>
       <c r="E4" t="s">
-        <v>432</v>
+        <v>379</v>
       </c>
       <c r="F4" t="s">
-        <v>455</v>
+        <v>399</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -2939,19 +2944,19 @@
         <v>36</v>
       </c>
       <c r="B5" t="s">
+        <v>219</v>
+      </c>
+      <c r="C5" t="s">
         <v>220</v>
       </c>
-      <c r="C5" t="s">
-        <v>221</v>
-      </c>
       <c r="D5" t="s">
-        <v>409</v>
+        <v>357</v>
       </c>
       <c r="E5" t="s">
-        <v>409</v>
+        <v>357</v>
       </c>
       <c r="F5" t="s">
-        <v>456</v>
+        <v>400</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -2980,19 +2985,19 @@
         <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D6" t="s">
-        <v>433</v>
+        <v>380</v>
       </c>
       <c r="E6" t="s">
-        <v>434</v>
+        <v>381</v>
       </c>
       <c r="F6" t="s">
-        <v>457</v>
+        <v>401</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -3021,16 +3026,16 @@
         <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D7" t="s">
-        <v>406</v>
+        <v>354</v>
       </c>
       <c r="E7" t="s">
-        <v>435</v>
+        <v>382</v>
       </c>
       <c r="F7">
         <v>401</v>
@@ -3062,19 +3067,19 @@
         <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D8" t="s">
-        <v>407</v>
+        <v>355</v>
       </c>
       <c r="E8" t="s">
-        <v>436</v>
+        <v>383</v>
       </c>
       <c r="F8" t="s">
-        <v>458</v>
+        <v>402</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -3103,19 +3108,19 @@
         <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D9" t="s">
-        <v>410</v>
+        <v>358</v>
       </c>
       <c r="E9" t="s">
-        <v>437</v>
+        <v>384</v>
       </c>
       <c r="F9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -3144,19 +3149,19 @@
         <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C10" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D10" t="s">
-        <v>411</v>
+        <v>359</v>
       </c>
       <c r="E10" t="s">
-        <v>438</v>
+        <v>483</v>
       </c>
       <c r="F10" t="s">
-        <v>459</v>
+        <v>403</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -3185,19 +3190,19 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C11" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D11" t="s">
-        <v>412</v>
+        <v>360</v>
       </c>
       <c r="E11" t="s">
-        <v>439</v>
+        <v>385</v>
       </c>
       <c r="F11" t="s">
-        <v>460</v>
+        <v>404</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -3226,19 +3231,19 @@
         <v>44</v>
       </c>
       <c r="B12" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C12" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D12" t="s">
-        <v>413</v>
+        <v>361</v>
       </c>
       <c r="E12" t="s">
-        <v>440</v>
+        <v>386</v>
       </c>
       <c r="F12" t="s">
-        <v>413</v>
+        <v>361</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -3267,19 +3272,19 @@
         <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C13" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D13" t="s">
-        <v>414</v>
+        <v>362</v>
       </c>
       <c r="E13" t="s">
-        <v>462</v>
+        <v>406</v>
       </c>
       <c r="F13" t="s">
-        <v>461</v>
+        <v>405</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -3308,19 +3313,19 @@
         <v>46</v>
       </c>
       <c r="B14" t="s">
+        <v>226</v>
+      </c>
+      <c r="C14" t="s">
         <v>227</v>
       </c>
-      <c r="C14" t="s">
-        <v>228</v>
-      </c>
       <c r="D14" t="s">
-        <v>415</v>
+        <v>363</v>
       </c>
       <c r="E14" t="s">
-        <v>441</v>
+        <v>387</v>
       </c>
       <c r="F14" t="s">
-        <v>463</v>
+        <v>407</v>
       </c>
       <c r="G14">
         <v>1</v>
@@ -3349,19 +3354,19 @@
         <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C15" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D15" t="s">
-        <v>416</v>
+        <v>364</v>
       </c>
       <c r="E15" t="s">
-        <v>464</v>
+        <v>488</v>
       </c>
       <c r="F15" t="s">
-        <v>465</v>
+        <v>489</v>
       </c>
       <c r="G15">
         <v>1</v>
@@ -3390,19 +3395,19 @@
         <v>48</v>
       </c>
       <c r="B16" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C16" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D16" t="s">
-        <v>417</v>
+        <v>365</v>
       </c>
       <c r="E16" t="s">
-        <v>442</v>
+        <v>388</v>
       </c>
       <c r="F16" t="s">
-        <v>466</v>
+        <v>408</v>
       </c>
       <c r="G16">
         <v>1</v>
@@ -3431,19 +3436,19 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C17" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D17" t="s">
-        <v>418</v>
+        <v>366</v>
       </c>
       <c r="E17" t="s">
-        <v>443</v>
+        <v>389</v>
       </c>
       <c r="F17" t="s">
-        <v>467</v>
+        <v>409</v>
       </c>
       <c r="G17">
         <v>1</v>
@@ -3472,10 +3477,10 @@
         <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C18" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D18" t="s">
         <v>177</v>
@@ -3513,19 +3518,19 @@
         <v>49</v>
       </c>
       <c r="B19" t="s">
+        <v>230</v>
+      </c>
+      <c r="C19" t="s">
         <v>231</v>
       </c>
-      <c r="C19" t="s">
-        <v>232</v>
-      </c>
       <c r="D19" t="s">
-        <v>419</v>
+        <v>367</v>
       </c>
       <c r="E19" t="s">
-        <v>444</v>
+        <v>390</v>
       </c>
       <c r="F19" t="s">
-        <v>468</v>
+        <v>486</v>
       </c>
       <c r="G19">
         <v>1</v>
@@ -3554,10 +3559,10 @@
         <v>50</v>
       </c>
       <c r="B20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D20" t="s">
         <v>148</v>
@@ -3595,19 +3600,19 @@
         <v>51</v>
       </c>
       <c r="B21" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C21" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D21" t="s">
-        <v>420</v>
+        <v>368</v>
       </c>
       <c r="E21" t="s">
-        <v>445</v>
+        <v>391</v>
       </c>
       <c r="F21" t="s">
-        <v>469</v>
+        <v>410</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -3636,19 +3641,19 @@
         <v>52</v>
       </c>
       <c r="B22" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C22" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D22" t="s">
-        <v>421</v>
+        <v>369</v>
       </c>
       <c r="E22" t="s">
-        <v>421</v>
+        <v>369</v>
       </c>
       <c r="F22" t="s">
-        <v>470</v>
+        <v>411</v>
       </c>
       <c r="G22">
         <v>1</v>
@@ -3677,19 +3682,19 @@
         <v>53</v>
       </c>
       <c r="B23" t="s">
+        <v>233</v>
+      </c>
+      <c r="C23" t="s">
         <v>234</v>
       </c>
-      <c r="C23" t="s">
-        <v>235</v>
-      </c>
       <c r="D23" t="s">
-        <v>422</v>
+        <v>370</v>
       </c>
       <c r="E23" t="s">
-        <v>422</v>
+        <v>370</v>
       </c>
       <c r="F23" t="s">
-        <v>422</v>
+        <v>370</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -3718,10 +3723,10 @@
         <v>54</v>
       </c>
       <c r="B24" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C24" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D24">
         <v>2780</v>
@@ -3759,19 +3764,19 @@
         <v>55</v>
       </c>
       <c r="B25" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C25" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D25" t="s">
-        <v>423</v>
+        <v>371</v>
       </c>
       <c r="E25" t="s">
-        <v>446</v>
+        <v>392</v>
       </c>
       <c r="F25" t="s">
-        <v>471</v>
+        <v>412</v>
       </c>
       <c r="G25">
         <v>1</v>
@@ -3800,10 +3805,10 @@
         <v>56</v>
       </c>
       <c r="B26" t="s">
+        <v>236</v>
+      </c>
+      <c r="C26" t="s">
         <v>237</v>
-      </c>
-      <c r="C26" t="s">
-        <v>238</v>
       </c>
       <c r="D26">
         <v>276</v>
@@ -3812,7 +3817,7 @@
         <v>276</v>
       </c>
       <c r="F26" t="s">
-        <v>472</v>
+        <v>413</v>
       </c>
       <c r="G26">
         <v>1</v>
@@ -3841,16 +3846,16 @@
         <v>57</v>
       </c>
       <c r="B27" t="s">
+        <v>238</v>
+      </c>
+      <c r="C27" t="s">
         <v>239</v>
-      </c>
-      <c r="C27" t="s">
-        <v>240</v>
       </c>
       <c r="D27">
         <v>2800</v>
       </c>
       <c r="E27" t="s">
-        <v>447</v>
+        <v>393</v>
       </c>
       <c r="F27">
         <v>2800</v>
@@ -3882,19 +3887,19 @@
         <v>58</v>
       </c>
       <c r="B28" t="s">
+        <v>240</v>
+      </c>
+      <c r="C28" t="s">
         <v>241</v>
       </c>
-      <c r="C28" t="s">
-        <v>242</v>
-      </c>
       <c r="D28" t="s">
-        <v>424</v>
+        <v>372</v>
       </c>
       <c r="E28" t="s">
-        <v>448</v>
+        <v>394</v>
       </c>
       <c r="F28" t="s">
-        <v>473</v>
+        <v>414</v>
       </c>
       <c r="G28">
         <v>1</v>
@@ -3923,19 +3928,19 @@
         <v>59</v>
       </c>
       <c r="B29" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C29" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D29" t="s">
-        <v>425</v>
+        <v>373</v>
       </c>
       <c r="E29" t="s">
-        <v>449</v>
+        <v>487</v>
       </c>
       <c r="F29" t="s">
-        <v>474</v>
+        <v>415</v>
       </c>
       <c r="G29">
         <v>1</v>
@@ -3964,19 +3969,19 @@
         <v>60</v>
       </c>
       <c r="B30" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C30" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D30" t="s">
-        <v>426</v>
+        <v>374</v>
       </c>
       <c r="E30" t="s">
-        <v>450</v>
+        <v>395</v>
       </c>
       <c r="F30" t="s">
-        <v>475</v>
+        <v>416</v>
       </c>
       <c r="G30">
         <v>1</v>
@@ -4005,19 +4010,19 @@
         <v>61</v>
       </c>
       <c r="B31" t="s">
+        <v>242</v>
+      </c>
+      <c r="C31" t="s">
         <v>243</v>
       </c>
-      <c r="C31" t="s">
-        <v>244</v>
-      </c>
       <c r="D31" t="s">
-        <v>427</v>
+        <v>375</v>
       </c>
       <c r="E31" t="s">
-        <v>427</v>
+        <v>375</v>
       </c>
       <c r="F31" t="s">
-        <v>476</v>
+        <v>417</v>
       </c>
       <c r="G31">
         <v>1</v>
@@ -4046,22 +4051,22 @@
         <v>62</v>
       </c>
       <c r="B32" t="s">
+        <v>244</v>
+      </c>
+      <c r="C32" t="s">
         <v>245</v>
       </c>
-      <c r="C32" t="s">
-        <v>246</v>
-      </c>
       <c r="D32" t="s">
-        <v>499</v>
+        <v>440</v>
       </c>
       <c r="E32" t="s">
-        <v>428</v>
+        <v>440</v>
       </c>
       <c r="F32" t="s">
-        <v>477</v>
+        <v>418</v>
       </c>
       <c r="G32" t="s">
-        <v>451</v>
+        <v>396</v>
       </c>
       <c r="H32">
         <v>1</v>
@@ -4093,7 +4098,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4109,7 +4114,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>481</v>
+        <v>422</v>
       </c>
       <c r="C1" t="s">
         <v>179</v>
@@ -4123,7 +4128,7 @@
         <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>70</v>
@@ -4134,7 +4139,7 @@
         <v>65</v>
       </c>
       <c r="B3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>70</v>
@@ -4145,7 +4150,7 @@
         <v>66</v>
       </c>
       <c r="B4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>71</v>
@@ -4156,7 +4161,7 @@
         <v>67</v>
       </c>
       <c r="B5" t="s">
-        <v>272</v>
+        <v>490</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>70</v>
@@ -4167,7 +4172,7 @@
         <v>68</v>
       </c>
       <c r="B6" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>70</v>
@@ -4178,7 +4183,7 @@
         <v>69</v>
       </c>
       <c r="B7" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>71</v>
@@ -4189,7 +4194,7 @@
         <v>178</v>
       </c>
       <c r="C8" t="s">
-        <v>478</v>
+        <v>419</v>
       </c>
       <c r="D8" t="s">
         <v>72</v>
@@ -4221,7 +4226,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>481</v>
+        <v>422</v>
       </c>
       <c r="C1" t="s">
         <v>179</v>
@@ -4229,24 +4234,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>399</v>
+        <v>347</v>
       </c>
       <c r="B2" t="s">
-        <v>400</v>
+        <v>348</v>
       </c>
       <c r="C2" t="s">
-        <v>401</v>
+        <v>349</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>402</v>
+        <v>350</v>
       </c>
       <c r="B3" t="s">
-        <v>403</v>
+        <v>351</v>
       </c>
       <c r="C3" t="s">
-        <v>404</v>
+        <v>352</v>
       </c>
     </row>
   </sheetData>
@@ -4275,7 +4280,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>481</v>
+        <v>422</v>
       </c>
       <c r="C1" t="s">
         <v>179</v>
@@ -4289,7 +4294,7 @@
         <v>64</v>
       </c>
       <c r="B2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>70</v>
@@ -4300,7 +4305,7 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>70</v>
@@ -4311,7 +4316,7 @@
         <v>75</v>
       </c>
       <c r="B4" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>71</v>
@@ -4322,7 +4327,7 @@
         <v>67</v>
       </c>
       <c r="B5" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>70</v>
@@ -4333,7 +4338,7 @@
         <v>68</v>
       </c>
       <c r="B6" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>70</v>
@@ -4344,7 +4349,7 @@
         <v>69</v>
       </c>
       <c r="B7" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>71</v>
@@ -4370,8 +4375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4388,7 +4393,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>496</v>
+        <v>437</v>
       </c>
       <c r="C1" t="s">
         <v>134</v>
@@ -4397,10 +4402,10 @@
         <v>90</v>
       </c>
       <c r="E1" t="s">
-        <v>497</v>
+        <v>438</v>
       </c>
       <c r="F1" t="s">
-        <v>489</v>
+        <v>430</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -4408,13 +4413,13 @@
         <v>91</v>
       </c>
       <c r="B2" t="s">
-        <v>279</v>
+        <v>480</v>
       </c>
       <c r="C2" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D2" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="E2">
         <v>6</v>
@@ -4428,13 +4433,13 @@
         <v>92</v>
       </c>
       <c r="B3" t="s">
-        <v>282</v>
+        <v>491</v>
       </c>
       <c r="C3" t="s">
-        <v>283</v>
+        <v>441</v>
       </c>
       <c r="D3" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="E3">
         <v>-1</v>
@@ -4448,13 +4453,13 @@
         <v>93</v>
       </c>
       <c r="B4" t="s">
-        <v>285</v>
+        <v>442</v>
       </c>
       <c r="C4" t="s">
-        <v>286</v>
+        <v>443</v>
       </c>
       <c r="D4" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -4468,13 +4473,13 @@
         <v>94</v>
       </c>
       <c r="B5" t="s">
-        <v>288</v>
+        <v>492</v>
       </c>
       <c r="C5" t="s">
-        <v>289</v>
+        <v>444</v>
       </c>
       <c r="D5" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -4488,13 +4493,13 @@
         <v>95</v>
       </c>
       <c r="B6" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="C6" t="s">
-        <v>292</v>
+        <v>445</v>
       </c>
       <c r="D6" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -4508,13 +4513,13 @@
         <v>96</v>
       </c>
       <c r="B7" t="s">
-        <v>294</v>
+        <v>446</v>
       </c>
       <c r="C7" t="s">
-        <v>295</v>
+        <v>447</v>
       </c>
       <c r="D7" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -4528,13 +4533,13 @@
         <v>97</v>
       </c>
       <c r="B8" t="s">
-        <v>297</v>
+        <v>448</v>
       </c>
       <c r="C8" t="s">
-        <v>298</v>
+        <v>285</v>
       </c>
       <c r="D8" t="s">
-        <v>299</v>
+        <v>286</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -4548,13 +4553,13 @@
         <v>98</v>
       </c>
       <c r="B9" t="s">
-        <v>300</v>
+        <v>287</v>
       </c>
       <c r="C9" t="s">
-        <v>301</v>
+        <v>288</v>
       </c>
       <c r="D9" t="s">
-        <v>302</v>
+        <v>289</v>
       </c>
       <c r="E9">
         <v>-1</v>
@@ -4568,13 +4573,13 @@
         <v>99</v>
       </c>
       <c r="B10" t="s">
-        <v>303</v>
+        <v>493</v>
       </c>
       <c r="C10" t="s">
-        <v>304</v>
+        <v>449</v>
       </c>
       <c r="D10" t="s">
-        <v>305</v>
+        <v>290</v>
       </c>
       <c r="E10">
         <v>2</v>
@@ -4588,13 +4593,13 @@
         <v>100</v>
       </c>
       <c r="B11" t="s">
-        <v>306</v>
+        <v>494</v>
       </c>
       <c r="C11" t="s">
-        <v>307</v>
+        <v>450</v>
       </c>
       <c r="D11" t="s">
-        <v>308</v>
+        <v>291</v>
       </c>
       <c r="E11">
         <v>2</v>
@@ -4608,13 +4613,13 @@
         <v>101</v>
       </c>
       <c r="B12" t="s">
-        <v>309</v>
+        <v>495</v>
       </c>
       <c r="C12" t="s">
-        <v>310</v>
+        <v>292</v>
       </c>
       <c r="D12" t="s">
-        <v>311</v>
+        <v>293</v>
       </c>
       <c r="E12">
         <v>2</v>
@@ -4628,13 +4633,13 @@
         <v>102</v>
       </c>
       <c r="B13" t="s">
-        <v>312</v>
+        <v>496</v>
       </c>
       <c r="C13" t="s">
-        <v>313</v>
+        <v>451</v>
       </c>
       <c r="D13" t="s">
-        <v>314</v>
+        <v>294</v>
       </c>
       <c r="E13">
         <v>2</v>
@@ -4648,13 +4653,13 @@
         <v>103</v>
       </c>
       <c r="B14" t="s">
-        <v>315</v>
+        <v>295</v>
       </c>
       <c r="C14" t="s">
-        <v>316</v>
+        <v>452</v>
       </c>
       <c r="D14" t="s">
-        <v>317</v>
+        <v>296</v>
       </c>
       <c r="E14">
         <v>2</v>
@@ -4668,13 +4673,13 @@
         <v>105</v>
       </c>
       <c r="B15" t="s">
-        <v>318</v>
+        <v>297</v>
       </c>
       <c r="C15" t="s">
-        <v>319</v>
+        <v>453</v>
       </c>
       <c r="D15" t="s">
-        <v>320</v>
+        <v>298</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -4688,13 +4693,13 @@
         <v>106</v>
       </c>
       <c r="B16" t="s">
-        <v>321</v>
+        <v>454</v>
       </c>
       <c r="C16" t="s">
-        <v>322</v>
+        <v>455</v>
       </c>
       <c r="D16" t="s">
-        <v>323</v>
+        <v>299</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -4708,13 +4713,13 @@
         <v>107</v>
       </c>
       <c r="B17" t="s">
-        <v>324</v>
+        <v>456</v>
       </c>
       <c r="C17" t="s">
-        <v>325</v>
+        <v>457</v>
       </c>
       <c r="D17" t="s">
-        <v>326</v>
+        <v>300</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -4728,13 +4733,13 @@
         <v>108</v>
       </c>
       <c r="B18" t="s">
-        <v>327</v>
+        <v>458</v>
       </c>
       <c r="C18" t="s">
-        <v>327</v>
+        <v>458</v>
       </c>
       <c r="D18" t="s">
-        <v>328</v>
+        <v>301</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -4748,7 +4753,7 @@
         <v>132</v>
       </c>
       <c r="B19" t="s">
-        <v>329</v>
+        <v>302</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -4759,13 +4764,13 @@
         <v>109</v>
       </c>
       <c r="B20" t="s">
-        <v>392</v>
+        <v>341</v>
       </c>
       <c r="C20" t="s">
-        <v>330</v>
+        <v>303</v>
       </c>
       <c r="D20" t="s">
-        <v>331</v>
+        <v>304</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -4776,13 +4781,13 @@
         <v>76</v>
       </c>
       <c r="B21" t="s">
-        <v>332</v>
+        <v>459</v>
       </c>
       <c r="C21" t="s">
-        <v>333</v>
+        <v>460</v>
       </c>
       <c r="D21" t="s">
-        <v>334</v>
+        <v>305</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -4796,13 +4801,13 @@
         <v>110</v>
       </c>
       <c r="B22" t="s">
-        <v>335</v>
+        <v>306</v>
       </c>
       <c r="C22" t="s">
-        <v>335</v>
+        <v>306</v>
       </c>
       <c r="D22" t="s">
-        <v>335</v>
+        <v>306</v>
       </c>
       <c r="E22">
         <v>4</v>
@@ -4816,13 +4821,13 @@
         <v>111</v>
       </c>
       <c r="B23" t="s">
-        <v>336</v>
+        <v>497</v>
       </c>
       <c r="C23" t="s">
-        <v>337</v>
+        <v>461</v>
       </c>
       <c r="D23" t="s">
-        <v>338</v>
+        <v>307</v>
       </c>
       <c r="E23">
         <v>-1</v>
@@ -4836,13 +4841,13 @@
         <v>112</v>
       </c>
       <c r="B24" t="s">
-        <v>339</v>
+        <v>498</v>
       </c>
       <c r="C24" t="s">
-        <v>340</v>
+        <v>462</v>
       </c>
       <c r="D24" t="s">
-        <v>341</v>
+        <v>308</v>
       </c>
       <c r="E24">
         <v>-1</v>
@@ -4856,13 +4861,13 @@
         <v>113</v>
       </c>
       <c r="B25" t="s">
-        <v>342</v>
+        <v>309</v>
       </c>
       <c r="C25" t="s">
-        <v>342</v>
+        <v>309</v>
       </c>
       <c r="D25" t="s">
-        <v>342</v>
+        <v>309</v>
       </c>
       <c r="E25">
         <v>2</v>
@@ -4876,7 +4881,7 @@
         <v>135</v>
       </c>
       <c r="B26" t="s">
-        <v>343</v>
+        <v>310</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -4890,7 +4895,7 @@
         <v>136</v>
       </c>
       <c r="B27" t="s">
-        <v>344</v>
+        <v>463</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -4904,13 +4909,13 @@
         <v>114</v>
       </c>
       <c r="B28" t="s">
-        <v>345</v>
+        <v>464</v>
       </c>
       <c r="C28" t="s">
-        <v>345</v>
+        <v>464</v>
       </c>
       <c r="D28" t="s">
-        <v>346</v>
+        <v>311</v>
       </c>
       <c r="E28">
         <v>-1</v>
@@ -4924,13 +4929,13 @@
         <v>115</v>
       </c>
       <c r="B29" t="s">
-        <v>393</v>
+        <v>342</v>
       </c>
       <c r="C29" t="s">
-        <v>347</v>
+        <v>312</v>
       </c>
       <c r="D29" t="s">
-        <v>348</v>
+        <v>313</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -4944,13 +4949,13 @@
         <v>116</v>
       </c>
       <c r="B30" t="s">
-        <v>349</v>
+        <v>499</v>
       </c>
       <c r="C30" t="s">
-        <v>350</v>
+        <v>465</v>
       </c>
       <c r="D30" t="s">
-        <v>351</v>
+        <v>314</v>
       </c>
       <c r="E30">
         <v>-1</v>
@@ -4964,13 +4969,13 @@
         <v>117</v>
       </c>
       <c r="B31" t="s">
-        <v>352</v>
+        <v>315</v>
       </c>
       <c r="C31" t="s">
-        <v>353</v>
+        <v>316</v>
       </c>
       <c r="D31" t="s">
-        <v>354</v>
+        <v>317</v>
       </c>
       <c r="E31">
         <v>2</v>
@@ -4984,13 +4989,13 @@
         <v>118</v>
       </c>
       <c r="B32" t="s">
-        <v>355</v>
+        <v>318</v>
       </c>
       <c r="C32" t="s">
-        <v>356</v>
+        <v>319</v>
       </c>
       <c r="D32" t="s">
-        <v>356</v>
+        <v>319</v>
       </c>
       <c r="E32">
         <v>3</v>
@@ -5004,13 +5009,13 @@
         <v>119</v>
       </c>
       <c r="B33" t="s">
-        <v>357</v>
+        <v>466</v>
       </c>
       <c r="C33" t="s">
-        <v>357</v>
+        <v>466</v>
       </c>
       <c r="D33" t="s">
-        <v>358</v>
+        <v>320</v>
       </c>
       <c r="E33">
         <v>2</v>
@@ -5024,13 +5029,13 @@
         <v>120</v>
       </c>
       <c r="B34" t="s">
-        <v>359</v>
+        <v>321</v>
       </c>
       <c r="C34" t="s">
-        <v>360</v>
+        <v>322</v>
       </c>
       <c r="D34" t="s">
-        <v>361</v>
+        <v>323</v>
       </c>
       <c r="E34">
         <v>0</v>
@@ -5044,13 +5049,13 @@
         <v>121</v>
       </c>
       <c r="B35" t="s">
-        <v>362</v>
+        <v>467</v>
       </c>
       <c r="C35" t="s">
-        <v>362</v>
+        <v>467</v>
       </c>
       <c r="D35" t="s">
-        <v>363</v>
+        <v>324</v>
       </c>
       <c r="E35">
         <v>-1</v>
@@ -5064,13 +5069,13 @@
         <v>122</v>
       </c>
       <c r="B36" t="s">
-        <v>394</v>
+        <v>468</v>
       </c>
       <c r="C36" t="s">
-        <v>364</v>
+        <v>469</v>
       </c>
       <c r="D36" t="s">
-        <v>365</v>
+        <v>325</v>
       </c>
       <c r="E36">
         <v>-1</v>
@@ -5084,13 +5089,13 @@
         <v>123</v>
       </c>
       <c r="B37" t="s">
-        <v>366</v>
+        <v>500</v>
       </c>
       <c r="C37" t="s">
-        <v>367</v>
+        <v>470</v>
       </c>
       <c r="D37" t="s">
-        <v>368</v>
+        <v>326</v>
       </c>
       <c r="E37">
         <v>3</v>
@@ -5104,13 +5109,13 @@
         <v>124</v>
       </c>
       <c r="B38" t="s">
-        <v>369</v>
+        <v>327</v>
       </c>
       <c r="C38" t="s">
-        <v>369</v>
+        <v>327</v>
       </c>
       <c r="D38" t="s">
-        <v>369</v>
+        <v>327</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -5124,13 +5129,13 @@
         <v>125</v>
       </c>
       <c r="B39" t="s">
-        <v>370</v>
+        <v>471</v>
       </c>
       <c r="C39" t="s">
-        <v>371</v>
+        <v>472</v>
       </c>
       <c r="D39" t="s">
-        <v>372</v>
+        <v>328</v>
       </c>
       <c r="E39">
         <v>3</v>
@@ -5144,13 +5149,13 @@
         <v>126</v>
       </c>
       <c r="B40" t="s">
-        <v>373</v>
+        <v>473</v>
       </c>
       <c r="C40" t="s">
-        <v>374</v>
+        <v>329</v>
       </c>
       <c r="D40" t="s">
-        <v>375</v>
+        <v>330</v>
       </c>
       <c r="E40">
         <v>0</v>
@@ -5164,13 +5169,13 @@
         <v>127</v>
       </c>
       <c r="B41" t="s">
-        <v>376</v>
+        <v>474</v>
       </c>
       <c r="C41" t="s">
-        <v>377</v>
+        <v>475</v>
       </c>
       <c r="D41" t="s">
-        <v>378</v>
+        <v>331</v>
       </c>
       <c r="E41">
         <v>6</v>
@@ -5184,7 +5189,7 @@
         <v>133</v>
       </c>
       <c r="B42" t="s">
-        <v>379</v>
+        <v>332</v>
       </c>
       <c r="E42">
         <v>6</v>
@@ -5198,13 +5203,13 @@
         <v>104</v>
       </c>
       <c r="B43" t="s">
-        <v>395</v>
+        <v>343</v>
       </c>
       <c r="C43" t="s">
-        <v>396</v>
+        <v>344</v>
       </c>
       <c r="D43" t="s">
-        <v>380</v>
+        <v>333</v>
       </c>
       <c r="E43">
         <v>6</v>
@@ -5218,13 +5223,13 @@
         <v>128</v>
       </c>
       <c r="B44" t="s">
-        <v>381</v>
+        <v>334</v>
       </c>
       <c r="C44" t="s">
-        <v>382</v>
+        <v>335</v>
       </c>
       <c r="D44" t="s">
-        <v>383</v>
+        <v>336</v>
       </c>
       <c r="E44">
         <v>6</v>
@@ -5238,13 +5243,13 @@
         <v>129</v>
       </c>
       <c r="B45" t="s">
-        <v>384</v>
+        <v>476</v>
       </c>
       <c r="C45" t="s">
-        <v>384</v>
+        <v>476</v>
       </c>
       <c r="D45" t="s">
-        <v>385</v>
+        <v>337</v>
       </c>
       <c r="E45">
         <v>2</v>
@@ -5258,13 +5263,13 @@
         <v>130</v>
       </c>
       <c r="B46" t="s">
-        <v>386</v>
+        <v>338</v>
       </c>
       <c r="C46" t="s">
-        <v>387</v>
+        <v>477</v>
       </c>
       <c r="D46" t="s">
-        <v>388</v>
+        <v>339</v>
       </c>
       <c r="E46">
         <v>0</v>
@@ -5278,13 +5283,13 @@
         <v>131</v>
       </c>
       <c r="B47" t="s">
-        <v>389</v>
+        <v>478</v>
       </c>
       <c r="C47" t="s">
-        <v>390</v>
+        <v>479</v>
       </c>
       <c r="D47" t="s">
-        <v>391</v>
+        <v>340</v>
       </c>
       <c r="F47">
         <v>1</v>
@@ -5318,10 +5323,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>481</v>
+        <v>422</v>
       </c>
       <c r="C1" t="s">
-        <v>498</v>
+        <v>439</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -5329,7 +5334,7 @@
         <v>77</v>
       </c>
       <c r="B2" t="s">
-        <v>397</v>
+        <v>345</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -5340,7 +5345,7 @@
         <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>398</v>
+        <v>346</v>
       </c>
       <c r="C3">
         <v>0</v>

</xml_diff>

<commit_message>
corrected misstake for hip_ae_hailer regex_kva codes for infection.
</commit_message>
<xml_diff>
--- a/data-raw/classcodes.xlsx
+++ b/data-raw/classcodes.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erik_\Documents\GitHub\coder\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\SHPR\Forskningsprojekt\Projekt 211-220\Projekt 217\coder\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A65391-0A99-4130-B081-D2B524FADE84}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32964" yWindow="0" windowWidth="14964" windowHeight="17868" tabRatio="500" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32964" yWindow="0" windowWidth="14964" windowHeight="17868" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ex_carbrands" sheetId="10" r:id="rId1"/>
@@ -1080,9 +1079,6 @@
     <t>(M(00(1|[0289]F?)|86([01]F|6F?)))|T(8(14|4(5[FX]?|7F?)))</t>
   </si>
   <si>
-    <t>NFS\\d{0,2}</t>
-  </si>
-  <si>
     <t>Dislocation</t>
   </si>
   <si>
@@ -1290,9 +1286,6 @@
     <t>29(6[235])|3(0(04|9)|11)</t>
   </si>
   <si>
-    <t>NF([CF-HJ-MS-TW]\\d{2}|A(02|1[12]|2[0-2])|Q09|U[013489]9)|QD(A10|B(0[05]|99)|E35|G30)|TNF(05|10)</t>
-  </si>
-  <si>
     <t>Chrysler|Fiat|Dodge|Ferrari|Maserati</t>
   </si>
   <si>
@@ -1534,12 +1527,18 @@
   </si>
   <si>
     <t>N02(A([A-W][0-9]{1}|X(0[0-26]|52))|BE51)</t>
+  </si>
+  <si>
+    <t>NFS[0-9]{0,2}</t>
+  </si>
+  <si>
+    <t>NF([CF-HJ-MS-TW][0-9]{2}|A(02|1[12]|2[0-2])|Q09|U[013489]9)|QD(A10|B(0[05]|99)|E35|G30)|TNF(05|10)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1605,7 +1604,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1882,7 +1881,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1931,7 +1930,7 @@
         <v>82</v>
       </c>
       <c r="B5" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -1955,7 +1954,7 @@
         <v>85</v>
       </c>
       <c r="B8" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
   </sheetData>
@@ -1964,7 +1963,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMO18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -1999,7 +1998,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>163</v>
@@ -2017,22 +2016,22 @@
         <v>150</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>426</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>427</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>428</v>
       </c>
       <c r="AMO1"/>
     </row>
@@ -2270,10 +2269,10 @@
         <v>166</v>
       </c>
       <c r="E7" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>157</v>
@@ -2317,7 +2316,7 @@
         <v>184</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>158</v>
@@ -2761,7 +2760,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2783,40 +2782,40 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C1" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F1" t="s">
         <v>164</v>
       </c>
       <c r="G1" t="s">
+        <v>428</v>
+      </c>
+      <c r="H1" t="s">
+        <v>429</v>
+      </c>
+      <c r="I1" t="s">
         <v>430</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>431</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>432</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>433</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>434</v>
-      </c>
-      <c r="L1" t="s">
-        <v>435</v>
-      </c>
-      <c r="M1" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -2830,13 +2829,13 @@
         <v>256</v>
       </c>
       <c r="D2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F2" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -2871,10 +2870,10 @@
         <v>257</v>
       </c>
       <c r="D3" t="s">
+        <v>396</v>
+      </c>
+      <c r="F3" t="s">
         <v>397</v>
-      </c>
-      <c r="F3" t="s">
-        <v>398</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -2909,13 +2908,13 @@
         <v>258</v>
       </c>
       <c r="D4" t="s">
+        <v>377</v>
+      </c>
+      <c r="E4" t="s">
         <v>378</v>
       </c>
-      <c r="E4" t="s">
-        <v>379</v>
-      </c>
       <c r="F4" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -2950,13 +2949,13 @@
         <v>220</v>
       </c>
       <c r="D5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F5" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -2991,13 +2990,13 @@
         <v>259</v>
       </c>
       <c r="D6" t="s">
+        <v>379</v>
+      </c>
+      <c r="E6" t="s">
         <v>380</v>
       </c>
-      <c r="E6" t="s">
-        <v>381</v>
-      </c>
       <c r="F6" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -3032,10 +3031,10 @@
         <v>221</v>
       </c>
       <c r="D7" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E7" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F7">
         <v>401</v>
@@ -3073,13 +3072,13 @@
         <v>222</v>
       </c>
       <c r="D8" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E8" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F8" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -3114,10 +3113,10 @@
         <v>223</v>
       </c>
       <c r="D9" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E9" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F9" t="s">
         <v>188</v>
@@ -3155,13 +3154,13 @@
         <v>260</v>
       </c>
       <c r="D10" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E10" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="F10" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -3196,13 +3195,13 @@
         <v>261</v>
       </c>
       <c r="D11" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E11" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F11" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -3237,13 +3236,13 @@
         <v>201</v>
       </c>
       <c r="D12" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E12" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F12" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -3278,13 +3277,13 @@
         <v>201</v>
       </c>
       <c r="D13" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E13" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F13" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -3319,13 +3318,13 @@
         <v>227</v>
       </c>
       <c r="D14" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E14" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F14" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="G14">
         <v>1</v>
@@ -3360,13 +3359,13 @@
         <v>262</v>
       </c>
       <c r="D15" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E15" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="F15" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="G15">
         <v>1</v>
@@ -3401,13 +3400,13 @@
         <v>263</v>
       </c>
       <c r="D16" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E16" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F16" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G16">
         <v>1</v>
@@ -3442,13 +3441,13 @@
         <v>196</v>
       </c>
       <c r="D17" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E17" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F17" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="G17">
         <v>1</v>
@@ -3524,13 +3523,13 @@
         <v>231</v>
       </c>
       <c r="D19" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E19" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="F19" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="G19">
         <v>1</v>
@@ -3606,13 +3605,13 @@
         <v>232</v>
       </c>
       <c r="D21" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E21" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F21" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -3647,13 +3646,13 @@
         <v>264</v>
       </c>
       <c r="D22" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E22" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F22" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="G22">
         <v>1</v>
@@ -3688,13 +3687,13 @@
         <v>234</v>
       </c>
       <c r="D23" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E23" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F23" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -3770,13 +3769,13 @@
         <v>265</v>
       </c>
       <c r="D25" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E25" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F25" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G25">
         <v>1</v>
@@ -3817,7 +3816,7 @@
         <v>276</v>
       </c>
       <c r="F26" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G26">
         <v>1</v>
@@ -3855,7 +3854,7 @@
         <v>2800</v>
       </c>
       <c r="E27" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F27">
         <v>2800</v>
@@ -3893,13 +3892,13 @@
         <v>241</v>
       </c>
       <c r="D28" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E28" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F28" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="G28">
         <v>1</v>
@@ -3934,13 +3933,13 @@
         <v>266</v>
       </c>
       <c r="D29" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E29" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="F29" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="G29">
         <v>1</v>
@@ -3975,13 +3974,13 @@
         <v>267</v>
       </c>
       <c r="D30" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E30" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F30" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="G30">
         <v>1</v>
@@ -4016,13 +4015,13 @@
         <v>243</v>
       </c>
       <c r="D31" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E31" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F31" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="G31">
         <v>1</v>
@@ -4057,16 +4056,16 @@
         <v>245</v>
       </c>
       <c r="D32" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E32" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="F32" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="G32" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="H32">
         <v>1</v>
@@ -4094,11 +4093,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4114,7 +4113,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C1" t="s">
         <v>179</v>
@@ -4161,7 +4160,7 @@
         <v>67</v>
       </c>
       <c r="B5" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>70</v>
@@ -4194,7 +4193,7 @@
         <v>178</v>
       </c>
       <c r="C8" t="s">
-        <v>419</v>
+        <v>500</v>
       </c>
       <c r="D8" t="s">
         <v>72</v>
@@ -4206,11 +4205,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4226,7 +4225,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C1" t="s">
         <v>179</v>
@@ -4240,18 +4239,18 @@
         <v>348</v>
       </c>
       <c r="C2" t="s">
-        <v>349</v>
+        <v>499</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>349</v>
+      </c>
+      <c r="B3" t="s">
         <v>350</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>351</v>
-      </c>
-      <c r="C3" t="s">
-        <v>352</v>
       </c>
     </row>
   </sheetData>
@@ -4260,7 +4259,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4280,7 +4279,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C1" t="s">
         <v>179</v>
@@ -4372,10 +4371,10 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
@@ -4393,7 +4392,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C1" t="s">
         <v>134</v>
@@ -4402,10 +4401,10 @@
         <v>90</v>
       </c>
       <c r="E1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="F1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -4413,7 +4412,7 @@
         <v>91</v>
       </c>
       <c r="B2" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C2" t="s">
         <v>277</v>
@@ -4433,10 +4432,10 @@
         <v>92</v>
       </c>
       <c r="B3" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C3" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D3" t="s">
         <v>279</v>
@@ -4453,10 +4452,10 @@
         <v>93</v>
       </c>
       <c r="B4" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C4" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D4" t="s">
         <v>280</v>
@@ -4473,10 +4472,10 @@
         <v>94</v>
       </c>
       <c r="B5" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="C5" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D5" t="s">
         <v>281</v>
@@ -4496,7 +4495,7 @@
         <v>282</v>
       </c>
       <c r="C6" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D6" t="s">
         <v>283</v>
@@ -4513,10 +4512,10 @@
         <v>96</v>
       </c>
       <c r="B7" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C7" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D7" t="s">
         <v>284</v>
@@ -4533,7 +4532,7 @@
         <v>97</v>
       </c>
       <c r="B8" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C8" t="s">
         <v>285</v>
@@ -4573,10 +4572,10 @@
         <v>99</v>
       </c>
       <c r="B10" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C10" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="D10" t="s">
         <v>290</v>
@@ -4593,10 +4592,10 @@
         <v>100</v>
       </c>
       <c r="B11" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C11" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="D11" t="s">
         <v>291</v>
@@ -4613,7 +4612,7 @@
         <v>101</v>
       </c>
       <c r="B12" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C12" t="s">
         <v>292</v>
@@ -4633,10 +4632,10 @@
         <v>102</v>
       </c>
       <c r="B13" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="C13" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D13" t="s">
         <v>294</v>
@@ -4656,7 +4655,7 @@
         <v>295</v>
       </c>
       <c r="C14" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="D14" t="s">
         <v>296</v>
@@ -4676,7 +4675,7 @@
         <v>297</v>
       </c>
       <c r="C15" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D15" t="s">
         <v>298</v>
@@ -4693,10 +4692,10 @@
         <v>106</v>
       </c>
       <c r="B16" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C16" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D16" t="s">
         <v>299</v>
@@ -4713,10 +4712,10 @@
         <v>107</v>
       </c>
       <c r="B17" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C17" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D17" t="s">
         <v>300</v>
@@ -4733,10 +4732,10 @@
         <v>108</v>
       </c>
       <c r="B18" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C18" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D18" t="s">
         <v>301</v>
@@ -4781,10 +4780,10 @@
         <v>76</v>
       </c>
       <c r="B21" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C21" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D21" t="s">
         <v>305</v>
@@ -4821,10 +4820,10 @@
         <v>111</v>
       </c>
       <c r="B23" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C23" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="D23" t="s">
         <v>307</v>
@@ -4841,10 +4840,10 @@
         <v>112</v>
       </c>
       <c r="B24" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="C24" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D24" t="s">
         <v>308</v>
@@ -4895,7 +4894,7 @@
         <v>136</v>
       </c>
       <c r="B27" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -4909,10 +4908,10 @@
         <v>114</v>
       </c>
       <c r="B28" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C28" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D28" t="s">
         <v>311</v>
@@ -4949,10 +4948,10 @@
         <v>116</v>
       </c>
       <c r="B30" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="C30" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D30" t="s">
         <v>314</v>
@@ -5009,10 +5008,10 @@
         <v>119</v>
       </c>
       <c r="B33" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C33" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D33" t="s">
         <v>320</v>
@@ -5049,10 +5048,10 @@
         <v>121</v>
       </c>
       <c r="B35" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="C35" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D35" t="s">
         <v>324</v>
@@ -5069,10 +5068,10 @@
         <v>122</v>
       </c>
       <c r="B36" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C36" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="D36" t="s">
         <v>325</v>
@@ -5089,10 +5088,10 @@
         <v>123</v>
       </c>
       <c r="B37" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="C37" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D37" t="s">
         <v>326</v>
@@ -5129,10 +5128,10 @@
         <v>125</v>
       </c>
       <c r="B39" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="C39" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D39" t="s">
         <v>328</v>
@@ -5149,7 +5148,7 @@
         <v>126</v>
       </c>
       <c r="B40" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="C40" t="s">
         <v>329</v>
@@ -5169,10 +5168,10 @@
         <v>127</v>
       </c>
       <c r="B41" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C41" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="D41" t="s">
         <v>331</v>
@@ -5243,10 +5242,10 @@
         <v>129</v>
       </c>
       <c r="B45" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C45" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="D45" t="s">
         <v>337</v>
@@ -5266,7 +5265,7 @@
         <v>338</v>
       </c>
       <c r="C46" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="D46" t="s">
         <v>339</v>
@@ -5283,10 +5282,10 @@
         <v>131</v>
       </c>
       <c r="B47" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C47" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="D47" t="s">
         <v>340</v>
@@ -5296,7 +5295,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D45">
+  <sortState ref="A2:D45">
     <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5305,7 +5304,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5323,10 +5322,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C1" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Remove toy example with cars. Fix #93.
</commit_message>
<xml_diff>
--- a/data-raw/classcodes.xlsx
+++ b/data-raw/classcodes.xlsx
@@ -1,35 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\SHPR\Forskningsprojekt\Projekt 211-220\Projekt 217\coder\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erik_\Documents\GitHub\coder\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{113D3CB6-524B-46E6-B326-18595D3E041E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32964" yWindow="0" windowWidth="14964" windowHeight="17868" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="18972" yWindow="444" windowWidth="26160" windowHeight="23808" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="ex_carbrands" sheetId="10" r:id="rId1"/>
-    <sheet name="charlson" sheetId="1" r:id="rId2"/>
-    <sheet name="elixhauser" sheetId="2" r:id="rId3"/>
-    <sheet name="hip_ae" sheetId="3" r:id="rId4"/>
-    <sheet name="hip_ae_hailer" sheetId="11" r:id="rId5"/>
-    <sheet name="knee_ae" sheetId="5" r:id="rId6"/>
-    <sheet name="rxriskv" sheetId="7" r:id="rId7"/>
-    <sheet name="cps" sheetId="9" r:id="rId8"/>
+    <sheet name="charlson" sheetId="1" r:id="rId1"/>
+    <sheet name="elixhauser" sheetId="2" r:id="rId2"/>
+    <sheet name="hip_ae" sheetId="3" r:id="rId3"/>
+    <sheet name="hip_ae_hailer" sheetId="11" r:id="rId4"/>
+    <sheet name="knee_ae" sheetId="5" r:id="rId5"/>
+    <sheet name="rxriskv" sheetId="7" r:id="rId6"/>
+    <sheet name="cps" sheetId="9" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">rxriskv!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">rxriskv!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="488">
   <si>
     <t>group</t>
   </si>
@@ -37,9 +37,6 @@
     <t>description</t>
   </si>
   <si>
-    <t>regex</t>
-  </si>
-  <si>
     <t>myocardial infarction</t>
   </si>
   <si>
@@ -266,36 +263,6 @@
   </si>
   <si>
     <t>special</t>
-  </si>
-  <si>
-    <t>Mazda</t>
-  </si>
-  <si>
-    <t>Mer-Ben</t>
-  </si>
-  <si>
-    <t>Ford</t>
-  </si>
-  <si>
-    <t>Fiat</t>
-  </si>
-  <si>
-    <t>Toyota</t>
-  </si>
-  <si>
-    <t>Volksw</t>
-  </si>
-  <si>
-    <t>Geely</t>
-  </si>
-  <si>
-    <t>Merc</t>
-  </si>
-  <si>
-    <t>Ford|Lincoln</t>
-  </si>
-  <si>
-    <t>Porsche</t>
   </si>
   <si>
     <t>malignancy</t>
@@ -1284,12 +1251,6 @@
   </si>
   <si>
     <t>29(6[235])|3(0(04|9)|11)</t>
-  </si>
-  <si>
-    <t>Chrysler|Fiat|Dodge|Ferrari|Maserati</t>
-  </si>
-  <si>
-    <t>Volvo|Lotus|Polestar</t>
   </si>
   <si>
     <t>regex_icd10</t>
@@ -1538,7 +1499,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1604,7 +1565,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1881,92 +1842,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="36.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>82</v>
-      </c>
-      <c r="B5" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>83</v>
-      </c>
-      <c r="B6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>84</v>
-      </c>
-      <c r="B7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>85</v>
-      </c>
-      <c r="B8" t="s">
-        <v>419</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMO18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="E16" sqref="E16"/>
     </sheetView>
@@ -1998,67 +1877,67 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>420</v>
+        <v>407</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>421</v>
+        <v>408</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>422</v>
+        <v>409</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>423</v>
+        <v>410</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>424</v>
+        <v>411</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>425</v>
+        <v>412</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>426</v>
+        <v>413</v>
       </c>
       <c r="AMO1"/>
     </row>
     <row r="2" spans="1:14 1029:1029" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>4</v>
-      </c>
       <c r="C2" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="I2">
         <v>1</v>
@@ -2081,28 +1960,28 @@
     </row>
     <row r="3" spans="1:14 1029:1029" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="C3" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="D3" s="6">
         <v>428</v>
       </c>
       <c r="E3" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="I3">
         <v>1</v>
@@ -2125,28 +2004,28 @@
     </row>
     <row r="4" spans="1:14 1029:1029" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="C4" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E4" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -2169,28 +2048,28 @@
     </row>
     <row r="5" spans="1:14 1029:1029" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="C5" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="E5" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="I5">
         <v>1</v>
@@ -2213,28 +2092,28 @@
     </row>
     <row r="6" spans="1:14 1029:1029" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="C6" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="D6" s="6">
         <v>290</v>
       </c>
       <c r="E6" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="I6">
         <v>1</v>
@@ -2257,28 +2136,28 @@
     </row>
     <row r="7" spans="1:14 1029:1029" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="C7" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="E7" t="s">
-        <v>479</v>
+        <v>466</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>482</v>
+        <v>469</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="I7">
         <v>1</v>
@@ -2301,28 +2180,28 @@
     </row>
     <row r="8" spans="1:14 1029:1029" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="C8" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="E8" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>480</v>
+        <v>467</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -2345,19 +2224,19 @@
     </row>
     <row r="9" spans="1:14 1029:1029" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="C9" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="E9" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="I9">
         <v>1</v>
@@ -2380,19 +2259,19 @@
     </row>
     <row r="10" spans="1:14 1029:1029" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="C10" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="E10" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="I10">
         <v>1</v>
@@ -2415,19 +2294,19 @@
     </row>
     <row r="11" spans="1:14 1029:1029" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="C11" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="E11" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="I11">
         <v>1</v>
@@ -2450,28 +2329,28 @@
     </row>
     <row r="12" spans="1:14 1029:1029" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="C12" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="E12" t="s">
+        <v>177</v>
+      </c>
+      <c r="F12" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>199</v>
       </c>
       <c r="G12" s="6">
         <v>344</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="I12">
         <v>2</v>
@@ -2494,28 +2373,28 @@
     </row>
     <row r="13" spans="1:14 1029:1029" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="C13" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="E13" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="I13">
         <v>2</v>
@@ -2538,22 +2417,22 @@
     </row>
     <row r="14" spans="1:14 1029:1029" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="C14" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="E14" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="G14" s="6">
         <v>250</v>
@@ -2582,28 +2461,28 @@
     </row>
     <row r="15" spans="1:14 1029:1029" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C15" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="E15" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="I15">
         <v>2</v>
@@ -2626,28 +2505,28 @@
     </row>
     <row r="16" spans="1:14 1029:1029" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="C16" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="E16" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="I16">
         <v>3</v>
@@ -2670,28 +2549,28 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="C17" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="E17" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="I17">
         <v>6</v>
@@ -2714,25 +2593,25 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="C18" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="E18" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="I18">
         <v>6</v>
@@ -2759,8 +2638,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2782,60 +2661,60 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>407</v>
+      </c>
+      <c r="C1" t="s">
+        <v>414</v>
+      </c>
+      <c r="D1" t="s">
+        <v>341</v>
+      </c>
+      <c r="E1" t="s">
+        <v>364</v>
+      </c>
+      <c r="F1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G1" t="s">
+        <v>415</v>
+      </c>
+      <c r="H1" t="s">
+        <v>416</v>
+      </c>
+      <c r="I1" t="s">
+        <v>417</v>
+      </c>
+      <c r="J1" t="s">
+        <v>418</v>
+      </c>
+      <c r="K1" t="s">
+        <v>419</v>
+      </c>
+      <c r="L1" t="s">
         <v>420</v>
       </c>
-      <c r="C1" t="s">
-        <v>427</v>
-      </c>
-      <c r="D1" t="s">
-        <v>352</v>
-      </c>
-      <c r="E1" t="s">
-        <v>375</v>
-      </c>
-      <c r="F1" t="s">
-        <v>164</v>
-      </c>
-      <c r="G1" t="s">
-        <v>428</v>
-      </c>
-      <c r="H1" t="s">
-        <v>429</v>
-      </c>
-      <c r="I1" t="s">
-        <v>430</v>
-      </c>
-      <c r="J1" t="s">
-        <v>431</v>
-      </c>
-      <c r="K1" t="s">
-        <v>432</v>
-      </c>
-      <c r="L1" t="s">
-        <v>433</v>
-      </c>
       <c r="M1" t="s">
-        <v>434</v>
+        <v>421</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="C2" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="D2" t="s">
-        <v>355</v>
+        <v>344</v>
       </c>
       <c r="E2" t="s">
-        <v>376</v>
+        <v>365</v>
       </c>
       <c r="F2" t="s">
-        <v>483</v>
+        <v>470</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -2861,19 +2740,19 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
+        <v>235</v>
+      </c>
+      <c r="C3" t="s">
         <v>246</v>
       </c>
-      <c r="C3" t="s">
-        <v>257</v>
-      </c>
       <c r="D3" t="s">
-        <v>396</v>
+        <v>385</v>
       </c>
       <c r="F3" t="s">
-        <v>397</v>
+        <v>386</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -2899,22 +2778,22 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
+        <v>236</v>
+      </c>
+      <c r="C4" t="s">
         <v>247</v>
       </c>
-      <c r="C4" t="s">
-        <v>258</v>
-      </c>
       <c r="D4" t="s">
-        <v>377</v>
+        <v>366</v>
       </c>
       <c r="E4" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
       <c r="F4" t="s">
-        <v>398</v>
+        <v>387</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -2940,22 +2819,22 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="C5" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="D5" t="s">
-        <v>356</v>
+        <v>345</v>
       </c>
       <c r="E5" t="s">
-        <v>356</v>
+        <v>345</v>
       </c>
       <c r="F5" t="s">
-        <v>399</v>
+        <v>388</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -2981,22 +2860,22 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="C6" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="D6" t="s">
-        <v>379</v>
+        <v>368</v>
       </c>
       <c r="E6" t="s">
-        <v>380</v>
+        <v>369</v>
       </c>
       <c r="F6" t="s">
-        <v>400</v>
+        <v>389</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -3022,19 +2901,19 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="C7" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="D7" t="s">
-        <v>353</v>
+        <v>342</v>
       </c>
       <c r="E7" t="s">
-        <v>381</v>
+        <v>370</v>
       </c>
       <c r="F7">
         <v>401</v>
@@ -3063,22 +2942,22 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="C8" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="D8" t="s">
-        <v>354</v>
+        <v>343</v>
       </c>
       <c r="E8" t="s">
-        <v>382</v>
+        <v>371</v>
       </c>
       <c r="F8" t="s">
-        <v>401</v>
+        <v>390</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -3104,22 +2983,22 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="C9" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="D9" t="s">
-        <v>357</v>
+        <v>346</v>
       </c>
       <c r="E9" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
       <c r="F9" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -3145,22 +3024,22 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="C10" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="D10" t="s">
-        <v>358</v>
+        <v>347</v>
       </c>
       <c r="E10" t="s">
-        <v>481</v>
+        <v>468</v>
       </c>
       <c r="F10" t="s">
-        <v>402</v>
+        <v>391</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -3186,22 +3065,22 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="C11" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="D11" t="s">
-        <v>359</v>
+        <v>348</v>
       </c>
       <c r="E11" t="s">
-        <v>384</v>
+        <v>373</v>
       </c>
       <c r="F11" t="s">
-        <v>403</v>
+        <v>392</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -3227,22 +3106,22 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B12" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="C12" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="D12" t="s">
-        <v>360</v>
+        <v>349</v>
       </c>
       <c r="E12" t="s">
-        <v>385</v>
+        <v>374</v>
       </c>
       <c r="F12" t="s">
-        <v>360</v>
+        <v>349</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -3268,22 +3147,22 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="C13" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="D13" t="s">
-        <v>361</v>
+        <v>350</v>
       </c>
       <c r="E13" t="s">
-        <v>405</v>
+        <v>394</v>
       </c>
       <c r="F13" t="s">
-        <v>404</v>
+        <v>393</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -3309,22 +3188,22 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="C14" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="D14" t="s">
-        <v>362</v>
+        <v>351</v>
       </c>
       <c r="E14" t="s">
-        <v>386</v>
+        <v>375</v>
       </c>
       <c r="F14" t="s">
-        <v>406</v>
+        <v>395</v>
       </c>
       <c r="G14">
         <v>1</v>
@@ -3350,22 +3229,22 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B15" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="C15" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="D15" t="s">
-        <v>363</v>
+        <v>352</v>
       </c>
       <c r="E15" t="s">
-        <v>486</v>
+        <v>473</v>
       </c>
       <c r="F15" t="s">
-        <v>487</v>
+        <v>474</v>
       </c>
       <c r="G15">
         <v>1</v>
@@ -3391,22 +3270,22 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B16" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="C16" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="D16" t="s">
-        <v>364</v>
+        <v>353</v>
       </c>
       <c r="E16" t="s">
-        <v>387</v>
+        <v>376</v>
       </c>
       <c r="F16" t="s">
-        <v>407</v>
+        <v>396</v>
       </c>
       <c r="G16">
         <v>1</v>
@@ -3432,22 +3311,22 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="C17" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="D17" t="s">
-        <v>365</v>
+        <v>354</v>
       </c>
       <c r="E17" t="s">
-        <v>388</v>
+        <v>377</v>
       </c>
       <c r="F17" t="s">
-        <v>408</v>
+        <v>397</v>
       </c>
       <c r="G17">
         <v>1</v>
@@ -3473,22 +3352,22 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="C18" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="D18" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="E18" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="F18" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="G18">
         <v>1</v>
@@ -3514,22 +3393,22 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B19" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="C19" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="D19" t="s">
-        <v>366</v>
+        <v>355</v>
       </c>
       <c r="E19" t="s">
-        <v>389</v>
+        <v>378</v>
       </c>
       <c r="F19" t="s">
-        <v>484</v>
+        <v>471</v>
       </c>
       <c r="G19">
         <v>1</v>
@@ -3555,22 +3434,22 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B20" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="C20" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="D20" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="E20" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="F20" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -3596,22 +3475,22 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B21" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="C21" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="D21" t="s">
-        <v>367</v>
+        <v>356</v>
       </c>
       <c r="E21" t="s">
-        <v>390</v>
+        <v>379</v>
       </c>
       <c r="F21" t="s">
-        <v>409</v>
+        <v>398</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -3637,22 +3516,22 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="C22" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="D22" t="s">
-        <v>368</v>
+        <v>357</v>
       </c>
       <c r="E22" t="s">
-        <v>368</v>
+        <v>357</v>
       </c>
       <c r="F22" t="s">
-        <v>410</v>
+        <v>399</v>
       </c>
       <c r="G22">
         <v>1</v>
@@ -3678,22 +3557,22 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B23" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="C23" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="D23" t="s">
-        <v>369</v>
+        <v>358</v>
       </c>
       <c r="E23" t="s">
-        <v>369</v>
+        <v>358</v>
       </c>
       <c r="F23" t="s">
-        <v>369</v>
+        <v>358</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -3719,13 +3598,13 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B24" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="C24" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="D24">
         <v>2780</v>
@@ -3760,22 +3639,22 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B25" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="C25" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="D25" t="s">
-        <v>370</v>
+        <v>359</v>
       </c>
       <c r="E25" t="s">
-        <v>391</v>
+        <v>380</v>
       </c>
       <c r="F25" t="s">
-        <v>411</v>
+        <v>400</v>
       </c>
       <c r="G25">
         <v>1</v>
@@ -3801,13 +3680,13 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B26" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="C26" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="D26">
         <v>276</v>
@@ -3816,7 +3695,7 @@
         <v>276</v>
       </c>
       <c r="F26" t="s">
-        <v>412</v>
+        <v>401</v>
       </c>
       <c r="G26">
         <v>1</v>
@@ -3842,19 +3721,19 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B27" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="C27" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="D27">
         <v>2800</v>
       </c>
       <c r="E27" t="s">
-        <v>392</v>
+        <v>381</v>
       </c>
       <c r="F27">
         <v>2800</v>
@@ -3883,22 +3762,22 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B28" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="C28" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="D28" t="s">
-        <v>371</v>
+        <v>360</v>
       </c>
       <c r="E28" t="s">
-        <v>393</v>
+        <v>382</v>
       </c>
       <c r="F28" t="s">
-        <v>413</v>
+        <v>402</v>
       </c>
       <c r="G28">
         <v>1</v>
@@ -3924,22 +3803,22 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B29" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="C29" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="D29" t="s">
-        <v>372</v>
+        <v>361</v>
       </c>
       <c r="E29" t="s">
-        <v>485</v>
+        <v>472</v>
       </c>
       <c r="F29" t="s">
-        <v>414</v>
+        <v>403</v>
       </c>
       <c r="G29">
         <v>1</v>
@@ -3965,22 +3844,22 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B30" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="C30" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="D30" t="s">
-        <v>373</v>
+        <v>362</v>
       </c>
       <c r="E30" t="s">
-        <v>394</v>
+        <v>383</v>
       </c>
       <c r="F30" t="s">
-        <v>415</v>
+        <v>404</v>
       </c>
       <c r="G30">
         <v>1</v>
@@ -4006,22 +3885,22 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B31" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="C31" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="D31" t="s">
-        <v>374</v>
+        <v>363</v>
       </c>
       <c r="E31" t="s">
-        <v>374</v>
+        <v>363</v>
       </c>
       <c r="F31" t="s">
-        <v>416</v>
+        <v>405</v>
       </c>
       <c r="G31">
         <v>1</v>
@@ -4047,25 +3926,25 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B32" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="C32" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="D32" t="s">
-        <v>438</v>
+        <v>425</v>
       </c>
       <c r="E32" t="s">
-        <v>438</v>
+        <v>425</v>
       </c>
       <c r="F32" t="s">
-        <v>417</v>
+        <v>406</v>
       </c>
       <c r="G32" t="s">
-        <v>395</v>
+        <v>384</v>
       </c>
       <c r="H32">
         <v>1</v>
@@ -4092,11 +3971,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -4113,90 +3992,90 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>420</v>
+        <v>407</v>
       </c>
       <c r="C1" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="D1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
-        <v>488</v>
+        <v>475</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B7" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="C8" t="s">
-        <v>500</v>
+        <v>487</v>
       </c>
       <c r="D8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -4204,8 +4083,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4225,32 +4104,32 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>420</v>
+        <v>407</v>
       </c>
       <c r="C1" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
       <c r="B2" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="C2" t="s">
-        <v>499</v>
+        <v>486</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>349</v>
+        <v>338</v>
       </c>
       <c r="B3" t="s">
-        <v>350</v>
+        <v>339</v>
       </c>
       <c r="C3" t="s">
-        <v>351</v>
+        <v>340</v>
       </c>
     </row>
   </sheetData>
@@ -4258,8 +4137,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4279,90 +4158,90 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>420</v>
+        <v>407</v>
       </c>
       <c r="C1" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="D1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B3" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B7" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="C8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -4370,8 +4249,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -4392,33 +4271,33 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>435</v>
+        <v>422</v>
       </c>
       <c r="C1" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="D1" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="E1" t="s">
-        <v>436</v>
+        <v>423</v>
       </c>
       <c r="F1" t="s">
-        <v>428</v>
+        <v>415</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="B2" t="s">
-        <v>478</v>
+        <v>465</v>
       </c>
       <c r="C2" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="D2" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="E2">
         <v>6</v>
@@ -4429,16 +4308,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="B3" t="s">
-        <v>489</v>
+        <v>476</v>
       </c>
       <c r="C3" t="s">
-        <v>439</v>
+        <v>426</v>
       </c>
       <c r="D3" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="E3">
         <v>-1</v>
@@ -4449,16 +4328,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="B4" t="s">
-        <v>440</v>
+        <v>427</v>
       </c>
       <c r="C4" t="s">
-        <v>441</v>
+        <v>428</v>
       </c>
       <c r="D4" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -4469,16 +4348,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="B5" t="s">
-        <v>490</v>
+        <v>477</v>
       </c>
       <c r="C5" t="s">
-        <v>442</v>
+        <v>429</v>
       </c>
       <c r="D5" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="E5">
         <v>2</v>
@@ -4489,16 +4368,16 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="B6" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="C6" t="s">
-        <v>443</v>
+        <v>430</v>
       </c>
       <c r="D6" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -4509,16 +4388,16 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B7" t="s">
-        <v>444</v>
+        <v>431</v>
       </c>
       <c r="C7" t="s">
-        <v>445</v>
+        <v>432</v>
       </c>
       <c r="D7" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -4529,16 +4408,16 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="B8" t="s">
-        <v>446</v>
+        <v>433</v>
       </c>
       <c r="C8" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="D8" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -4549,16 +4428,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="B9" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="C9" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
       <c r="D9" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="E9">
         <v>-1</v>
@@ -4569,16 +4448,16 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="B10" t="s">
-        <v>491</v>
+        <v>478</v>
       </c>
       <c r="C10" t="s">
-        <v>447</v>
+        <v>434</v>
       </c>
       <c r="D10" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="E10">
         <v>2</v>
@@ -4589,16 +4468,16 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="B11" t="s">
-        <v>492</v>
+        <v>479</v>
       </c>
       <c r="C11" t="s">
-        <v>448</v>
+        <v>435</v>
       </c>
       <c r="D11" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="E11">
         <v>2</v>
@@ -4609,16 +4488,16 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="B12" t="s">
-        <v>493</v>
+        <v>480</v>
       </c>
       <c r="C12" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="D12" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="E12">
         <v>2</v>
@@ -4629,16 +4508,16 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="B13" t="s">
-        <v>494</v>
+        <v>481</v>
       </c>
       <c r="C13" t="s">
-        <v>449</v>
+        <v>436</v>
       </c>
       <c r="D13" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="E13">
         <v>2</v>
@@ -4649,16 +4528,16 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="B14" t="s">
-        <v>295</v>
+        <v>284</v>
       </c>
       <c r="C14" t="s">
-        <v>450</v>
+        <v>437</v>
       </c>
       <c r="D14" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="E14">
         <v>2</v>
@@ -4669,16 +4548,16 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="B15" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="C15" t="s">
-        <v>451</v>
+        <v>438</v>
       </c>
       <c r="D15" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -4689,16 +4568,16 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="B16" t="s">
-        <v>452</v>
+        <v>439</v>
       </c>
       <c r="C16" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
       <c r="D16" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -4709,16 +4588,16 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="B17" t="s">
-        <v>454</v>
+        <v>441</v>
       </c>
       <c r="C17" t="s">
-        <v>455</v>
+        <v>442</v>
       </c>
       <c r="D17" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -4729,16 +4608,16 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="B18" t="s">
-        <v>456</v>
+        <v>443</v>
       </c>
       <c r="C18" t="s">
-        <v>456</v>
+        <v>443</v>
       </c>
       <c r="D18" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -4749,10 +4628,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="B19" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -4760,16 +4639,16 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="B20" t="s">
-        <v>341</v>
+        <v>330</v>
       </c>
       <c r="C20" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="D20" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -4777,16 +4656,16 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B21" t="s">
-        <v>457</v>
+        <v>444</v>
       </c>
       <c r="C21" t="s">
-        <v>458</v>
+        <v>445</v>
       </c>
       <c r="D21" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -4797,16 +4676,16 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="B22" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="C22" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="D22" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="E22">
         <v>4</v>
@@ -4817,16 +4696,16 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="B23" t="s">
-        <v>495</v>
+        <v>482</v>
       </c>
       <c r="C23" t="s">
-        <v>459</v>
+        <v>446</v>
       </c>
       <c r="D23" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="E23">
         <v>-1</v>
@@ -4837,16 +4716,16 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="B24" t="s">
-        <v>496</v>
+        <v>483</v>
       </c>
       <c r="C24" t="s">
-        <v>460</v>
+        <v>447</v>
       </c>
       <c r="D24" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="E24">
         <v>-1</v>
@@ -4857,16 +4736,16 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="B25" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
       <c r="C25" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
       <c r="D25" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
       <c r="E25">
         <v>2</v>
@@ -4877,10 +4756,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="B26" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -4891,10 +4770,10 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="B27" t="s">
-        <v>461</v>
+        <v>448</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -4905,16 +4784,16 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="B28" t="s">
-        <v>462</v>
+        <v>449</v>
       </c>
       <c r="C28" t="s">
-        <v>462</v>
+        <v>449</v>
       </c>
       <c r="D28" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
       <c r="E28">
         <v>-1</v>
@@ -4925,16 +4804,16 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="B29" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
       <c r="C29" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
       <c r="D29" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -4945,16 +4824,16 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="B30" t="s">
-        <v>497</v>
+        <v>484</v>
       </c>
       <c r="C30" t="s">
-        <v>463</v>
+        <v>450</v>
       </c>
       <c r="D30" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="E30">
         <v>-1</v>
@@ -4965,16 +4844,16 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="B31" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="C31" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="D31" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
       <c r="E31">
         <v>2</v>
@@ -4985,16 +4864,16 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="B32" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
       <c r="C32" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
       <c r="D32" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
       <c r="E32">
         <v>3</v>
@@ -5005,16 +4884,16 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="B33" t="s">
-        <v>464</v>
+        <v>451</v>
       </c>
       <c r="C33" t="s">
-        <v>464</v>
+        <v>451</v>
       </c>
       <c r="D33" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
       <c r="E33">
         <v>2</v>
@@ -5025,16 +4904,16 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="B34" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
       <c r="C34" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
       <c r="D34" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
       <c r="E34">
         <v>0</v>
@@ -5045,16 +4924,16 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="B35" t="s">
-        <v>465</v>
+        <v>452</v>
       </c>
       <c r="C35" t="s">
-        <v>465</v>
+        <v>452</v>
       </c>
       <c r="D35" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
       <c r="E35">
         <v>-1</v>
@@ -5065,16 +4944,16 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="B36" t="s">
-        <v>466</v>
+        <v>453</v>
       </c>
       <c r="C36" t="s">
-        <v>467</v>
+        <v>454</v>
       </c>
       <c r="D36" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
       <c r="E36">
         <v>-1</v>
@@ -5085,16 +4964,16 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="B37" t="s">
-        <v>498</v>
+        <v>485</v>
       </c>
       <c r="C37" t="s">
-        <v>468</v>
+        <v>455</v>
       </c>
       <c r="D37" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
       <c r="E37">
         <v>3</v>
@@ -5105,16 +4984,16 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="B38" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
       <c r="C38" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
       <c r="D38" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -5125,16 +5004,16 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="B39" t="s">
-        <v>469</v>
+        <v>456</v>
       </c>
       <c r="C39" t="s">
-        <v>470</v>
+        <v>457</v>
       </c>
       <c r="D39" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
       <c r="E39">
         <v>3</v>
@@ -5145,16 +5024,16 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="B40" t="s">
-        <v>471</v>
+        <v>458</v>
       </c>
       <c r="C40" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
       <c r="D40" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
       <c r="E40">
         <v>0</v>
@@ -5165,16 +5044,16 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="B41" t="s">
-        <v>472</v>
+        <v>459</v>
       </c>
       <c r="C41" t="s">
-        <v>473</v>
+        <v>460</v>
       </c>
       <c r="D41" t="s">
-        <v>331</v>
+        <v>320</v>
       </c>
       <c r="E41">
         <v>6</v>
@@ -5185,10 +5064,10 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="B42" t="s">
-        <v>332</v>
+        <v>321</v>
       </c>
       <c r="E42">
         <v>6</v>
@@ -5199,16 +5078,16 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="B43" t="s">
-        <v>343</v>
+        <v>332</v>
       </c>
       <c r="C43" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="D43" t="s">
-        <v>333</v>
+        <v>322</v>
       </c>
       <c r="E43">
         <v>6</v>
@@ -5219,16 +5098,16 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="B44" t="s">
-        <v>334</v>
+        <v>323</v>
       </c>
       <c r="C44" t="s">
-        <v>335</v>
+        <v>324</v>
       </c>
       <c r="D44" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
       <c r="E44">
         <v>6</v>
@@ -5239,16 +5118,16 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="B45" t="s">
-        <v>474</v>
+        <v>461</v>
       </c>
       <c r="C45" t="s">
-        <v>474</v>
+        <v>461</v>
       </c>
       <c r="D45" t="s">
-        <v>337</v>
+        <v>326</v>
       </c>
       <c r="E45">
         <v>2</v>
@@ -5259,16 +5138,16 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="B46" t="s">
-        <v>338</v>
+        <v>327</v>
       </c>
       <c r="C46" t="s">
-        <v>475</v>
+        <v>462</v>
       </c>
       <c r="D46" t="s">
-        <v>339</v>
+        <v>328</v>
       </c>
       <c r="E46">
         <v>0</v>
@@ -5279,23 +5158,23 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="B47" t="s">
-        <v>476</v>
+        <v>463</v>
       </c>
       <c r="C47" t="s">
-        <v>477</v>
+        <v>464</v>
       </c>
       <c r="D47" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="F47">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D45">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D45">
     <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5303,8 +5182,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5322,18 +5201,18 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>420</v>
+        <v>407</v>
       </c>
       <c r="C1" t="s">
-        <v>437</v>
+        <v>424</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -5341,10 +5220,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="C3">
         <v>0</v>

</xml_diff>

<commit_message>
added T846F to hip_ae_hailer
Fix #69
</commit_message>
<xml_diff>
--- a/data-raw/classcodes.xlsx
+++ b/data-raw/classcodes.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erik_\Documents\GitHub\coder\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\SHPR\Forskningsprojekt\Projekt 211-220\Projekt 217\coder\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581C680A-F71B-428E-910A-7FE0AD579675}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2712" yWindow="828" windowWidth="25284" windowHeight="23808" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2712" yWindow="828" windowWidth="25284" windowHeight="23808" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="charlson" sheetId="1" r:id="rId1"/>
@@ -1025,9 +1024,6 @@
     <t>Infection</t>
   </si>
   <si>
-    <t>(M(00(1|[0289]F?)|86([01]F|6F?)))|T(8(14|4(5[FX]?|7F?)))</t>
-  </si>
-  <si>
     <t>Dislocation</t>
   </si>
   <si>
@@ -1497,12 +1493,15 @@
   </si>
   <si>
     <t>regex_atc_garland</t>
+  </si>
+  <si>
+    <t>(M(00(1|[0289]F?)|86([01]F|6F?)))|T(8(14|4(5[FX]?|6F|7F?)))</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1568,7 +1567,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1845,7 +1844,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMO18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -1880,7 +1879,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>150</v>
@@ -1898,22 +1897,22 @@
         <v>137</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>405</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>406</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>407</v>
       </c>
       <c r="AMO1"/>
     </row>
@@ -2151,10 +2150,10 @@
         <v>153</v>
       </c>
       <c r="E7" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>144</v>
@@ -2198,7 +2197,7 @@
         <v>171</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>145</v>
@@ -2642,7 +2641,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2664,40 +2663,40 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="F1" t="s">
         <v>151</v>
       </c>
       <c r="G1" t="s">
+        <v>408</v>
+      </c>
+      <c r="H1" t="s">
         <v>409</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>410</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>411</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>412</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>413</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>414</v>
-      </c>
-      <c r="M1" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -2711,13 +2710,13 @@
         <v>243</v>
       </c>
       <c r="D2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -2752,10 +2751,10 @@
         <v>244</v>
       </c>
       <c r="D3" t="s">
+        <v>378</v>
+      </c>
+      <c r="F3" t="s">
         <v>379</v>
-      </c>
-      <c r="F3" t="s">
-        <v>380</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -2790,13 +2789,13 @@
         <v>245</v>
       </c>
       <c r="D4" t="s">
+        <v>359</v>
+      </c>
+      <c r="E4" t="s">
         <v>360</v>
       </c>
-      <c r="E4" t="s">
-        <v>361</v>
-      </c>
       <c r="F4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -2831,13 +2830,13 @@
         <v>207</v>
       </c>
       <c r="D5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -2872,13 +2871,13 @@
         <v>246</v>
       </c>
       <c r="D6" t="s">
+        <v>361</v>
+      </c>
+      <c r="E6" t="s">
         <v>362</v>
       </c>
-      <c r="E6" t="s">
-        <v>363</v>
-      </c>
       <c r="F6" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -2913,10 +2912,10 @@
         <v>208</v>
       </c>
       <c r="D7" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E7" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F7">
         <v>401</v>
@@ -2954,13 +2953,13 @@
         <v>209</v>
       </c>
       <c r="D8" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F8" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -2995,10 +2994,10 @@
         <v>210</v>
       </c>
       <c r="D9" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E9" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F9" t="s">
         <v>175</v>
@@ -3036,13 +3035,13 @@
         <v>247</v>
       </c>
       <c r="D10" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E10" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="F10" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -3077,13 +3076,13 @@
         <v>248</v>
       </c>
       <c r="D11" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E11" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F11" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -3118,13 +3117,13 @@
         <v>188</v>
       </c>
       <c r="D12" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E12" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F12" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -3159,13 +3158,13 @@
         <v>188</v>
       </c>
       <c r="D13" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E13" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="F13" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -3200,13 +3199,13 @@
         <v>214</v>
       </c>
       <c r="D14" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E14" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F14" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G14">
         <v>1</v>
@@ -3241,13 +3240,13 @@
         <v>249</v>
       </c>
       <c r="D15" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E15" t="s">
+        <v>465</v>
+      </c>
+      <c r="F15" t="s">
         <v>466</v>
-      </c>
-      <c r="F15" t="s">
-        <v>467</v>
       </c>
       <c r="G15">
         <v>1</v>
@@ -3282,13 +3281,13 @@
         <v>250</v>
       </c>
       <c r="D16" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E16" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="F16" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="G16">
         <v>1</v>
@@ -3323,13 +3322,13 @@
         <v>183</v>
       </c>
       <c r="D17" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E17" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F17" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G17">
         <v>1</v>
@@ -3405,13 +3404,13 @@
         <v>218</v>
       </c>
       <c r="D19" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E19" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F19" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="G19">
         <v>1</v>
@@ -3487,13 +3486,13 @@
         <v>219</v>
       </c>
       <c r="D21" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E21" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F21" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -3528,13 +3527,13 @@
         <v>251</v>
       </c>
       <c r="D22" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E22" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F22" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G22">
         <v>1</v>
@@ -3569,13 +3568,13 @@
         <v>221</v>
       </c>
       <c r="D23" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E23" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F23" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -3651,13 +3650,13 @@
         <v>252</v>
       </c>
       <c r="D25" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E25" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F25" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G25">
         <v>1</v>
@@ -3698,7 +3697,7 @@
         <v>276</v>
       </c>
       <c r="F26" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G26">
         <v>1</v>
@@ -3736,7 +3735,7 @@
         <v>2800</v>
       </c>
       <c r="E27" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F27">
         <v>2800</v>
@@ -3774,13 +3773,13 @@
         <v>228</v>
       </c>
       <c r="D28" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E28" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F28" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G28">
         <v>1</v>
@@ -3815,13 +3814,13 @@
         <v>253</v>
       </c>
       <c r="D29" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E29" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="F29" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="G29">
         <v>1</v>
@@ -3856,13 +3855,13 @@
         <v>254</v>
       </c>
       <c r="D30" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E30" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F30" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G30">
         <v>1</v>
@@ -3897,13 +3896,13 @@
         <v>230</v>
       </c>
       <c r="D31" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E31" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="F31" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G31">
         <v>1</v>
@@ -3938,16 +3937,16 @@
         <v>232</v>
       </c>
       <c r="D32" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E32" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F32" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G32" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H32">
         <v>1</v>
@@ -3975,7 +3974,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3995,7 +3994,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C1" t="s">
         <v>166</v>
@@ -4020,7 +4019,7 @@
         <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>69</v>
@@ -4042,7 +4041,7 @@
         <v>66</v>
       </c>
       <c r="B5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>69</v>
@@ -4053,7 +4052,7 @@
         <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>69</v>
@@ -4064,7 +4063,7 @@
         <v>68</v>
       </c>
       <c r="B7" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>70</v>
@@ -4075,7 +4074,7 @@
         <v>165</v>
       </c>
       <c r="C8" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D8" t="s">
         <v>71</v>
@@ -4087,11 +4086,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4107,7 +4106,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C1" t="s">
         <v>166</v>
@@ -4118,21 +4117,21 @@
         <v>330</v>
       </c>
       <c r="B2" t="s">
-        <v>331</v>
+        <v>488</v>
       </c>
       <c r="C2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>331</v>
+      </c>
+      <c r="B3" t="s">
         <v>332</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>333</v>
-      </c>
-      <c r="C3" t="s">
-        <v>334</v>
       </c>
     </row>
   </sheetData>
@@ -4141,7 +4140,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4161,7 +4160,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C1" t="s">
         <v>166</v>
@@ -4208,7 +4207,7 @@
         <v>66</v>
       </c>
       <c r="B5" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>69</v>
@@ -4219,7 +4218,7 @@
         <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>69</v>
@@ -4230,7 +4229,7 @@
         <v>68</v>
       </c>
       <c r="B7" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>70</v>
@@ -4253,10 +4252,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -4274,19 +4273,19 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>485</v>
+      </c>
+      <c r="C1" t="s">
         <v>486</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>487</v>
       </c>
-      <c r="D1" t="s">
-        <v>488</v>
-      </c>
       <c r="E1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -4294,7 +4293,7 @@
         <v>79</v>
       </c>
       <c r="B2" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C2" t="s">
         <v>260</v>
@@ -4314,10 +4313,10 @@
         <v>80</v>
       </c>
       <c r="B3" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D3" t="s">
         <v>262</v>
@@ -4334,10 +4333,10 @@
         <v>81</v>
       </c>
       <c r="B4" t="s">
+        <v>419</v>
+      </c>
+      <c r="C4" t="s">
         <v>420</v>
-      </c>
-      <c r="C4" t="s">
-        <v>421</v>
       </c>
       <c r="D4" t="s">
         <v>263</v>
@@ -4354,10 +4353,10 @@
         <v>82</v>
       </c>
       <c r="B5" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C5" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D5" t="s">
         <v>264</v>
@@ -4377,7 +4376,7 @@
         <v>265</v>
       </c>
       <c r="C6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D6" t="s">
         <v>266</v>
@@ -4394,10 +4393,10 @@
         <v>84</v>
       </c>
       <c r="B7" t="s">
+        <v>423</v>
+      </c>
+      <c r="C7" t="s">
         <v>424</v>
-      </c>
-      <c r="C7" t="s">
-        <v>425</v>
       </c>
       <c r="D7" t="s">
         <v>267</v>
@@ -4414,7 +4413,7 @@
         <v>85</v>
       </c>
       <c r="B8" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C8" t="s">
         <v>268</v>
@@ -4454,10 +4453,10 @@
         <v>87</v>
       </c>
       <c r="B10" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C10" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D10" t="s">
         <v>273</v>
@@ -4474,10 +4473,10 @@
         <v>88</v>
       </c>
       <c r="B11" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C11" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D11" t="s">
         <v>274</v>
@@ -4494,7 +4493,7 @@
         <v>89</v>
       </c>
       <c r="B12" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C12" t="s">
         <v>275</v>
@@ -4514,10 +4513,10 @@
         <v>90</v>
       </c>
       <c r="B13" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C13" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D13" t="s">
         <v>277</v>
@@ -4537,7 +4536,7 @@
         <v>278</v>
       </c>
       <c r="C14" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D14" t="s">
         <v>279</v>
@@ -4557,7 +4556,7 @@
         <v>280</v>
       </c>
       <c r="C15" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D15" t="s">
         <v>281</v>
@@ -4574,10 +4573,10 @@
         <v>94</v>
       </c>
       <c r="B16" t="s">
+        <v>431</v>
+      </c>
+      <c r="C16" t="s">
         <v>432</v>
-      </c>
-      <c r="C16" t="s">
-        <v>433</v>
       </c>
       <c r="D16" t="s">
         <v>282</v>
@@ -4594,10 +4593,10 @@
         <v>95</v>
       </c>
       <c r="B17" t="s">
+        <v>433</v>
+      </c>
+      <c r="C17" t="s">
         <v>434</v>
-      </c>
-      <c r="C17" t="s">
-        <v>435</v>
       </c>
       <c r="D17" t="s">
         <v>283</v>
@@ -4614,10 +4613,10 @@
         <v>96</v>
       </c>
       <c r="B18" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C18" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D18" t="s">
         <v>284</v>
@@ -4662,10 +4661,10 @@
         <v>75</v>
       </c>
       <c r="B21" t="s">
+        <v>436</v>
+      </c>
+      <c r="C21" t="s">
         <v>437</v>
-      </c>
-      <c r="C21" t="s">
-        <v>438</v>
       </c>
       <c r="D21" t="s">
         <v>288</v>
@@ -4702,10 +4701,10 @@
         <v>99</v>
       </c>
       <c r="B23" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C23" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D23" t="s">
         <v>290</v>
@@ -4722,10 +4721,10 @@
         <v>100</v>
       </c>
       <c r="B24" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C24" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D24" t="s">
         <v>291</v>
@@ -4776,7 +4775,7 @@
         <v>123</v>
       </c>
       <c r="B27" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -4790,10 +4789,10 @@
         <v>102</v>
       </c>
       <c r="B28" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C28" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D28" t="s">
         <v>294</v>
@@ -4830,10 +4829,10 @@
         <v>104</v>
       </c>
       <c r="B30" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C30" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D30" t="s">
         <v>297</v>
@@ -4890,10 +4889,10 @@
         <v>107</v>
       </c>
       <c r="B33" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C33" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D33" t="s">
         <v>303</v>
@@ -4930,10 +4929,10 @@
         <v>109</v>
       </c>
       <c r="B35" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C35" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D35" t="s">
         <v>307</v>
@@ -4950,10 +4949,10 @@
         <v>110</v>
       </c>
       <c r="B36" t="s">
+        <v>445</v>
+      </c>
+      <c r="C36" t="s">
         <v>446</v>
-      </c>
-      <c r="C36" t="s">
-        <v>447</v>
       </c>
       <c r="D36" t="s">
         <v>308</v>
@@ -4970,10 +4969,10 @@
         <v>111</v>
       </c>
       <c r="B37" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C37" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D37" t="s">
         <v>309</v>
@@ -5010,10 +5009,10 @@
         <v>113</v>
       </c>
       <c r="B39" t="s">
+        <v>448</v>
+      </c>
+      <c r="C39" t="s">
         <v>449</v>
-      </c>
-      <c r="C39" t="s">
-        <v>450</v>
       </c>
       <c r="D39" t="s">
         <v>311</v>
@@ -5030,7 +5029,7 @@
         <v>114</v>
       </c>
       <c r="B40" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C40" t="s">
         <v>312</v>
@@ -5050,10 +5049,10 @@
         <v>115</v>
       </c>
       <c r="B41" t="s">
+        <v>451</v>
+      </c>
+      <c r="C41" t="s">
         <v>452</v>
-      </c>
-      <c r="C41" t="s">
-        <v>453</v>
       </c>
       <c r="D41" t="s">
         <v>314</v>
@@ -5124,10 +5123,10 @@
         <v>117</v>
       </c>
       <c r="B45" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C45" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D45" t="s">
         <v>320</v>
@@ -5147,7 +5146,7 @@
         <v>321</v>
       </c>
       <c r="C46" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D46" t="s">
         <v>322</v>
@@ -5164,10 +5163,10 @@
         <v>119</v>
       </c>
       <c r="B47" t="s">
+        <v>455</v>
+      </c>
+      <c r="C47" t="s">
         <v>456</v>
-      </c>
-      <c r="C47" t="s">
-        <v>457</v>
       </c>
       <c r="D47" t="s">
         <v>323</v>
@@ -5177,7 +5176,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D45">
+  <sortState ref="A2:D45">
     <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5186,7 +5185,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5204,10 +5203,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added Swedish version of ICD 10
#148
</commit_message>
<xml_diff>
--- a/data-raw/classcodes.xlsx
+++ b/data-raw/classcodes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erik_\Documents\GitHub\coder\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xbuler/Documents/GitHub/coder/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C877AF-3BFC-4449-8FDE-F2890A0B217E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD508C7B-3429-2649-B55F-806C1149A770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5460" yWindow="5460" windowWidth="43200" windowHeight="23535" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="charlson" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="505">
   <si>
     <t>group</t>
   </si>
@@ -1497,13 +1497,61 @@
   </si>
   <si>
     <t>NF(S[0-59]|W[56])9</t>
+  </si>
+  <si>
+    <t>regex_icd10_swe</t>
+  </si>
+  <si>
+    <t>I((1(1[13]0|32))|255|42[06-9]|43|50)</t>
+  </si>
+  <si>
+    <t>(I7([01]|3[189]|71|9[02]))|K55</t>
+  </si>
+  <si>
+    <t>G45|I6[0-479]</t>
+  </si>
+  <si>
+    <t>F0([0-3]|51)|G3(0|1[19])</t>
+  </si>
+  <si>
+    <t>J(4[1-7]|6|70)</t>
+  </si>
+  <si>
+    <t>M(0([568]|7[0-3])|1(23|31)|3([02-4]|1[3-6]|5[013])|4[56])</t>
+  </si>
+  <si>
+    <t>B1[5-9]|K7(0[39]|3|46|54)</t>
+  </si>
+  <si>
+    <t>E1([0-4][01])</t>
+  </si>
+  <si>
+    <t>G(114|8([0-2]|3[[0-38]]))</t>
+  </si>
+  <si>
+    <t>I1(20|31)|N(0[35][2-7]|(1[189]|250))|Q61[1-4]|Z(49|940|992)</t>
+  </si>
+  <si>
+    <t>E1(0[2-57]|[1-4][2-7])</t>
+  </si>
+  <si>
+    <t>C([0-36]|4[0135-9]|5[0-8]|7[0-6]|8[1-689]|9[0-7])</t>
+  </si>
+  <si>
+    <t>I((85[09])|98[23])</t>
+  </si>
+  <si>
+    <t>C(7[789]|80)</t>
+  </si>
+  <si>
+    <t>B2[0-4]|F024|O987|R75|Z219|Z717</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1525,6 +1573,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1554,15 +1615,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1846,85 +1909,88 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMO18"/>
+  <dimension ref="A1:AMP18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" customWidth="1"/>
-    <col min="2" max="2" width="53.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="61.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="61.42578125" customWidth="1"/>
-    <col min="6" max="6" width="61.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="61.42578125" style="6" customWidth="1"/>
-    <col min="8" max="8" width="55.7109375" style="6" customWidth="1"/>
-    <col min="9" max="9" width="8.42578125" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" customWidth="1"/>
-    <col min="11" max="11" width="11" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" customWidth="1"/>
-    <col min="13" max="13" width="17.42578125" customWidth="1"/>
-    <col min="14" max="14" width="14.42578125" customWidth="1"/>
-    <col min="15" max="1030" width="8.42578125" customWidth="1"/>
+    <col min="1" max="1" width="37.5" customWidth="1"/>
+    <col min="2" max="2" width="53.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="61.5" style="5" customWidth="1"/>
+    <col min="6" max="6" width="61.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="61.5" style="6" customWidth="1"/>
+    <col min="9" max="9" width="55.6640625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="22.33203125" customWidth="1"/>
+    <col min="11" max="11" width="14.1640625" customWidth="1"/>
+    <col min="12" max="12" width="11" customWidth="1"/>
+    <col min="13" max="13" width="13.6640625" customWidth="1"/>
+    <col min="14" max="14" width="17.5" customWidth="1"/>
+    <col min="15" max="15" width="14.5" customWidth="1"/>
+    <col min="16" max="1031" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14 1029:1029" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15 1030:1030" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>400</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
+        <v>489</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>405</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="AMO1"/>
-    </row>
-    <row r="2" spans="1:14 1029:1029" x14ac:dyDescent="0.25">
+      <c r="AMP1"/>
+    </row>
+    <row r="2" spans="1:15 1030:1030" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="5" t="s">
         <v>179</v>
       </c>
       <c r="D2" s="6" t="s">
@@ -1937,14 +2003,14 @@
         <v>181</v>
       </c>
       <c r="G2" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
       <c r="J2">
         <v>1</v>
       </c>
@@ -1958,37 +2024,40 @@
         <v>1</v>
       </c>
       <c r="N2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14 1029:1029" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15 1030:1030" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="5" t="s">
         <v>193</v>
       </c>
       <c r="D3" s="6">
         <v>428</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="5" t="s">
         <v>167</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>180</v>
       </c>
       <c r="G3" s="6" t="s">
+        <v>490</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="I3" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
       <c r="J3">
         <v>1</v>
       </c>
@@ -1996,43 +2065,46 @@
         <v>1</v>
       </c>
       <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
         <v>4</v>
       </c>
-      <c r="M3">
-        <v>1</v>
-      </c>
       <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:14 1029:1029" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15 1030:1030" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="5" t="s">
         <v>194</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="5" t="s">
         <v>168</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>201</v>
       </c>
       <c r="G4" s="6" t="s">
+        <v>491</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="I4" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
       <c r="J4">
         <v>1</v>
       </c>
@@ -2040,43 +2112,46 @@
         <v>1</v>
       </c>
       <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
         <v>2</v>
       </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
       <c r="N4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14 1029:1029" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15 1030:1030" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="5" t="s">
         <v>195</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="5" t="s">
         <v>169</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>202</v>
       </c>
       <c r="G5" s="6" t="s">
+        <v>492</v>
+      </c>
+      <c r="H5" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="I5" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
       <c r="J5">
         <v>1</v>
       </c>
@@ -2090,37 +2165,40 @@
         <v>1</v>
       </c>
       <c r="N5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14 1029:1029" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15 1030:1030" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="5" t="s">
         <v>196</v>
       </c>
       <c r="D6" s="6">
         <v>290</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="5" t="s">
         <v>170</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>203</v>
       </c>
       <c r="G6" s="6" t="s">
+        <v>493</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="I6" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
       <c r="J6">
         <v>1</v>
       </c>
@@ -2128,43 +2206,46 @@
         <v>1</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:14 1029:1029" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15 1030:1030" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="5" t="s">
         <v>197</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="5" t="s">
         <v>458</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>461</v>
       </c>
       <c r="G7" s="6" t="s">
+        <v>494</v>
+      </c>
+      <c r="H7" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="I7" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
       <c r="J7">
         <v>1</v>
       </c>
@@ -2172,43 +2253,46 @@
         <v>1</v>
       </c>
       <c r="L7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:14 1029:1029" x14ac:dyDescent="0.25">
+      <c r="O7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15 1030:1030" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" t="s">
         <v>15</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="5" t="s">
         <v>182</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="5" t="s">
         <v>171</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>459</v>
       </c>
       <c r="G8" s="6" t="s">
+        <v>495</v>
+      </c>
+      <c r="H8" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="I8" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
       <c r="J8">
         <v>1</v>
       </c>
@@ -2216,33 +2300,36 @@
         <v>1</v>
       </c>
       <c r="L8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:14 1029:1029" x14ac:dyDescent="0.25">
+      <c r="O8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15 1030:1030" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" t="s">
         <v>17</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="5" t="s">
         <v>183</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="I9">
-        <v>1</v>
+      <c r="G9" s="6" t="s">
+        <v>183</v>
       </c>
       <c r="J9">
         <v>1</v>
@@ -2251,33 +2338,36 @@
         <v>1</v>
       </c>
       <c r="L9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14 1029:1029" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15 1030:1030" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" t="s">
         <v>19</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="5" t="s">
         <v>198</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="I10">
-        <v>1</v>
+      <c r="G10" s="6" t="s">
+        <v>496</v>
       </c>
       <c r="J10">
         <v>1</v>
@@ -2286,33 +2376,36 @@
         <v>1</v>
       </c>
       <c r="L10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:14 1029:1029" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15 1030:1030" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" t="s">
         <v>21</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="5" t="s">
         <v>184</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="I11">
-        <v>1</v>
+      <c r="G11" s="6" t="s">
+        <v>497</v>
       </c>
       <c r="J11">
         <v>1</v>
@@ -2321,317 +2414,341 @@
         <v>1</v>
       </c>
       <c r="L11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14 1029:1029" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15 1030:1030" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" t="s">
         <v>23</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="5" t="s">
         <v>185</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="5" t="s">
         <v>175</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="6" t="s">
+        <v>498</v>
+      </c>
+      <c r="H12" s="6">
         <v>344</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="I12" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>2</v>
       </c>
-      <c r="J12">
-        <v>1</v>
-      </c>
       <c r="K12">
         <v>1</v>
       </c>
       <c r="L12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N12">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:14 1029:1029" x14ac:dyDescent="0.25">
+      <c r="O12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15 1030:1030" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" t="s">
         <v>25</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="5" t="s">
         <v>199</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="5" t="s">
         <v>176</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>204</v>
       </c>
       <c r="G13" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="H13" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="I13" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>2</v>
       </c>
-      <c r="J13">
-        <v>1</v>
-      </c>
       <c r="K13">
         <v>1</v>
       </c>
       <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13">
         <v>3</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>2</v>
       </c>
-      <c r="N13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14 1029:1029" x14ac:dyDescent="0.25">
+      <c r="O13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15 1030:1030" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" t="s">
         <v>27</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="5" t="s">
         <v>187</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="5" t="s">
         <v>174</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="G14" s="6">
-        <v>250</v>
+      <c r="G14" s="6" t="s">
+        <v>500</v>
       </c>
       <c r="H14" s="6">
         <v>250</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="6">
+        <v>250</v>
+      </c>
+      <c r="J14">
         <v>2</v>
       </c>
-      <c r="J14">
-        <v>1</v>
-      </c>
       <c r="K14">
         <v>1</v>
       </c>
       <c r="L14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
         <v>2</v>
       </c>
-      <c r="N14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14 1029:1029" x14ac:dyDescent="0.25">
+      <c r="O14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15 1030:1030" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>78</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" t="s">
         <v>28</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="5" t="s">
         <v>189</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="5" t="s">
         <v>177</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>189</v>
       </c>
       <c r="G15" s="6" t="s">
+        <v>501</v>
+      </c>
+      <c r="H15" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="I15" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>2</v>
       </c>
-      <c r="J15">
-        <v>1</v>
-      </c>
       <c r="K15">
         <v>1</v>
       </c>
       <c r="L15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N15">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:14 1029:1029" ht="30" x14ac:dyDescent="0.25">
+      <c r="O15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15 1030:1030" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" t="s">
         <v>30</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="5" t="s">
         <v>200</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="5" t="s">
         <v>178</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>205</v>
       </c>
       <c r="G16" s="7" t="s">
+        <v>502</v>
+      </c>
+      <c r="H16" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="H16" s="7" t="s">
+      <c r="I16" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>3</v>
       </c>
-      <c r="J16">
-        <v>1</v>
-      </c>
       <c r="K16">
         <v>1</v>
       </c>
       <c r="L16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
         <v>3</v>
       </c>
-      <c r="N16">
+      <c r="O16">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" t="s">
         <v>32</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="5" t="s">
         <v>190</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="5" t="s">
         <v>135</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>190</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>135</v>
+        <v>503</v>
       </c>
       <c r="H17" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="J17">
         <v>6</v>
       </c>
-      <c r="J17">
-        <v>1</v>
-      </c>
       <c r="K17">
         <v>1</v>
       </c>
       <c r="L17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M17">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="N17">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" t="s">
         <v>34</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="5" t="s">
         <v>191</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="5" t="s">
         <v>164</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="H18" s="6" t="s">
+      <c r="G18" s="6" t="s">
+        <v>504</v>
+      </c>
+      <c r="I18" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <v>6</v>
       </c>
-      <c r="J18">
-        <v>1</v>
-      </c>
       <c r="K18">
         <v>1</v>
       </c>
       <c r="L18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
         <v>6</v>
       </c>
-      <c r="N18">
+      <c r="O18">
         <v>4</v>
       </c>
     </row>
@@ -2650,16 +2767,16 @@
       <selection pane="topRight" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="62.42578125" customWidth="1"/>
-    <col min="12" max="12" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="62.5" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2700,7 +2817,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2741,7 +2858,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -2779,7 +2896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -2820,7 +2937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -2861,7 +2978,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -2902,7 +3019,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -2943,7 +3060,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -2984,7 +3101,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -3025,7 +3142,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -3066,7 +3183,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -3107,7 +3224,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -3148,7 +3265,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -3189,7 +3306,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -3230,7 +3347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -3271,7 +3388,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>47</v>
       </c>
@@ -3312,7 +3429,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -3353,7 +3470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -3394,7 +3511,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -3435,7 +3552,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -3476,7 +3593,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>50</v>
       </c>
@@ -3517,7 +3634,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -3558,7 +3675,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>52</v>
       </c>
@@ -3599,7 +3716,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>53</v>
       </c>
@@ -3640,7 +3757,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>54</v>
       </c>
@@ -3681,7 +3798,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>55</v>
       </c>
@@ -3722,7 +3839,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>56</v>
       </c>
@@ -3763,7 +3880,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>57</v>
       </c>
@@ -3804,7 +3921,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>58</v>
       </c>
@@ -3845,7 +3962,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>59</v>
       </c>
@@ -3886,7 +4003,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>60</v>
       </c>
@@ -3927,7 +4044,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>61</v>
       </c>
@@ -3982,15 +4099,15 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.5703125" customWidth="1"/>
-    <col min="3" max="3" width="38.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.5" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4004,7 +4121,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>63</v>
       </c>
@@ -4015,7 +4132,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>64</v>
       </c>
@@ -4026,7 +4143,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>65</v>
       </c>
@@ -4037,7 +4154,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>66</v>
       </c>
@@ -4048,7 +4165,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>67</v>
       </c>
@@ -4059,7 +4176,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>68</v>
       </c>
@@ -4070,7 +4187,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>165</v>
       </c>
@@ -4090,19 +4207,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4113,7 +4230,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>330</v>
       </c>
@@ -4124,7 +4241,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>331</v>
       </c>
@@ -4148,15 +4265,15 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="61.7109375" customWidth="1"/>
-    <col min="3" max="3" width="33.28515625" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.6640625" customWidth="1"/>
+    <col min="3" max="3" width="33.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4170,7 +4287,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>63</v>
       </c>
@@ -4181,7 +4298,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>73</v>
       </c>
@@ -4192,7 +4309,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>74</v>
       </c>
@@ -4203,7 +4320,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>66</v>
       </c>
@@ -4214,7 +4331,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>67</v>
       </c>
@@ -4225,7 +4342,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>68</v>
       </c>
@@ -4236,7 +4353,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>165</v>
       </c>
@@ -4260,16 +4377,16 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="33.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="144.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="144.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4289,7 +4406,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>79</v>
       </c>
@@ -4309,7 +4426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>80</v>
       </c>
@@ -4329,7 +4446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>81</v>
       </c>
@@ -4349,7 +4466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>82</v>
       </c>
@@ -4369,7 +4486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>83</v>
       </c>
@@ -4389,7 +4506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>84</v>
       </c>
@@ -4409,7 +4526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>85</v>
       </c>
@@ -4429,7 +4546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>86</v>
       </c>
@@ -4449,7 +4566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>87</v>
       </c>
@@ -4469,7 +4586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>88</v>
       </c>
@@ -4489,7 +4606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>89</v>
       </c>
@@ -4509,7 +4626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>90</v>
       </c>
@@ -4529,7 +4646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>91</v>
       </c>
@@ -4549,7 +4666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>93</v>
       </c>
@@ -4569,7 +4686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>94</v>
       </c>
@@ -4589,7 +4706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>95</v>
       </c>
@@ -4609,7 +4726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>96</v>
       </c>
@@ -4629,7 +4746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>120</v>
       </c>
@@ -4640,7 +4757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>97</v>
       </c>
@@ -4657,7 +4774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>75</v>
       </c>
@@ -4677,7 +4794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>98</v>
       </c>
@@ -4697,7 +4814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>99</v>
       </c>
@@ -4717,7 +4834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>100</v>
       </c>
@@ -4737,7 +4854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>101</v>
       </c>
@@ -4757,7 +4874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>122</v>
       </c>
@@ -4771,7 +4888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>123</v>
       </c>
@@ -4785,7 +4902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>102</v>
       </c>
@@ -4805,7 +4922,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>103</v>
       </c>
@@ -4825,7 +4942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>104</v>
       </c>
@@ -4845,7 +4962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>105</v>
       </c>
@@ -4865,7 +4982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>106</v>
       </c>
@@ -4885,7 +5002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>107</v>
       </c>
@@ -4905,7 +5022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>108</v>
       </c>
@@ -4925,7 +5042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>109</v>
       </c>
@@ -4945,7 +5062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>110</v>
       </c>
@@ -4965,7 +5082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>111</v>
       </c>
@@ -4985,7 +5102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>112</v>
       </c>
@@ -5005,7 +5122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>113</v>
       </c>
@@ -5025,7 +5142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>114</v>
       </c>
@@ -5045,7 +5162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>115</v>
       </c>
@@ -5065,7 +5182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>121</v>
       </c>
@@ -5079,7 +5196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>92</v>
       </c>
@@ -5099,7 +5216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>116</v>
       </c>
@@ -5119,7 +5236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>117</v>
       </c>
@@ -5139,7 +5256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>118</v>
       </c>
@@ -5159,7 +5276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>119</v>
       </c>
@@ -5193,13 +5310,13 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="39.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5210,7 +5327,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>76</v>
       </c>
@@ -5221,7 +5338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>77</v>
       </c>

</xml_diff>